<commit_message>
Updated the ROSC frequency for EBG from 120 -> 240 Mhz
[git-p4: depot-paths = "//depot/projects/coe/CSME/": change = 758435]
</commit_message>
<xml_diff>
--- a/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
+++ b/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="10000" windowHeight="4670" activeTab="1"/>
+    <workbookView xWindow="1170" yWindow="105" windowWidth="10005" windowHeight="4665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="2" r:id="rId1"/>
     <sheet name="CSE CSME IE OCS Features" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateCount="5"/>
 </workbook>
 </file>
 
@@ -6768,6 +6768,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -6884,12 +6890,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7210,17 +7210,17 @@
       <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.36328125" style="26" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="221" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="78.7265625" style="284" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="26"/>
+    <col min="1" max="1" width="3.42578125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="221" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="26" customWidth="1"/>
+    <col min="5" max="5" width="78.7109375" style="284" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="26"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="219" t="s">
         <v>321</v>
       </c>
@@ -7234,7 +7234,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="220">
         <v>1</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B4" s="220">
         <v>2</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="220">
         <v>3</v>
       </c>
@@ -7276,7 +7276,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="220">
         <v>4</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="220">
         <v>5</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="220">
         <v>6</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="220">
         <v>7</v>
       </c>
@@ -7332,7 +7332,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="220">
         <v>8</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="220">
         <v>9</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="220">
         <v>10</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="220">
         <v>11</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="220">
         <v>12</v>
       </c>
@@ -7402,7 +7402,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="220">
         <v>13</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="220">
         <v>14</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="220">
         <v>15</v>
       </c>
@@ -7444,7 +7444,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="220">
         <v>16</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="220">
         <v>17</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="220">
         <v>18</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="220">
         <v>19</v>
       </c>
@@ -7500,7 +7500,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="220">
         <v>20</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="220">
         <v>21</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B24" s="220">
         <v>22</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="220">
         <v>23</v>
       </c>
@@ -7556,7 +7556,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="220">
         <v>24</v>
       </c>
@@ -7570,7 +7570,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="220">
         <v>25</v>
       </c>
@@ -7584,7 +7584,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" s="220">
         <v>26</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="220">
         <v>27</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B30" s="220">
         <v>28</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="220">
         <v>29</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="220">
         <v>30</v>
       </c>
@@ -7654,7 +7654,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="220">
         <v>31</v>
       </c>
@@ -7668,7 +7668,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="220">
         <v>32</v>
       </c>
@@ -7682,7 +7682,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="220">
         <v>33</v>
       </c>
@@ -7696,7 +7696,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="220">
         <v>34</v>
       </c>
@@ -7710,7 +7710,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="220">
         <v>35</v>
       </c>
@@ -7724,7 +7724,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="220">
         <v>36</v>
       </c>
@@ -7738,7 +7738,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="220">
         <v>37</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="220">
         <v>28</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="220">
         <v>29</v>
       </c>
@@ -7780,7 +7780,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="220">
         <v>30</v>
       </c>
@@ -7794,7 +7794,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="220">
         <v>31</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="220">
         <v>32</v>
       </c>
@@ -7822,7 +7822,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="220">
         <v>33</v>
       </c>
@@ -7836,7 +7836,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="220">
         <v>34</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="220">
         <v>35</v>
       </c>
@@ -7864,25 +7864,25 @@
         <v>396</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="220"/>
       <c r="C48" s="9"/>
       <c r="D48" s="10"/>
       <c r="E48" s="4"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="220"/>
       <c r="C49" s="9"/>
       <c r="D49" s="10"/>
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="220"/>
       <c r="C50" s="9"/>
       <c r="D50" s="10"/>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="220"/>
       <c r="C51" s="9"/>
       <c r="D51" s="10"/>
@@ -7900,67 +7900,67 @@
   <dimension ref="A1:AD175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="X32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AC123" sqref="AC123"/>
+      <selection pane="bottomRight" activeCell="AA38" sqref="AA38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.08984375" style="250" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="250" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="12" customWidth="1"/>
-    <col min="3" max="3" width="43.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="10.453125" style="17" customWidth="1"/>
-    <col min="11" max="14" width="10.453125" style="27" customWidth="1"/>
-    <col min="15" max="18" width="10.453125" style="17" customWidth="1"/>
-    <col min="19" max="19" width="10.453125" style="251" customWidth="1"/>
-    <col min="20" max="28" width="10.453125" style="17" customWidth="1"/>
-    <col min="29" max="29" width="9.7265625" style="17" customWidth="1"/>
-    <col min="30" max="30" width="32.90625" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="43.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="10.42578125" style="17" customWidth="1"/>
+    <col min="11" max="14" width="10.42578125" style="27" customWidth="1"/>
+    <col min="15" max="18" width="10.42578125" style="17" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" style="251" customWidth="1"/>
+    <col min="20" max="28" width="10.42578125" style="17" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" style="17" customWidth="1"/>
+    <col min="30" max="30" width="32.85546875" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="230"/>
       <c r="C1" s="307" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="323" t="s">
+    <row r="2" spans="1:30" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="325" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="319" t="s">
+      <c r="C2" s="321" t="s">
         <v>280</v>
       </c>
-      <c r="D2" s="320"/>
-      <c r="E2" s="345" t="s">
+      <c r="D2" s="322"/>
+      <c r="E2" s="347" t="s">
         <v>241</v>
       </c>
-      <c r="F2" s="346"/>
-      <c r="G2" s="346"/>
-      <c r="H2" s="346"/>
-      <c r="I2" s="346"/>
-      <c r="J2" s="347"/>
-      <c r="K2" s="326" t="s">
+      <c r="F2" s="348"/>
+      <c r="G2" s="348"/>
+      <c r="H2" s="348"/>
+      <c r="I2" s="348"/>
+      <c r="J2" s="349"/>
+      <c r="K2" s="328" t="s">
         <v>315</v>
       </c>
-      <c r="L2" s="327"/>
-      <c r="M2" s="328" t="s">
+      <c r="L2" s="329"/>
+      <c r="M2" s="330" t="s">
         <v>316</v>
       </c>
-      <c r="N2" s="329"/>
-      <c r="O2" s="332" t="s">
+      <c r="N2" s="331"/>
+      <c r="O2" s="334" t="s">
         <v>317</v>
       </c>
-      <c r="P2" s="330"/>
-      <c r="Q2" s="333"/>
-      <c r="R2" s="330" t="s">
+      <c r="P2" s="332"/>
+      <c r="Q2" s="335"/>
+      <c r="R2" s="332" t="s">
         <v>160</v>
       </c>
-      <c r="S2" s="331"/>
+      <c r="S2" s="333"/>
       <c r="T2" s="190" t="s">
         <v>102</v>
       </c>
@@ -7991,16 +7991,16 @@
       <c r="AC2" s="242" t="s">
         <v>391</v>
       </c>
-      <c r="AD2" s="315" t="s">
+      <c r="AD2" s="317" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="324"/>
-      <c r="C3" s="321" t="s">
+    <row r="3" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="326"/>
+      <c r="C3" s="323" t="s">
         <v>281</v>
       </c>
-      <c r="D3" s="322"/>
+      <c r="D3" s="324"/>
       <c r="E3" s="247" t="s">
         <v>237</v>
       </c>
@@ -8076,10 +8076,10 @@
       <c r="AC3" s="214" t="s">
         <v>333</v>
       </c>
-      <c r="AD3" s="316"/>
-    </row>
-    <row r="4" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="325"/>
+      <c r="AD3" s="318"/>
+    </row>
+    <row r="4" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="327"/>
       <c r="C4" s="244" t="s">
         <v>0</v>
       </c>
@@ -8161,10 +8161,10 @@
       <c r="AC4" s="215" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="317"/>
-    </row>
-    <row r="5" spans="1:30" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="318"/>
+      <c r="AD4" s="319"/>
+    </row>
+    <row r="5" spans="1:30" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="320"/>
       <c r="B5" s="297" t="s">
         <v>312</v>
       </c>
@@ -8174,39 +8174,39 @@
       <c r="D5" s="299" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="348" t="s">
+      <c r="E5" s="350" t="s">
         <v>355</v>
       </c>
-      <c r="F5" s="337"/>
-      <c r="G5" s="337"/>
-      <c r="H5" s="337"/>
-      <c r="I5" s="337"/>
-      <c r="J5" s="349"/>
-      <c r="K5" s="336" t="s">
+      <c r="F5" s="339"/>
+      <c r="G5" s="339"/>
+      <c r="H5" s="339"/>
+      <c r="I5" s="339"/>
+      <c r="J5" s="351"/>
+      <c r="K5" s="338" t="s">
         <v>357</v>
       </c>
-      <c r="L5" s="337"/>
-      <c r="M5" s="337"/>
-      <c r="N5" s="337"/>
-      <c r="O5" s="337"/>
-      <c r="P5" s="337"/>
-      <c r="Q5" s="337"/>
-      <c r="R5" s="337"/>
-      <c r="S5" s="337"/>
-      <c r="T5" s="337"/>
-      <c r="U5" s="337"/>
-      <c r="V5" s="337"/>
-      <c r="W5" s="337"/>
-      <c r="X5" s="337"/>
-      <c r="Y5" s="337"/>
-      <c r="Z5" s="337"/>
-      <c r="AA5" s="337"/>
-      <c r="AB5" s="337"/>
-      <c r="AC5" s="338"/>
+      <c r="L5" s="339"/>
+      <c r="M5" s="339"/>
+      <c r="N5" s="339"/>
+      <c r="O5" s="339"/>
+      <c r="P5" s="339"/>
+      <c r="Q5" s="339"/>
+      <c r="R5" s="339"/>
+      <c r="S5" s="339"/>
+      <c r="T5" s="339"/>
+      <c r="U5" s="339"/>
+      <c r="V5" s="339"/>
+      <c r="W5" s="339"/>
+      <c r="X5" s="339"/>
+      <c r="Y5" s="339"/>
+      <c r="Z5" s="339"/>
+      <c r="AA5" s="339"/>
+      <c r="AB5" s="339"/>
+      <c r="AC5" s="340"/>
       <c r="AD5" s="245"/>
     </row>
-    <row r="6" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="318"/>
+    <row r="6" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="320"/>
       <c r="B6" s="300"/>
       <c r="C6" s="301" t="s">
         <v>9</v>
@@ -8214,35 +8214,35 @@
       <c r="D6" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="350"/>
-      <c r="F6" s="340"/>
-      <c r="G6" s="340"/>
-      <c r="H6" s="340"/>
-      <c r="I6" s="340"/>
-      <c r="J6" s="351"/>
-      <c r="K6" s="339"/>
-      <c r="L6" s="340"/>
-      <c r="M6" s="340"/>
-      <c r="N6" s="340"/>
-      <c r="O6" s="340"/>
-      <c r="P6" s="340"/>
-      <c r="Q6" s="340"/>
-      <c r="R6" s="340"/>
-      <c r="S6" s="340"/>
-      <c r="T6" s="340"/>
-      <c r="U6" s="340"/>
-      <c r="V6" s="340"/>
-      <c r="W6" s="340"/>
-      <c r="X6" s="340"/>
-      <c r="Y6" s="340"/>
-      <c r="Z6" s="340"/>
-      <c r="AA6" s="340"/>
-      <c r="AB6" s="340"/>
-      <c r="AC6" s="341"/>
+      <c r="E6" s="352"/>
+      <c r="F6" s="342"/>
+      <c r="G6" s="342"/>
+      <c r="H6" s="342"/>
+      <c r="I6" s="342"/>
+      <c r="J6" s="353"/>
+      <c r="K6" s="341"/>
+      <c r="L6" s="342"/>
+      <c r="M6" s="342"/>
+      <c r="N6" s="342"/>
+      <c r="O6" s="342"/>
+      <c r="P6" s="342"/>
+      <c r="Q6" s="342"/>
+      <c r="R6" s="342"/>
+      <c r="S6" s="342"/>
+      <c r="T6" s="342"/>
+      <c r="U6" s="342"/>
+      <c r="V6" s="342"/>
+      <c r="W6" s="342"/>
+      <c r="X6" s="342"/>
+      <c r="Y6" s="342"/>
+      <c r="Z6" s="342"/>
+      <c r="AA6" s="342"/>
+      <c r="AB6" s="342"/>
+      <c r="AC6" s="343"/>
       <c r="AD6" s="246"/>
     </row>
-    <row r="7" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="318"/>
+    <row r="7" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="320"/>
       <c r="B7" s="300"/>
       <c r="C7" s="301" t="s">
         <v>12</v>
@@ -8250,35 +8250,35 @@
       <c r="D7" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="350"/>
-      <c r="F7" s="340"/>
-      <c r="G7" s="340"/>
-      <c r="H7" s="340"/>
-      <c r="I7" s="340"/>
-      <c r="J7" s="351"/>
-      <c r="K7" s="339"/>
-      <c r="L7" s="340"/>
-      <c r="M7" s="340"/>
-      <c r="N7" s="340"/>
-      <c r="O7" s="340"/>
-      <c r="P7" s="340"/>
-      <c r="Q7" s="340"/>
-      <c r="R7" s="340"/>
-      <c r="S7" s="340"/>
-      <c r="T7" s="340"/>
-      <c r="U7" s="340"/>
-      <c r="V7" s="340"/>
-      <c r="W7" s="340"/>
-      <c r="X7" s="340"/>
-      <c r="Y7" s="340"/>
-      <c r="Z7" s="340"/>
-      <c r="AA7" s="340"/>
-      <c r="AB7" s="340"/>
-      <c r="AC7" s="341"/>
+      <c r="E7" s="352"/>
+      <c r="F7" s="342"/>
+      <c r="G7" s="342"/>
+      <c r="H7" s="342"/>
+      <c r="I7" s="342"/>
+      <c r="J7" s="353"/>
+      <c r="K7" s="341"/>
+      <c r="L7" s="342"/>
+      <c r="M7" s="342"/>
+      <c r="N7" s="342"/>
+      <c r="O7" s="342"/>
+      <c r="P7" s="342"/>
+      <c r="Q7" s="342"/>
+      <c r="R7" s="342"/>
+      <c r="S7" s="342"/>
+      <c r="T7" s="342"/>
+      <c r="U7" s="342"/>
+      <c r="V7" s="342"/>
+      <c r="W7" s="342"/>
+      <c r="X7" s="342"/>
+      <c r="Y7" s="342"/>
+      <c r="Z7" s="342"/>
+      <c r="AA7" s="342"/>
+      <c r="AB7" s="342"/>
+      <c r="AC7" s="343"/>
       <c r="AD7" s="246"/>
     </row>
-    <row r="8" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="318"/>
+    <row r="8" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="320"/>
       <c r="B8" s="300"/>
       <c r="C8" s="301" t="s">
         <v>13</v>
@@ -8286,35 +8286,35 @@
       <c r="D8" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="350"/>
-      <c r="F8" s="340"/>
-      <c r="G8" s="340"/>
-      <c r="H8" s="340"/>
-      <c r="I8" s="340"/>
-      <c r="J8" s="351"/>
-      <c r="K8" s="339"/>
-      <c r="L8" s="340"/>
-      <c r="M8" s="340"/>
-      <c r="N8" s="340"/>
-      <c r="O8" s="340"/>
-      <c r="P8" s="340"/>
-      <c r="Q8" s="340"/>
-      <c r="R8" s="340"/>
-      <c r="S8" s="340"/>
-      <c r="T8" s="340"/>
-      <c r="U8" s="340"/>
-      <c r="V8" s="340"/>
-      <c r="W8" s="340"/>
-      <c r="X8" s="340"/>
-      <c r="Y8" s="340"/>
-      <c r="Z8" s="340"/>
-      <c r="AA8" s="340"/>
-      <c r="AB8" s="340"/>
-      <c r="AC8" s="341"/>
+      <c r="E8" s="352"/>
+      <c r="F8" s="342"/>
+      <c r="G8" s="342"/>
+      <c r="H8" s="342"/>
+      <c r="I8" s="342"/>
+      <c r="J8" s="353"/>
+      <c r="K8" s="341"/>
+      <c r="L8" s="342"/>
+      <c r="M8" s="342"/>
+      <c r="N8" s="342"/>
+      <c r="O8" s="342"/>
+      <c r="P8" s="342"/>
+      <c r="Q8" s="342"/>
+      <c r="R8" s="342"/>
+      <c r="S8" s="342"/>
+      <c r="T8" s="342"/>
+      <c r="U8" s="342"/>
+      <c r="V8" s="342"/>
+      <c r="W8" s="342"/>
+      <c r="X8" s="342"/>
+      <c r="Y8" s="342"/>
+      <c r="Z8" s="342"/>
+      <c r="AA8" s="342"/>
+      <c r="AB8" s="342"/>
+      <c r="AC8" s="343"/>
       <c r="AD8" s="246"/>
     </row>
-    <row r="9" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="318"/>
+    <row r="9" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="320"/>
       <c r="B9" s="300"/>
       <c r="C9" s="301" t="s">
         <v>341</v>
@@ -8322,35 +8322,35 @@
       <c r="D9" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="350"/>
-      <c r="F9" s="340"/>
-      <c r="G9" s="340"/>
-      <c r="H9" s="340"/>
-      <c r="I9" s="340"/>
-      <c r="J9" s="351"/>
-      <c r="K9" s="339"/>
-      <c r="L9" s="340"/>
-      <c r="M9" s="340"/>
-      <c r="N9" s="340"/>
-      <c r="O9" s="340"/>
-      <c r="P9" s="340"/>
-      <c r="Q9" s="340"/>
-      <c r="R9" s="340"/>
-      <c r="S9" s="340"/>
-      <c r="T9" s="340"/>
-      <c r="U9" s="340"/>
-      <c r="V9" s="340"/>
-      <c r="W9" s="340"/>
-      <c r="X9" s="340"/>
-      <c r="Y9" s="340"/>
-      <c r="Z9" s="340"/>
-      <c r="AA9" s="340"/>
-      <c r="AB9" s="340"/>
-      <c r="AC9" s="341"/>
+      <c r="E9" s="352"/>
+      <c r="F9" s="342"/>
+      <c r="G9" s="342"/>
+      <c r="H9" s="342"/>
+      <c r="I9" s="342"/>
+      <c r="J9" s="353"/>
+      <c r="K9" s="341"/>
+      <c r="L9" s="342"/>
+      <c r="M9" s="342"/>
+      <c r="N9" s="342"/>
+      <c r="O9" s="342"/>
+      <c r="P9" s="342"/>
+      <c r="Q9" s="342"/>
+      <c r="R9" s="342"/>
+      <c r="S9" s="342"/>
+      <c r="T9" s="342"/>
+      <c r="U9" s="342"/>
+      <c r="V9" s="342"/>
+      <c r="W9" s="342"/>
+      <c r="X9" s="342"/>
+      <c r="Y9" s="342"/>
+      <c r="Z9" s="342"/>
+      <c r="AA9" s="342"/>
+      <c r="AB9" s="342"/>
+      <c r="AC9" s="343"/>
       <c r="AD9" s="246"/>
     </row>
-    <row r="10" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="318"/>
+    <row r="10" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="320"/>
       <c r="B10" s="300"/>
       <c r="C10" s="301" t="s">
         <v>183</v>
@@ -8358,35 +8358,35 @@
       <c r="D10" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="350"/>
-      <c r="F10" s="340"/>
-      <c r="G10" s="340"/>
-      <c r="H10" s="340"/>
-      <c r="I10" s="340"/>
-      <c r="J10" s="351"/>
-      <c r="K10" s="339"/>
-      <c r="L10" s="340"/>
-      <c r="M10" s="340"/>
-      <c r="N10" s="340"/>
-      <c r="O10" s="340"/>
-      <c r="P10" s="340"/>
-      <c r="Q10" s="340"/>
-      <c r="R10" s="340"/>
-      <c r="S10" s="340"/>
-      <c r="T10" s="340"/>
-      <c r="U10" s="340"/>
-      <c r="V10" s="340"/>
-      <c r="W10" s="340"/>
-      <c r="X10" s="340"/>
-      <c r="Y10" s="340"/>
-      <c r="Z10" s="340"/>
-      <c r="AA10" s="340"/>
-      <c r="AB10" s="340"/>
-      <c r="AC10" s="341"/>
+      <c r="E10" s="352"/>
+      <c r="F10" s="342"/>
+      <c r="G10" s="342"/>
+      <c r="H10" s="342"/>
+      <c r="I10" s="342"/>
+      <c r="J10" s="353"/>
+      <c r="K10" s="341"/>
+      <c r="L10" s="342"/>
+      <c r="M10" s="342"/>
+      <c r="N10" s="342"/>
+      <c r="O10" s="342"/>
+      <c r="P10" s="342"/>
+      <c r="Q10" s="342"/>
+      <c r="R10" s="342"/>
+      <c r="S10" s="342"/>
+      <c r="T10" s="342"/>
+      <c r="U10" s="342"/>
+      <c r="V10" s="342"/>
+      <c r="W10" s="342"/>
+      <c r="X10" s="342"/>
+      <c r="Y10" s="342"/>
+      <c r="Z10" s="342"/>
+      <c r="AA10" s="342"/>
+      <c r="AB10" s="342"/>
+      <c r="AC10" s="343"/>
       <c r="AD10" s="246"/>
     </row>
-    <row r="11" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="318"/>
+    <row r="11" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="320"/>
       <c r="B11" s="300"/>
       <c r="C11" s="301" t="s">
         <v>17</v>
@@ -8394,35 +8394,35 @@
       <c r="D11" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="350"/>
-      <c r="F11" s="340"/>
-      <c r="G11" s="340"/>
-      <c r="H11" s="340"/>
-      <c r="I11" s="340"/>
-      <c r="J11" s="351"/>
-      <c r="K11" s="339"/>
-      <c r="L11" s="340"/>
-      <c r="M11" s="340"/>
-      <c r="N11" s="340"/>
-      <c r="O11" s="340"/>
-      <c r="P11" s="340"/>
-      <c r="Q11" s="340"/>
-      <c r="R11" s="340"/>
-      <c r="S11" s="340"/>
-      <c r="T11" s="340"/>
-      <c r="U11" s="340"/>
-      <c r="V11" s="340"/>
-      <c r="W11" s="340"/>
-      <c r="X11" s="340"/>
-      <c r="Y11" s="340"/>
-      <c r="Z11" s="340"/>
-      <c r="AA11" s="340"/>
-      <c r="AB11" s="340"/>
-      <c r="AC11" s="341"/>
+      <c r="E11" s="352"/>
+      <c r="F11" s="342"/>
+      <c r="G11" s="342"/>
+      <c r="H11" s="342"/>
+      <c r="I11" s="342"/>
+      <c r="J11" s="353"/>
+      <c r="K11" s="341"/>
+      <c r="L11" s="342"/>
+      <c r="M11" s="342"/>
+      <c r="N11" s="342"/>
+      <c r="O11" s="342"/>
+      <c r="P11" s="342"/>
+      <c r="Q11" s="342"/>
+      <c r="R11" s="342"/>
+      <c r="S11" s="342"/>
+      <c r="T11" s="342"/>
+      <c r="U11" s="342"/>
+      <c r="V11" s="342"/>
+      <c r="W11" s="342"/>
+      <c r="X11" s="342"/>
+      <c r="Y11" s="342"/>
+      <c r="Z11" s="342"/>
+      <c r="AA11" s="342"/>
+      <c r="AB11" s="342"/>
+      <c r="AC11" s="343"/>
       <c r="AD11" s="246"/>
     </row>
-    <row r="12" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="318"/>
+    <row r="12" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="320"/>
       <c r="B12" s="300"/>
       <c r="C12" s="301" t="s">
         <v>18</v>
@@ -8430,35 +8430,35 @@
       <c r="D12" s="303" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="350"/>
-      <c r="F12" s="340"/>
-      <c r="G12" s="340"/>
-      <c r="H12" s="340"/>
-      <c r="I12" s="340"/>
-      <c r="J12" s="351"/>
-      <c r="K12" s="339"/>
-      <c r="L12" s="340"/>
-      <c r="M12" s="340"/>
-      <c r="N12" s="340"/>
-      <c r="O12" s="340"/>
-      <c r="P12" s="340"/>
-      <c r="Q12" s="340"/>
-      <c r="R12" s="340"/>
-      <c r="S12" s="340"/>
-      <c r="T12" s="340"/>
-      <c r="U12" s="340"/>
-      <c r="V12" s="340"/>
-      <c r="W12" s="340"/>
-      <c r="X12" s="340"/>
-      <c r="Y12" s="340"/>
-      <c r="Z12" s="340"/>
-      <c r="AA12" s="340"/>
-      <c r="AB12" s="340"/>
-      <c r="AC12" s="341"/>
+      <c r="E12" s="352"/>
+      <c r="F12" s="342"/>
+      <c r="G12" s="342"/>
+      <c r="H12" s="342"/>
+      <c r="I12" s="342"/>
+      <c r="J12" s="353"/>
+      <c r="K12" s="341"/>
+      <c r="L12" s="342"/>
+      <c r="M12" s="342"/>
+      <c r="N12" s="342"/>
+      <c r="O12" s="342"/>
+      <c r="P12" s="342"/>
+      <c r="Q12" s="342"/>
+      <c r="R12" s="342"/>
+      <c r="S12" s="342"/>
+      <c r="T12" s="342"/>
+      <c r="U12" s="342"/>
+      <c r="V12" s="342"/>
+      <c r="W12" s="342"/>
+      <c r="X12" s="342"/>
+      <c r="Y12" s="342"/>
+      <c r="Z12" s="342"/>
+      <c r="AA12" s="342"/>
+      <c r="AB12" s="342"/>
+      <c r="AC12" s="343"/>
       <c r="AD12" s="246"/>
     </row>
-    <row r="13" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="318"/>
+    <row r="13" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="320"/>
       <c r="B13" s="300"/>
       <c r="C13" s="301" t="s">
         <v>20</v>
@@ -8466,35 +8466,35 @@
       <c r="D13" s="303">
         <v>32</v>
       </c>
-      <c r="E13" s="350"/>
-      <c r="F13" s="340"/>
-      <c r="G13" s="340"/>
-      <c r="H13" s="340"/>
-      <c r="I13" s="340"/>
-      <c r="J13" s="351"/>
-      <c r="K13" s="339"/>
-      <c r="L13" s="340"/>
-      <c r="M13" s="340"/>
-      <c r="N13" s="340"/>
-      <c r="O13" s="340"/>
-      <c r="P13" s="340"/>
-      <c r="Q13" s="340"/>
-      <c r="R13" s="340"/>
-      <c r="S13" s="340"/>
-      <c r="T13" s="340"/>
-      <c r="U13" s="340"/>
-      <c r="V13" s="340"/>
-      <c r="W13" s="340"/>
-      <c r="X13" s="340"/>
-      <c r="Y13" s="340"/>
-      <c r="Z13" s="340"/>
-      <c r="AA13" s="340"/>
-      <c r="AB13" s="340"/>
-      <c r="AC13" s="341"/>
+      <c r="E13" s="352"/>
+      <c r="F13" s="342"/>
+      <c r="G13" s="342"/>
+      <c r="H13" s="342"/>
+      <c r="I13" s="342"/>
+      <c r="J13" s="353"/>
+      <c r="K13" s="341"/>
+      <c r="L13" s="342"/>
+      <c r="M13" s="342"/>
+      <c r="N13" s="342"/>
+      <c r="O13" s="342"/>
+      <c r="P13" s="342"/>
+      <c r="Q13" s="342"/>
+      <c r="R13" s="342"/>
+      <c r="S13" s="342"/>
+      <c r="T13" s="342"/>
+      <c r="U13" s="342"/>
+      <c r="V13" s="342"/>
+      <c r="W13" s="342"/>
+      <c r="X13" s="342"/>
+      <c r="Y13" s="342"/>
+      <c r="Z13" s="342"/>
+      <c r="AA13" s="342"/>
+      <c r="AB13" s="342"/>
+      <c r="AC13" s="343"/>
       <c r="AD13" s="246"/>
     </row>
-    <row r="14" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="318"/>
+    <row r="14" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="320"/>
       <c r="B14" s="300"/>
       <c r="C14" s="301" t="s">
         <v>21</v>
@@ -8502,35 +8502,35 @@
       <c r="D14" s="303">
         <v>32</v>
       </c>
-      <c r="E14" s="350"/>
-      <c r="F14" s="340"/>
-      <c r="G14" s="340"/>
-      <c r="H14" s="340"/>
-      <c r="I14" s="340"/>
-      <c r="J14" s="351"/>
-      <c r="K14" s="339"/>
-      <c r="L14" s="340"/>
-      <c r="M14" s="340"/>
-      <c r="N14" s="340"/>
-      <c r="O14" s="340"/>
-      <c r="P14" s="340"/>
-      <c r="Q14" s="340"/>
-      <c r="R14" s="340"/>
-      <c r="S14" s="340"/>
-      <c r="T14" s="340"/>
-      <c r="U14" s="340"/>
-      <c r="V14" s="340"/>
-      <c r="W14" s="340"/>
-      <c r="X14" s="340"/>
-      <c r="Y14" s="340"/>
-      <c r="Z14" s="340"/>
-      <c r="AA14" s="340"/>
-      <c r="AB14" s="340"/>
-      <c r="AC14" s="341"/>
+      <c r="E14" s="352"/>
+      <c r="F14" s="342"/>
+      <c r="G14" s="342"/>
+      <c r="H14" s="342"/>
+      <c r="I14" s="342"/>
+      <c r="J14" s="353"/>
+      <c r="K14" s="341"/>
+      <c r="L14" s="342"/>
+      <c r="M14" s="342"/>
+      <c r="N14" s="342"/>
+      <c r="O14" s="342"/>
+      <c r="P14" s="342"/>
+      <c r="Q14" s="342"/>
+      <c r="R14" s="342"/>
+      <c r="S14" s="342"/>
+      <c r="T14" s="342"/>
+      <c r="U14" s="342"/>
+      <c r="V14" s="342"/>
+      <c r="W14" s="342"/>
+      <c r="X14" s="342"/>
+      <c r="Y14" s="342"/>
+      <c r="Z14" s="342"/>
+      <c r="AA14" s="342"/>
+      <c r="AB14" s="342"/>
+      <c r="AC14" s="343"/>
       <c r="AD14" s="246"/>
     </row>
-    <row r="15" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="318"/>
+    <row r="15" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="320"/>
       <c r="B15" s="300"/>
       <c r="C15" s="301" t="s">
         <v>22</v>
@@ -8538,35 +8538,35 @@
       <c r="D15" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="350"/>
-      <c r="F15" s="340"/>
-      <c r="G15" s="340"/>
-      <c r="H15" s="340"/>
-      <c r="I15" s="340"/>
-      <c r="J15" s="351"/>
-      <c r="K15" s="339"/>
-      <c r="L15" s="340"/>
-      <c r="M15" s="340"/>
-      <c r="N15" s="340"/>
-      <c r="O15" s="340"/>
-      <c r="P15" s="340"/>
-      <c r="Q15" s="340"/>
-      <c r="R15" s="340"/>
-      <c r="S15" s="340"/>
-      <c r="T15" s="340"/>
-      <c r="U15" s="340"/>
-      <c r="V15" s="340"/>
-      <c r="W15" s="340"/>
-      <c r="X15" s="340"/>
-      <c r="Y15" s="340"/>
-      <c r="Z15" s="340"/>
-      <c r="AA15" s="340"/>
-      <c r="AB15" s="340"/>
-      <c r="AC15" s="341"/>
+      <c r="E15" s="352"/>
+      <c r="F15" s="342"/>
+      <c r="G15" s="342"/>
+      <c r="H15" s="342"/>
+      <c r="I15" s="342"/>
+      <c r="J15" s="353"/>
+      <c r="K15" s="341"/>
+      <c r="L15" s="342"/>
+      <c r="M15" s="342"/>
+      <c r="N15" s="342"/>
+      <c r="O15" s="342"/>
+      <c r="P15" s="342"/>
+      <c r="Q15" s="342"/>
+      <c r="R15" s="342"/>
+      <c r="S15" s="342"/>
+      <c r="T15" s="342"/>
+      <c r="U15" s="342"/>
+      <c r="V15" s="342"/>
+      <c r="W15" s="342"/>
+      <c r="X15" s="342"/>
+      <c r="Y15" s="342"/>
+      <c r="Z15" s="342"/>
+      <c r="AA15" s="342"/>
+      <c r="AB15" s="342"/>
+      <c r="AC15" s="343"/>
       <c r="AD15" s="246"/>
     </row>
-    <row r="16" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="318"/>
+    <row r="16" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="320"/>
       <c r="B16" s="300" t="s">
         <v>23</v>
       </c>
@@ -8576,35 +8576,35 @@
       <c r="D16" s="302" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="350"/>
-      <c r="F16" s="340"/>
-      <c r="G16" s="340"/>
-      <c r="H16" s="340"/>
-      <c r="I16" s="340"/>
-      <c r="J16" s="351"/>
-      <c r="K16" s="339"/>
-      <c r="L16" s="340"/>
-      <c r="M16" s="340"/>
-      <c r="N16" s="340"/>
-      <c r="O16" s="340"/>
-      <c r="P16" s="340"/>
-      <c r="Q16" s="340"/>
-      <c r="R16" s="340"/>
-      <c r="S16" s="340"/>
-      <c r="T16" s="340"/>
-      <c r="U16" s="340"/>
-      <c r="V16" s="340"/>
-      <c r="W16" s="340"/>
-      <c r="X16" s="340"/>
-      <c r="Y16" s="340"/>
-      <c r="Z16" s="340"/>
-      <c r="AA16" s="340"/>
-      <c r="AB16" s="340"/>
-      <c r="AC16" s="341"/>
+      <c r="E16" s="352"/>
+      <c r="F16" s="342"/>
+      <c r="G16" s="342"/>
+      <c r="H16" s="342"/>
+      <c r="I16" s="342"/>
+      <c r="J16" s="353"/>
+      <c r="K16" s="341"/>
+      <c r="L16" s="342"/>
+      <c r="M16" s="342"/>
+      <c r="N16" s="342"/>
+      <c r="O16" s="342"/>
+      <c r="P16" s="342"/>
+      <c r="Q16" s="342"/>
+      <c r="R16" s="342"/>
+      <c r="S16" s="342"/>
+      <c r="T16" s="342"/>
+      <c r="U16" s="342"/>
+      <c r="V16" s="342"/>
+      <c r="W16" s="342"/>
+      <c r="X16" s="342"/>
+      <c r="Y16" s="342"/>
+      <c r="Z16" s="342"/>
+      <c r="AA16" s="342"/>
+      <c r="AB16" s="342"/>
+      <c r="AC16" s="343"/>
       <c r="AD16" s="246"/>
     </row>
-    <row r="17" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="318"/>
+    <row r="17" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="320"/>
       <c r="B17" s="300"/>
       <c r="C17" s="301" t="s">
         <v>27</v>
@@ -8612,35 +8612,35 @@
       <c r="D17" s="302">
         <v>128</v>
       </c>
-      <c r="E17" s="350"/>
-      <c r="F17" s="340"/>
-      <c r="G17" s="340"/>
-      <c r="H17" s="340"/>
-      <c r="I17" s="340"/>
-      <c r="J17" s="351"/>
-      <c r="K17" s="339"/>
-      <c r="L17" s="340"/>
-      <c r="M17" s="340"/>
-      <c r="N17" s="340"/>
-      <c r="O17" s="340"/>
-      <c r="P17" s="340"/>
-      <c r="Q17" s="340"/>
-      <c r="R17" s="340"/>
-      <c r="S17" s="340"/>
-      <c r="T17" s="340"/>
-      <c r="U17" s="340"/>
-      <c r="V17" s="340"/>
-      <c r="W17" s="340"/>
-      <c r="X17" s="340"/>
-      <c r="Y17" s="340"/>
-      <c r="Z17" s="340"/>
-      <c r="AA17" s="340"/>
-      <c r="AB17" s="340"/>
-      <c r="AC17" s="341"/>
+      <c r="E17" s="352"/>
+      <c r="F17" s="342"/>
+      <c r="G17" s="342"/>
+      <c r="H17" s="342"/>
+      <c r="I17" s="342"/>
+      <c r="J17" s="353"/>
+      <c r="K17" s="341"/>
+      <c r="L17" s="342"/>
+      <c r="M17" s="342"/>
+      <c r="N17" s="342"/>
+      <c r="O17" s="342"/>
+      <c r="P17" s="342"/>
+      <c r="Q17" s="342"/>
+      <c r="R17" s="342"/>
+      <c r="S17" s="342"/>
+      <c r="T17" s="342"/>
+      <c r="U17" s="342"/>
+      <c r="V17" s="342"/>
+      <c r="W17" s="342"/>
+      <c r="X17" s="342"/>
+      <c r="Y17" s="342"/>
+      <c r="Z17" s="342"/>
+      <c r="AA17" s="342"/>
+      <c r="AB17" s="342"/>
+      <c r="AC17" s="343"/>
       <c r="AD17" s="246"/>
     </row>
-    <row r="18" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="318"/>
+    <row r="18" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="320"/>
       <c r="B18" s="300"/>
       <c r="C18" s="301" t="s">
         <v>28</v>
@@ -8648,35 +8648,35 @@
       <c r="D18" s="302" t="s">
         <v>339</v>
       </c>
-      <c r="E18" s="350"/>
-      <c r="F18" s="340"/>
-      <c r="G18" s="340"/>
-      <c r="H18" s="340"/>
-      <c r="I18" s="340"/>
-      <c r="J18" s="351"/>
-      <c r="K18" s="339"/>
-      <c r="L18" s="340"/>
-      <c r="M18" s="340"/>
-      <c r="N18" s="340"/>
-      <c r="O18" s="340"/>
-      <c r="P18" s="340"/>
-      <c r="Q18" s="340"/>
-      <c r="R18" s="340"/>
-      <c r="S18" s="340"/>
-      <c r="T18" s="340"/>
-      <c r="U18" s="340"/>
-      <c r="V18" s="340"/>
-      <c r="W18" s="340"/>
-      <c r="X18" s="340"/>
-      <c r="Y18" s="340"/>
-      <c r="Z18" s="340"/>
-      <c r="AA18" s="340"/>
-      <c r="AB18" s="340"/>
-      <c r="AC18" s="341"/>
+      <c r="E18" s="352"/>
+      <c r="F18" s="342"/>
+      <c r="G18" s="342"/>
+      <c r="H18" s="342"/>
+      <c r="I18" s="342"/>
+      <c r="J18" s="353"/>
+      <c r="K18" s="341"/>
+      <c r="L18" s="342"/>
+      <c r="M18" s="342"/>
+      <c r="N18" s="342"/>
+      <c r="O18" s="342"/>
+      <c r="P18" s="342"/>
+      <c r="Q18" s="342"/>
+      <c r="R18" s="342"/>
+      <c r="S18" s="342"/>
+      <c r="T18" s="342"/>
+      <c r="U18" s="342"/>
+      <c r="V18" s="342"/>
+      <c r="W18" s="342"/>
+      <c r="X18" s="342"/>
+      <c r="Y18" s="342"/>
+      <c r="Z18" s="342"/>
+      <c r="AA18" s="342"/>
+      <c r="AB18" s="342"/>
+      <c r="AC18" s="343"/>
       <c r="AD18" s="246"/>
     </row>
-    <row r="19" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="318"/>
+    <row r="19" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="320"/>
       <c r="B19" s="300"/>
       <c r="C19" s="301" t="s">
         <v>29</v>
@@ -8684,35 +8684,35 @@
       <c r="D19" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="350"/>
-      <c r="F19" s="340"/>
-      <c r="G19" s="340"/>
-      <c r="H19" s="340"/>
-      <c r="I19" s="340"/>
-      <c r="J19" s="351"/>
-      <c r="K19" s="339"/>
-      <c r="L19" s="340"/>
-      <c r="M19" s="340"/>
-      <c r="N19" s="340"/>
-      <c r="O19" s="340"/>
-      <c r="P19" s="340"/>
-      <c r="Q19" s="340"/>
-      <c r="R19" s="340"/>
-      <c r="S19" s="340"/>
-      <c r="T19" s="340"/>
-      <c r="U19" s="340"/>
-      <c r="V19" s="340"/>
-      <c r="W19" s="340"/>
-      <c r="X19" s="340"/>
-      <c r="Y19" s="340"/>
-      <c r="Z19" s="340"/>
-      <c r="AA19" s="340"/>
-      <c r="AB19" s="340"/>
-      <c r="AC19" s="341"/>
+      <c r="E19" s="352"/>
+      <c r="F19" s="342"/>
+      <c r="G19" s="342"/>
+      <c r="H19" s="342"/>
+      <c r="I19" s="342"/>
+      <c r="J19" s="353"/>
+      <c r="K19" s="341"/>
+      <c r="L19" s="342"/>
+      <c r="M19" s="342"/>
+      <c r="N19" s="342"/>
+      <c r="O19" s="342"/>
+      <c r="P19" s="342"/>
+      <c r="Q19" s="342"/>
+      <c r="R19" s="342"/>
+      <c r="S19" s="342"/>
+      <c r="T19" s="342"/>
+      <c r="U19" s="342"/>
+      <c r="V19" s="342"/>
+      <c r="W19" s="342"/>
+      <c r="X19" s="342"/>
+      <c r="Y19" s="342"/>
+      <c r="Z19" s="342"/>
+      <c r="AA19" s="342"/>
+      <c r="AB19" s="342"/>
+      <c r="AC19" s="343"/>
       <c r="AD19" s="246"/>
     </row>
-    <row r="20" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="318"/>
+    <row r="20" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="320"/>
       <c r="B20" s="300" t="s">
         <v>101</v>
       </c>
@@ -8722,35 +8722,35 @@
       <c r="D20" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="350"/>
-      <c r="F20" s="340"/>
-      <c r="G20" s="340"/>
-      <c r="H20" s="340"/>
-      <c r="I20" s="340"/>
-      <c r="J20" s="351"/>
-      <c r="K20" s="339"/>
-      <c r="L20" s="340"/>
-      <c r="M20" s="340"/>
-      <c r="N20" s="340"/>
-      <c r="O20" s="340"/>
-      <c r="P20" s="340"/>
-      <c r="Q20" s="340"/>
-      <c r="R20" s="340"/>
-      <c r="S20" s="340"/>
-      <c r="T20" s="340"/>
-      <c r="U20" s="340"/>
-      <c r="V20" s="340"/>
-      <c r="W20" s="340"/>
-      <c r="X20" s="340"/>
-      <c r="Y20" s="340"/>
-      <c r="Z20" s="340"/>
-      <c r="AA20" s="340"/>
-      <c r="AB20" s="340"/>
-      <c r="AC20" s="341"/>
+      <c r="E20" s="352"/>
+      <c r="F20" s="342"/>
+      <c r="G20" s="342"/>
+      <c r="H20" s="342"/>
+      <c r="I20" s="342"/>
+      <c r="J20" s="353"/>
+      <c r="K20" s="341"/>
+      <c r="L20" s="342"/>
+      <c r="M20" s="342"/>
+      <c r="N20" s="342"/>
+      <c r="O20" s="342"/>
+      <c r="P20" s="342"/>
+      <c r="Q20" s="342"/>
+      <c r="R20" s="342"/>
+      <c r="S20" s="342"/>
+      <c r="T20" s="342"/>
+      <c r="U20" s="342"/>
+      <c r="V20" s="342"/>
+      <c r="W20" s="342"/>
+      <c r="X20" s="342"/>
+      <c r="Y20" s="342"/>
+      <c r="Z20" s="342"/>
+      <c r="AA20" s="342"/>
+      <c r="AB20" s="342"/>
+      <c r="AC20" s="343"/>
       <c r="AD20" s="246"/>
     </row>
-    <row r="21" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="318"/>
+    <row r="21" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="320"/>
       <c r="B21" s="300" t="s">
         <v>46</v>
       </c>
@@ -8760,35 +8760,35 @@
       <c r="D21" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="350"/>
-      <c r="F21" s="340"/>
-      <c r="G21" s="340"/>
-      <c r="H21" s="340"/>
-      <c r="I21" s="340"/>
-      <c r="J21" s="351"/>
-      <c r="K21" s="339"/>
-      <c r="L21" s="340"/>
-      <c r="M21" s="340"/>
-      <c r="N21" s="340"/>
-      <c r="O21" s="340"/>
-      <c r="P21" s="340"/>
-      <c r="Q21" s="340"/>
-      <c r="R21" s="340"/>
-      <c r="S21" s="340"/>
-      <c r="T21" s="340"/>
-      <c r="U21" s="340"/>
-      <c r="V21" s="340"/>
-      <c r="W21" s="340"/>
-      <c r="X21" s="340"/>
-      <c r="Y21" s="340"/>
-      <c r="Z21" s="340"/>
-      <c r="AA21" s="340"/>
-      <c r="AB21" s="340"/>
-      <c r="AC21" s="341"/>
+      <c r="E21" s="352"/>
+      <c r="F21" s="342"/>
+      <c r="G21" s="342"/>
+      <c r="H21" s="342"/>
+      <c r="I21" s="342"/>
+      <c r="J21" s="353"/>
+      <c r="K21" s="341"/>
+      <c r="L21" s="342"/>
+      <c r="M21" s="342"/>
+      <c r="N21" s="342"/>
+      <c r="O21" s="342"/>
+      <c r="P21" s="342"/>
+      <c r="Q21" s="342"/>
+      <c r="R21" s="342"/>
+      <c r="S21" s="342"/>
+      <c r="T21" s="342"/>
+      <c r="U21" s="342"/>
+      <c r="V21" s="342"/>
+      <c r="W21" s="342"/>
+      <c r="X21" s="342"/>
+      <c r="Y21" s="342"/>
+      <c r="Z21" s="342"/>
+      <c r="AA21" s="342"/>
+      <c r="AB21" s="342"/>
+      <c r="AC21" s="343"/>
       <c r="AD21" s="201"/>
     </row>
-    <row r="22" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="318"/>
+    <row r="22" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="320"/>
       <c r="B22" s="300"/>
       <c r="C22" s="301" t="s">
         <v>340</v>
@@ -8796,35 +8796,35 @@
       <c r="D22" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="350"/>
-      <c r="F22" s="340"/>
-      <c r="G22" s="340"/>
-      <c r="H22" s="340"/>
-      <c r="I22" s="340"/>
-      <c r="J22" s="351"/>
-      <c r="K22" s="339"/>
-      <c r="L22" s="340"/>
-      <c r="M22" s="340"/>
-      <c r="N22" s="340"/>
-      <c r="O22" s="340"/>
-      <c r="P22" s="340"/>
-      <c r="Q22" s="340"/>
-      <c r="R22" s="340"/>
-      <c r="S22" s="340"/>
-      <c r="T22" s="340"/>
-      <c r="U22" s="340"/>
-      <c r="V22" s="340"/>
-      <c r="W22" s="340"/>
-      <c r="X22" s="340"/>
-      <c r="Y22" s="340"/>
-      <c r="Z22" s="340"/>
-      <c r="AA22" s="340"/>
-      <c r="AB22" s="340"/>
-      <c r="AC22" s="341"/>
+      <c r="E22" s="352"/>
+      <c r="F22" s="342"/>
+      <c r="G22" s="342"/>
+      <c r="H22" s="342"/>
+      <c r="I22" s="342"/>
+      <c r="J22" s="353"/>
+      <c r="K22" s="341"/>
+      <c r="L22" s="342"/>
+      <c r="M22" s="342"/>
+      <c r="N22" s="342"/>
+      <c r="O22" s="342"/>
+      <c r="P22" s="342"/>
+      <c r="Q22" s="342"/>
+      <c r="R22" s="342"/>
+      <c r="S22" s="342"/>
+      <c r="T22" s="342"/>
+      <c r="U22" s="342"/>
+      <c r="V22" s="342"/>
+      <c r="W22" s="342"/>
+      <c r="X22" s="342"/>
+      <c r="Y22" s="342"/>
+      <c r="Z22" s="342"/>
+      <c r="AA22" s="342"/>
+      <c r="AB22" s="342"/>
+      <c r="AC22" s="343"/>
       <c r="AD22" s="201"/>
     </row>
-    <row r="23" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="318"/>
+    <row r="23" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="320"/>
       <c r="B23" s="300"/>
       <c r="C23" s="301" t="s">
         <v>188</v>
@@ -8832,35 +8832,35 @@
       <c r="D23" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="350"/>
-      <c r="F23" s="340"/>
-      <c r="G23" s="340"/>
-      <c r="H23" s="340"/>
-      <c r="I23" s="340"/>
-      <c r="J23" s="351"/>
-      <c r="K23" s="339"/>
-      <c r="L23" s="340"/>
-      <c r="M23" s="340"/>
-      <c r="N23" s="340"/>
-      <c r="O23" s="340"/>
-      <c r="P23" s="340"/>
-      <c r="Q23" s="340"/>
-      <c r="R23" s="340"/>
-      <c r="S23" s="340"/>
-      <c r="T23" s="340"/>
-      <c r="U23" s="340"/>
-      <c r="V23" s="340"/>
-      <c r="W23" s="340"/>
-      <c r="X23" s="340"/>
-      <c r="Y23" s="340"/>
-      <c r="Z23" s="340"/>
-      <c r="AA23" s="340"/>
-      <c r="AB23" s="340"/>
-      <c r="AC23" s="341"/>
+      <c r="E23" s="352"/>
+      <c r="F23" s="342"/>
+      <c r="G23" s="342"/>
+      <c r="H23" s="342"/>
+      <c r="I23" s="342"/>
+      <c r="J23" s="353"/>
+      <c r="K23" s="341"/>
+      <c r="L23" s="342"/>
+      <c r="M23" s="342"/>
+      <c r="N23" s="342"/>
+      <c r="O23" s="342"/>
+      <c r="P23" s="342"/>
+      <c r="Q23" s="342"/>
+      <c r="R23" s="342"/>
+      <c r="S23" s="342"/>
+      <c r="T23" s="342"/>
+      <c r="U23" s="342"/>
+      <c r="V23" s="342"/>
+      <c r="W23" s="342"/>
+      <c r="X23" s="342"/>
+      <c r="Y23" s="342"/>
+      <c r="Z23" s="342"/>
+      <c r="AA23" s="342"/>
+      <c r="AB23" s="342"/>
+      <c r="AC23" s="343"/>
       <c r="AD23" s="201"/>
     </row>
-    <row r="24" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="318"/>
+    <row r="24" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="320"/>
       <c r="B24" s="300"/>
       <c r="C24" s="301" t="s">
         <v>190</v>
@@ -8868,35 +8868,35 @@
       <c r="D24" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="350"/>
-      <c r="F24" s="340"/>
-      <c r="G24" s="340"/>
-      <c r="H24" s="340"/>
-      <c r="I24" s="340"/>
-      <c r="J24" s="351"/>
-      <c r="K24" s="339"/>
-      <c r="L24" s="340"/>
-      <c r="M24" s="340"/>
-      <c r="N24" s="340"/>
-      <c r="O24" s="340"/>
-      <c r="P24" s="340"/>
-      <c r="Q24" s="340"/>
-      <c r="R24" s="340"/>
-      <c r="S24" s="340"/>
-      <c r="T24" s="340"/>
-      <c r="U24" s="340"/>
-      <c r="V24" s="340"/>
-      <c r="W24" s="340"/>
-      <c r="X24" s="340"/>
-      <c r="Y24" s="340"/>
-      <c r="Z24" s="340"/>
-      <c r="AA24" s="340"/>
-      <c r="AB24" s="340"/>
-      <c r="AC24" s="341"/>
+      <c r="E24" s="352"/>
+      <c r="F24" s="342"/>
+      <c r="G24" s="342"/>
+      <c r="H24" s="342"/>
+      <c r="I24" s="342"/>
+      <c r="J24" s="353"/>
+      <c r="K24" s="341"/>
+      <c r="L24" s="342"/>
+      <c r="M24" s="342"/>
+      <c r="N24" s="342"/>
+      <c r="O24" s="342"/>
+      <c r="P24" s="342"/>
+      <c r="Q24" s="342"/>
+      <c r="R24" s="342"/>
+      <c r="S24" s="342"/>
+      <c r="T24" s="342"/>
+      <c r="U24" s="342"/>
+      <c r="V24" s="342"/>
+      <c r="W24" s="342"/>
+      <c r="X24" s="342"/>
+      <c r="Y24" s="342"/>
+      <c r="Z24" s="342"/>
+      <c r="AA24" s="342"/>
+      <c r="AB24" s="342"/>
+      <c r="AC24" s="343"/>
       <c r="AD24" s="201"/>
     </row>
-    <row r="25" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="318"/>
+    <row r="25" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="320"/>
       <c r="B25" s="300"/>
       <c r="C25" s="301" t="s">
         <v>307</v>
@@ -8904,35 +8904,35 @@
       <c r="D25" s="302" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="350"/>
-      <c r="F25" s="340"/>
-      <c r="G25" s="340"/>
-      <c r="H25" s="340"/>
-      <c r="I25" s="340"/>
-      <c r="J25" s="351"/>
-      <c r="K25" s="339"/>
-      <c r="L25" s="340"/>
-      <c r="M25" s="340"/>
-      <c r="N25" s="340"/>
-      <c r="O25" s="340"/>
-      <c r="P25" s="340"/>
-      <c r="Q25" s="340"/>
-      <c r="R25" s="340"/>
-      <c r="S25" s="340"/>
-      <c r="T25" s="340"/>
-      <c r="U25" s="340"/>
-      <c r="V25" s="340"/>
-      <c r="W25" s="340"/>
-      <c r="X25" s="340"/>
-      <c r="Y25" s="340"/>
-      <c r="Z25" s="340"/>
-      <c r="AA25" s="340"/>
-      <c r="AB25" s="340"/>
-      <c r="AC25" s="341"/>
+      <c r="E25" s="352"/>
+      <c r="F25" s="342"/>
+      <c r="G25" s="342"/>
+      <c r="H25" s="342"/>
+      <c r="I25" s="342"/>
+      <c r="J25" s="353"/>
+      <c r="K25" s="341"/>
+      <c r="L25" s="342"/>
+      <c r="M25" s="342"/>
+      <c r="N25" s="342"/>
+      <c r="O25" s="342"/>
+      <c r="P25" s="342"/>
+      <c r="Q25" s="342"/>
+      <c r="R25" s="342"/>
+      <c r="S25" s="342"/>
+      <c r="T25" s="342"/>
+      <c r="U25" s="342"/>
+      <c r="V25" s="342"/>
+      <c r="W25" s="342"/>
+      <c r="X25" s="342"/>
+      <c r="Y25" s="342"/>
+      <c r="Z25" s="342"/>
+      <c r="AA25" s="342"/>
+      <c r="AB25" s="342"/>
+      <c r="AC25" s="343"/>
       <c r="AD25" s="201"/>
     </row>
-    <row r="26" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="318"/>
+    <row r="26" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="320"/>
       <c r="B26" s="300"/>
       <c r="C26" s="301" t="s">
         <v>199</v>
@@ -8940,35 +8940,35 @@
       <c r="D26" s="302" t="s">
         <v>200</v>
       </c>
-      <c r="E26" s="350"/>
-      <c r="F26" s="340"/>
-      <c r="G26" s="340"/>
-      <c r="H26" s="340"/>
-      <c r="I26" s="340"/>
-      <c r="J26" s="351"/>
-      <c r="K26" s="339"/>
-      <c r="L26" s="340"/>
-      <c r="M26" s="340"/>
-      <c r="N26" s="340"/>
-      <c r="O26" s="340"/>
-      <c r="P26" s="340"/>
-      <c r="Q26" s="340"/>
-      <c r="R26" s="340"/>
-      <c r="S26" s="340"/>
-      <c r="T26" s="340"/>
-      <c r="U26" s="340"/>
-      <c r="V26" s="340"/>
-      <c r="W26" s="340"/>
-      <c r="X26" s="340"/>
-      <c r="Y26" s="340"/>
-      <c r="Z26" s="340"/>
-      <c r="AA26" s="340"/>
-      <c r="AB26" s="340"/>
-      <c r="AC26" s="341"/>
+      <c r="E26" s="352"/>
+      <c r="F26" s="342"/>
+      <c r="G26" s="342"/>
+      <c r="H26" s="342"/>
+      <c r="I26" s="342"/>
+      <c r="J26" s="353"/>
+      <c r="K26" s="341"/>
+      <c r="L26" s="342"/>
+      <c r="M26" s="342"/>
+      <c r="N26" s="342"/>
+      <c r="O26" s="342"/>
+      <c r="P26" s="342"/>
+      <c r="Q26" s="342"/>
+      <c r="R26" s="342"/>
+      <c r="S26" s="342"/>
+      <c r="T26" s="342"/>
+      <c r="U26" s="342"/>
+      <c r="V26" s="342"/>
+      <c r="W26" s="342"/>
+      <c r="X26" s="342"/>
+      <c r="Y26" s="342"/>
+      <c r="Z26" s="342"/>
+      <c r="AA26" s="342"/>
+      <c r="AB26" s="342"/>
+      <c r="AC26" s="343"/>
       <c r="AD26" s="201"/>
     </row>
-    <row r="27" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="318"/>
+    <row r="27" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="320"/>
       <c r="B27" s="300"/>
       <c r="C27" s="301" t="s">
         <v>202</v>
@@ -8976,37 +8976,37 @@
       <c r="D27" s="302" t="s">
         <v>201</v>
       </c>
-      <c r="E27" s="350"/>
-      <c r="F27" s="340"/>
-      <c r="G27" s="340"/>
-      <c r="H27" s="340"/>
-      <c r="I27" s="340"/>
-      <c r="J27" s="351"/>
-      <c r="K27" s="339"/>
-      <c r="L27" s="340"/>
-      <c r="M27" s="340"/>
-      <c r="N27" s="340"/>
-      <c r="O27" s="340"/>
-      <c r="P27" s="340"/>
-      <c r="Q27" s="340"/>
-      <c r="R27" s="340"/>
-      <c r="S27" s="340"/>
-      <c r="T27" s="340"/>
-      <c r="U27" s="340"/>
-      <c r="V27" s="340"/>
-      <c r="W27" s="340"/>
-      <c r="X27" s="340"/>
-      <c r="Y27" s="340"/>
-      <c r="Z27" s="340"/>
-      <c r="AA27" s="340"/>
-      <c r="AB27" s="340"/>
-      <c r="AC27" s="341"/>
+      <c r="E27" s="352"/>
+      <c r="F27" s="342"/>
+      <c r="G27" s="342"/>
+      <c r="H27" s="342"/>
+      <c r="I27" s="342"/>
+      <c r="J27" s="353"/>
+      <c r="K27" s="341"/>
+      <c r="L27" s="342"/>
+      <c r="M27" s="342"/>
+      <c r="N27" s="342"/>
+      <c r="O27" s="342"/>
+      <c r="P27" s="342"/>
+      <c r="Q27" s="342"/>
+      <c r="R27" s="342"/>
+      <c r="S27" s="342"/>
+      <c r="T27" s="342"/>
+      <c r="U27" s="342"/>
+      <c r="V27" s="342"/>
+      <c r="W27" s="342"/>
+      <c r="X27" s="342"/>
+      <c r="Y27" s="342"/>
+      <c r="Z27" s="342"/>
+      <c r="AA27" s="342"/>
+      <c r="AB27" s="342"/>
+      <c r="AC27" s="343"/>
       <c r="AD27" s="201" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="318"/>
+    <row r="28" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="320"/>
       <c r="B28" s="300"/>
       <c r="C28" s="301" t="s">
         <v>191</v>
@@ -9014,35 +9014,35 @@
       <c r="D28" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="350"/>
-      <c r="F28" s="340"/>
-      <c r="G28" s="340"/>
-      <c r="H28" s="340"/>
-      <c r="I28" s="340"/>
-      <c r="J28" s="351"/>
-      <c r="K28" s="339"/>
-      <c r="L28" s="340"/>
-      <c r="M28" s="340"/>
-      <c r="N28" s="340"/>
-      <c r="O28" s="340"/>
-      <c r="P28" s="340"/>
-      <c r="Q28" s="340"/>
-      <c r="R28" s="340"/>
-      <c r="S28" s="340"/>
-      <c r="T28" s="340"/>
-      <c r="U28" s="340"/>
-      <c r="V28" s="340"/>
-      <c r="W28" s="340"/>
-      <c r="X28" s="340"/>
-      <c r="Y28" s="340"/>
-      <c r="Z28" s="340"/>
-      <c r="AA28" s="340"/>
-      <c r="AB28" s="340"/>
-      <c r="AC28" s="341"/>
+      <c r="E28" s="352"/>
+      <c r="F28" s="342"/>
+      <c r="G28" s="342"/>
+      <c r="H28" s="342"/>
+      <c r="I28" s="342"/>
+      <c r="J28" s="353"/>
+      <c r="K28" s="341"/>
+      <c r="L28" s="342"/>
+      <c r="M28" s="342"/>
+      <c r="N28" s="342"/>
+      <c r="O28" s="342"/>
+      <c r="P28" s="342"/>
+      <c r="Q28" s="342"/>
+      <c r="R28" s="342"/>
+      <c r="S28" s="342"/>
+      <c r="T28" s="342"/>
+      <c r="U28" s="342"/>
+      <c r="V28" s="342"/>
+      <c r="W28" s="342"/>
+      <c r="X28" s="342"/>
+      <c r="Y28" s="342"/>
+      <c r="Z28" s="342"/>
+      <c r="AA28" s="342"/>
+      <c r="AB28" s="342"/>
+      <c r="AC28" s="343"/>
       <c r="AD28" s="201"/>
     </row>
-    <row r="29" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="318"/>
+    <row r="29" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="320"/>
       <c r="B29" s="300"/>
       <c r="C29" s="301" t="s">
         <v>68</v>
@@ -9050,35 +9050,35 @@
       <c r="D29" s="302" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="350"/>
-      <c r="F29" s="340"/>
-      <c r="G29" s="340"/>
-      <c r="H29" s="340"/>
-      <c r="I29" s="340"/>
-      <c r="J29" s="351"/>
-      <c r="K29" s="339"/>
-      <c r="L29" s="340"/>
-      <c r="M29" s="340"/>
-      <c r="N29" s="340"/>
-      <c r="O29" s="340"/>
-      <c r="P29" s="340"/>
-      <c r="Q29" s="340"/>
-      <c r="R29" s="340"/>
-      <c r="S29" s="340"/>
-      <c r="T29" s="340"/>
-      <c r="U29" s="340"/>
-      <c r="V29" s="340"/>
-      <c r="W29" s="340"/>
-      <c r="X29" s="340"/>
-      <c r="Y29" s="340"/>
-      <c r="Z29" s="340"/>
-      <c r="AA29" s="340"/>
-      <c r="AB29" s="340"/>
-      <c r="AC29" s="341"/>
+      <c r="E29" s="352"/>
+      <c r="F29" s="342"/>
+      <c r="G29" s="342"/>
+      <c r="H29" s="342"/>
+      <c r="I29" s="342"/>
+      <c r="J29" s="353"/>
+      <c r="K29" s="341"/>
+      <c r="L29" s="342"/>
+      <c r="M29" s="342"/>
+      <c r="N29" s="342"/>
+      <c r="O29" s="342"/>
+      <c r="P29" s="342"/>
+      <c r="Q29" s="342"/>
+      <c r="R29" s="342"/>
+      <c r="S29" s="342"/>
+      <c r="T29" s="342"/>
+      <c r="U29" s="342"/>
+      <c r="V29" s="342"/>
+      <c r="W29" s="342"/>
+      <c r="X29" s="342"/>
+      <c r="Y29" s="342"/>
+      <c r="Z29" s="342"/>
+      <c r="AA29" s="342"/>
+      <c r="AB29" s="342"/>
+      <c r="AC29" s="343"/>
       <c r="AD29" s="201"/>
     </row>
-    <row r="30" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="318"/>
+    <row r="30" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="320"/>
       <c r="B30" s="300"/>
       <c r="C30" s="301" t="s">
         <v>70</v>
@@ -9086,35 +9086,35 @@
       <c r="D30" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="350"/>
-      <c r="F30" s="340"/>
-      <c r="G30" s="340"/>
-      <c r="H30" s="340"/>
-      <c r="I30" s="340"/>
-      <c r="J30" s="351"/>
-      <c r="K30" s="339"/>
-      <c r="L30" s="340"/>
-      <c r="M30" s="340"/>
-      <c r="N30" s="340"/>
-      <c r="O30" s="340"/>
-      <c r="P30" s="340"/>
-      <c r="Q30" s="340"/>
-      <c r="R30" s="340"/>
-      <c r="S30" s="340"/>
-      <c r="T30" s="340"/>
-      <c r="U30" s="340"/>
-      <c r="V30" s="340"/>
-      <c r="W30" s="340"/>
-      <c r="X30" s="340"/>
-      <c r="Y30" s="340"/>
-      <c r="Z30" s="340"/>
-      <c r="AA30" s="340"/>
-      <c r="AB30" s="340"/>
-      <c r="AC30" s="341"/>
+      <c r="E30" s="352"/>
+      <c r="F30" s="342"/>
+      <c r="G30" s="342"/>
+      <c r="H30" s="342"/>
+      <c r="I30" s="342"/>
+      <c r="J30" s="353"/>
+      <c r="K30" s="341"/>
+      <c r="L30" s="342"/>
+      <c r="M30" s="342"/>
+      <c r="N30" s="342"/>
+      <c r="O30" s="342"/>
+      <c r="P30" s="342"/>
+      <c r="Q30" s="342"/>
+      <c r="R30" s="342"/>
+      <c r="S30" s="342"/>
+      <c r="T30" s="342"/>
+      <c r="U30" s="342"/>
+      <c r="V30" s="342"/>
+      <c r="W30" s="342"/>
+      <c r="X30" s="342"/>
+      <c r="Y30" s="342"/>
+      <c r="Z30" s="342"/>
+      <c r="AA30" s="342"/>
+      <c r="AB30" s="342"/>
+      <c r="AC30" s="343"/>
       <c r="AD30" s="201"/>
     </row>
-    <row r="31" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="318"/>
+    <row r="31" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="320"/>
       <c r="B31" s="300"/>
       <c r="C31" s="301" t="s">
         <v>75</v>
@@ -9122,35 +9122,35 @@
       <c r="D31" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="350"/>
-      <c r="F31" s="340"/>
-      <c r="G31" s="340"/>
-      <c r="H31" s="340"/>
-      <c r="I31" s="340"/>
-      <c r="J31" s="351"/>
-      <c r="K31" s="339"/>
-      <c r="L31" s="340"/>
-      <c r="M31" s="340"/>
-      <c r="N31" s="340"/>
-      <c r="O31" s="340"/>
-      <c r="P31" s="340"/>
-      <c r="Q31" s="340"/>
-      <c r="R31" s="340"/>
-      <c r="S31" s="340"/>
-      <c r="T31" s="340"/>
-      <c r="U31" s="340"/>
-      <c r="V31" s="340"/>
-      <c r="W31" s="340"/>
-      <c r="X31" s="340"/>
-      <c r="Y31" s="340"/>
-      <c r="Z31" s="340"/>
-      <c r="AA31" s="340"/>
-      <c r="AB31" s="340"/>
-      <c r="AC31" s="341"/>
+      <c r="E31" s="352"/>
+      <c r="F31" s="342"/>
+      <c r="G31" s="342"/>
+      <c r="H31" s="342"/>
+      <c r="I31" s="342"/>
+      <c r="J31" s="353"/>
+      <c r="K31" s="341"/>
+      <c r="L31" s="342"/>
+      <c r="M31" s="342"/>
+      <c r="N31" s="342"/>
+      <c r="O31" s="342"/>
+      <c r="P31" s="342"/>
+      <c r="Q31" s="342"/>
+      <c r="R31" s="342"/>
+      <c r="S31" s="342"/>
+      <c r="T31" s="342"/>
+      <c r="U31" s="342"/>
+      <c r="V31" s="342"/>
+      <c r="W31" s="342"/>
+      <c r="X31" s="342"/>
+      <c r="Y31" s="342"/>
+      <c r="Z31" s="342"/>
+      <c r="AA31" s="342"/>
+      <c r="AB31" s="342"/>
+      <c r="AC31" s="343"/>
       <c r="AD31" s="201"/>
     </row>
-    <row r="32" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="318"/>
+    <row r="32" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="320"/>
       <c r="B32" s="300"/>
       <c r="C32" s="301" t="s">
         <v>76</v>
@@ -9158,35 +9158,35 @@
       <c r="D32" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="350"/>
-      <c r="F32" s="340"/>
-      <c r="G32" s="340"/>
-      <c r="H32" s="340"/>
-      <c r="I32" s="340"/>
-      <c r="J32" s="351"/>
-      <c r="K32" s="339"/>
-      <c r="L32" s="340"/>
-      <c r="M32" s="340"/>
-      <c r="N32" s="340"/>
-      <c r="O32" s="340"/>
-      <c r="P32" s="340"/>
-      <c r="Q32" s="340"/>
-      <c r="R32" s="340"/>
-      <c r="S32" s="340"/>
-      <c r="T32" s="340"/>
-      <c r="U32" s="340"/>
-      <c r="V32" s="340"/>
-      <c r="W32" s="340"/>
-      <c r="X32" s="340"/>
-      <c r="Y32" s="340"/>
-      <c r="Z32" s="340"/>
-      <c r="AA32" s="340"/>
-      <c r="AB32" s="340"/>
-      <c r="AC32" s="341"/>
+      <c r="E32" s="352"/>
+      <c r="F32" s="342"/>
+      <c r="G32" s="342"/>
+      <c r="H32" s="342"/>
+      <c r="I32" s="342"/>
+      <c r="J32" s="353"/>
+      <c r="K32" s="341"/>
+      <c r="L32" s="342"/>
+      <c r="M32" s="342"/>
+      <c r="N32" s="342"/>
+      <c r="O32" s="342"/>
+      <c r="P32" s="342"/>
+      <c r="Q32" s="342"/>
+      <c r="R32" s="342"/>
+      <c r="S32" s="342"/>
+      <c r="T32" s="342"/>
+      <c r="U32" s="342"/>
+      <c r="V32" s="342"/>
+      <c r="W32" s="342"/>
+      <c r="X32" s="342"/>
+      <c r="Y32" s="342"/>
+      <c r="Z32" s="342"/>
+      <c r="AA32" s="342"/>
+      <c r="AB32" s="342"/>
+      <c r="AC32" s="343"/>
       <c r="AD32" s="201"/>
     </row>
-    <row r="33" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="318"/>
+    <row r="33" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="320"/>
       <c r="B33" s="300"/>
       <c r="C33" s="301" t="s">
         <v>77</v>
@@ -9194,35 +9194,35 @@
       <c r="D33" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="350"/>
-      <c r="F33" s="340"/>
-      <c r="G33" s="340"/>
-      <c r="H33" s="340"/>
-      <c r="I33" s="340"/>
-      <c r="J33" s="351"/>
-      <c r="K33" s="339"/>
-      <c r="L33" s="340"/>
-      <c r="M33" s="340"/>
-      <c r="N33" s="340"/>
-      <c r="O33" s="340"/>
-      <c r="P33" s="340"/>
-      <c r="Q33" s="340"/>
-      <c r="R33" s="340"/>
-      <c r="S33" s="340"/>
-      <c r="T33" s="340"/>
-      <c r="U33" s="340"/>
-      <c r="V33" s="340"/>
-      <c r="W33" s="340"/>
-      <c r="X33" s="340"/>
-      <c r="Y33" s="340"/>
-      <c r="Z33" s="340"/>
-      <c r="AA33" s="340"/>
-      <c r="AB33" s="340"/>
-      <c r="AC33" s="341"/>
+      <c r="E33" s="352"/>
+      <c r="F33" s="342"/>
+      <c r="G33" s="342"/>
+      <c r="H33" s="342"/>
+      <c r="I33" s="342"/>
+      <c r="J33" s="353"/>
+      <c r="K33" s="341"/>
+      <c r="L33" s="342"/>
+      <c r="M33" s="342"/>
+      <c r="N33" s="342"/>
+      <c r="O33" s="342"/>
+      <c r="P33" s="342"/>
+      <c r="Q33" s="342"/>
+      <c r="R33" s="342"/>
+      <c r="S33" s="342"/>
+      <c r="T33" s="342"/>
+      <c r="U33" s="342"/>
+      <c r="V33" s="342"/>
+      <c r="W33" s="342"/>
+      <c r="X33" s="342"/>
+      <c r="Y33" s="342"/>
+      <c r="Z33" s="342"/>
+      <c r="AA33" s="342"/>
+      <c r="AB33" s="342"/>
+      <c r="AC33" s="343"/>
       <c r="AD33" s="201"/>
     </row>
-    <row r="34" spans="1:30" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="318"/>
+    <row r="34" spans="1:30" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="320"/>
       <c r="B34" s="304"/>
       <c r="C34" s="305" t="s">
         <v>78</v>
@@ -9230,42 +9230,42 @@
       <c r="D34" s="306" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="352"/>
-      <c r="F34" s="343"/>
-      <c r="G34" s="343"/>
-      <c r="H34" s="343"/>
-      <c r="I34" s="343"/>
-      <c r="J34" s="353"/>
-      <c r="K34" s="342"/>
-      <c r="L34" s="343"/>
-      <c r="M34" s="343"/>
-      <c r="N34" s="343"/>
-      <c r="O34" s="343"/>
-      <c r="P34" s="343"/>
-      <c r="Q34" s="343"/>
-      <c r="R34" s="343"/>
-      <c r="S34" s="343"/>
-      <c r="T34" s="343"/>
-      <c r="U34" s="343"/>
-      <c r="V34" s="343"/>
-      <c r="W34" s="343"/>
-      <c r="X34" s="343"/>
-      <c r="Y34" s="343"/>
-      <c r="Z34" s="343"/>
-      <c r="AA34" s="343"/>
-      <c r="AB34" s="343"/>
-      <c r="AC34" s="344"/>
+      <c r="E34" s="354"/>
+      <c r="F34" s="345"/>
+      <c r="G34" s="345"/>
+      <c r="H34" s="345"/>
+      <c r="I34" s="345"/>
+      <c r="J34" s="355"/>
+      <c r="K34" s="344"/>
+      <c r="L34" s="345"/>
+      <c r="M34" s="345"/>
+      <c r="N34" s="345"/>
+      <c r="O34" s="345"/>
+      <c r="P34" s="345"/>
+      <c r="Q34" s="345"/>
+      <c r="R34" s="345"/>
+      <c r="S34" s="345"/>
+      <c r="T34" s="345"/>
+      <c r="U34" s="345"/>
+      <c r="V34" s="345"/>
+      <c r="W34" s="345"/>
+      <c r="X34" s="345"/>
+      <c r="Y34" s="345"/>
+      <c r="Z34" s="345"/>
+      <c r="AA34" s="345"/>
+      <c r="AB34" s="345"/>
+      <c r="AC34" s="346"/>
       <c r="AD34" s="201"/>
     </row>
-    <row r="35" spans="1:30" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="318"/>
+    <row r="35" spans="1:30" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="320"/>
       <c r="B35" s="47" t="s">
         <v>312</v>
       </c>
       <c r="C35" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="334" t="s">
+      <c r="D35" s="336" t="s">
         <v>386</v>
       </c>
       <c r="E35" s="116"/>
@@ -9333,13 +9333,13 @@
       </c>
       <c r="AD35" s="73"/>
     </row>
-    <row r="36" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="318"/>
+    <row r="36" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="320"/>
       <c r="B36" s="53"/>
       <c r="C36" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="334"/>
+      <c r="D36" s="336"/>
       <c r="E36" s="117"/>
       <c r="F36" s="36"/>
       <c r="G36" s="36"/>
@@ -9405,13 +9405,13 @@
       </c>
       <c r="AD36" s="201"/>
     </row>
-    <row r="37" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="318"/>
+    <row r="37" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="320"/>
       <c r="B37" s="53"/>
       <c r="C37" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="D37" s="334"/>
+      <c r="D37" s="336"/>
       <c r="E37" s="117"/>
       <c r="F37" s="36"/>
       <c r="G37" s="36"/>
@@ -9477,13 +9477,13 @@
       </c>
       <c r="AD37" s="201"/>
     </row>
-    <row r="38" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="318"/>
+    <row r="38" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="320"/>
       <c r="B38" s="53"/>
       <c r="C38" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="D38" s="334"/>
+      <c r="D38" s="336"/>
       <c r="E38" s="117"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -9539,7 +9539,7 @@
         <v>200</v>
       </c>
       <c r="AA38" s="16">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="AB38" s="42">
         <v>200</v>
@@ -9549,13 +9549,13 @@
       </c>
       <c r="AD38" s="201"/>
     </row>
-    <row r="39" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="318"/>
+    <row r="39" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="320"/>
       <c r="B39" s="53"/>
       <c r="C39" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="D39" s="334"/>
+      <c r="D39" s="336"/>
       <c r="E39" s="117"/>
       <c r="F39" s="36"/>
       <c r="G39" s="36"/>
@@ -9621,13 +9621,13 @@
       </c>
       <c r="AD39" s="201"/>
     </row>
-    <row r="40" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="318"/>
+    <row r="40" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="320"/>
       <c r="B40" s="53"/>
       <c r="C40" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="D40" s="334"/>
+      <c r="D40" s="336"/>
       <c r="E40" s="117"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -9693,13 +9693,13 @@
       </c>
       <c r="AD40" s="201"/>
     </row>
-    <row r="41" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="318"/>
+    <row r="41" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="320"/>
       <c r="B41" s="53"/>
       <c r="C41" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="334"/>
+      <c r="D41" s="336"/>
       <c r="E41" s="117"/>
       <c r="F41" s="36"/>
       <c r="G41" s="36"/>
@@ -9765,13 +9765,13 @@
       </c>
       <c r="AD41" s="201"/>
     </row>
-    <row r="42" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="318"/>
+    <row r="42" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="320"/>
       <c r="B42" s="53"/>
       <c r="C42" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D42" s="334"/>
+      <c r="D42" s="336"/>
       <c r="E42" s="117"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -9811,13 +9811,13 @@
       </c>
       <c r="AD42" s="202"/>
     </row>
-    <row r="43" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="318"/>
+    <row r="43" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="320"/>
       <c r="B43" s="53"/>
       <c r="C43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="334"/>
+      <c r="D43" s="336"/>
       <c r="E43" s="117"/>
       <c r="F43" s="36"/>
       <c r="G43" s="36"/>
@@ -9883,13 +9883,13 @@
       </c>
       <c r="AD43" s="201"/>
     </row>
-    <row r="44" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="318"/>
+    <row r="44" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="320"/>
       <c r="B44" s="53"/>
       <c r="C44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="334"/>
+      <c r="D44" s="336"/>
       <c r="E44" s="117"/>
       <c r="F44" s="36"/>
       <c r="G44" s="36"/>
@@ -9947,13 +9947,13 @@
       </c>
       <c r="AD44" s="201"/>
     </row>
-    <row r="45" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="318"/>
+    <row r="45" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="320"/>
       <c r="B45" s="53"/>
       <c r="C45" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="334"/>
+      <c r="D45" s="336"/>
       <c r="E45" s="117"/>
       <c r="F45" s="36"/>
       <c r="G45" s="36"/>
@@ -10013,13 +10013,13 @@
         <v>338</v>
       </c>
     </row>
-    <row r="46" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="318"/>
+    <row r="46" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="320"/>
       <c r="B46" s="53"/>
       <c r="C46" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D46" s="334"/>
+      <c r="D46" s="336"/>
       <c r="E46" s="117"/>
       <c r="F46" s="36"/>
       <c r="G46" s="36"/>
@@ -10067,13 +10067,13 @@
       </c>
       <c r="AD46" s="201"/>
     </row>
-    <row r="47" spans="1:30" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="318"/>
+    <row r="47" spans="1:30" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="320"/>
       <c r="B47" s="74"/>
       <c r="C47" s="75" t="s">
         <v>288</v>
       </c>
-      <c r="D47" s="334"/>
+      <c r="D47" s="336"/>
       <c r="E47" s="119"/>
       <c r="F47" s="76"/>
       <c r="G47" s="76"/>
@@ -10107,15 +10107,15 @@
       </c>
       <c r="AD47" s="203"/>
     </row>
-    <row r="48" spans="1:30" ht="15.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="318"/>
+    <row r="48" spans="1:30" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="320"/>
       <c r="B48" s="53" t="s">
         <v>23</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D48" s="334"/>
+      <c r="D48" s="336"/>
       <c r="E48" s="117"/>
       <c r="F48" s="36"/>
       <c r="G48" s="36"/>
@@ -10181,13 +10181,13 @@
       </c>
       <c r="AD48" s="201"/>
     </row>
-    <row r="49" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="318"/>
+    <row r="49" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="320"/>
       <c r="B49" s="53"/>
       <c r="C49" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D49" s="334"/>
+      <c r="D49" s="336"/>
       <c r="E49" s="117"/>
       <c r="F49" s="36"/>
       <c r="G49" s="36"/>
@@ -10219,13 +10219,13 @@
       </c>
       <c r="AD49" s="201"/>
     </row>
-    <row r="50" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="318"/>
+    <row r="50" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="320"/>
       <c r="B50" s="53"/>
       <c r="C50" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="D50" s="334"/>
+      <c r="D50" s="336"/>
       <c r="E50" s="117"/>
       <c r="F50" s="36"/>
       <c r="G50" s="36"/>
@@ -10257,13 +10257,13 @@
       </c>
       <c r="AD50" s="201"/>
     </row>
-    <row r="51" spans="1:30" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="318"/>
+    <row r="51" spans="1:30" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="320"/>
       <c r="B51" s="74"/>
       <c r="C51" s="75" t="s">
         <v>292</v>
       </c>
-      <c r="D51" s="334"/>
+      <c r="D51" s="336"/>
       <c r="E51" s="119"/>
       <c r="F51" s="76"/>
       <c r="G51" s="76"/>
@@ -10284,16 +10284,16 @@
       <c r="V51" s="77"/>
       <c r="W51" s="158"/>
       <c r="X51" s="111"/>
-      <c r="Y51" s="354" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z51" s="354" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA51" s="354" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB51" s="355" t="s">
+      <c r="Y51" s="315" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z51" s="315" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA51" s="315" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB51" s="316" t="s">
         <v>10</v>
       </c>
       <c r="AC51" s="243" t="s">
@@ -10301,15 +10301,15 @@
       </c>
       <c r="AD51" s="203"/>
     </row>
-    <row r="52" spans="1:30" ht="15.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="318"/>
+    <row r="52" spans="1:30" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="320"/>
       <c r="B52" s="47" t="s">
         <v>101</v>
       </c>
       <c r="C52" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="D52" s="334"/>
+      <c r="D52" s="336"/>
       <c r="E52" s="116"/>
       <c r="F52" s="49"/>
       <c r="G52" s="49"/>
@@ -10377,13 +10377,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="318"/>
+    <row r="53" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="320"/>
       <c r="B53" s="53"/>
       <c r="C53" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="334"/>
+      <c r="D53" s="336"/>
       <c r="E53" s="117"/>
       <c r="F53" s="36"/>
       <c r="G53" s="36"/>
@@ -10451,13 +10451,13 @@
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:30" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="318"/>
+    <row r="54" spans="1:30" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="320"/>
       <c r="B54" s="79"/>
       <c r="C54" s="75" t="s">
         <v>178</v>
       </c>
-      <c r="D54" s="334"/>
+      <c r="D54" s="336"/>
       <c r="E54" s="120"/>
       <c r="F54" s="80"/>
       <c r="G54" s="80"/>
@@ -10497,15 +10497,15 @@
       </c>
       <c r="AD54" s="204"/>
     </row>
-    <row r="55" spans="1:30" s="44" customFormat="1" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="318"/>
+    <row r="55" spans="1:30" s="44" customFormat="1" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="320"/>
       <c r="B55" s="81" t="s">
         <v>308</v>
       </c>
       <c r="C55" s="82" t="s">
         <v>309</v>
       </c>
-      <c r="D55" s="334"/>
+      <c r="D55" s="336"/>
       <c r="E55" s="121"/>
       <c r="F55" s="83"/>
       <c r="G55" s="83"/>
@@ -10537,15 +10537,15 @@
       </c>
       <c r="AD55" s="205"/>
     </row>
-    <row r="56" spans="1:30" ht="15.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="318"/>
+    <row r="56" spans="1:30" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="320"/>
       <c r="B56" s="47" t="s">
         <v>36</v>
       </c>
       <c r="C56" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="334"/>
+      <c r="D56" s="336"/>
       <c r="E56" s="116" t="s">
         <v>19</v>
       </c>
@@ -10623,13 +10623,13 @@
       </c>
       <c r="AD56" s="73"/>
     </row>
-    <row r="57" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="318"/>
+    <row r="57" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="320"/>
       <c r="B57" s="54"/>
       <c r="C57" s="45" t="s">
         <v>284</v>
       </c>
-      <c r="D57" s="334"/>
+      <c r="D57" s="336"/>
       <c r="E57" s="122"/>
       <c r="F57" s="46" t="s">
         <v>10</v>
@@ -10705,13 +10705,13 @@
       </c>
       <c r="AD57" s="206"/>
     </row>
-    <row r="58" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="318"/>
+    <row r="58" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="320"/>
       <c r="B58" s="54"/>
       <c r="C58" s="45" t="s">
         <v>285</v>
       </c>
-      <c r="D58" s="334"/>
+      <c r="D58" s="336"/>
       <c r="E58" s="124" t="s">
         <v>10</v>
       </c>
@@ -10789,13 +10789,13 @@
       </c>
       <c r="AD58" s="206"/>
     </row>
-    <row r="59" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="318"/>
+    <row r="59" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="320"/>
       <c r="B59" s="53"/>
       <c r="C59" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="D59" s="334"/>
+      <c r="D59" s="336"/>
       <c r="E59" s="117" t="s">
         <v>10</v>
       </c>
@@ -10873,13 +10873,13 @@
       </c>
       <c r="AD59" s="201"/>
     </row>
-    <row r="60" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="318"/>
+    <row r="60" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="320"/>
       <c r="B60" s="53"/>
       <c r="C60" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="D60" s="334"/>
+      <c r="D60" s="336"/>
       <c r="E60" s="125"/>
       <c r="F60" s="41"/>
       <c r="G60" s="41"/>
@@ -10931,13 +10931,13 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="318"/>
+    <row r="61" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="320"/>
       <c r="B61" s="53"/>
       <c r="C61" s="224" t="s">
         <v>287</v>
       </c>
-      <c r="D61" s="334"/>
+      <c r="D61" s="336"/>
       <c r="E61" s="117" t="s">
         <v>19</v>
       </c>
@@ -11015,13 +11015,13 @@
       </c>
       <c r="AD61" s="201"/>
     </row>
-    <row r="62" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="318"/>
+    <row r="62" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="320"/>
       <c r="B62" s="53"/>
       <c r="C62" s="225" t="s">
         <v>245</v>
       </c>
-      <c r="D62" s="334"/>
+      <c r="D62" s="336"/>
       <c r="E62" s="125"/>
       <c r="F62" s="41"/>
       <c r="G62" s="41"/>
@@ -11073,13 +11073,13 @@
         <v>243</v>
       </c>
     </row>
-    <row r="63" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="318"/>
+    <row r="63" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="320"/>
       <c r="B63" s="53"/>
       <c r="C63" s="224" t="s">
         <v>38</v>
       </c>
-      <c r="D63" s="334"/>
+      <c r="D63" s="336"/>
       <c r="E63" s="117" t="s">
         <v>10</v>
       </c>
@@ -11157,13 +11157,13 @@
       </c>
       <c r="AD63" s="201"/>
     </row>
-    <row r="64" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="318"/>
+    <row r="64" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="320"/>
       <c r="B64" s="53"/>
       <c r="C64" s="224" t="s">
         <v>246</v>
       </c>
-      <c r="D64" s="334"/>
+      <c r="D64" s="336"/>
       <c r="E64" s="117" t="s">
         <v>10</v>
       </c>
@@ -11241,13 +11241,13 @@
       </c>
       <c r="AD64" s="201"/>
     </row>
-    <row r="65" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="318"/>
+    <row r="65" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="320"/>
       <c r="B65" s="53"/>
       <c r="C65" s="224" t="s">
         <v>247</v>
       </c>
-      <c r="D65" s="334"/>
+      <c r="D65" s="336"/>
       <c r="E65" s="117" t="s">
         <v>10</v>
       </c>
@@ -11325,13 +11325,13 @@
       </c>
       <c r="AD65" s="201"/>
     </row>
-    <row r="66" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="318"/>
+    <row r="66" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="320"/>
       <c r="B66" s="53"/>
       <c r="C66" s="224" t="s">
         <v>248</v>
       </c>
-      <c r="D66" s="334"/>
+      <c r="D66" s="336"/>
       <c r="E66" s="117" t="s">
         <v>10</v>
       </c>
@@ -11409,13 +11409,13 @@
       </c>
       <c r="AD66" s="201"/>
     </row>
-    <row r="67" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="318"/>
+    <row r="67" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="320"/>
       <c r="B67" s="53"/>
       <c r="C67" s="224" t="s">
         <v>238</v>
       </c>
-      <c r="D67" s="334"/>
+      <c r="D67" s="336"/>
       <c r="E67" s="126"/>
       <c r="F67" s="40"/>
       <c r="G67" s="40"/>
@@ -11461,13 +11461,13 @@
       </c>
       <c r="AD67" s="201"/>
     </row>
-    <row r="68" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="318"/>
+    <row r="68" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="320"/>
       <c r="B68" s="53"/>
       <c r="C68" s="225" t="s">
         <v>39</v>
       </c>
-      <c r="D68" s="334"/>
+      <c r="D68" s="336"/>
       <c r="E68" s="125"/>
       <c r="F68" s="41"/>
       <c r="G68" s="41"/>
@@ -11517,13 +11517,13 @@
       </c>
       <c r="AD68" s="201"/>
     </row>
-    <row r="69" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="318"/>
+    <row r="69" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="320"/>
       <c r="B69" s="53"/>
       <c r="C69" s="225" t="s">
         <v>40</v>
       </c>
-      <c r="D69" s="334"/>
+      <c r="D69" s="336"/>
       <c r="E69" s="125"/>
       <c r="F69" s="41"/>
       <c r="G69" s="41"/>
@@ -11573,13 +11573,13 @@
       </c>
       <c r="AD69" s="201"/>
     </row>
-    <row r="70" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="318"/>
+    <row r="70" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="320"/>
       <c r="B70" s="53"/>
       <c r="C70" s="224" t="s">
         <v>250</v>
       </c>
-      <c r="D70" s="334"/>
+      <c r="D70" s="336"/>
       <c r="E70" s="117" t="s">
         <v>10</v>
       </c>
@@ -11657,13 +11657,13 @@
       </c>
       <c r="AD70" s="201"/>
     </row>
-    <row r="71" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="318"/>
+    <row r="71" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="320"/>
       <c r="B71" s="53"/>
       <c r="C71" s="224" t="s">
         <v>249</v>
       </c>
-      <c r="D71" s="334"/>
+      <c r="D71" s="336"/>
       <c r="E71" s="117" t="s">
         <v>10</v>
       </c>
@@ -11741,13 +11741,13 @@
       </c>
       <c r="AD71" s="201"/>
     </row>
-    <row r="72" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="318"/>
+    <row r="72" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="320"/>
       <c r="B72" s="53"/>
       <c r="C72" s="224" t="s">
         <v>251</v>
       </c>
-      <c r="D72" s="334"/>
+      <c r="D72" s="336"/>
       <c r="E72" s="117" t="s">
         <v>10</v>
       </c>
@@ -11825,13 +11825,13 @@
       </c>
       <c r="AD72" s="201"/>
     </row>
-    <row r="73" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="318"/>
+    <row r="73" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="320"/>
       <c r="B73" s="53"/>
       <c r="C73" s="224" t="s">
         <v>252</v>
       </c>
-      <c r="D73" s="334"/>
+      <c r="D73" s="336"/>
       <c r="E73" s="117" t="s">
         <v>10</v>
       </c>
@@ -11909,13 +11909,13 @@
       </c>
       <c r="AD73" s="201"/>
     </row>
-    <row r="74" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="318"/>
+    <row r="74" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="320"/>
       <c r="B74" s="53"/>
       <c r="C74" s="224" t="s">
         <v>41</v>
       </c>
-      <c r="D74" s="334"/>
+      <c r="D74" s="336"/>
       <c r="E74" s="126"/>
       <c r="F74" s="40"/>
       <c r="G74" s="40"/>
@@ -11965,13 +11965,13 @@
       </c>
       <c r="AD74" s="201"/>
     </row>
-    <row r="75" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="318"/>
+    <row r="75" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="320"/>
       <c r="B75" s="53"/>
       <c r="C75" s="224" t="s">
         <v>275</v>
       </c>
-      <c r="D75" s="334"/>
+      <c r="D75" s="336"/>
       <c r="E75" s="126"/>
       <c r="F75" s="40"/>
       <c r="G75" s="40"/>
@@ -12013,13 +12013,13 @@
       </c>
       <c r="AD75" s="201"/>
     </row>
-    <row r="76" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="318"/>
+    <row r="76" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="320"/>
       <c r="B76" s="53"/>
       <c r="C76" s="224" t="s">
         <v>290</v>
       </c>
-      <c r="D76" s="334"/>
+      <c r="D76" s="336"/>
       <c r="E76" s="126"/>
       <c r="F76" s="40"/>
       <c r="G76" s="40"/>
@@ -12065,13 +12065,13 @@
       </c>
       <c r="AD76" s="201"/>
     </row>
-    <row r="77" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="318"/>
+    <row r="77" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="320"/>
       <c r="B77" s="53"/>
       <c r="C77" s="224" t="s">
         <v>42</v>
       </c>
-      <c r="D77" s="334"/>
+      <c r="D77" s="336"/>
       <c r="E77" s="117" t="s">
         <v>19</v>
       </c>
@@ -12149,13 +12149,13 @@
       </c>
       <c r="AD77" s="201"/>
     </row>
-    <row r="78" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="318"/>
+    <row r="78" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="320"/>
       <c r="B78" s="53"/>
       <c r="C78" s="224" t="s">
         <v>231</v>
       </c>
-      <c r="D78" s="334"/>
+      <c r="D78" s="336"/>
       <c r="E78" s="117" t="s">
         <v>10</v>
       </c>
@@ -12233,13 +12233,13 @@
       </c>
       <c r="AD78" s="201"/>
     </row>
-    <row r="79" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="318"/>
+    <row r="79" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="320"/>
       <c r="B79" s="53"/>
       <c r="C79" s="224" t="s">
         <v>232</v>
       </c>
-      <c r="D79" s="334"/>
+      <c r="D79" s="336"/>
       <c r="E79" s="126"/>
       <c r="F79" s="40"/>
       <c r="G79" s="40"/>
@@ -12281,13 +12281,13 @@
       </c>
       <c r="AD79" s="201"/>
     </row>
-    <row r="80" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="318"/>
+    <row r="80" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="320"/>
       <c r="B80" s="53"/>
       <c r="C80" s="224" t="s">
         <v>43</v>
       </c>
-      <c r="D80" s="334"/>
+      <c r="D80" s="336"/>
       <c r="E80" s="117" t="s">
         <v>19</v>
       </c>
@@ -12367,13 +12367,13 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="318"/>
+    <row r="81" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="320"/>
       <c r="B81" s="53"/>
       <c r="C81" s="224" t="s">
         <v>113</v>
       </c>
-      <c r="D81" s="334"/>
+      <c r="D81" s="336"/>
       <c r="E81" s="117" t="s">
         <v>10</v>
       </c>
@@ -12451,13 +12451,13 @@
       </c>
       <c r="AD81" s="201"/>
     </row>
-    <row r="82" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="318"/>
+    <row r="82" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="320"/>
       <c r="B82" s="53"/>
       <c r="C82" s="224" t="s">
         <v>44</v>
       </c>
-      <c r="D82" s="334"/>
+      <c r="D82" s="336"/>
       <c r="E82" s="117" t="s">
         <v>19</v>
       </c>
@@ -12537,13 +12537,13 @@
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="318"/>
+    <row r="83" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="320"/>
       <c r="B83" s="53"/>
       <c r="C83" s="224" t="s">
         <v>324</v>
       </c>
-      <c r="D83" s="334"/>
+      <c r="D83" s="336"/>
       <c r="E83" s="126"/>
       <c r="F83" s="40"/>
       <c r="G83" s="40"/>
@@ -12585,13 +12585,13 @@
       </c>
       <c r="AD83" s="201"/>
     </row>
-    <row r="84" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="318"/>
+    <row r="84" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="320"/>
       <c r="B84" s="290"/>
       <c r="C84" s="291" t="s">
         <v>260</v>
       </c>
-      <c r="D84" s="334"/>
+      <c r="D84" s="336"/>
       <c r="E84" s="36" t="s">
         <v>384</v>
       </c>
@@ -12669,13 +12669,13 @@
       </c>
       <c r="AD84" s="296"/>
     </row>
-    <row r="85" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="318"/>
+    <row r="85" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="320"/>
       <c r="B85" s="53"/>
       <c r="C85" s="224" t="s">
         <v>373</v>
       </c>
-      <c r="D85" s="334"/>
+      <c r="D85" s="336"/>
       <c r="E85" s="228"/>
       <c r="F85" s="40"/>
       <c r="G85" s="40"/>
@@ -12705,13 +12705,13 @@
       <c r="AC85" s="150"/>
       <c r="AD85" s="201"/>
     </row>
-    <row r="86" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="318"/>
+    <row r="86" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="320"/>
       <c r="B86" s="53"/>
       <c r="C86" s="224" t="s">
         <v>254</v>
       </c>
-      <c r="D86" s="334"/>
+      <c r="D86" s="336"/>
       <c r="E86" s="127" t="s">
         <v>19</v>
       </c>
@@ -12789,13 +12789,13 @@
       </c>
       <c r="AD86" s="201"/>
     </row>
-    <row r="87" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="318"/>
+    <row r="87" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="320"/>
       <c r="B87" s="53"/>
       <c r="C87" s="224" t="s">
         <v>211</v>
       </c>
-      <c r="D87" s="334"/>
+      <c r="D87" s="336"/>
       <c r="E87" s="126"/>
       <c r="F87" s="40"/>
       <c r="G87" s="40"/>
@@ -12849,13 +12849,13 @@
       </c>
       <c r="AD87" s="201"/>
     </row>
-    <row r="88" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="318"/>
+    <row r="88" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="320"/>
       <c r="B88" s="53"/>
       <c r="C88" s="224" t="s">
         <v>114</v>
       </c>
-      <c r="D88" s="334"/>
+      <c r="D88" s="336"/>
       <c r="E88" s="126"/>
       <c r="F88" s="40"/>
       <c r="G88" s="40"/>
@@ -12905,13 +12905,13 @@
       </c>
       <c r="AD88" s="201"/>
     </row>
-    <row r="89" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="318"/>
+    <row r="89" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="320"/>
       <c r="B89" s="53"/>
       <c r="C89" s="224" t="s">
         <v>115</v>
       </c>
-      <c r="D89" s="334"/>
+      <c r="D89" s="336"/>
       <c r="E89" s="126"/>
       <c r="F89" s="40"/>
       <c r="G89" s="40"/>
@@ -12957,13 +12957,13 @@
       </c>
       <c r="AD89" s="201"/>
     </row>
-    <row r="90" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="318"/>
+    <row r="90" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="320"/>
       <c r="B90" s="53"/>
       <c r="C90" s="224" t="s">
         <v>236</v>
       </c>
-      <c r="D90" s="334"/>
+      <c r="D90" s="336"/>
       <c r="E90" s="126"/>
       <c r="F90" s="40"/>
       <c r="G90" s="40"/>
@@ -13013,13 +13013,13 @@
       </c>
       <c r="AD90" s="201"/>
     </row>
-    <row r="91" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="318"/>
+    <row r="91" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="320"/>
       <c r="B91" s="53"/>
       <c r="C91" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="D91" s="334"/>
+      <c r="D91" s="336"/>
       <c r="E91" s="126"/>
       <c r="F91" s="40"/>
       <c r="G91" s="40"/>
@@ -13069,13 +13069,13 @@
       </c>
       <c r="AD91" s="201"/>
     </row>
-    <row r="92" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="318"/>
+    <row r="92" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="320"/>
       <c r="B92" s="55"/>
       <c r="C92" s="86" t="s">
         <v>374</v>
       </c>
-      <c r="D92" s="334"/>
+      <c r="D92" s="336"/>
       <c r="E92" s="275"/>
       <c r="F92" s="276"/>
       <c r="G92" s="276"/>
@@ -13105,13 +13105,13 @@
       <c r="AC92" s="150"/>
       <c r="AD92" s="207"/>
     </row>
-    <row r="93" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="318"/>
+    <row r="93" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="320"/>
       <c r="B93" s="55"/>
       <c r="C93" s="86" t="s">
         <v>305</v>
       </c>
-      <c r="D93" s="334"/>
+      <c r="D93" s="336"/>
       <c r="E93" s="129" t="s">
         <v>258</v>
       </c>
@@ -13189,13 +13189,13 @@
       </c>
       <c r="AD93" s="207"/>
     </row>
-    <row r="94" spans="1:30" s="44" customFormat="1" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="318"/>
+    <row r="94" spans="1:30" s="44" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="320"/>
       <c r="B94" s="85"/>
       <c r="C94" s="86" t="s">
         <v>239</v>
       </c>
-      <c r="D94" s="334"/>
+      <c r="D94" s="336"/>
       <c r="E94" s="129" t="s">
         <v>240</v>
       </c>
@@ -13273,15 +13273,15 @@
       </c>
       <c r="AD94" s="208"/>
     </row>
-    <row r="95" spans="1:30" ht="15.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="318"/>
+    <row r="95" spans="1:30" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="320"/>
       <c r="B95" s="47" t="s">
         <v>46</v>
       </c>
       <c r="C95" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="D95" s="334"/>
+      <c r="D95" s="336"/>
       <c r="E95" s="116"/>
       <c r="F95" s="49"/>
       <c r="G95" s="49"/>
@@ -13347,13 +13347,13 @@
       </c>
       <c r="AD95" s="73"/>
     </row>
-    <row r="96" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="318"/>
+    <row r="96" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="320"/>
       <c r="B96" s="54"/>
       <c r="C96" s="45" t="s">
         <v>325</v>
       </c>
-      <c r="D96" s="334"/>
+      <c r="D96" s="336"/>
       <c r="E96" s="124"/>
       <c r="F96" s="46"/>
       <c r="G96" s="46"/>
@@ -13393,13 +13393,13 @@
       </c>
       <c r="AD96" s="206"/>
     </row>
-    <row r="97" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="318"/>
+    <row r="97" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="320"/>
       <c r="B97" s="53"/>
       <c r="C97" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D97" s="334"/>
+      <c r="D97" s="336"/>
       <c r="E97" s="117"/>
       <c r="F97" s="36"/>
       <c r="G97" s="36"/>
@@ -13465,13 +13465,13 @@
       </c>
       <c r="AD97" s="201"/>
     </row>
-    <row r="98" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="318"/>
+    <row r="98" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="320"/>
       <c r="B98" s="53"/>
       <c r="C98" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D98" s="334"/>
+      <c r="D98" s="336"/>
       <c r="E98" s="117"/>
       <c r="F98" s="36"/>
       <c r="G98" s="36"/>
@@ -13537,13 +13537,13 @@
       </c>
       <c r="AD98" s="201"/>
     </row>
-    <row r="99" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="318"/>
+    <row r="99" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="320"/>
       <c r="B99" s="53"/>
       <c r="C99" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D99" s="334"/>
+      <c r="D99" s="336"/>
       <c r="E99" s="117"/>
       <c r="F99" s="36"/>
       <c r="G99" s="36"/>
@@ -13609,13 +13609,13 @@
       </c>
       <c r="AD99" s="201"/>
     </row>
-    <row r="100" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="318"/>
+    <row r="100" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="320"/>
       <c r="B100" s="53"/>
       <c r="C100" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D100" s="334"/>
+      <c r="D100" s="336"/>
       <c r="E100" s="117"/>
       <c r="F100" s="36"/>
       <c r="G100" s="36"/>
@@ -13683,13 +13683,13 @@
         <v>53</v>
       </c>
     </row>
-    <row r="101" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="318"/>
+    <row r="101" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="320"/>
       <c r="B101" s="53"/>
       <c r="C101" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D101" s="334"/>
+      <c r="D101" s="336"/>
       <c r="E101" s="117"/>
       <c r="F101" s="36"/>
       <c r="G101" s="36"/>
@@ -13755,13 +13755,13 @@
       </c>
       <c r="AD101" s="201"/>
     </row>
-    <row r="102" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="318"/>
+    <row r="102" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="320"/>
       <c r="B102" s="53"/>
       <c r="C102" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D102" s="334"/>
+      <c r="D102" s="336"/>
       <c r="E102" s="117"/>
       <c r="F102" s="36"/>
       <c r="G102" s="36"/>
@@ -13829,13 +13829,13 @@
         <v>53</v>
       </c>
     </row>
-    <row r="103" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="318"/>
+    <row r="103" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="320"/>
       <c r="B103" s="53"/>
       <c r="C103" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D103" s="334"/>
+      <c r="D103" s="336"/>
       <c r="E103" s="117"/>
       <c r="F103" s="36"/>
       <c r="G103" s="36"/>
@@ -13903,13 +13903,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="318"/>
+    <row r="104" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="320"/>
       <c r="B104" s="53"/>
       <c r="C104" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D104" s="334"/>
+      <c r="D104" s="336"/>
       <c r="E104" s="117"/>
       <c r="F104" s="36"/>
       <c r="G104" s="36"/>
@@ -13977,13 +13977,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="318"/>
+    <row r="105" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="320"/>
       <c r="B105" s="53"/>
       <c r="C105" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D105" s="334"/>
+      <c r="D105" s="336"/>
       <c r="E105" s="117"/>
       <c r="F105" s="36"/>
       <c r="G105" s="36"/>
@@ -14051,13 +14051,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="318"/>
+    <row r="106" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="320"/>
       <c r="B106" s="53"/>
       <c r="C106" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D106" s="334"/>
+      <c r="D106" s="336"/>
       <c r="E106" s="117"/>
       <c r="F106" s="36"/>
       <c r="G106" s="36"/>
@@ -14097,13 +14097,13 @@
       </c>
       <c r="AD106" s="201"/>
     </row>
-    <row r="107" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="318"/>
+    <row r="107" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="320"/>
       <c r="B107" s="53"/>
       <c r="C107" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D107" s="334"/>
+      <c r="D107" s="336"/>
       <c r="E107" s="117"/>
       <c r="F107" s="36"/>
       <c r="G107" s="36"/>
@@ -14151,13 +14151,13 @@
       </c>
       <c r="AD107" s="201"/>
     </row>
-    <row r="108" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="318"/>
+    <row r="108" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="320"/>
       <c r="B108" s="53"/>
       <c r="C108" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D108" s="334"/>
+      <c r="D108" s="336"/>
       <c r="E108" s="117"/>
       <c r="F108" s="36"/>
       <c r="G108" s="36"/>
@@ -14223,13 +14223,13 @@
       </c>
       <c r="AD108" s="201"/>
     </row>
-    <row r="109" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="318"/>
+    <row r="109" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="320"/>
       <c r="B109" s="53"/>
       <c r="C109" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D109" s="334"/>
+      <c r="D109" s="336"/>
       <c r="E109" s="117"/>
       <c r="F109" s="36"/>
       <c r="G109" s="36"/>
@@ -14287,13 +14287,13 @@
       </c>
       <c r="AD109" s="201"/>
     </row>
-    <row r="110" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="318"/>
+    <row r="110" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="320"/>
       <c r="B110" s="53"/>
       <c r="C110" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="D110" s="334"/>
+      <c r="D110" s="336"/>
       <c r="E110" s="117"/>
       <c r="F110" s="36"/>
       <c r="G110" s="36"/>
@@ -14359,13 +14359,13 @@
       </c>
       <c r="AD110" s="209"/>
     </row>
-    <row r="111" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="318"/>
+    <row r="111" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="320"/>
       <c r="B111" s="53"/>
       <c r="C111" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="D111" s="334"/>
+      <c r="D111" s="336"/>
       <c r="E111" s="117"/>
       <c r="F111" s="36"/>
       <c r="G111" s="36"/>
@@ -14431,13 +14431,13 @@
       </c>
       <c r="AD111" s="201"/>
     </row>
-    <row r="112" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="318"/>
+    <row r="112" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="320"/>
       <c r="B112" s="53"/>
       <c r="C112" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="D112" s="334"/>
+      <c r="D112" s="336"/>
       <c r="E112" s="117"/>
       <c r="F112" s="36"/>
       <c r="G112" s="36"/>
@@ -14503,13 +14503,13 @@
       </c>
       <c r="AD112" s="201"/>
     </row>
-    <row r="113" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="318"/>
+    <row r="113" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="320"/>
       <c r="B113" s="53"/>
       <c r="C113" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="D113" s="334"/>
+      <c r="D113" s="336"/>
       <c r="E113" s="117"/>
       <c r="F113" s="36"/>
       <c r="G113" s="36"/>
@@ -14575,13 +14575,13 @@
       </c>
       <c r="AD113" s="209"/>
     </row>
-    <row r="114" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="318"/>
+    <row r="114" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="320"/>
       <c r="B114" s="53"/>
       <c r="C114" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="D114" s="334"/>
+      <c r="D114" s="336"/>
       <c r="E114" s="117"/>
       <c r="F114" s="36"/>
       <c r="G114" s="36"/>
@@ -14647,13 +14647,13 @@
       </c>
       <c r="AD114" s="201"/>
     </row>
-    <row r="115" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="318"/>
+    <row r="115" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="320"/>
       <c r="B115" s="53"/>
       <c r="C115" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="D115" s="334"/>
+      <c r="D115" s="336"/>
       <c r="E115" s="117"/>
       <c r="F115" s="36"/>
       <c r="G115" s="36"/>
@@ -14719,13 +14719,13 @@
       </c>
       <c r="AD115" s="209"/>
     </row>
-    <row r="116" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="318"/>
+    <row r="116" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="320"/>
       <c r="B116" s="53"/>
       <c r="C116" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="D116" s="334"/>
+      <c r="D116" s="336"/>
       <c r="E116" s="117"/>
       <c r="F116" s="36"/>
       <c r="G116" s="36"/>
@@ -14791,13 +14791,13 @@
       </c>
       <c r="AD116" s="201"/>
     </row>
-    <row r="117" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="318"/>
+    <row r="117" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="320"/>
       <c r="B117" s="53"/>
       <c r="C117" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="D117" s="334"/>
+      <c r="D117" s="336"/>
       <c r="E117" s="117"/>
       <c r="F117" s="36"/>
       <c r="G117" s="36"/>
@@ -14863,13 +14863,13 @@
       </c>
       <c r="AD117" s="201"/>
     </row>
-    <row r="118" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="318"/>
+    <row r="118" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="320"/>
       <c r="B118" s="53"/>
       <c r="C118" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D118" s="334"/>
+      <c r="D118" s="336"/>
       <c r="E118" s="117"/>
       <c r="F118" s="36"/>
       <c r="G118" s="36"/>
@@ -14937,13 +14937,13 @@
         <v>174</v>
       </c>
     </row>
-    <row r="119" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="318"/>
+    <row r="119" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="320"/>
       <c r="B119" s="53"/>
       <c r="C119" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D119" s="334"/>
+      <c r="D119" s="336"/>
       <c r="E119" s="117"/>
       <c r="F119" s="36"/>
       <c r="G119" s="36"/>
@@ -15011,13 +15011,13 @@
         <v>174</v>
       </c>
     </row>
-    <row r="120" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="318"/>
+    <row r="120" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="320"/>
       <c r="B120" s="53"/>
       <c r="C120" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D120" s="334"/>
+      <c r="D120" s="336"/>
       <c r="E120" s="117"/>
       <c r="F120" s="36"/>
       <c r="G120" s="36"/>
@@ -15083,13 +15083,13 @@
       </c>
       <c r="AD120" s="201"/>
     </row>
-    <row r="121" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="318"/>
+    <row r="121" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="320"/>
       <c r="B121" s="53"/>
       <c r="C121" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D121" s="334"/>
+      <c r="D121" s="336"/>
       <c r="E121" s="117"/>
       <c r="F121" s="36"/>
       <c r="G121" s="36"/>
@@ -15155,13 +15155,13 @@
       </c>
       <c r="AD121" s="201"/>
     </row>
-    <row r="122" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="318"/>
+    <row r="122" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="320"/>
       <c r="B122" s="53"/>
       <c r="C122" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D122" s="334"/>
+      <c r="D122" s="336"/>
       <c r="E122" s="117"/>
       <c r="F122" s="36"/>
       <c r="G122" s="36"/>
@@ -15229,13 +15229,13 @@
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="318"/>
+    <row r="123" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="320"/>
       <c r="B123" s="53"/>
       <c r="C123" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D123" s="334"/>
+      <c r="D123" s="336"/>
       <c r="E123" s="117"/>
       <c r="F123" s="36"/>
       <c r="G123" s="36"/>
@@ -15303,13 +15303,13 @@
         <v>174</v>
       </c>
     </row>
-    <row r="124" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="318"/>
+    <row r="124" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="320"/>
       <c r="B124" s="53"/>
       <c r="C124" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D124" s="334"/>
+      <c r="D124" s="336"/>
       <c r="E124" s="117"/>
       <c r="F124" s="36"/>
       <c r="G124" s="36"/>
@@ -15377,13 +15377,13 @@
         <v>174</v>
       </c>
     </row>
-    <row r="125" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="318"/>
+    <row r="125" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="320"/>
       <c r="B125" s="53"/>
       <c r="C125" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D125" s="334"/>
+      <c r="D125" s="336"/>
       <c r="E125" s="117"/>
       <c r="F125" s="36"/>
       <c r="G125" s="36"/>
@@ -15425,13 +15425,13 @@
       </c>
       <c r="AD125" s="201"/>
     </row>
-    <row r="126" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="318"/>
+    <row r="126" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="320"/>
       <c r="B126" s="53"/>
       <c r="C126" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D126" s="334"/>
+      <c r="D126" s="336"/>
       <c r="E126" s="117"/>
       <c r="F126" s="36"/>
       <c r="G126" s="36"/>
@@ -15473,13 +15473,13 @@
       </c>
       <c r="AD126" s="201"/>
     </row>
-    <row r="127" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="318"/>
+    <row r="127" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="320"/>
       <c r="B127" s="53"/>
       <c r="C127" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D127" s="334"/>
+      <c r="D127" s="336"/>
       <c r="E127" s="117"/>
       <c r="F127" s="36"/>
       <c r="G127" s="36"/>
@@ -15521,13 +15521,13 @@
       </c>
       <c r="AD127" s="201"/>
     </row>
-    <row r="128" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="318"/>
+    <row r="128" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="320"/>
       <c r="B128" s="53"/>
       <c r="C128" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D128" s="334"/>
+      <c r="D128" s="336"/>
       <c r="E128" s="117"/>
       <c r="F128" s="36"/>
       <c r="G128" s="36"/>
@@ -15569,13 +15569,13 @@
       </c>
       <c r="AD128" s="201"/>
     </row>
-    <row r="129" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="318"/>
+    <row r="129" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="320"/>
       <c r="B129" s="53"/>
       <c r="C129" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D129" s="334"/>
+      <c r="D129" s="336"/>
       <c r="E129" s="117"/>
       <c r="F129" s="36"/>
       <c r="G129" s="36"/>
@@ -15617,13 +15617,13 @@
       </c>
       <c r="AD129" s="201"/>
     </row>
-    <row r="130" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="318"/>
+    <row r="130" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="320"/>
       <c r="B130" s="53"/>
       <c r="C130" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D130" s="334"/>
+      <c r="D130" s="336"/>
       <c r="E130" s="117"/>
       <c r="F130" s="36"/>
       <c r="G130" s="36"/>
@@ -15665,13 +15665,13 @@
       </c>
       <c r="AD130" s="201"/>
     </row>
-    <row r="131" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="318"/>
+    <row r="131" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="320"/>
       <c r="B131" s="53"/>
       <c r="C131" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D131" s="334"/>
+      <c r="D131" s="336"/>
       <c r="E131" s="117"/>
       <c r="F131" s="36"/>
       <c r="G131" s="36"/>
@@ -15713,13 +15713,13 @@
       </c>
       <c r="AD131" s="201"/>
     </row>
-    <row r="132" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="318"/>
+    <row r="132" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="320"/>
       <c r="B132" s="53"/>
       <c r="C132" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D132" s="334"/>
+      <c r="D132" s="336"/>
       <c r="E132" s="117"/>
       <c r="F132" s="36"/>
       <c r="G132" s="36"/>
@@ -15761,13 +15761,13 @@
       </c>
       <c r="AD132" s="201"/>
     </row>
-    <row r="133" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="318"/>
+    <row r="133" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="320"/>
       <c r="B133" s="53"/>
       <c r="C133" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D133" s="334"/>
+      <c r="D133" s="336"/>
       <c r="E133" s="117"/>
       <c r="F133" s="36"/>
       <c r="G133" s="36"/>
@@ -15809,13 +15809,13 @@
       </c>
       <c r="AD133" s="201"/>
     </row>
-    <row r="134" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="318"/>
+    <row r="134" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="320"/>
       <c r="B134" s="53"/>
       <c r="C134" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D134" s="334"/>
+      <c r="D134" s="336"/>
       <c r="E134" s="117"/>
       <c r="F134" s="36"/>
       <c r="G134" s="36"/>
@@ -15857,13 +15857,13 @@
       </c>
       <c r="AD134" s="201"/>
     </row>
-    <row r="135" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="318"/>
+    <row r="135" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="320"/>
       <c r="B135" s="53"/>
       <c r="C135" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D135" s="334"/>
+      <c r="D135" s="336"/>
       <c r="E135" s="117"/>
       <c r="F135" s="36"/>
       <c r="G135" s="36"/>
@@ -15905,13 +15905,13 @@
       </c>
       <c r="AD135" s="201"/>
     </row>
-    <row r="136" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="318"/>
+    <row r="136" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="320"/>
       <c r="B136" s="53"/>
       <c r="C136" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D136" s="334"/>
+      <c r="D136" s="336"/>
       <c r="E136" s="117"/>
       <c r="F136" s="36"/>
       <c r="G136" s="36"/>
@@ -15965,13 +15965,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="137" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="318"/>
+    <row r="137" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="320"/>
       <c r="B137" s="53"/>
       <c r="C137" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D137" s="334"/>
+      <c r="D137" s="336"/>
       <c r="E137" s="117"/>
       <c r="F137" s="36"/>
       <c r="G137" s="36"/>
@@ -16037,13 +16037,13 @@
       </c>
       <c r="AD137" s="201"/>
     </row>
-    <row r="138" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="318"/>
+    <row r="138" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="320"/>
       <c r="B138" s="53"/>
       <c r="C138" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D138" s="334"/>
+      <c r="D138" s="336"/>
       <c r="E138" s="131"/>
       <c r="F138" s="37"/>
       <c r="G138" s="37"/>
@@ -16071,13 +16071,13 @@
       <c r="AC138" s="150"/>
       <c r="AD138" s="201"/>
     </row>
-    <row r="139" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="318"/>
+    <row r="139" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="320"/>
       <c r="B139" s="53"/>
       <c r="C139" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D139" s="334"/>
+      <c r="D139" s="336"/>
       <c r="E139" s="131"/>
       <c r="F139" s="37"/>
       <c r="G139" s="37"/>
@@ -16143,13 +16143,13 @@
       </c>
       <c r="AD139" s="201"/>
     </row>
-    <row r="140" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="318"/>
+    <row r="140" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="320"/>
       <c r="B140" s="53"/>
       <c r="C140" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D140" s="334"/>
+      <c r="D140" s="336"/>
       <c r="E140" s="131"/>
       <c r="F140" s="37"/>
       <c r="G140" s="37"/>
@@ -16215,13 +16215,13 @@
       </c>
       <c r="AD140" s="201"/>
     </row>
-    <row r="141" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="318"/>
+    <row r="141" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="320"/>
       <c r="B141" s="53"/>
       <c r="C141" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="D141" s="334"/>
+      <c r="D141" s="336"/>
       <c r="E141" s="131"/>
       <c r="F141" s="37"/>
       <c r="G141" s="37"/>
@@ -16289,13 +16289,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="142" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="318"/>
+    <row r="142" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="320"/>
       <c r="B142" s="53"/>
       <c r="C142" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D142" s="334"/>
+      <c r="D142" s="336"/>
       <c r="E142" s="131"/>
       <c r="F142" s="37"/>
       <c r="G142" s="37"/>
@@ -16361,13 +16361,13 @@
       </c>
       <c r="AD142" s="201"/>
     </row>
-    <row r="143" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="318"/>
+    <row r="143" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="320"/>
       <c r="B143" s="53"/>
       <c r="C143" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D143" s="334"/>
+      <c r="D143" s="336"/>
       <c r="E143" s="131"/>
       <c r="F143" s="37"/>
       <c r="G143" s="37"/>
@@ -16411,13 +16411,13 @@
       </c>
       <c r="AD143" s="201"/>
     </row>
-    <row r="144" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="318"/>
+    <row r="144" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="320"/>
       <c r="B144" s="53"/>
       <c r="C144" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D144" s="334"/>
+      <c r="D144" s="336"/>
       <c r="E144" s="131"/>
       <c r="F144" s="37"/>
       <c r="G144" s="37"/>
@@ -16483,13 +16483,13 @@
       </c>
       <c r="AD144" s="201"/>
     </row>
-    <row r="145" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="318"/>
+    <row r="145" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="320"/>
       <c r="B145" s="53"/>
       <c r="C145" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D145" s="334"/>
+      <c r="D145" s="336"/>
       <c r="E145" s="131"/>
       <c r="F145" s="37"/>
       <c r="G145" s="37"/>
@@ -16555,13 +16555,13 @@
       </c>
       <c r="AD145" s="201"/>
     </row>
-    <row r="146" spans="1:30" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="318"/>
+    <row r="146" spans="1:30" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="320"/>
       <c r="B146" s="74"/>
       <c r="C146" s="75" t="s">
         <v>235</v>
       </c>
-      <c r="D146" s="334"/>
+      <c r="D146" s="336"/>
       <c r="E146" s="120"/>
       <c r="F146" s="80"/>
       <c r="G146" s="80"/>
@@ -16603,15 +16603,15 @@
       </c>
       <c r="AD146" s="203"/>
     </row>
-    <row r="147" spans="1:30" ht="39.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="318"/>
+    <row r="147" spans="1:30" ht="39" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="320"/>
       <c r="B147" s="97" t="s">
         <v>79</v>
       </c>
       <c r="C147" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="D147" s="334"/>
+      <c r="D147" s="336"/>
       <c r="E147" s="132"/>
       <c r="F147" s="98"/>
       <c r="G147" s="98"/>
@@ -16679,13 +16679,13 @@
         <v>203</v>
       </c>
     </row>
-    <row r="148" spans="1:30" ht="26" x14ac:dyDescent="0.35">
-      <c r="A148" s="318"/>
+    <row r="148" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A148" s="320"/>
       <c r="B148" s="53"/>
       <c r="C148" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D148" s="334"/>
+      <c r="D148" s="336"/>
       <c r="E148" s="131"/>
       <c r="F148" s="37"/>
       <c r="G148" s="37"/>
@@ -16753,13 +16753,13 @@
         <v>82</v>
       </c>
     </row>
-    <row r="149" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="318"/>
+    <row r="149" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="320"/>
       <c r="B149" s="53"/>
       <c r="C149" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D149" s="334"/>
+      <c r="D149" s="336"/>
       <c r="E149" s="131"/>
       <c r="F149" s="37"/>
       <c r="G149" s="37"/>
@@ -16825,13 +16825,13 @@
       </c>
       <c r="AD149" s="201"/>
     </row>
-    <row r="150" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="318"/>
+    <row r="150" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="320"/>
       <c r="B150" s="53"/>
       <c r="C150" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D150" s="334"/>
+      <c r="D150" s="336"/>
       <c r="E150" s="131"/>
       <c r="F150" s="37"/>
       <c r="G150" s="37"/>
@@ -16897,13 +16897,13 @@
       </c>
       <c r="AD150" s="201"/>
     </row>
-    <row r="151" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="318"/>
+    <row r="151" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="320"/>
       <c r="B151" s="53"/>
       <c r="C151" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D151" s="334"/>
+      <c r="D151" s="336"/>
       <c r="E151" s="131"/>
       <c r="F151" s="37"/>
       <c r="G151" s="37"/>
@@ -16969,13 +16969,13 @@
       </c>
       <c r="AD151" s="201"/>
     </row>
-    <row r="152" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="318"/>
+    <row r="152" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="320"/>
       <c r="B152" s="53"/>
       <c r="C152" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D152" s="334"/>
+      <c r="D152" s="336"/>
       <c r="E152" s="131"/>
       <c r="F152" s="37"/>
       <c r="G152" s="37"/>
@@ -17041,13 +17041,13 @@
       </c>
       <c r="AD152" s="201"/>
     </row>
-    <row r="153" spans="1:30" ht="52" x14ac:dyDescent="0.35">
-      <c r="A153" s="318"/>
+    <row r="153" spans="1:30" ht="51" x14ac:dyDescent="0.25">
+      <c r="A153" s="320"/>
       <c r="B153" s="53"/>
       <c r="C153" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D153" s="334"/>
+      <c r="D153" s="336"/>
       <c r="E153" s="131"/>
       <c r="F153" s="37"/>
       <c r="G153" s="37"/>
@@ -17115,13 +17115,13 @@
         <v>88</v>
       </c>
     </row>
-    <row r="154" spans="1:30" ht="39" x14ac:dyDescent="0.35">
-      <c r="A154" s="318"/>
+    <row r="154" spans="1:30" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A154" s="320"/>
       <c r="B154" s="53"/>
       <c r="C154" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D154" s="334"/>
+      <c r="D154" s="336"/>
       <c r="E154" s="131"/>
       <c r="F154" s="37"/>
       <c r="G154" s="37"/>
@@ -17187,13 +17187,13 @@
       </c>
       <c r="AD154" s="209"/>
     </row>
-    <row r="155" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="318"/>
+    <row r="155" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="320"/>
       <c r="B155" s="53"/>
       <c r="C155" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D155" s="334"/>
+      <c r="D155" s="336"/>
       <c r="E155" s="131"/>
       <c r="F155" s="37"/>
       <c r="G155" s="37"/>
@@ -17259,13 +17259,13 @@
       </c>
       <c r="AD155" s="209"/>
     </row>
-    <row r="156" spans="1:30" ht="39" x14ac:dyDescent="0.35">
-      <c r="A156" s="318"/>
+    <row r="156" spans="1:30" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A156" s="320"/>
       <c r="B156" s="53"/>
       <c r="C156" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D156" s="334"/>
+      <c r="D156" s="336"/>
       <c r="E156" s="131"/>
       <c r="F156" s="37"/>
       <c r="G156" s="37"/>
@@ -17333,13 +17333,13 @@
         <v>132</v>
       </c>
     </row>
-    <row r="157" spans="1:30" ht="26" x14ac:dyDescent="0.35">
-      <c r="A157" s="318"/>
+    <row r="157" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A157" s="320"/>
       <c r="B157" s="53"/>
       <c r="C157" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D157" s="334"/>
+      <c r="D157" s="336"/>
       <c r="E157" s="131"/>
       <c r="F157" s="37"/>
       <c r="G157" s="37"/>
@@ -17407,13 +17407,13 @@
         <v>204</v>
       </c>
     </row>
-    <row r="158" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="318"/>
+    <row r="158" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="320"/>
       <c r="B158" s="53"/>
       <c r="C158" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D158" s="334"/>
+      <c r="D158" s="336"/>
       <c r="E158" s="131"/>
       <c r="F158" s="37"/>
       <c r="G158" s="37"/>
@@ -17479,13 +17479,13 @@
       </c>
       <c r="AD158" s="201"/>
     </row>
-    <row r="159" spans="1:30" ht="39" x14ac:dyDescent="0.35">
-      <c r="A159" s="318"/>
+    <row r="159" spans="1:30" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A159" s="320"/>
       <c r="B159" s="53"/>
       <c r="C159" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D159" s="334"/>
+      <c r="D159" s="336"/>
       <c r="E159" s="131"/>
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
@@ -17553,13 +17553,13 @@
         <v>129</v>
       </c>
     </row>
-    <row r="160" spans="1:30" ht="52" x14ac:dyDescent="0.35">
-      <c r="A160" s="318"/>
+    <row r="160" spans="1:30" ht="51" x14ac:dyDescent="0.25">
+      <c r="A160" s="320"/>
       <c r="B160" s="53"/>
       <c r="C160" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D160" s="334"/>
+      <c r="D160" s="336"/>
       <c r="E160" s="131"/>
       <c r="F160" s="37"/>
       <c r="G160" s="37"/>
@@ -17625,13 +17625,13 @@
       </c>
       <c r="AD160" s="201"/>
     </row>
-    <row r="161" spans="1:30" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A161" s="318"/>
+    <row r="161" spans="1:30" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="320"/>
       <c r="B161" s="74"/>
       <c r="C161" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="D161" s="334"/>
+      <c r="D161" s="336"/>
       <c r="E161" s="120"/>
       <c r="F161" s="80"/>
       <c r="G161" s="80"/>
@@ -17683,15 +17683,15 @@
       </c>
       <c r="AD161" s="203"/>
     </row>
-    <row r="162" spans="1:30" ht="15.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="318"/>
+    <row r="162" spans="1:30" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="320"/>
       <c r="B162" s="62" t="s">
         <v>139</v>
       </c>
       <c r="C162" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="D162" s="334"/>
+      <c r="D162" s="336"/>
       <c r="E162" s="133"/>
       <c r="F162" s="64"/>
       <c r="G162" s="64"/>
@@ -17757,13 +17757,13 @@
       </c>
       <c r="AD162" s="210"/>
     </row>
-    <row r="163" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="318"/>
+    <row r="163" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="320"/>
       <c r="B163" s="66"/>
       <c r="C163" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D163" s="334"/>
+      <c r="D163" s="336"/>
       <c r="E163" s="134"/>
       <c r="F163" s="38"/>
       <c r="G163" s="38"/>
@@ -17829,13 +17829,13 @@
       </c>
       <c r="AD163" s="211"/>
     </row>
-    <row r="164" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="318"/>
+    <row r="164" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="320"/>
       <c r="B164" s="66"/>
       <c r="C164" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D164" s="334"/>
+      <c r="D164" s="336"/>
       <c r="E164" s="134"/>
       <c r="F164" s="38"/>
       <c r="G164" s="38"/>
@@ -17903,13 +17903,13 @@
         <v>197</v>
       </c>
     </row>
-    <row r="165" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="318"/>
+    <row r="165" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="320"/>
       <c r="B165" s="66"/>
       <c r="C165" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D165" s="334"/>
+      <c r="D165" s="336"/>
       <c r="E165" s="134"/>
       <c r="F165" s="38"/>
       <c r="G165" s="38"/>
@@ -17975,13 +17975,13 @@
       </c>
       <c r="AD165" s="211"/>
     </row>
-    <row r="166" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="318"/>
+    <row r="166" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="320"/>
       <c r="B166" s="66"/>
       <c r="C166" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D166" s="334"/>
+      <c r="D166" s="336"/>
       <c r="E166" s="134"/>
       <c r="F166" s="38"/>
       <c r="G166" s="38"/>
@@ -18047,13 +18047,13 @@
       </c>
       <c r="AD166" s="211"/>
     </row>
-    <row r="167" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="318"/>
+    <row r="167" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="320"/>
       <c r="B167" s="66"/>
       <c r="C167" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D167" s="334"/>
+      <c r="D167" s="336"/>
       <c r="E167" s="134"/>
       <c r="F167" s="38"/>
       <c r="G167" s="38"/>
@@ -18121,13 +18121,13 @@
         <v>327</v>
       </c>
     </row>
-    <row r="168" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="318"/>
+    <row r="168" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="320"/>
       <c r="B168" s="66"/>
       <c r="C168" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D168" s="334"/>
+      <c r="D168" s="336"/>
       <c r="E168" s="134"/>
       <c r="F168" s="38"/>
       <c r="G168" s="38"/>
@@ -18193,13 +18193,13 @@
       </c>
       <c r="AD168" s="211"/>
     </row>
-    <row r="169" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="318"/>
+    <row r="169" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="320"/>
       <c r="B169" s="66"/>
       <c r="C169" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D169" s="334"/>
+      <c r="D169" s="336"/>
       <c r="E169" s="134"/>
       <c r="F169" s="38"/>
       <c r="G169" s="38"/>
@@ -18265,13 +18265,13 @@
       </c>
       <c r="AD169" s="211"/>
     </row>
-    <row r="170" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="318"/>
+    <row r="170" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="320"/>
       <c r="B170" s="66"/>
       <c r="C170" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D170" s="334"/>
+      <c r="D170" s="336"/>
       <c r="E170" s="134"/>
       <c r="F170" s="38"/>
       <c r="G170" s="38"/>
@@ -18337,13 +18337,13 @@
       </c>
       <c r="AD170" s="211"/>
     </row>
-    <row r="171" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="318"/>
+    <row r="171" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="320"/>
       <c r="B171" s="66"/>
       <c r="C171" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="D171" s="334"/>
+      <c r="D171" s="336"/>
       <c r="E171" s="134"/>
       <c r="F171" s="38"/>
       <c r="G171" s="38"/>
@@ -18411,13 +18411,13 @@
         <v>153</v>
       </c>
     </row>
-    <row r="172" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="318"/>
+    <row r="172" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="320"/>
       <c r="B172" s="66"/>
       <c r="C172" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D172" s="334"/>
+      <c r="D172" s="336"/>
       <c r="E172" s="134"/>
       <c r="F172" s="38"/>
       <c r="G172" s="38"/>
@@ -18483,13 +18483,13 @@
       </c>
       <c r="AD172" s="211"/>
     </row>
-    <row r="173" spans="1:30" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="318"/>
+    <row r="173" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="320"/>
       <c r="B173" s="66"/>
       <c r="C173" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D173" s="334"/>
+      <c r="D173" s="336"/>
       <c r="E173" s="134"/>
       <c r="F173" s="38"/>
       <c r="G173" s="38"/>
@@ -18555,13 +18555,13 @@
       </c>
       <c r="AD173" s="211"/>
     </row>
-    <row r="174" spans="1:30" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="318"/>
+    <row r="174" spans="1:30" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="320"/>
       <c r="B174" s="67"/>
       <c r="C174" s="68" t="s">
         <v>154</v>
       </c>
-      <c r="D174" s="335"/>
+      <c r="D174" s="337"/>
       <c r="E174" s="135"/>
       <c r="F174" s="69"/>
       <c r="G174" s="69"/>
@@ -18627,7 +18627,7 @@
       </c>
       <c r="AD174" s="213"/>
     </row>
-    <row r="175" spans="1:30" ht="13.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="175" spans="1:30" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="AD2:AD4"/>

</xml_diff>

<commit_message>
updated the SRAM size for GSC
[git-p4: depot-paths = "//depot/projects/coe/CSME/": change = 759686]
</commit_message>
<xml_diff>
--- a/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
+++ b/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="105" windowWidth="10005" windowHeight="4665"/>
+    <workbookView xWindow="5820" yWindow="105" windowWidth="10005" windowHeight="4665"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="2" r:id="rId1"/>
     <sheet name="CSE CSME IE OCS Features" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" iterateCount="5"/>
+  <calcPr calcId="152511" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -3064,7 +3064,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2778" uniqueCount="443">
   <si>
     <t>Feature</t>
   </si>
@@ -4712,6 +4712,12 @@
 (https://hsdes.intel.com/appstore/article/#/1407023163)
 [DG1] RAVDM transaction routing for GSC
 https://hsdes.intel.com/appstore/no-ie/?srcUrl=https%3A%2F%2Fhsdes.intel.com%2Fappstore%2Farticle%2F%23%2F1407181570</t>
+  </si>
+  <si>
+    <t>1024 KB</t>
+  </si>
+  <si>
+    <t>Updated SRAM size 1 MB</t>
   </si>
 </sst>
 </file>
@@ -7477,7 +7483,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E59" sqref="E59"/>
+      <selection pane="bottomRight" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8191,10 +8197,18 @@
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="220"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="4"/>
+      <c r="B52" s="220">
+        <v>40</v>
+      </c>
+      <c r="C52" s="9">
+        <v>43244</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="220"/>
@@ -8291,9 +8305,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF182"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A45" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="3" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z98" sqref="Z98"/>
+      <selection pane="topRight" activeCell="AD54" sqref="AD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10832,7 +10846,7 @@
         <v>30</v>
       </c>
       <c r="AD52" s="310" t="s">
-        <v>363</v>
+        <v>441</v>
       </c>
       <c r="AE52" s="73" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
added 2 SMS for GSC
[git-p4: depot-paths = "//depot/projects/coe/CSME/": change = 760543]
</commit_message>
<xml_diff>
--- a/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
+++ b/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8610" yWindow="105" windowWidth="10005" windowHeight="4665"/>
+    <workbookView xWindow="9540" yWindow="105" windowWidth="10005" windowHeight="4665"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="2" r:id="rId1"/>
@@ -3088,7 +3088,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="449">
   <si>
     <t>Feature</t>
   </si>
@@ -4754,6 +4754,12 @@
   </si>
   <si>
     <t>Updated SRAM size 1.5 MB , ROSC clk is not used for GSC , No support for PG</t>
+  </si>
+  <si>
+    <t>Yes(x2)</t>
+  </si>
+  <si>
+    <t>Added 2 SMS for GSC</t>
   </si>
 </sst>
 </file>
@@ -7095,6 +7101,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -7217,27 +7244,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7555,7 +7561,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E53" sqref="E53"/>
+      <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8297,10 +8303,18 @@
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="220"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="4"/>
+      <c r="B54" s="220">
+        <v>42</v>
+      </c>
+      <c r="C54" s="9">
+        <v>43270</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="220"/>
@@ -8385,9 +8399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF184"/>
   <sheetViews>
-    <sheetView topLeftCell="A188" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="A171" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD182" sqref="AD182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8415,38 +8429,38 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="354" t="s">
+      <c r="B2" s="361" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="349" t="s">
+      <c r="C2" s="356" t="s">
         <v>277</v>
       </c>
-      <c r="D2" s="350"/>
-      <c r="E2" s="377" t="s">
+      <c r="D2" s="357"/>
+      <c r="E2" s="384" t="s">
         <v>238</v>
       </c>
-      <c r="F2" s="378"/>
-      <c r="G2" s="378"/>
-      <c r="H2" s="378"/>
-      <c r="I2" s="378"/>
-      <c r="J2" s="379"/>
-      <c r="K2" s="357" t="s">
+      <c r="F2" s="385"/>
+      <c r="G2" s="385"/>
+      <c r="H2" s="385"/>
+      <c r="I2" s="385"/>
+      <c r="J2" s="386"/>
+      <c r="K2" s="364" t="s">
         <v>312</v>
       </c>
-      <c r="L2" s="358"/>
-      <c r="M2" s="359" t="s">
+      <c r="L2" s="365"/>
+      <c r="M2" s="366" t="s">
         <v>313</v>
       </c>
-      <c r="N2" s="360"/>
-      <c r="O2" s="363" t="s">
+      <c r="N2" s="367"/>
+      <c r="O2" s="370" t="s">
         <v>314</v>
       </c>
-      <c r="P2" s="361"/>
-      <c r="Q2" s="364"/>
-      <c r="R2" s="361" t="s">
+      <c r="P2" s="368"/>
+      <c r="Q2" s="371"/>
+      <c r="R2" s="368" t="s">
         <v>159</v>
       </c>
-      <c r="S2" s="362"/>
+      <c r="S2" s="369"/>
       <c r="T2" s="190" t="s">
         <v>101</v>
       </c>
@@ -8480,16 +8494,16 @@
       <c r="AD2" s="319" t="s">
         <v>2</v>
       </c>
-      <c r="AE2" s="345" t="s">
+      <c r="AE2" s="352" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="355"/>
-      <c r="C3" s="351" t="s">
+      <c r="B3" s="362"/>
+      <c r="C3" s="358" t="s">
         <v>278</v>
       </c>
-      <c r="D3" s="352"/>
+      <c r="D3" s="359"/>
       <c r="E3" s="247" t="s">
         <v>234</v>
       </c>
@@ -8568,10 +8582,10 @@
       <c r="AD3" s="320" t="s">
         <v>408</v>
       </c>
-      <c r="AE3" s="346"/>
+      <c r="AE3" s="353"/>
     </row>
     <row r="4" spans="1:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="356"/>
+      <c r="B4" s="363"/>
       <c r="C4" s="244" t="s">
         <v>0</v>
       </c>
@@ -8656,10 +8670,10 @@
       <c r="AD4" s="321" t="s">
         <v>409</v>
       </c>
-      <c r="AE4" s="347"/>
+      <c r="AE4" s="354"/>
     </row>
     <row r="5" spans="1:31" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="348"/>
+      <c r="A5" s="355"/>
       <c r="B5" s="297" t="s">
         <v>309</v>
       </c>
@@ -8669,40 +8683,40 @@
       <c r="D5" s="299" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="380" t="s">
+      <c r="E5" s="387" t="s">
         <v>352</v>
       </c>
-      <c r="F5" s="369"/>
-      <c r="G5" s="369"/>
-      <c r="H5" s="369"/>
-      <c r="I5" s="369"/>
-      <c r="J5" s="381"/>
-      <c r="K5" s="368" t="s">
+      <c r="F5" s="376"/>
+      <c r="G5" s="376"/>
+      <c r="H5" s="376"/>
+      <c r="I5" s="376"/>
+      <c r="J5" s="388"/>
+      <c r="K5" s="375" t="s">
         <v>354</v>
       </c>
-      <c r="L5" s="369"/>
-      <c r="M5" s="369"/>
-      <c r="N5" s="369"/>
-      <c r="O5" s="369"/>
-      <c r="P5" s="369"/>
-      <c r="Q5" s="369"/>
-      <c r="R5" s="369"/>
-      <c r="S5" s="369"/>
-      <c r="T5" s="369"/>
-      <c r="U5" s="369"/>
-      <c r="V5" s="369"/>
-      <c r="W5" s="369"/>
-      <c r="X5" s="369"/>
-      <c r="Y5" s="369"/>
-      <c r="Z5" s="369"/>
-      <c r="AA5" s="369"/>
-      <c r="AB5" s="369"/>
-      <c r="AC5" s="370"/>
+      <c r="L5" s="376"/>
+      <c r="M5" s="376"/>
+      <c r="N5" s="376"/>
+      <c r="O5" s="376"/>
+      <c r="P5" s="376"/>
+      <c r="Q5" s="376"/>
+      <c r="R5" s="376"/>
+      <c r="S5" s="376"/>
+      <c r="T5" s="376"/>
+      <c r="U5" s="376"/>
+      <c r="V5" s="376"/>
+      <c r="W5" s="376"/>
+      <c r="X5" s="376"/>
+      <c r="Y5" s="376"/>
+      <c r="Z5" s="376"/>
+      <c r="AA5" s="376"/>
+      <c r="AB5" s="376"/>
+      <c r="AC5" s="377"/>
       <c r="AD5" s="317"/>
       <c r="AE5" s="245"/>
     </row>
     <row r="6" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="348"/>
+      <c r="A6" s="355"/>
       <c r="B6" s="300"/>
       <c r="C6" s="301" t="s">
         <v>9</v>
@@ -8710,36 +8724,36 @@
       <c r="D6" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="382"/>
-      <c r="F6" s="372"/>
-      <c r="G6" s="372"/>
-      <c r="H6" s="372"/>
-      <c r="I6" s="372"/>
-      <c r="J6" s="383"/>
-      <c r="K6" s="371"/>
-      <c r="L6" s="372"/>
-      <c r="M6" s="372"/>
-      <c r="N6" s="372"/>
-      <c r="O6" s="372"/>
-      <c r="P6" s="372"/>
-      <c r="Q6" s="372"/>
-      <c r="R6" s="372"/>
-      <c r="S6" s="372"/>
-      <c r="T6" s="372"/>
-      <c r="U6" s="372"/>
-      <c r="V6" s="372"/>
-      <c r="W6" s="372"/>
-      <c r="X6" s="372"/>
-      <c r="Y6" s="372"/>
-      <c r="Z6" s="372"/>
-      <c r="AA6" s="372"/>
-      <c r="AB6" s="372"/>
-      <c r="AC6" s="373"/>
+      <c r="E6" s="389"/>
+      <c r="F6" s="379"/>
+      <c r="G6" s="379"/>
+      <c r="H6" s="379"/>
+      <c r="I6" s="379"/>
+      <c r="J6" s="390"/>
+      <c r="K6" s="378"/>
+      <c r="L6" s="379"/>
+      <c r="M6" s="379"/>
+      <c r="N6" s="379"/>
+      <c r="O6" s="379"/>
+      <c r="P6" s="379"/>
+      <c r="Q6" s="379"/>
+      <c r="R6" s="379"/>
+      <c r="S6" s="379"/>
+      <c r="T6" s="379"/>
+      <c r="U6" s="379"/>
+      <c r="V6" s="379"/>
+      <c r="W6" s="379"/>
+      <c r="X6" s="379"/>
+      <c r="Y6" s="379"/>
+      <c r="Z6" s="379"/>
+      <c r="AA6" s="379"/>
+      <c r="AB6" s="379"/>
+      <c r="AC6" s="380"/>
       <c r="AD6" s="318"/>
       <c r="AE6" s="246"/>
     </row>
     <row r="7" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="348"/>
+      <c r="A7" s="355"/>
       <c r="B7" s="300"/>
       <c r="C7" s="301" t="s">
         <v>12</v>
@@ -8747,36 +8761,36 @@
       <c r="D7" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="382"/>
-      <c r="F7" s="372"/>
-      <c r="G7" s="372"/>
-      <c r="H7" s="372"/>
-      <c r="I7" s="372"/>
-      <c r="J7" s="383"/>
-      <c r="K7" s="371"/>
-      <c r="L7" s="372"/>
-      <c r="M7" s="372"/>
-      <c r="N7" s="372"/>
-      <c r="O7" s="372"/>
-      <c r="P7" s="372"/>
-      <c r="Q7" s="372"/>
-      <c r="R7" s="372"/>
-      <c r="S7" s="372"/>
-      <c r="T7" s="372"/>
-      <c r="U7" s="372"/>
-      <c r="V7" s="372"/>
-      <c r="W7" s="372"/>
-      <c r="X7" s="372"/>
-      <c r="Y7" s="372"/>
-      <c r="Z7" s="372"/>
-      <c r="AA7" s="372"/>
-      <c r="AB7" s="372"/>
-      <c r="AC7" s="373"/>
+      <c r="E7" s="389"/>
+      <c r="F7" s="379"/>
+      <c r="G7" s="379"/>
+      <c r="H7" s="379"/>
+      <c r="I7" s="379"/>
+      <c r="J7" s="390"/>
+      <c r="K7" s="378"/>
+      <c r="L7" s="379"/>
+      <c r="M7" s="379"/>
+      <c r="N7" s="379"/>
+      <c r="O7" s="379"/>
+      <c r="P7" s="379"/>
+      <c r="Q7" s="379"/>
+      <c r="R7" s="379"/>
+      <c r="S7" s="379"/>
+      <c r="T7" s="379"/>
+      <c r="U7" s="379"/>
+      <c r="V7" s="379"/>
+      <c r="W7" s="379"/>
+      <c r="X7" s="379"/>
+      <c r="Y7" s="379"/>
+      <c r="Z7" s="379"/>
+      <c r="AA7" s="379"/>
+      <c r="AB7" s="379"/>
+      <c r="AC7" s="380"/>
       <c r="AD7" s="318"/>
       <c r="AE7" s="246"/>
     </row>
     <row r="8" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="348"/>
+      <c r="A8" s="355"/>
       <c r="B8" s="300"/>
       <c r="C8" s="301" t="s">
         <v>13</v>
@@ -8784,36 +8798,36 @@
       <c r="D8" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="382"/>
-      <c r="F8" s="372"/>
-      <c r="G8" s="372"/>
-      <c r="H8" s="372"/>
-      <c r="I8" s="372"/>
-      <c r="J8" s="383"/>
-      <c r="K8" s="371"/>
-      <c r="L8" s="372"/>
-      <c r="M8" s="372"/>
-      <c r="N8" s="372"/>
-      <c r="O8" s="372"/>
-      <c r="P8" s="372"/>
-      <c r="Q8" s="372"/>
-      <c r="R8" s="372"/>
-      <c r="S8" s="372"/>
-      <c r="T8" s="372"/>
-      <c r="U8" s="372"/>
-      <c r="V8" s="372"/>
-      <c r="W8" s="372"/>
-      <c r="X8" s="372"/>
-      <c r="Y8" s="372"/>
-      <c r="Z8" s="372"/>
-      <c r="AA8" s="372"/>
-      <c r="AB8" s="372"/>
-      <c r="AC8" s="373"/>
+      <c r="E8" s="389"/>
+      <c r="F8" s="379"/>
+      <c r="G8" s="379"/>
+      <c r="H8" s="379"/>
+      <c r="I8" s="379"/>
+      <c r="J8" s="390"/>
+      <c r="K8" s="378"/>
+      <c r="L8" s="379"/>
+      <c r="M8" s="379"/>
+      <c r="N8" s="379"/>
+      <c r="O8" s="379"/>
+      <c r="P8" s="379"/>
+      <c r="Q8" s="379"/>
+      <c r="R8" s="379"/>
+      <c r="S8" s="379"/>
+      <c r="T8" s="379"/>
+      <c r="U8" s="379"/>
+      <c r="V8" s="379"/>
+      <c r="W8" s="379"/>
+      <c r="X8" s="379"/>
+      <c r="Y8" s="379"/>
+      <c r="Z8" s="379"/>
+      <c r="AA8" s="379"/>
+      <c r="AB8" s="379"/>
+      <c r="AC8" s="380"/>
       <c r="AD8" s="318"/>
       <c r="AE8" s="246"/>
     </row>
     <row r="9" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="348"/>
+      <c r="A9" s="355"/>
       <c r="B9" s="300"/>
       <c r="C9" s="301" t="s">
         <v>338</v>
@@ -8821,36 +8835,36 @@
       <c r="D9" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="382"/>
-      <c r="F9" s="372"/>
-      <c r="G9" s="372"/>
-      <c r="H9" s="372"/>
-      <c r="I9" s="372"/>
-      <c r="J9" s="383"/>
-      <c r="K9" s="371"/>
-      <c r="L9" s="372"/>
-      <c r="M9" s="372"/>
-      <c r="N9" s="372"/>
-      <c r="O9" s="372"/>
-      <c r="P9" s="372"/>
-      <c r="Q9" s="372"/>
-      <c r="R9" s="372"/>
-      <c r="S9" s="372"/>
-      <c r="T9" s="372"/>
-      <c r="U9" s="372"/>
-      <c r="V9" s="372"/>
-      <c r="W9" s="372"/>
-      <c r="X9" s="372"/>
-      <c r="Y9" s="372"/>
-      <c r="Z9" s="372"/>
-      <c r="AA9" s="372"/>
-      <c r="AB9" s="372"/>
-      <c r="AC9" s="373"/>
+      <c r="E9" s="389"/>
+      <c r="F9" s="379"/>
+      <c r="G9" s="379"/>
+      <c r="H9" s="379"/>
+      <c r="I9" s="379"/>
+      <c r="J9" s="390"/>
+      <c r="K9" s="378"/>
+      <c r="L9" s="379"/>
+      <c r="M9" s="379"/>
+      <c r="N9" s="379"/>
+      <c r="O9" s="379"/>
+      <c r="P9" s="379"/>
+      <c r="Q9" s="379"/>
+      <c r="R9" s="379"/>
+      <c r="S9" s="379"/>
+      <c r="T9" s="379"/>
+      <c r="U9" s="379"/>
+      <c r="V9" s="379"/>
+      <c r="W9" s="379"/>
+      <c r="X9" s="379"/>
+      <c r="Y9" s="379"/>
+      <c r="Z9" s="379"/>
+      <c r="AA9" s="379"/>
+      <c r="AB9" s="379"/>
+      <c r="AC9" s="380"/>
       <c r="AD9" s="318"/>
       <c r="AE9" s="246"/>
     </row>
     <row r="10" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="348"/>
+      <c r="A10" s="355"/>
       <c r="B10" s="300"/>
       <c r="C10" s="301" t="s">
         <v>181</v>
@@ -8858,36 +8872,36 @@
       <c r="D10" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="382"/>
-      <c r="F10" s="372"/>
-      <c r="G10" s="372"/>
-      <c r="H10" s="372"/>
-      <c r="I10" s="372"/>
-      <c r="J10" s="383"/>
-      <c r="K10" s="371"/>
-      <c r="L10" s="372"/>
-      <c r="M10" s="372"/>
-      <c r="N10" s="372"/>
-      <c r="O10" s="372"/>
-      <c r="P10" s="372"/>
-      <c r="Q10" s="372"/>
-      <c r="R10" s="372"/>
-      <c r="S10" s="372"/>
-      <c r="T10" s="372"/>
-      <c r="U10" s="372"/>
-      <c r="V10" s="372"/>
-      <c r="W10" s="372"/>
-      <c r="X10" s="372"/>
-      <c r="Y10" s="372"/>
-      <c r="Z10" s="372"/>
-      <c r="AA10" s="372"/>
-      <c r="AB10" s="372"/>
-      <c r="AC10" s="373"/>
+      <c r="E10" s="389"/>
+      <c r="F10" s="379"/>
+      <c r="G10" s="379"/>
+      <c r="H10" s="379"/>
+      <c r="I10" s="379"/>
+      <c r="J10" s="390"/>
+      <c r="K10" s="378"/>
+      <c r="L10" s="379"/>
+      <c r="M10" s="379"/>
+      <c r="N10" s="379"/>
+      <c r="O10" s="379"/>
+      <c r="P10" s="379"/>
+      <c r="Q10" s="379"/>
+      <c r="R10" s="379"/>
+      <c r="S10" s="379"/>
+      <c r="T10" s="379"/>
+      <c r="U10" s="379"/>
+      <c r="V10" s="379"/>
+      <c r="W10" s="379"/>
+      <c r="X10" s="379"/>
+      <c r="Y10" s="379"/>
+      <c r="Z10" s="379"/>
+      <c r="AA10" s="379"/>
+      <c r="AB10" s="379"/>
+      <c r="AC10" s="380"/>
       <c r="AD10" s="318"/>
       <c r="AE10" s="246"/>
     </row>
     <row r="11" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="348"/>
+      <c r="A11" s="355"/>
       <c r="B11" s="300"/>
       <c r="C11" s="301" t="s">
         <v>17</v>
@@ -8895,36 +8909,36 @@
       <c r="D11" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="382"/>
-      <c r="F11" s="372"/>
-      <c r="G11" s="372"/>
-      <c r="H11" s="372"/>
-      <c r="I11" s="372"/>
-      <c r="J11" s="383"/>
-      <c r="K11" s="371"/>
-      <c r="L11" s="372"/>
-      <c r="M11" s="372"/>
-      <c r="N11" s="372"/>
-      <c r="O11" s="372"/>
-      <c r="P11" s="372"/>
-      <c r="Q11" s="372"/>
-      <c r="R11" s="372"/>
-      <c r="S11" s="372"/>
-      <c r="T11" s="372"/>
-      <c r="U11" s="372"/>
-      <c r="V11" s="372"/>
-      <c r="W11" s="372"/>
-      <c r="X11" s="372"/>
-      <c r="Y11" s="372"/>
-      <c r="Z11" s="372"/>
-      <c r="AA11" s="372"/>
-      <c r="AB11" s="372"/>
-      <c r="AC11" s="373"/>
+      <c r="E11" s="389"/>
+      <c r="F11" s="379"/>
+      <c r="G11" s="379"/>
+      <c r="H11" s="379"/>
+      <c r="I11" s="379"/>
+      <c r="J11" s="390"/>
+      <c r="K11" s="378"/>
+      <c r="L11" s="379"/>
+      <c r="M11" s="379"/>
+      <c r="N11" s="379"/>
+      <c r="O11" s="379"/>
+      <c r="P11" s="379"/>
+      <c r="Q11" s="379"/>
+      <c r="R11" s="379"/>
+      <c r="S11" s="379"/>
+      <c r="T11" s="379"/>
+      <c r="U11" s="379"/>
+      <c r="V11" s="379"/>
+      <c r="W11" s="379"/>
+      <c r="X11" s="379"/>
+      <c r="Y11" s="379"/>
+      <c r="Z11" s="379"/>
+      <c r="AA11" s="379"/>
+      <c r="AB11" s="379"/>
+      <c r="AC11" s="380"/>
       <c r="AD11" s="318"/>
       <c r="AE11" s="246"/>
     </row>
     <row r="12" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="348"/>
+      <c r="A12" s="355"/>
       <c r="B12" s="300"/>
       <c r="C12" s="301" t="s">
         <v>18</v>
@@ -8932,36 +8946,36 @@
       <c r="D12" s="303" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="382"/>
-      <c r="F12" s="372"/>
-      <c r="G12" s="372"/>
-      <c r="H12" s="372"/>
-      <c r="I12" s="372"/>
-      <c r="J12" s="383"/>
-      <c r="K12" s="371"/>
-      <c r="L12" s="372"/>
-      <c r="M12" s="372"/>
-      <c r="N12" s="372"/>
-      <c r="O12" s="372"/>
-      <c r="P12" s="372"/>
-      <c r="Q12" s="372"/>
-      <c r="R12" s="372"/>
-      <c r="S12" s="372"/>
-      <c r="T12" s="372"/>
-      <c r="U12" s="372"/>
-      <c r="V12" s="372"/>
-      <c r="W12" s="372"/>
-      <c r="X12" s="372"/>
-      <c r="Y12" s="372"/>
-      <c r="Z12" s="372"/>
-      <c r="AA12" s="372"/>
-      <c r="AB12" s="372"/>
-      <c r="AC12" s="373"/>
+      <c r="E12" s="389"/>
+      <c r="F12" s="379"/>
+      <c r="G12" s="379"/>
+      <c r="H12" s="379"/>
+      <c r="I12" s="379"/>
+      <c r="J12" s="390"/>
+      <c r="K12" s="378"/>
+      <c r="L12" s="379"/>
+      <c r="M12" s="379"/>
+      <c r="N12" s="379"/>
+      <c r="O12" s="379"/>
+      <c r="P12" s="379"/>
+      <c r="Q12" s="379"/>
+      <c r="R12" s="379"/>
+      <c r="S12" s="379"/>
+      <c r="T12" s="379"/>
+      <c r="U12" s="379"/>
+      <c r="V12" s="379"/>
+      <c r="W12" s="379"/>
+      <c r="X12" s="379"/>
+      <c r="Y12" s="379"/>
+      <c r="Z12" s="379"/>
+      <c r="AA12" s="379"/>
+      <c r="AB12" s="379"/>
+      <c r="AC12" s="380"/>
       <c r="AD12" s="318"/>
       <c r="AE12" s="246"/>
     </row>
     <row r="13" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="348"/>
+      <c r="A13" s="355"/>
       <c r="B13" s="300"/>
       <c r="C13" s="301" t="s">
         <v>20</v>
@@ -8969,36 +8983,36 @@
       <c r="D13" s="303">
         <v>32</v>
       </c>
-      <c r="E13" s="382"/>
-      <c r="F13" s="372"/>
-      <c r="G13" s="372"/>
-      <c r="H13" s="372"/>
-      <c r="I13" s="372"/>
-      <c r="J13" s="383"/>
-      <c r="K13" s="371"/>
-      <c r="L13" s="372"/>
-      <c r="M13" s="372"/>
-      <c r="N13" s="372"/>
-      <c r="O13" s="372"/>
-      <c r="P13" s="372"/>
-      <c r="Q13" s="372"/>
-      <c r="R13" s="372"/>
-      <c r="S13" s="372"/>
-      <c r="T13" s="372"/>
-      <c r="U13" s="372"/>
-      <c r="V13" s="372"/>
-      <c r="W13" s="372"/>
-      <c r="X13" s="372"/>
-      <c r="Y13" s="372"/>
-      <c r="Z13" s="372"/>
-      <c r="AA13" s="372"/>
-      <c r="AB13" s="372"/>
-      <c r="AC13" s="373"/>
+      <c r="E13" s="389"/>
+      <c r="F13" s="379"/>
+      <c r="G13" s="379"/>
+      <c r="H13" s="379"/>
+      <c r="I13" s="379"/>
+      <c r="J13" s="390"/>
+      <c r="K13" s="378"/>
+      <c r="L13" s="379"/>
+      <c r="M13" s="379"/>
+      <c r="N13" s="379"/>
+      <c r="O13" s="379"/>
+      <c r="P13" s="379"/>
+      <c r="Q13" s="379"/>
+      <c r="R13" s="379"/>
+      <c r="S13" s="379"/>
+      <c r="T13" s="379"/>
+      <c r="U13" s="379"/>
+      <c r="V13" s="379"/>
+      <c r="W13" s="379"/>
+      <c r="X13" s="379"/>
+      <c r="Y13" s="379"/>
+      <c r="Z13" s="379"/>
+      <c r="AA13" s="379"/>
+      <c r="AB13" s="379"/>
+      <c r="AC13" s="380"/>
       <c r="AD13" s="318"/>
       <c r="AE13" s="246"/>
     </row>
     <row r="14" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="348"/>
+      <c r="A14" s="355"/>
       <c r="B14" s="300"/>
       <c r="C14" s="301" t="s">
         <v>21</v>
@@ -9006,36 +9020,36 @@
       <c r="D14" s="303">
         <v>32</v>
       </c>
-      <c r="E14" s="382"/>
-      <c r="F14" s="372"/>
-      <c r="G14" s="372"/>
-      <c r="H14" s="372"/>
-      <c r="I14" s="372"/>
-      <c r="J14" s="383"/>
-      <c r="K14" s="371"/>
-      <c r="L14" s="372"/>
-      <c r="M14" s="372"/>
-      <c r="N14" s="372"/>
-      <c r="O14" s="372"/>
-      <c r="P14" s="372"/>
-      <c r="Q14" s="372"/>
-      <c r="R14" s="372"/>
-      <c r="S14" s="372"/>
-      <c r="T14" s="372"/>
-      <c r="U14" s="372"/>
-      <c r="V14" s="372"/>
-      <c r="W14" s="372"/>
-      <c r="X14" s="372"/>
-      <c r="Y14" s="372"/>
-      <c r="Z14" s="372"/>
-      <c r="AA14" s="372"/>
-      <c r="AB14" s="372"/>
-      <c r="AC14" s="373"/>
+      <c r="E14" s="389"/>
+      <c r="F14" s="379"/>
+      <c r="G14" s="379"/>
+      <c r="H14" s="379"/>
+      <c r="I14" s="379"/>
+      <c r="J14" s="390"/>
+      <c r="K14" s="378"/>
+      <c r="L14" s="379"/>
+      <c r="M14" s="379"/>
+      <c r="N14" s="379"/>
+      <c r="O14" s="379"/>
+      <c r="P14" s="379"/>
+      <c r="Q14" s="379"/>
+      <c r="R14" s="379"/>
+      <c r="S14" s="379"/>
+      <c r="T14" s="379"/>
+      <c r="U14" s="379"/>
+      <c r="V14" s="379"/>
+      <c r="W14" s="379"/>
+      <c r="X14" s="379"/>
+      <c r="Y14" s="379"/>
+      <c r="Z14" s="379"/>
+      <c r="AA14" s="379"/>
+      <c r="AB14" s="379"/>
+      <c r="AC14" s="380"/>
       <c r="AD14" s="318"/>
       <c r="AE14" s="246"/>
     </row>
     <row r="15" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="348"/>
+      <c r="A15" s="355"/>
       <c r="B15" s="300"/>
       <c r="C15" s="301" t="s">
         <v>22</v>
@@ -9043,36 +9057,36 @@
       <c r="D15" s="303" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="382"/>
-      <c r="F15" s="372"/>
-      <c r="G15" s="372"/>
-      <c r="H15" s="372"/>
-      <c r="I15" s="372"/>
-      <c r="J15" s="383"/>
-      <c r="K15" s="371"/>
-      <c r="L15" s="372"/>
-      <c r="M15" s="372"/>
-      <c r="N15" s="372"/>
-      <c r="O15" s="372"/>
-      <c r="P15" s="372"/>
-      <c r="Q15" s="372"/>
-      <c r="R15" s="372"/>
-      <c r="S15" s="372"/>
-      <c r="T15" s="372"/>
-      <c r="U15" s="372"/>
-      <c r="V15" s="372"/>
-      <c r="W15" s="372"/>
-      <c r="X15" s="372"/>
-      <c r="Y15" s="372"/>
-      <c r="Z15" s="372"/>
-      <c r="AA15" s="372"/>
-      <c r="AB15" s="372"/>
-      <c r="AC15" s="373"/>
+      <c r="E15" s="389"/>
+      <c r="F15" s="379"/>
+      <c r="G15" s="379"/>
+      <c r="H15" s="379"/>
+      <c r="I15" s="379"/>
+      <c r="J15" s="390"/>
+      <c r="K15" s="378"/>
+      <c r="L15" s="379"/>
+      <c r="M15" s="379"/>
+      <c r="N15" s="379"/>
+      <c r="O15" s="379"/>
+      <c r="P15" s="379"/>
+      <c r="Q15" s="379"/>
+      <c r="R15" s="379"/>
+      <c r="S15" s="379"/>
+      <c r="T15" s="379"/>
+      <c r="U15" s="379"/>
+      <c r="V15" s="379"/>
+      <c r="W15" s="379"/>
+      <c r="X15" s="379"/>
+      <c r="Y15" s="379"/>
+      <c r="Z15" s="379"/>
+      <c r="AA15" s="379"/>
+      <c r="AB15" s="379"/>
+      <c r="AC15" s="380"/>
       <c r="AD15" s="318"/>
       <c r="AE15" s="246"/>
     </row>
     <row r="16" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="348"/>
+      <c r="A16" s="355"/>
       <c r="B16" s="300" t="s">
         <v>23</v>
       </c>
@@ -9082,36 +9096,36 @@
       <c r="D16" s="302" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="382"/>
-      <c r="F16" s="372"/>
-      <c r="G16" s="372"/>
-      <c r="H16" s="372"/>
-      <c r="I16" s="372"/>
-      <c r="J16" s="383"/>
-      <c r="K16" s="371"/>
-      <c r="L16" s="372"/>
-      <c r="M16" s="372"/>
-      <c r="N16" s="372"/>
-      <c r="O16" s="372"/>
-      <c r="P16" s="372"/>
-      <c r="Q16" s="372"/>
-      <c r="R16" s="372"/>
-      <c r="S16" s="372"/>
-      <c r="T16" s="372"/>
-      <c r="U16" s="372"/>
-      <c r="V16" s="372"/>
-      <c r="W16" s="372"/>
-      <c r="X16" s="372"/>
-      <c r="Y16" s="372"/>
-      <c r="Z16" s="372"/>
-      <c r="AA16" s="372"/>
-      <c r="AB16" s="372"/>
-      <c r="AC16" s="373"/>
+      <c r="E16" s="389"/>
+      <c r="F16" s="379"/>
+      <c r="G16" s="379"/>
+      <c r="H16" s="379"/>
+      <c r="I16" s="379"/>
+      <c r="J16" s="390"/>
+      <c r="K16" s="378"/>
+      <c r="L16" s="379"/>
+      <c r="M16" s="379"/>
+      <c r="N16" s="379"/>
+      <c r="O16" s="379"/>
+      <c r="P16" s="379"/>
+      <c r="Q16" s="379"/>
+      <c r="R16" s="379"/>
+      <c r="S16" s="379"/>
+      <c r="T16" s="379"/>
+      <c r="U16" s="379"/>
+      <c r="V16" s="379"/>
+      <c r="W16" s="379"/>
+      <c r="X16" s="379"/>
+      <c r="Y16" s="379"/>
+      <c r="Z16" s="379"/>
+      <c r="AA16" s="379"/>
+      <c r="AB16" s="379"/>
+      <c r="AC16" s="380"/>
       <c r="AD16" s="318"/>
       <c r="AE16" s="246"/>
     </row>
     <row r="17" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="348"/>
+      <c r="A17" s="355"/>
       <c r="B17" s="300"/>
       <c r="C17" s="301" t="s">
         <v>27</v>
@@ -9119,36 +9133,36 @@
       <c r="D17" s="302">
         <v>128</v>
       </c>
-      <c r="E17" s="382"/>
-      <c r="F17" s="372"/>
-      <c r="G17" s="372"/>
-      <c r="H17" s="372"/>
-      <c r="I17" s="372"/>
-      <c r="J17" s="383"/>
-      <c r="K17" s="371"/>
-      <c r="L17" s="372"/>
-      <c r="M17" s="372"/>
-      <c r="N17" s="372"/>
-      <c r="O17" s="372"/>
-      <c r="P17" s="372"/>
-      <c r="Q17" s="372"/>
-      <c r="R17" s="372"/>
-      <c r="S17" s="372"/>
-      <c r="T17" s="372"/>
-      <c r="U17" s="372"/>
-      <c r="V17" s="372"/>
-      <c r="W17" s="372"/>
-      <c r="X17" s="372"/>
-      <c r="Y17" s="372"/>
-      <c r="Z17" s="372"/>
-      <c r="AA17" s="372"/>
-      <c r="AB17" s="372"/>
-      <c r="AC17" s="373"/>
+      <c r="E17" s="389"/>
+      <c r="F17" s="379"/>
+      <c r="G17" s="379"/>
+      <c r="H17" s="379"/>
+      <c r="I17" s="379"/>
+      <c r="J17" s="390"/>
+      <c r="K17" s="378"/>
+      <c r="L17" s="379"/>
+      <c r="M17" s="379"/>
+      <c r="N17" s="379"/>
+      <c r="O17" s="379"/>
+      <c r="P17" s="379"/>
+      <c r="Q17" s="379"/>
+      <c r="R17" s="379"/>
+      <c r="S17" s="379"/>
+      <c r="T17" s="379"/>
+      <c r="U17" s="379"/>
+      <c r="V17" s="379"/>
+      <c r="W17" s="379"/>
+      <c r="X17" s="379"/>
+      <c r="Y17" s="379"/>
+      <c r="Z17" s="379"/>
+      <c r="AA17" s="379"/>
+      <c r="AB17" s="379"/>
+      <c r="AC17" s="380"/>
       <c r="AD17" s="318"/>
       <c r="AE17" s="246"/>
     </row>
     <row r="18" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="348"/>
+      <c r="A18" s="355"/>
       <c r="B18" s="300"/>
       <c r="C18" s="301" t="s">
         <v>28</v>
@@ -9156,36 +9170,36 @@
       <c r="D18" s="302" t="s">
         <v>336</v>
       </c>
-      <c r="E18" s="382"/>
-      <c r="F18" s="372"/>
-      <c r="G18" s="372"/>
-      <c r="H18" s="372"/>
-      <c r="I18" s="372"/>
-      <c r="J18" s="383"/>
-      <c r="K18" s="371"/>
-      <c r="L18" s="372"/>
-      <c r="M18" s="372"/>
-      <c r="N18" s="372"/>
-      <c r="O18" s="372"/>
-      <c r="P18" s="372"/>
-      <c r="Q18" s="372"/>
-      <c r="R18" s="372"/>
-      <c r="S18" s="372"/>
-      <c r="T18" s="372"/>
-      <c r="U18" s="372"/>
-      <c r="V18" s="372"/>
-      <c r="W18" s="372"/>
-      <c r="X18" s="372"/>
-      <c r="Y18" s="372"/>
-      <c r="Z18" s="372"/>
-      <c r="AA18" s="372"/>
-      <c r="AB18" s="372"/>
-      <c r="AC18" s="373"/>
+      <c r="E18" s="389"/>
+      <c r="F18" s="379"/>
+      <c r="G18" s="379"/>
+      <c r="H18" s="379"/>
+      <c r="I18" s="379"/>
+      <c r="J18" s="390"/>
+      <c r="K18" s="378"/>
+      <c r="L18" s="379"/>
+      <c r="M18" s="379"/>
+      <c r="N18" s="379"/>
+      <c r="O18" s="379"/>
+      <c r="P18" s="379"/>
+      <c r="Q18" s="379"/>
+      <c r="R18" s="379"/>
+      <c r="S18" s="379"/>
+      <c r="T18" s="379"/>
+      <c r="U18" s="379"/>
+      <c r="V18" s="379"/>
+      <c r="W18" s="379"/>
+      <c r="X18" s="379"/>
+      <c r="Y18" s="379"/>
+      <c r="Z18" s="379"/>
+      <c r="AA18" s="379"/>
+      <c r="AB18" s="379"/>
+      <c r="AC18" s="380"/>
       <c r="AD18" s="318"/>
       <c r="AE18" s="246"/>
     </row>
     <row r="19" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="348"/>
+      <c r="A19" s="355"/>
       <c r="B19" s="300"/>
       <c r="C19" s="301" t="s">
         <v>29</v>
@@ -9193,36 +9207,36 @@
       <c r="D19" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="382"/>
-      <c r="F19" s="372"/>
-      <c r="G19" s="372"/>
-      <c r="H19" s="372"/>
-      <c r="I19" s="372"/>
-      <c r="J19" s="383"/>
-      <c r="K19" s="371"/>
-      <c r="L19" s="372"/>
-      <c r="M19" s="372"/>
-      <c r="N19" s="372"/>
-      <c r="O19" s="372"/>
-      <c r="P19" s="372"/>
-      <c r="Q19" s="372"/>
-      <c r="R19" s="372"/>
-      <c r="S19" s="372"/>
-      <c r="T19" s="372"/>
-      <c r="U19" s="372"/>
-      <c r="V19" s="372"/>
-      <c r="W19" s="372"/>
-      <c r="X19" s="372"/>
-      <c r="Y19" s="372"/>
-      <c r="Z19" s="372"/>
-      <c r="AA19" s="372"/>
-      <c r="AB19" s="372"/>
-      <c r="AC19" s="373"/>
+      <c r="E19" s="389"/>
+      <c r="F19" s="379"/>
+      <c r="G19" s="379"/>
+      <c r="H19" s="379"/>
+      <c r="I19" s="379"/>
+      <c r="J19" s="390"/>
+      <c r="K19" s="378"/>
+      <c r="L19" s="379"/>
+      <c r="M19" s="379"/>
+      <c r="N19" s="379"/>
+      <c r="O19" s="379"/>
+      <c r="P19" s="379"/>
+      <c r="Q19" s="379"/>
+      <c r="R19" s="379"/>
+      <c r="S19" s="379"/>
+      <c r="T19" s="379"/>
+      <c r="U19" s="379"/>
+      <c r="V19" s="379"/>
+      <c r="W19" s="379"/>
+      <c r="X19" s="379"/>
+      <c r="Y19" s="379"/>
+      <c r="Z19" s="379"/>
+      <c r="AA19" s="379"/>
+      <c r="AB19" s="379"/>
+      <c r="AC19" s="380"/>
       <c r="AD19" s="318"/>
       <c r="AE19" s="246"/>
     </row>
     <row r="20" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="348"/>
+      <c r="A20" s="355"/>
       <c r="B20" s="300" t="s">
         <v>100</v>
       </c>
@@ -9232,36 +9246,36 @@
       <c r="D20" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="382"/>
-      <c r="F20" s="372"/>
-      <c r="G20" s="372"/>
-      <c r="H20" s="372"/>
-      <c r="I20" s="372"/>
-      <c r="J20" s="383"/>
-      <c r="K20" s="371"/>
-      <c r="L20" s="372"/>
-      <c r="M20" s="372"/>
-      <c r="N20" s="372"/>
-      <c r="O20" s="372"/>
-      <c r="P20" s="372"/>
-      <c r="Q20" s="372"/>
-      <c r="R20" s="372"/>
-      <c r="S20" s="372"/>
-      <c r="T20" s="372"/>
-      <c r="U20" s="372"/>
-      <c r="V20" s="372"/>
-      <c r="W20" s="372"/>
-      <c r="X20" s="372"/>
-      <c r="Y20" s="372"/>
-      <c r="Z20" s="372"/>
-      <c r="AA20" s="372"/>
-      <c r="AB20" s="372"/>
-      <c r="AC20" s="373"/>
+      <c r="E20" s="389"/>
+      <c r="F20" s="379"/>
+      <c r="G20" s="379"/>
+      <c r="H20" s="379"/>
+      <c r="I20" s="379"/>
+      <c r="J20" s="390"/>
+      <c r="K20" s="378"/>
+      <c r="L20" s="379"/>
+      <c r="M20" s="379"/>
+      <c r="N20" s="379"/>
+      <c r="O20" s="379"/>
+      <c r="P20" s="379"/>
+      <c r="Q20" s="379"/>
+      <c r="R20" s="379"/>
+      <c r="S20" s="379"/>
+      <c r="T20" s="379"/>
+      <c r="U20" s="379"/>
+      <c r="V20" s="379"/>
+      <c r="W20" s="379"/>
+      <c r="X20" s="379"/>
+      <c r="Y20" s="379"/>
+      <c r="Z20" s="379"/>
+      <c r="AA20" s="379"/>
+      <c r="AB20" s="379"/>
+      <c r="AC20" s="380"/>
       <c r="AD20" s="318"/>
       <c r="AE20" s="246"/>
     </row>
     <row r="21" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="348"/>
+      <c r="A21" s="355"/>
       <c r="B21" s="300" t="s">
         <v>46</v>
       </c>
@@ -9271,36 +9285,36 @@
       <c r="D21" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="382"/>
-      <c r="F21" s="372"/>
-      <c r="G21" s="372"/>
-      <c r="H21" s="372"/>
-      <c r="I21" s="372"/>
-      <c r="J21" s="383"/>
-      <c r="K21" s="371"/>
-      <c r="L21" s="372"/>
-      <c r="M21" s="372"/>
-      <c r="N21" s="372"/>
-      <c r="O21" s="372"/>
-      <c r="P21" s="372"/>
-      <c r="Q21" s="372"/>
-      <c r="R21" s="372"/>
-      <c r="S21" s="372"/>
-      <c r="T21" s="372"/>
-      <c r="U21" s="372"/>
-      <c r="V21" s="372"/>
-      <c r="W21" s="372"/>
-      <c r="X21" s="372"/>
-      <c r="Y21" s="372"/>
-      <c r="Z21" s="372"/>
-      <c r="AA21" s="372"/>
-      <c r="AB21" s="372"/>
-      <c r="AC21" s="373"/>
+      <c r="E21" s="389"/>
+      <c r="F21" s="379"/>
+      <c r="G21" s="379"/>
+      <c r="H21" s="379"/>
+      <c r="I21" s="379"/>
+      <c r="J21" s="390"/>
+      <c r="K21" s="378"/>
+      <c r="L21" s="379"/>
+      <c r="M21" s="379"/>
+      <c r="N21" s="379"/>
+      <c r="O21" s="379"/>
+      <c r="P21" s="379"/>
+      <c r="Q21" s="379"/>
+      <c r="R21" s="379"/>
+      <c r="S21" s="379"/>
+      <c r="T21" s="379"/>
+      <c r="U21" s="379"/>
+      <c r="V21" s="379"/>
+      <c r="W21" s="379"/>
+      <c r="X21" s="379"/>
+      <c r="Y21" s="379"/>
+      <c r="Z21" s="379"/>
+      <c r="AA21" s="379"/>
+      <c r="AB21" s="379"/>
+      <c r="AC21" s="380"/>
       <c r="AD21" s="318"/>
       <c r="AE21" s="201"/>
     </row>
     <row r="22" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="348"/>
+      <c r="A22" s="355"/>
       <c r="B22" s="300"/>
       <c r="C22" s="301" t="s">
         <v>337</v>
@@ -9308,104 +9322,104 @@
       <c r="D22" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="382"/>
-      <c r="F22" s="372"/>
-      <c r="G22" s="372"/>
-      <c r="H22" s="372"/>
-      <c r="I22" s="372"/>
-      <c r="J22" s="383"/>
-      <c r="K22" s="371"/>
-      <c r="L22" s="372"/>
-      <c r="M22" s="372"/>
-      <c r="N22" s="372"/>
-      <c r="O22" s="372"/>
-      <c r="P22" s="372"/>
-      <c r="Q22" s="372"/>
-      <c r="R22" s="372"/>
-      <c r="S22" s="372"/>
-      <c r="T22" s="372"/>
-      <c r="U22" s="372"/>
-      <c r="V22" s="372"/>
-      <c r="W22" s="372"/>
-      <c r="X22" s="372"/>
-      <c r="Y22" s="372"/>
-      <c r="Z22" s="372"/>
-      <c r="AA22" s="372"/>
-      <c r="AB22" s="372"/>
-      <c r="AC22" s="373"/>
+      <c r="E22" s="389"/>
+      <c r="F22" s="379"/>
+      <c r="G22" s="379"/>
+      <c r="H22" s="379"/>
+      <c r="I22" s="379"/>
+      <c r="J22" s="390"/>
+      <c r="K22" s="378"/>
+      <c r="L22" s="379"/>
+      <c r="M22" s="379"/>
+      <c r="N22" s="379"/>
+      <c r="O22" s="379"/>
+      <c r="P22" s="379"/>
+      <c r="Q22" s="379"/>
+      <c r="R22" s="379"/>
+      <c r="S22" s="379"/>
+      <c r="T22" s="379"/>
+      <c r="U22" s="379"/>
+      <c r="V22" s="379"/>
+      <c r="W22" s="379"/>
+      <c r="X22" s="379"/>
+      <c r="Y22" s="379"/>
+      <c r="Z22" s="379"/>
+      <c r="AA22" s="379"/>
+      <c r="AB22" s="379"/>
+      <c r="AC22" s="380"/>
       <c r="AD22" s="318"/>
       <c r="AE22" s="201"/>
     </row>
     <row r="23" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="348"/>
+      <c r="A23" s="355"/>
       <c r="B23" s="300"/>
       <c r="C23" s="301"/>
       <c r="D23" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="382"/>
-      <c r="F23" s="372"/>
-      <c r="G23" s="372"/>
-      <c r="H23" s="372"/>
-      <c r="I23" s="372"/>
-      <c r="J23" s="383"/>
-      <c r="K23" s="371"/>
-      <c r="L23" s="372"/>
-      <c r="M23" s="372"/>
-      <c r="N23" s="372"/>
-      <c r="O23" s="372"/>
-      <c r="P23" s="372"/>
-      <c r="Q23" s="372"/>
-      <c r="R23" s="372"/>
-      <c r="S23" s="372"/>
-      <c r="T23" s="372"/>
-      <c r="U23" s="372"/>
-      <c r="V23" s="372"/>
-      <c r="W23" s="372"/>
-      <c r="X23" s="372"/>
-      <c r="Y23" s="372"/>
-      <c r="Z23" s="372"/>
-      <c r="AA23" s="372"/>
-      <c r="AB23" s="372"/>
-      <c r="AC23" s="373"/>
+      <c r="E23" s="389"/>
+      <c r="F23" s="379"/>
+      <c r="G23" s="379"/>
+      <c r="H23" s="379"/>
+      <c r="I23" s="379"/>
+      <c r="J23" s="390"/>
+      <c r="K23" s="378"/>
+      <c r="L23" s="379"/>
+      <c r="M23" s="379"/>
+      <c r="N23" s="379"/>
+      <c r="O23" s="379"/>
+      <c r="P23" s="379"/>
+      <c r="Q23" s="379"/>
+      <c r="R23" s="379"/>
+      <c r="S23" s="379"/>
+      <c r="T23" s="379"/>
+      <c r="U23" s="379"/>
+      <c r="V23" s="379"/>
+      <c r="W23" s="379"/>
+      <c r="X23" s="379"/>
+      <c r="Y23" s="379"/>
+      <c r="Z23" s="379"/>
+      <c r="AA23" s="379"/>
+      <c r="AB23" s="379"/>
+      <c r="AC23" s="380"/>
       <c r="AD23" s="318"/>
       <c r="AE23" s="201"/>
     </row>
     <row r="24" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="348"/>
+      <c r="A24" s="355"/>
       <c r="B24" s="300"/>
       <c r="C24" s="301"/>
       <c r="D24" s="302"/>
-      <c r="E24" s="382"/>
-      <c r="F24" s="372"/>
-      <c r="G24" s="372"/>
-      <c r="H24" s="372"/>
-      <c r="I24" s="372"/>
-      <c r="J24" s="383"/>
-      <c r="K24" s="371"/>
-      <c r="L24" s="372"/>
-      <c r="M24" s="372"/>
-      <c r="N24" s="372"/>
-      <c r="O24" s="372"/>
-      <c r="P24" s="372"/>
-      <c r="Q24" s="372"/>
-      <c r="R24" s="372"/>
-      <c r="S24" s="372"/>
-      <c r="T24" s="372"/>
-      <c r="U24" s="372"/>
-      <c r="V24" s="372"/>
-      <c r="W24" s="372"/>
-      <c r="X24" s="372"/>
-      <c r="Y24" s="372"/>
-      <c r="Z24" s="372"/>
-      <c r="AA24" s="372"/>
-      <c r="AB24" s="372"/>
-      <c r="AC24" s="373"/>
+      <c r="E24" s="389"/>
+      <c r="F24" s="379"/>
+      <c r="G24" s="379"/>
+      <c r="H24" s="379"/>
+      <c r="I24" s="379"/>
+      <c r="J24" s="390"/>
+      <c r="K24" s="378"/>
+      <c r="L24" s="379"/>
+      <c r="M24" s="379"/>
+      <c r="N24" s="379"/>
+      <c r="O24" s="379"/>
+      <c r="P24" s="379"/>
+      <c r="Q24" s="379"/>
+      <c r="R24" s="379"/>
+      <c r="S24" s="379"/>
+      <c r="T24" s="379"/>
+      <c r="U24" s="379"/>
+      <c r="V24" s="379"/>
+      <c r="W24" s="379"/>
+      <c r="X24" s="379"/>
+      <c r="Y24" s="379"/>
+      <c r="Z24" s="379"/>
+      <c r="AA24" s="379"/>
+      <c r="AB24" s="379"/>
+      <c r="AC24" s="380"/>
       <c r="AD24" s="318"/>
       <c r="AE24" s="201"/>
     </row>
     <row r="25" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="348"/>
+      <c r="A25" s="355"/>
       <c r="B25" s="300"/>
       <c r="C25" s="301" t="s">
         <v>304</v>
@@ -9413,104 +9427,104 @@
       <c r="D25" s="302" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="382"/>
-      <c r="F25" s="372"/>
-      <c r="G25" s="372"/>
-      <c r="H25" s="372"/>
-      <c r="I25" s="372"/>
-      <c r="J25" s="383"/>
-      <c r="K25" s="371"/>
-      <c r="L25" s="372"/>
-      <c r="M25" s="372"/>
-      <c r="N25" s="372"/>
-      <c r="O25" s="372"/>
-      <c r="P25" s="372"/>
-      <c r="Q25" s="372"/>
-      <c r="R25" s="372"/>
-      <c r="S25" s="372"/>
-      <c r="T25" s="372"/>
-      <c r="U25" s="372"/>
-      <c r="V25" s="372"/>
-      <c r="W25" s="372"/>
-      <c r="X25" s="372"/>
-      <c r="Y25" s="372"/>
-      <c r="Z25" s="372"/>
-      <c r="AA25" s="372"/>
-      <c r="AB25" s="372"/>
-      <c r="AC25" s="373"/>
+      <c r="E25" s="389"/>
+      <c r="F25" s="379"/>
+      <c r="G25" s="379"/>
+      <c r="H25" s="379"/>
+      <c r="I25" s="379"/>
+      <c r="J25" s="390"/>
+      <c r="K25" s="378"/>
+      <c r="L25" s="379"/>
+      <c r="M25" s="379"/>
+      <c r="N25" s="379"/>
+      <c r="O25" s="379"/>
+      <c r="P25" s="379"/>
+      <c r="Q25" s="379"/>
+      <c r="R25" s="379"/>
+      <c r="S25" s="379"/>
+      <c r="T25" s="379"/>
+      <c r="U25" s="379"/>
+      <c r="V25" s="379"/>
+      <c r="W25" s="379"/>
+      <c r="X25" s="379"/>
+      <c r="Y25" s="379"/>
+      <c r="Z25" s="379"/>
+      <c r="AA25" s="379"/>
+      <c r="AB25" s="379"/>
+      <c r="AC25" s="380"/>
       <c r="AD25" s="318"/>
       <c r="AE25" s="201"/>
     </row>
     <row r="26" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="348"/>
+      <c r="A26" s="355"/>
       <c r="B26" s="300"/>
       <c r="C26" s="301"/>
       <c r="D26" s="302"/>
-      <c r="E26" s="382"/>
-      <c r="F26" s="372"/>
-      <c r="G26" s="372"/>
-      <c r="H26" s="372"/>
-      <c r="I26" s="372"/>
-      <c r="J26" s="383"/>
-      <c r="K26" s="371"/>
-      <c r="L26" s="372"/>
-      <c r="M26" s="372"/>
-      <c r="N26" s="372"/>
-      <c r="O26" s="372"/>
-      <c r="P26" s="372"/>
-      <c r="Q26" s="372"/>
-      <c r="R26" s="372"/>
-      <c r="S26" s="372"/>
-      <c r="T26" s="372"/>
-      <c r="U26" s="372"/>
-      <c r="V26" s="372"/>
-      <c r="W26" s="372"/>
-      <c r="X26" s="372"/>
-      <c r="Y26" s="372"/>
-      <c r="Z26" s="372"/>
-      <c r="AA26" s="372"/>
-      <c r="AB26" s="372"/>
-      <c r="AC26" s="373"/>
+      <c r="E26" s="389"/>
+      <c r="F26" s="379"/>
+      <c r="G26" s="379"/>
+      <c r="H26" s="379"/>
+      <c r="I26" s="379"/>
+      <c r="J26" s="390"/>
+      <c r="K26" s="378"/>
+      <c r="L26" s="379"/>
+      <c r="M26" s="379"/>
+      <c r="N26" s="379"/>
+      <c r="O26" s="379"/>
+      <c r="P26" s="379"/>
+      <c r="Q26" s="379"/>
+      <c r="R26" s="379"/>
+      <c r="S26" s="379"/>
+      <c r="T26" s="379"/>
+      <c r="U26" s="379"/>
+      <c r="V26" s="379"/>
+      <c r="W26" s="379"/>
+      <c r="X26" s="379"/>
+      <c r="Y26" s="379"/>
+      <c r="Z26" s="379"/>
+      <c r="AA26" s="379"/>
+      <c r="AB26" s="379"/>
+      <c r="AC26" s="380"/>
       <c r="AD26" s="318"/>
       <c r="AE26" s="201"/>
     </row>
     <row r="27" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="348"/>
+      <c r="A27" s="355"/>
       <c r="B27" s="300"/>
       <c r="C27" s="301"/>
       <c r="D27" s="302"/>
-      <c r="E27" s="382"/>
-      <c r="F27" s="372"/>
-      <c r="G27" s="372"/>
-      <c r="H27" s="372"/>
-      <c r="I27" s="372"/>
-      <c r="J27" s="383"/>
-      <c r="K27" s="371"/>
-      <c r="L27" s="372"/>
-      <c r="M27" s="372"/>
-      <c r="N27" s="372"/>
-      <c r="O27" s="372"/>
-      <c r="P27" s="372"/>
-      <c r="Q27" s="372"/>
-      <c r="R27" s="372"/>
-      <c r="S27" s="372"/>
-      <c r="T27" s="372"/>
-      <c r="U27" s="372"/>
-      <c r="V27" s="372"/>
-      <c r="W27" s="372"/>
-      <c r="X27" s="372"/>
-      <c r="Y27" s="372"/>
-      <c r="Z27" s="372"/>
-      <c r="AA27" s="372"/>
-      <c r="AB27" s="372"/>
-      <c r="AC27" s="373"/>
+      <c r="E27" s="389"/>
+      <c r="F27" s="379"/>
+      <c r="G27" s="379"/>
+      <c r="H27" s="379"/>
+      <c r="I27" s="379"/>
+      <c r="J27" s="390"/>
+      <c r="K27" s="378"/>
+      <c r="L27" s="379"/>
+      <c r="M27" s="379"/>
+      <c r="N27" s="379"/>
+      <c r="O27" s="379"/>
+      <c r="P27" s="379"/>
+      <c r="Q27" s="379"/>
+      <c r="R27" s="379"/>
+      <c r="S27" s="379"/>
+      <c r="T27" s="379"/>
+      <c r="U27" s="379"/>
+      <c r="V27" s="379"/>
+      <c r="W27" s="379"/>
+      <c r="X27" s="379"/>
+      <c r="Y27" s="379"/>
+      <c r="Z27" s="379"/>
+      <c r="AA27" s="379"/>
+      <c r="AB27" s="379"/>
+      <c r="AC27" s="380"/>
       <c r="AD27" s="318"/>
       <c r="AE27" s="201" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="348"/>
+      <c r="A28" s="355"/>
       <c r="B28" s="300"/>
       <c r="C28" s="301" t="s">
         <v>189</v>
@@ -9518,102 +9532,102 @@
       <c r="D28" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="382"/>
-      <c r="F28" s="372"/>
-      <c r="G28" s="372"/>
-      <c r="H28" s="372"/>
-      <c r="I28" s="372"/>
-      <c r="J28" s="383"/>
-      <c r="K28" s="371"/>
-      <c r="L28" s="372"/>
-      <c r="M28" s="372"/>
-      <c r="N28" s="372"/>
-      <c r="O28" s="372"/>
-      <c r="P28" s="372"/>
-      <c r="Q28" s="372"/>
-      <c r="R28" s="372"/>
-      <c r="S28" s="372"/>
-      <c r="T28" s="372"/>
-      <c r="U28" s="372"/>
-      <c r="V28" s="372"/>
-      <c r="W28" s="372"/>
-      <c r="X28" s="372"/>
-      <c r="Y28" s="372"/>
-      <c r="Z28" s="372"/>
-      <c r="AA28" s="372"/>
-      <c r="AB28" s="372"/>
-      <c r="AC28" s="373"/>
+      <c r="E28" s="389"/>
+      <c r="F28" s="379"/>
+      <c r="G28" s="379"/>
+      <c r="H28" s="379"/>
+      <c r="I28" s="379"/>
+      <c r="J28" s="390"/>
+      <c r="K28" s="378"/>
+      <c r="L28" s="379"/>
+      <c r="M28" s="379"/>
+      <c r="N28" s="379"/>
+      <c r="O28" s="379"/>
+      <c r="P28" s="379"/>
+      <c r="Q28" s="379"/>
+      <c r="R28" s="379"/>
+      <c r="S28" s="379"/>
+      <c r="T28" s="379"/>
+      <c r="U28" s="379"/>
+      <c r="V28" s="379"/>
+      <c r="W28" s="379"/>
+      <c r="X28" s="379"/>
+      <c r="Y28" s="379"/>
+      <c r="Z28" s="379"/>
+      <c r="AA28" s="379"/>
+      <c r="AB28" s="379"/>
+      <c r="AC28" s="380"/>
       <c r="AD28" s="318"/>
       <c r="AE28" s="201"/>
     </row>
     <row r="29" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="348"/>
+      <c r="A29" s="355"/>
       <c r="B29" s="300"/>
       <c r="C29" s="301"/>
       <c r="D29" s="302"/>
-      <c r="E29" s="382"/>
-      <c r="F29" s="372"/>
-      <c r="G29" s="372"/>
-      <c r="H29" s="372"/>
-      <c r="I29" s="372"/>
-      <c r="J29" s="383"/>
-      <c r="K29" s="371"/>
-      <c r="L29" s="372"/>
-      <c r="M29" s="372"/>
-      <c r="N29" s="372"/>
-      <c r="O29" s="372"/>
-      <c r="P29" s="372"/>
-      <c r="Q29" s="372"/>
-      <c r="R29" s="372"/>
-      <c r="S29" s="372"/>
-      <c r="T29" s="372"/>
-      <c r="U29" s="372"/>
-      <c r="V29" s="372"/>
-      <c r="W29" s="372"/>
-      <c r="X29" s="372"/>
-      <c r="Y29" s="372"/>
-      <c r="Z29" s="372"/>
-      <c r="AA29" s="372"/>
-      <c r="AB29" s="372"/>
-      <c r="AC29" s="373"/>
+      <c r="E29" s="389"/>
+      <c r="F29" s="379"/>
+      <c r="G29" s="379"/>
+      <c r="H29" s="379"/>
+      <c r="I29" s="379"/>
+      <c r="J29" s="390"/>
+      <c r="K29" s="378"/>
+      <c r="L29" s="379"/>
+      <c r="M29" s="379"/>
+      <c r="N29" s="379"/>
+      <c r="O29" s="379"/>
+      <c r="P29" s="379"/>
+      <c r="Q29" s="379"/>
+      <c r="R29" s="379"/>
+      <c r="S29" s="379"/>
+      <c r="T29" s="379"/>
+      <c r="U29" s="379"/>
+      <c r="V29" s="379"/>
+      <c r="W29" s="379"/>
+      <c r="X29" s="379"/>
+      <c r="Y29" s="379"/>
+      <c r="Z29" s="379"/>
+      <c r="AA29" s="379"/>
+      <c r="AB29" s="379"/>
+      <c r="AC29" s="380"/>
       <c r="AD29" s="318"/>
       <c r="AE29" s="201"/>
     </row>
     <row r="30" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="348"/>
+      <c r="A30" s="355"/>
       <c r="B30" s="300"/>
       <c r="C30" s="301"/>
       <c r="D30" s="302"/>
-      <c r="E30" s="382"/>
-      <c r="F30" s="372"/>
-      <c r="G30" s="372"/>
-      <c r="H30" s="372"/>
-      <c r="I30" s="372"/>
-      <c r="J30" s="383"/>
-      <c r="K30" s="371"/>
-      <c r="L30" s="372"/>
-      <c r="M30" s="372"/>
-      <c r="N30" s="372"/>
-      <c r="O30" s="372"/>
-      <c r="P30" s="372"/>
-      <c r="Q30" s="372"/>
-      <c r="R30" s="372"/>
-      <c r="S30" s="372"/>
-      <c r="T30" s="372"/>
-      <c r="U30" s="372"/>
-      <c r="V30" s="372"/>
-      <c r="W30" s="372"/>
-      <c r="X30" s="372"/>
-      <c r="Y30" s="372"/>
-      <c r="Z30" s="372"/>
-      <c r="AA30" s="372"/>
-      <c r="AB30" s="372"/>
-      <c r="AC30" s="373"/>
+      <c r="E30" s="389"/>
+      <c r="F30" s="379"/>
+      <c r="G30" s="379"/>
+      <c r="H30" s="379"/>
+      <c r="I30" s="379"/>
+      <c r="J30" s="390"/>
+      <c r="K30" s="378"/>
+      <c r="L30" s="379"/>
+      <c r="M30" s="379"/>
+      <c r="N30" s="379"/>
+      <c r="O30" s="379"/>
+      <c r="P30" s="379"/>
+      <c r="Q30" s="379"/>
+      <c r="R30" s="379"/>
+      <c r="S30" s="379"/>
+      <c r="T30" s="379"/>
+      <c r="U30" s="379"/>
+      <c r="V30" s="379"/>
+      <c r="W30" s="379"/>
+      <c r="X30" s="379"/>
+      <c r="Y30" s="379"/>
+      <c r="Z30" s="379"/>
+      <c r="AA30" s="379"/>
+      <c r="AB30" s="379"/>
+      <c r="AC30" s="380"/>
       <c r="AD30" s="318"/>
       <c r="AE30" s="201"/>
     </row>
     <row r="31" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="348"/>
+      <c r="A31" s="355"/>
       <c r="B31" s="300"/>
       <c r="C31" s="301" t="s">
         <v>74</v>
@@ -9621,36 +9635,36 @@
       <c r="D31" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="382"/>
-      <c r="F31" s="372"/>
-      <c r="G31" s="372"/>
-      <c r="H31" s="372"/>
-      <c r="I31" s="372"/>
-      <c r="J31" s="383"/>
-      <c r="K31" s="371"/>
-      <c r="L31" s="372"/>
-      <c r="M31" s="372"/>
-      <c r="N31" s="372"/>
-      <c r="O31" s="372"/>
-      <c r="P31" s="372"/>
-      <c r="Q31" s="372"/>
-      <c r="R31" s="372"/>
-      <c r="S31" s="372"/>
-      <c r="T31" s="372"/>
-      <c r="U31" s="372"/>
-      <c r="V31" s="372"/>
-      <c r="W31" s="372"/>
-      <c r="X31" s="372"/>
-      <c r="Y31" s="372"/>
-      <c r="Z31" s="372"/>
-      <c r="AA31" s="372"/>
-      <c r="AB31" s="372"/>
-      <c r="AC31" s="373"/>
+      <c r="E31" s="389"/>
+      <c r="F31" s="379"/>
+      <c r="G31" s="379"/>
+      <c r="H31" s="379"/>
+      <c r="I31" s="379"/>
+      <c r="J31" s="390"/>
+      <c r="K31" s="378"/>
+      <c r="L31" s="379"/>
+      <c r="M31" s="379"/>
+      <c r="N31" s="379"/>
+      <c r="O31" s="379"/>
+      <c r="P31" s="379"/>
+      <c r="Q31" s="379"/>
+      <c r="R31" s="379"/>
+      <c r="S31" s="379"/>
+      <c r="T31" s="379"/>
+      <c r="U31" s="379"/>
+      <c r="V31" s="379"/>
+      <c r="W31" s="379"/>
+      <c r="X31" s="379"/>
+      <c r="Y31" s="379"/>
+      <c r="Z31" s="379"/>
+      <c r="AA31" s="379"/>
+      <c r="AB31" s="379"/>
+      <c r="AC31" s="380"/>
       <c r="AD31" s="318"/>
       <c r="AE31" s="201"/>
     </row>
     <row r="32" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="348"/>
+      <c r="A32" s="355"/>
       <c r="B32" s="300"/>
       <c r="C32" s="301" t="s">
         <v>75</v>
@@ -9658,69 +9672,69 @@
       <c r="D32" s="302" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="382"/>
-      <c r="F32" s="372"/>
-      <c r="G32" s="372"/>
-      <c r="H32" s="372"/>
-      <c r="I32" s="372"/>
-      <c r="J32" s="383"/>
-      <c r="K32" s="371"/>
-      <c r="L32" s="372"/>
-      <c r="M32" s="372"/>
-      <c r="N32" s="372"/>
-      <c r="O32" s="372"/>
-      <c r="P32" s="372"/>
-      <c r="Q32" s="372"/>
-      <c r="R32" s="372"/>
-      <c r="S32" s="372"/>
-      <c r="T32" s="372"/>
-      <c r="U32" s="372"/>
-      <c r="V32" s="372"/>
-      <c r="W32" s="372"/>
-      <c r="X32" s="372"/>
-      <c r="Y32" s="372"/>
-      <c r="Z32" s="372"/>
-      <c r="AA32" s="372"/>
-      <c r="AB32" s="372"/>
-      <c r="AC32" s="373"/>
+      <c r="E32" s="389"/>
+      <c r="F32" s="379"/>
+      <c r="G32" s="379"/>
+      <c r="H32" s="379"/>
+      <c r="I32" s="379"/>
+      <c r="J32" s="390"/>
+      <c r="K32" s="378"/>
+      <c r="L32" s="379"/>
+      <c r="M32" s="379"/>
+      <c r="N32" s="379"/>
+      <c r="O32" s="379"/>
+      <c r="P32" s="379"/>
+      <c r="Q32" s="379"/>
+      <c r="R32" s="379"/>
+      <c r="S32" s="379"/>
+      <c r="T32" s="379"/>
+      <c r="U32" s="379"/>
+      <c r="V32" s="379"/>
+      <c r="W32" s="379"/>
+      <c r="X32" s="379"/>
+      <c r="Y32" s="379"/>
+      <c r="Z32" s="379"/>
+      <c r="AA32" s="379"/>
+      <c r="AB32" s="379"/>
+      <c r="AC32" s="380"/>
       <c r="AD32" s="318"/>
       <c r="AE32" s="201"/>
     </row>
     <row r="33" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="348"/>
+      <c r="A33" s="355"/>
       <c r="B33" s="300"/>
       <c r="C33" s="301"/>
       <c r="D33" s="302"/>
-      <c r="E33" s="382"/>
-      <c r="F33" s="372"/>
-      <c r="G33" s="372"/>
-      <c r="H33" s="372"/>
-      <c r="I33" s="372"/>
-      <c r="J33" s="383"/>
-      <c r="K33" s="371"/>
-      <c r="L33" s="372"/>
-      <c r="M33" s="372"/>
-      <c r="N33" s="372"/>
-      <c r="O33" s="372"/>
-      <c r="P33" s="372"/>
-      <c r="Q33" s="372"/>
-      <c r="R33" s="372"/>
-      <c r="S33" s="372"/>
-      <c r="T33" s="372"/>
-      <c r="U33" s="372"/>
-      <c r="V33" s="372"/>
-      <c r="W33" s="372"/>
-      <c r="X33" s="372"/>
-      <c r="Y33" s="372"/>
-      <c r="Z33" s="372"/>
-      <c r="AA33" s="372"/>
-      <c r="AB33" s="372"/>
-      <c r="AC33" s="373"/>
+      <c r="E33" s="389"/>
+      <c r="F33" s="379"/>
+      <c r="G33" s="379"/>
+      <c r="H33" s="379"/>
+      <c r="I33" s="379"/>
+      <c r="J33" s="390"/>
+      <c r="K33" s="378"/>
+      <c r="L33" s="379"/>
+      <c r="M33" s="379"/>
+      <c r="N33" s="379"/>
+      <c r="O33" s="379"/>
+      <c r="P33" s="379"/>
+      <c r="Q33" s="379"/>
+      <c r="R33" s="379"/>
+      <c r="S33" s="379"/>
+      <c r="T33" s="379"/>
+      <c r="U33" s="379"/>
+      <c r="V33" s="379"/>
+      <c r="W33" s="379"/>
+      <c r="X33" s="379"/>
+      <c r="Y33" s="379"/>
+      <c r="Z33" s="379"/>
+      <c r="AA33" s="379"/>
+      <c r="AB33" s="379"/>
+      <c r="AC33" s="380"/>
       <c r="AD33" s="318"/>
       <c r="AE33" s="201"/>
     </row>
     <row r="34" spans="1:31" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="348"/>
+      <c r="A34" s="355"/>
       <c r="B34" s="304"/>
       <c r="C34" s="305" t="s">
         <v>77</v>
@@ -9728,43 +9742,43 @@
       <c r="D34" s="306" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="384"/>
-      <c r="F34" s="375"/>
-      <c r="G34" s="375"/>
-      <c r="H34" s="375"/>
-      <c r="I34" s="375"/>
-      <c r="J34" s="385"/>
-      <c r="K34" s="374"/>
-      <c r="L34" s="375"/>
-      <c r="M34" s="375"/>
-      <c r="N34" s="375"/>
-      <c r="O34" s="375"/>
-      <c r="P34" s="375"/>
-      <c r="Q34" s="375"/>
-      <c r="R34" s="375"/>
-      <c r="S34" s="375"/>
-      <c r="T34" s="375"/>
-      <c r="U34" s="375"/>
-      <c r="V34" s="375"/>
-      <c r="W34" s="375"/>
-      <c r="X34" s="375"/>
-      <c r="Y34" s="375"/>
-      <c r="Z34" s="375"/>
-      <c r="AA34" s="375"/>
-      <c r="AB34" s="375"/>
-      <c r="AC34" s="376"/>
+      <c r="E34" s="391"/>
+      <c r="F34" s="382"/>
+      <c r="G34" s="382"/>
+      <c r="H34" s="382"/>
+      <c r="I34" s="382"/>
+      <c r="J34" s="392"/>
+      <c r="K34" s="381"/>
+      <c r="L34" s="382"/>
+      <c r="M34" s="382"/>
+      <c r="N34" s="382"/>
+      <c r="O34" s="382"/>
+      <c r="P34" s="382"/>
+      <c r="Q34" s="382"/>
+      <c r="R34" s="382"/>
+      <c r="S34" s="382"/>
+      <c r="T34" s="382"/>
+      <c r="U34" s="382"/>
+      <c r="V34" s="382"/>
+      <c r="W34" s="382"/>
+      <c r="X34" s="382"/>
+      <c r="Y34" s="382"/>
+      <c r="Z34" s="382"/>
+      <c r="AA34" s="382"/>
+      <c r="AB34" s="382"/>
+      <c r="AC34" s="383"/>
       <c r="AD34" s="318"/>
       <c r="AE34" s="201"/>
     </row>
     <row r="35" spans="1:31" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="348"/>
+      <c r="A35" s="355"/>
       <c r="B35" s="47" t="s">
         <v>309</v>
       </c>
       <c r="C35" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="365" t="s">
+      <c r="D35" s="372" t="s">
         <v>383</v>
       </c>
       <c r="E35" s="116"/>
@@ -9836,12 +9850,12 @@
       <c r="AE35" s="73"/>
     </row>
     <row r="36" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="348"/>
+      <c r="A36" s="355"/>
       <c r="B36" s="53"/>
       <c r="C36" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="365"/>
+      <c r="D36" s="372"/>
       <c r="E36" s="117"/>
       <c r="F36" s="36"/>
       <c r="G36" s="36"/>
@@ -9911,12 +9925,12 @@
       <c r="AE36" s="201"/>
     </row>
     <row r="37" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="348"/>
+      <c r="A37" s="355"/>
       <c r="B37" s="53"/>
       <c r="C37" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="D37" s="365"/>
+      <c r="D37" s="372"/>
       <c r="E37" s="117"/>
       <c r="F37" s="36"/>
       <c r="G37" s="36"/>
@@ -9986,12 +10000,12 @@
       <c r="AE37" s="201"/>
     </row>
     <row r="38" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="348"/>
+      <c r="A38" s="355"/>
       <c r="B38" s="53"/>
       <c r="C38" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="D38" s="365"/>
+      <c r="D38" s="372"/>
       <c r="E38" s="117"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -10063,12 +10077,12 @@
       </c>
     </row>
     <row r="39" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="348"/>
+      <c r="A39" s="355"/>
       <c r="B39" s="53"/>
       <c r="C39" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="D39" s="365"/>
+      <c r="D39" s="372"/>
       <c r="E39" s="117"/>
       <c r="F39" s="36"/>
       <c r="G39" s="36"/>
@@ -10138,12 +10152,12 @@
       <c r="AE39" s="201"/>
     </row>
     <row r="40" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="348"/>
+      <c r="A40" s="355"/>
       <c r="B40" s="53"/>
       <c r="C40" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="D40" s="365"/>
+      <c r="D40" s="372"/>
       <c r="E40" s="117"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -10213,12 +10227,12 @@
       <c r="AE40" s="201"/>
     </row>
     <row r="41" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="348"/>
+      <c r="A41" s="355"/>
       <c r="B41" s="53"/>
       <c r="C41" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D41" s="365"/>
+      <c r="D41" s="372"/>
       <c r="E41" s="117"/>
       <c r="F41" s="36"/>
       <c r="G41" s="36"/>
@@ -10288,12 +10302,12 @@
       <c r="AE41" s="201"/>
     </row>
     <row r="42" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="348"/>
+      <c r="A42" s="355"/>
       <c r="B42" s="53"/>
       <c r="C42" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D42" s="365"/>
+      <c r="D42" s="372"/>
       <c r="E42" s="117"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -10337,12 +10351,12 @@
       <c r="AE42" s="202"/>
     </row>
     <row r="43" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="348"/>
+      <c r="A43" s="355"/>
       <c r="B43" s="53"/>
       <c r="C43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="365"/>
+      <c r="D43" s="372"/>
       <c r="E43" s="117"/>
       <c r="F43" s="36"/>
       <c r="G43" s="36"/>
@@ -10412,12 +10426,12 @@
       <c r="AE43" s="201"/>
     </row>
     <row r="44" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="348"/>
+      <c r="A44" s="355"/>
       <c r="B44" s="53"/>
       <c r="C44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="365"/>
+      <c r="D44" s="372"/>
       <c r="E44" s="117"/>
       <c r="F44" s="36"/>
       <c r="G44" s="36"/>
@@ -10479,12 +10493,12 @@
       <c r="AE44" s="201"/>
     </row>
     <row r="45" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="348"/>
+      <c r="A45" s="355"/>
       <c r="B45" s="53"/>
       <c r="C45" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="365"/>
+      <c r="D45" s="372"/>
       <c r="E45" s="117"/>
       <c r="F45" s="36"/>
       <c r="G45" s="36"/>
@@ -10548,12 +10562,12 @@
       </c>
     </row>
     <row r="46" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="348"/>
+      <c r="A46" s="355"/>
       <c r="B46" s="53"/>
       <c r="C46" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D46" s="365"/>
+      <c r="D46" s="372"/>
       <c r="E46" s="117"/>
       <c r="F46" s="36"/>
       <c r="G46" s="36"/>
@@ -10605,12 +10619,12 @@
       <c r="AE46" s="201"/>
     </row>
     <row r="47" spans="1:31" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="348"/>
+      <c r="A47" s="355"/>
       <c r="B47" s="74"/>
       <c r="C47" s="75" t="s">
         <v>285</v>
       </c>
-      <c r="D47" s="365"/>
+      <c r="D47" s="372"/>
       <c r="E47" s="119"/>
       <c r="F47" s="76"/>
       <c r="G47" s="76"/>
@@ -10640,14 +10654,14 @@
       <c r="AE47" s="203"/>
     </row>
     <row r="48" spans="1:31" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="348"/>
+      <c r="A48" s="355"/>
       <c r="B48" s="53" t="s">
         <v>23</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D48" s="365"/>
+      <c r="D48" s="372"/>
       <c r="E48" s="117"/>
       <c r="F48" s="36"/>
       <c r="G48" s="36"/>
@@ -10717,12 +10731,12 @@
       <c r="AE48" s="201"/>
     </row>
     <row r="49" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="348"/>
+      <c r="A49" s="355"/>
       <c r="B49" s="53"/>
       <c r="C49" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D49" s="365"/>
+      <c r="D49" s="372"/>
       <c r="E49" s="117"/>
       <c r="F49" s="36"/>
       <c r="G49" s="36"/>
@@ -10758,12 +10772,12 @@
       <c r="AE49" s="201"/>
     </row>
     <row r="50" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="348"/>
+      <c r="A50" s="355"/>
       <c r="B50" s="53"/>
       <c r="C50" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="D50" s="365"/>
+      <c r="D50" s="372"/>
       <c r="E50" s="117"/>
       <c r="F50" s="36"/>
       <c r="G50" s="36"/>
@@ -10799,12 +10813,12 @@
       <c r="AE50" s="201"/>
     </row>
     <row r="51" spans="1:32" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="348"/>
+      <c r="A51" s="355"/>
       <c r="B51" s="74"/>
       <c r="C51" s="75" t="s">
         <v>289</v>
       </c>
-      <c r="D51" s="365"/>
+      <c r="D51" s="372"/>
       <c r="E51" s="119"/>
       <c r="F51" s="76"/>
       <c r="G51" s="76"/>
@@ -10846,14 +10860,14 @@
       <c r="AE51" s="203"/>
     </row>
     <row r="52" spans="1:32" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="348"/>
+      <c r="A52" s="355"/>
       <c r="B52" s="47" t="s">
         <v>100</v>
       </c>
       <c r="C52" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="365"/>
+      <c r="D52" s="372"/>
       <c r="E52" s="116"/>
       <c r="F52" s="49"/>
       <c r="G52" s="49"/>
@@ -10925,12 +10939,12 @@
       </c>
     </row>
     <row r="53" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="348"/>
+      <c r="A53" s="355"/>
       <c r="B53" s="53"/>
       <c r="C53" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="365"/>
+      <c r="D53" s="372"/>
       <c r="E53" s="117"/>
       <c r="F53" s="36"/>
       <c r="G53" s="36"/>
@@ -11005,12 +11019,12 @@
       </c>
     </row>
     <row r="54" spans="1:32" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="348"/>
+      <c r="A54" s="355"/>
       <c r="B54" s="79"/>
       <c r="C54" s="75" t="s">
         <v>176</v>
       </c>
-      <c r="D54" s="365"/>
+      <c r="D54" s="372"/>
       <c r="E54" s="120"/>
       <c r="F54" s="80"/>
       <c r="G54" s="80"/>
@@ -11054,14 +11068,14 @@
       <c r="AE54" s="204"/>
     </row>
     <row r="55" spans="1:32" s="44" customFormat="1" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="348"/>
+      <c r="A55" s="355"/>
       <c r="B55" s="81" t="s">
         <v>305</v>
       </c>
       <c r="C55" s="82" t="s">
         <v>306</v>
       </c>
-      <c r="D55" s="365"/>
+      <c r="D55" s="372"/>
       <c r="E55" s="121"/>
       <c r="F55" s="83"/>
       <c r="G55" s="83"/>
@@ -11097,14 +11111,14 @@
       <c r="AE55" s="205"/>
     </row>
     <row r="56" spans="1:32" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="348"/>
+      <c r="A56" s="355"/>
       <c r="B56" s="47" t="s">
         <v>36</v>
       </c>
       <c r="C56" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="365"/>
+      <c r="D56" s="372"/>
       <c r="E56" s="116" t="s">
         <v>19</v>
       </c>
@@ -11186,12 +11200,12 @@
       <c r="AE56" s="73"/>
     </row>
     <row r="57" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="348"/>
+      <c r="A57" s="355"/>
       <c r="B57" s="54"/>
       <c r="C57" s="45" t="s">
         <v>281</v>
       </c>
-      <c r="D57" s="365"/>
+      <c r="D57" s="372"/>
       <c r="E57" s="122"/>
       <c r="F57" s="46" t="s">
         <v>10</v>
@@ -11271,12 +11285,12 @@
       <c r="AE57" s="206"/>
     </row>
     <row r="58" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="348"/>
+      <c r="A58" s="355"/>
       <c r="B58" s="54"/>
       <c r="C58" s="45" t="s">
         <v>282</v>
       </c>
-      <c r="D58" s="365"/>
+      <c r="D58" s="372"/>
       <c r="E58" s="124" t="s">
         <v>10</v>
       </c>
@@ -11358,12 +11372,12 @@
       <c r="AE58" s="206"/>
     </row>
     <row r="59" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="348"/>
+      <c r="A59" s="355"/>
       <c r="B59" s="53"/>
       <c r="C59" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D59" s="365"/>
+      <c r="D59" s="372"/>
       <c r="E59" s="117" t="s">
         <v>10</v>
       </c>
@@ -11445,12 +11459,12 @@
       <c r="AE59" s="201"/>
     </row>
     <row r="60" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="348"/>
+      <c r="A60" s="355"/>
       <c r="B60" s="53"/>
       <c r="C60" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D60" s="365"/>
+      <c r="D60" s="372"/>
       <c r="E60" s="125"/>
       <c r="F60" s="41"/>
       <c r="G60" s="41"/>
@@ -11506,12 +11520,12 @@
       </c>
     </row>
     <row r="61" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="348"/>
+      <c r="A61" s="355"/>
       <c r="B61" s="53"/>
       <c r="C61" s="224" t="s">
         <v>284</v>
       </c>
-      <c r="D61" s="365"/>
+      <c r="D61" s="372"/>
       <c r="E61" s="117" t="s">
         <v>19</v>
       </c>
@@ -11593,12 +11607,12 @@
       <c r="AE61" s="201"/>
     </row>
     <row r="62" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="348"/>
+      <c r="A62" s="355"/>
       <c r="B62" s="53"/>
       <c r="C62" s="225" t="s">
         <v>242</v>
       </c>
-      <c r="D62" s="365"/>
+      <c r="D62" s="372"/>
       <c r="E62" s="125"/>
       <c r="F62" s="41"/>
       <c r="G62" s="41"/>
@@ -11654,12 +11668,12 @@
       </c>
     </row>
     <row r="63" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="348"/>
+      <c r="A63" s="355"/>
       <c r="B63" s="53"/>
       <c r="C63" s="224" t="s">
         <v>38</v>
       </c>
-      <c r="D63" s="365"/>
+      <c r="D63" s="372"/>
       <c r="E63" s="117" t="s">
         <v>10</v>
       </c>
@@ -11741,12 +11755,12 @@
       <c r="AE63" s="201"/>
     </row>
     <row r="64" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="348"/>
+      <c r="A64" s="355"/>
       <c r="B64" s="53"/>
       <c r="C64" s="224" t="s">
         <v>243</v>
       </c>
-      <c r="D64" s="365"/>
+      <c r="D64" s="372"/>
       <c r="E64" s="117" t="s">
         <v>10</v>
       </c>
@@ -11828,12 +11842,12 @@
       <c r="AE64" s="201"/>
     </row>
     <row r="65" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="348"/>
+      <c r="A65" s="355"/>
       <c r="B65" s="53"/>
       <c r="C65" s="224" t="s">
         <v>244</v>
       </c>
-      <c r="D65" s="365"/>
+      <c r="D65" s="372"/>
       <c r="E65" s="117" t="s">
         <v>10</v>
       </c>
@@ -11915,12 +11929,12 @@
       <c r="AE65" s="201"/>
     </row>
     <row r="66" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="348"/>
+      <c r="A66" s="355"/>
       <c r="B66" s="53"/>
       <c r="C66" s="224" t="s">
         <v>245</v>
       </c>
-      <c r="D66" s="365"/>
+      <c r="D66" s="372"/>
       <c r="E66" s="117" t="s">
         <v>10</v>
       </c>
@@ -12002,12 +12016,12 @@
       <c r="AE66" s="201"/>
     </row>
     <row r="67" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="348"/>
+      <c r="A67" s="355"/>
       <c r="B67" s="53"/>
       <c r="C67" s="224" t="s">
         <v>235</v>
       </c>
-      <c r="D67" s="365"/>
+      <c r="D67" s="372"/>
       <c r="E67" s="126"/>
       <c r="F67" s="40"/>
       <c r="G67" s="40"/>
@@ -12057,12 +12071,12 @@
       <c r="AE67" s="201"/>
     </row>
     <row r="68" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="348"/>
+      <c r="A68" s="355"/>
       <c r="B68" s="53"/>
       <c r="C68" s="225" t="s">
         <v>39</v>
       </c>
-      <c r="D68" s="365"/>
+      <c r="D68" s="372"/>
       <c r="E68" s="125"/>
       <c r="F68" s="41"/>
       <c r="G68" s="41"/>
@@ -12116,12 +12130,12 @@
       <c r="AE68" s="202"/>
     </row>
     <row r="69" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="348"/>
+      <c r="A69" s="355"/>
       <c r="B69" s="53"/>
       <c r="C69" s="225" t="s">
         <v>40</v>
       </c>
-      <c r="D69" s="365"/>
+      <c r="D69" s="372"/>
       <c r="E69" s="125"/>
       <c r="F69" s="41"/>
       <c r="G69" s="41"/>
@@ -12175,12 +12189,12 @@
       <c r="AE69" s="201"/>
     </row>
     <row r="70" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="348"/>
+      <c r="A70" s="355"/>
       <c r="B70" s="53"/>
       <c r="C70" s="224" t="s">
         <v>247</v>
       </c>
-      <c r="D70" s="365"/>
+      <c r="D70" s="372"/>
       <c r="E70" s="117" t="s">
         <v>10</v>
       </c>
@@ -12262,12 +12276,12 @@
       <c r="AE70" s="201"/>
     </row>
     <row r="71" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="348"/>
+      <c r="A71" s="355"/>
       <c r="B71" s="53"/>
       <c r="C71" s="224" t="s">
         <v>246</v>
       </c>
-      <c r="D71" s="365"/>
+      <c r="D71" s="372"/>
       <c r="E71" s="117" t="s">
         <v>10</v>
       </c>
@@ -12349,12 +12363,12 @@
       <c r="AE71" s="201"/>
     </row>
     <row r="72" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="348"/>
+      <c r="A72" s="355"/>
       <c r="B72" s="53"/>
       <c r="C72" s="224" t="s">
         <v>248</v>
       </c>
-      <c r="D72" s="365"/>
+      <c r="D72" s="372"/>
       <c r="E72" s="117" t="s">
         <v>10</v>
       </c>
@@ -12436,12 +12450,12 @@
       <c r="AE72" s="201"/>
     </row>
     <row r="73" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="348"/>
+      <c r="A73" s="355"/>
       <c r="B73" s="53"/>
       <c r="C73" s="224" t="s">
         <v>249</v>
       </c>
-      <c r="D73" s="365"/>
+      <c r="D73" s="372"/>
       <c r="E73" s="117" t="s">
         <v>10</v>
       </c>
@@ -12523,12 +12537,12 @@
       <c r="AE73" s="201"/>
     </row>
     <row r="74" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="348"/>
+      <c r="A74" s="355"/>
       <c r="B74" s="53"/>
       <c r="C74" s="224" t="s">
         <v>41</v>
       </c>
-      <c r="D74" s="365"/>
+      <c r="D74" s="372"/>
       <c r="E74" s="126"/>
       <c r="F74" s="40"/>
       <c r="G74" s="40"/>
@@ -12582,12 +12596,12 @@
       <c r="AE74" s="201"/>
     </row>
     <row r="75" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="348"/>
+      <c r="A75" s="355"/>
       <c r="B75" s="53"/>
       <c r="C75" s="224" t="s">
         <v>272</v>
       </c>
-      <c r="D75" s="365"/>
+      <c r="D75" s="372"/>
       <c r="E75" s="126"/>
       <c r="F75" s="40"/>
       <c r="G75" s="40"/>
@@ -12633,12 +12647,12 @@
       <c r="AE75" s="201"/>
     </row>
     <row r="76" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="348"/>
+      <c r="A76" s="355"/>
       <c r="B76" s="53"/>
       <c r="C76" s="224" t="s">
         <v>287</v>
       </c>
-      <c r="D76" s="365"/>
+      <c r="D76" s="372"/>
       <c r="E76" s="126"/>
       <c r="F76" s="40"/>
       <c r="G76" s="40"/>
@@ -12688,12 +12702,12 @@
       <c r="AE76" s="201"/>
     </row>
     <row r="77" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="348"/>
+      <c r="A77" s="355"/>
       <c r="B77" s="53"/>
       <c r="C77" s="224" t="s">
         <v>42</v>
       </c>
-      <c r="D77" s="365"/>
+      <c r="D77" s="372"/>
       <c r="E77" s="117" t="s">
         <v>19</v>
       </c>
@@ -12775,12 +12789,12 @@
       <c r="AE77" s="201"/>
     </row>
     <row r="78" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="348"/>
+      <c r="A78" s="355"/>
       <c r="B78" s="53"/>
       <c r="C78" s="224" t="s">
         <v>228</v>
       </c>
-      <c r="D78" s="365"/>
+      <c r="D78" s="372"/>
       <c r="E78" s="117" t="s">
         <v>10</v>
       </c>
@@ -12862,12 +12876,12 @@
       <c r="AE78" s="201"/>
     </row>
     <row r="79" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="348"/>
+      <c r="A79" s="355"/>
       <c r="B79" s="53"/>
       <c r="C79" s="224" t="s">
         <v>229</v>
       </c>
-      <c r="D79" s="365"/>
+      <c r="D79" s="372"/>
       <c r="E79" s="126"/>
       <c r="F79" s="40"/>
       <c r="G79" s="40"/>
@@ -12913,12 +12927,12 @@
       <c r="AE79" s="201"/>
     </row>
     <row r="80" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="348"/>
+      <c r="A80" s="355"/>
       <c r="B80" s="53"/>
       <c r="C80" s="224" t="s">
         <v>43</v>
       </c>
-      <c r="D80" s="365"/>
+      <c r="D80" s="372"/>
       <c r="E80" s="117" t="s">
         <v>19</v>
       </c>
@@ -13002,12 +13016,12 @@
       </c>
     </row>
     <row r="81" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="348"/>
+      <c r="A81" s="355"/>
       <c r="B81" s="53"/>
       <c r="C81" s="224" t="s">
         <v>112</v>
       </c>
-      <c r="D81" s="365"/>
+      <c r="D81" s="372"/>
       <c r="E81" s="117" t="s">
         <v>10</v>
       </c>
@@ -13089,12 +13103,12 @@
       <c r="AE81" s="201"/>
     </row>
     <row r="82" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="348"/>
+      <c r="A82" s="355"/>
       <c r="B82" s="53"/>
       <c r="C82" s="224" t="s">
         <v>44</v>
       </c>
-      <c r="D82" s="365"/>
+      <c r="D82" s="372"/>
       <c r="E82" s="117" t="s">
         <v>19</v>
       </c>
@@ -13178,12 +13192,12 @@
       </c>
     </row>
     <row r="83" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="348"/>
+      <c r="A83" s="355"/>
       <c r="B83" s="53"/>
       <c r="C83" s="224" t="s">
         <v>321</v>
       </c>
-      <c r="D83" s="365"/>
+      <c r="D83" s="372"/>
       <c r="E83" s="126"/>
       <c r="F83" s="40"/>
       <c r="G83" s="40"/>
@@ -13229,12 +13243,12 @@
       <c r="AE83" s="201"/>
     </row>
     <row r="84" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="348"/>
+      <c r="A84" s="355"/>
       <c r="B84" s="290"/>
       <c r="C84" s="291" t="s">
         <v>257</v>
       </c>
-      <c r="D84" s="365"/>
+      <c r="D84" s="372"/>
       <c r="E84" s="36" t="s">
         <v>381</v>
       </c>
@@ -13316,12 +13330,12 @@
       <c r="AE84" s="296"/>
     </row>
     <row r="85" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="348"/>
+      <c r="A85" s="355"/>
       <c r="B85" s="53"/>
       <c r="C85" s="224" t="s">
         <v>370</v>
       </c>
-      <c r="D85" s="365"/>
+      <c r="D85" s="372"/>
       <c r="E85" s="228"/>
       <c r="F85" s="40"/>
       <c r="G85" s="40"/>
@@ -13353,12 +13367,12 @@
       <c r="AE85" s="201"/>
     </row>
     <row r="86" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="348"/>
+      <c r="A86" s="355"/>
       <c r="B86" s="53"/>
       <c r="C86" s="224" t="s">
         <v>251</v>
       </c>
-      <c r="D86" s="365"/>
+      <c r="D86" s="372"/>
       <c r="E86" s="127" t="s">
         <v>19</v>
       </c>
@@ -13440,12 +13454,12 @@
       <c r="AE86" s="201"/>
     </row>
     <row r="87" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="348"/>
+      <c r="A87" s="355"/>
       <c r="B87" s="53"/>
       <c r="C87" s="224" t="s">
         <v>208</v>
       </c>
-      <c r="D87" s="365"/>
+      <c r="D87" s="372"/>
       <c r="E87" s="126"/>
       <c r="F87" s="40"/>
       <c r="G87" s="40"/>
@@ -13503,12 +13517,12 @@
       <c r="AE87" s="201"/>
     </row>
     <row r="88" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="348"/>
+      <c r="A88" s="355"/>
       <c r="B88" s="53"/>
       <c r="C88" s="224" t="s">
         <v>113</v>
       </c>
-      <c r="D88" s="365"/>
+      <c r="D88" s="372"/>
       <c r="E88" s="126"/>
       <c r="F88" s="40"/>
       <c r="G88" s="40"/>
@@ -13562,12 +13576,12 @@
       <c r="AE88" s="201"/>
     </row>
     <row r="89" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="348"/>
+      <c r="A89" s="355"/>
       <c r="B89" s="53"/>
       <c r="C89" s="224" t="s">
         <v>114</v>
       </c>
-      <c r="D89" s="365"/>
+      <c r="D89" s="372"/>
       <c r="E89" s="126"/>
       <c r="F89" s="40"/>
       <c r="G89" s="40"/>
@@ -13617,12 +13631,12 @@
       <c r="AE89" s="201"/>
     </row>
     <row r="90" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="348"/>
+      <c r="A90" s="355"/>
       <c r="B90" s="53"/>
       <c r="C90" s="224" t="s">
         <v>233</v>
       </c>
-      <c r="D90" s="365"/>
+      <c r="D90" s="372"/>
       <c r="E90" s="126"/>
       <c r="F90" s="40"/>
       <c r="G90" s="40"/>
@@ -13676,12 +13690,12 @@
       <c r="AE90" s="201"/>
     </row>
     <row r="91" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="348"/>
+      <c r="A91" s="355"/>
       <c r="B91" s="53"/>
       <c r="C91" s="224" t="s">
         <v>202</v>
       </c>
-      <c r="D91" s="365"/>
+      <c r="D91" s="372"/>
       <c r="E91" s="126"/>
       <c r="F91" s="40"/>
       <c r="G91" s="40"/>
@@ -13735,12 +13749,12 @@
       <c r="AE91" s="201"/>
     </row>
     <row r="92" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="348"/>
+      <c r="A92" s="355"/>
       <c r="B92" s="55"/>
       <c r="C92" s="86" t="s">
         <v>371</v>
       </c>
-      <c r="D92" s="365"/>
+      <c r="D92" s="372"/>
       <c r="E92" s="275"/>
       <c r="F92" s="276"/>
       <c r="G92" s="276"/>
@@ -13772,12 +13786,12 @@
       <c r="AE92" s="207"/>
     </row>
     <row r="93" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="348"/>
+      <c r="A93" s="355"/>
       <c r="B93" s="55"/>
       <c r="C93" s="86" t="s">
         <v>302</v>
       </c>
-      <c r="D93" s="365"/>
+      <c r="D93" s="372"/>
       <c r="E93" s="129" t="s">
         <v>255</v>
       </c>
@@ -13859,12 +13873,12 @@
       <c r="AE93" s="207"/>
     </row>
     <row r="94" spans="1:32" s="44" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="348"/>
+      <c r="A94" s="355"/>
       <c r="B94" s="85"/>
       <c r="C94" s="86" t="s">
         <v>236</v>
       </c>
-      <c r="D94" s="365"/>
+      <c r="D94" s="372"/>
       <c r="E94" s="129" t="s">
         <v>237</v>
       </c>
@@ -13949,14 +13963,14 @@
       </c>
     </row>
     <row r="95" spans="1:32" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="348"/>
+      <c r="A95" s="355"/>
       <c r="B95" s="47" t="s">
         <v>46</v>
       </c>
       <c r="C95" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="D95" s="365"/>
+      <c r="D95" s="372"/>
       <c r="E95" s="116"/>
       <c r="F95" s="49"/>
       <c r="G95" s="49"/>
@@ -14028,12 +14042,12 @@
       </c>
     </row>
     <row r="96" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="348"/>
+      <c r="A96" s="355"/>
       <c r="B96" s="54"/>
       <c r="C96" s="45" t="s">
         <v>322</v>
       </c>
-      <c r="D96" s="365"/>
+      <c r="D96" s="372"/>
       <c r="E96" s="124"/>
       <c r="F96" s="46"/>
       <c r="G96" s="46"/>
@@ -14077,12 +14091,12 @@
       <c r="AE96" s="206"/>
     </row>
     <row r="97" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="348"/>
+      <c r="A97" s="355"/>
       <c r="B97" s="53"/>
       <c r="C97" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D97" s="365"/>
+      <c r="D97" s="372"/>
       <c r="E97" s="117"/>
       <c r="F97" s="36"/>
       <c r="G97" s="36"/>
@@ -14152,12 +14166,12 @@
       <c r="AE97" s="201"/>
     </row>
     <row r="98" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="348"/>
+      <c r="A98" s="355"/>
       <c r="B98" s="53"/>
       <c r="C98" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D98" s="365"/>
+      <c r="D98" s="372"/>
       <c r="E98" s="117"/>
       <c r="F98" s="36"/>
       <c r="G98" s="36"/>
@@ -14227,12 +14241,12 @@
       <c r="AE98" s="201"/>
     </row>
     <row r="99" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="348"/>
+      <c r="A99" s="355"/>
       <c r="B99" s="53"/>
       <c r="C99" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D99" s="365"/>
+      <c r="D99" s="372"/>
       <c r="E99" s="117"/>
       <c r="F99" s="36"/>
       <c r="G99" s="36"/>
@@ -14302,12 +14316,12 @@
       <c r="AE99" s="201"/>
     </row>
     <row r="100" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="348"/>
+      <c r="A100" s="355"/>
       <c r="B100" s="53"/>
       <c r="C100" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D100" s="365"/>
+      <c r="D100" s="372"/>
       <c r="E100" s="117"/>
       <c r="F100" s="36"/>
       <c r="G100" s="36"/>
@@ -14382,12 +14396,12 @@
       </c>
     </row>
     <row r="101" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="348"/>
+      <c r="A101" s="355"/>
       <c r="B101" s="53"/>
       <c r="C101" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D101" s="365"/>
+      <c r="D101" s="372"/>
       <c r="E101" s="117"/>
       <c r="F101" s="36"/>
       <c r="G101" s="36"/>
@@ -14460,12 +14474,12 @@
       </c>
     </row>
     <row r="102" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="348"/>
+      <c r="A102" s="355"/>
       <c r="B102" s="53"/>
       <c r="C102" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D102" s="365"/>
+      <c r="D102" s="372"/>
       <c r="E102" s="117"/>
       <c r="F102" s="36"/>
       <c r="G102" s="36"/>
@@ -14540,12 +14554,12 @@
       </c>
     </row>
     <row r="103" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="348"/>
+      <c r="A103" s="355"/>
       <c r="B103" s="53"/>
       <c r="C103" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D103" s="365"/>
+      <c r="D103" s="372"/>
       <c r="E103" s="117"/>
       <c r="F103" s="36"/>
       <c r="G103" s="36"/>
@@ -14617,12 +14631,12 @@
       </c>
     </row>
     <row r="104" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="348"/>
+      <c r="A104" s="355"/>
       <c r="B104" s="53"/>
       <c r="C104" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D104" s="365"/>
+      <c r="D104" s="372"/>
       <c r="E104" s="117"/>
       <c r="F104" s="36"/>
       <c r="G104" s="36"/>
@@ -14694,12 +14708,12 @@
       </c>
     </row>
     <row r="105" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="348"/>
+      <c r="A105" s="355"/>
       <c r="B105" s="53"/>
       <c r="C105" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D105" s="365"/>
+      <c r="D105" s="372"/>
       <c r="E105" s="117"/>
       <c r="F105" s="36"/>
       <c r="G105" s="36"/>
@@ -14771,12 +14785,12 @@
       </c>
     </row>
     <row r="106" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="348"/>
+      <c r="A106" s="355"/>
       <c r="B106" s="53"/>
       <c r="C106" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D106" s="365"/>
+      <c r="D106" s="372"/>
       <c r="E106" s="117"/>
       <c r="F106" s="36"/>
       <c r="G106" s="36"/>
@@ -14820,12 +14834,12 @@
       <c r="AE106" s="201"/>
     </row>
     <row r="107" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="348"/>
+      <c r="A107" s="355"/>
       <c r="B107" s="53"/>
       <c r="C107" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D107" s="365"/>
+      <c r="D107" s="372"/>
       <c r="E107" s="117"/>
       <c r="F107" s="36"/>
       <c r="G107" s="36"/>
@@ -14877,12 +14891,12 @@
       <c r="AE107" s="201"/>
     </row>
     <row r="108" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="348"/>
+      <c r="A108" s="355"/>
       <c r="B108" s="55"/>
       <c r="C108" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D108" s="365"/>
+      <c r="D108" s="372"/>
       <c r="E108" s="117"/>
       <c r="F108" s="36"/>
       <c r="G108" s="36"/>
@@ -14952,12 +14966,12 @@
       <c r="AE108" s="201"/>
     </row>
     <row r="109" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="353"/>
+      <c r="A109" s="360"/>
       <c r="B109" s="343"/>
       <c r="C109" s="342" t="s">
         <v>186</v>
       </c>
-      <c r="D109" s="365"/>
+      <c r="D109" s="372"/>
       <c r="E109" s="117"/>
       <c r="F109" s="36"/>
       <c r="G109" s="36"/>
@@ -15027,12 +15041,12 @@
       <c r="AE109" s="201"/>
     </row>
     <row r="110" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="348"/>
+      <c r="A110" s="355"/>
       <c r="B110" s="54"/>
       <c r="C110" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D110" s="365"/>
+      <c r="D110" s="372"/>
       <c r="E110" s="117"/>
       <c r="F110" s="36"/>
       <c r="G110" s="36"/>
@@ -15096,12 +15110,12 @@
       </c>
     </row>
     <row r="111" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="348"/>
+      <c r="A111" s="355"/>
       <c r="B111" s="53"/>
       <c r="C111" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="D111" s="365"/>
+      <c r="D111" s="372"/>
       <c r="E111" s="117"/>
       <c r="F111" s="36"/>
       <c r="G111" s="36"/>
@@ -15171,12 +15185,12 @@
       <c r="AE111" s="209"/>
     </row>
     <row r="112" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="348"/>
+      <c r="A112" s="355"/>
       <c r="B112" s="53"/>
       <c r="C112" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="D112" s="365"/>
+      <c r="D112" s="372"/>
       <c r="E112" s="117"/>
       <c r="F112" s="36"/>
       <c r="G112" s="36"/>
@@ -15246,12 +15260,12 @@
       <c r="AE112" s="201"/>
     </row>
     <row r="113" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="348"/>
+      <c r="A113" s="355"/>
       <c r="B113" s="53"/>
       <c r="C113" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="D113" s="365"/>
+      <c r="D113" s="372"/>
       <c r="E113" s="117"/>
       <c r="F113" s="36"/>
       <c r="G113" s="36"/>
@@ -15321,12 +15335,12 @@
       <c r="AE113" s="201"/>
     </row>
     <row r="114" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="348"/>
+      <c r="A114" s="355"/>
       <c r="B114" s="53"/>
       <c r="C114" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="D114" s="365"/>
+      <c r="D114" s="372"/>
       <c r="E114" s="117"/>
       <c r="F114" s="36"/>
       <c r="G114" s="36"/>
@@ -15396,12 +15410,12 @@
       <c r="AE114" s="209"/>
     </row>
     <row r="115" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="348"/>
+      <c r="A115" s="355"/>
       <c r="B115" s="53"/>
       <c r="C115" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="D115" s="365"/>
+      <c r="D115" s="372"/>
       <c r="E115" s="117"/>
       <c r="F115" s="36"/>
       <c r="G115" s="36"/>
@@ -15471,12 +15485,12 @@
       <c r="AE115" s="201"/>
     </row>
     <row r="116" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="348"/>
+      <c r="A116" s="355"/>
       <c r="B116" s="53"/>
       <c r="C116" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="D116" s="365"/>
+      <c r="D116" s="372"/>
       <c r="E116" s="117"/>
       <c r="F116" s="36"/>
       <c r="G116" s="36"/>
@@ -15546,12 +15560,12 @@
       <c r="AE116" s="209"/>
     </row>
     <row r="117" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="348"/>
+      <c r="A117" s="355"/>
       <c r="B117" s="53"/>
       <c r="C117" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="D117" s="365"/>
+      <c r="D117" s="372"/>
       <c r="E117" s="117"/>
       <c r="F117" s="36"/>
       <c r="G117" s="36"/>
@@ -15621,12 +15635,12 @@
       <c r="AE117" s="201"/>
     </row>
     <row r="118" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="348"/>
+      <c r="A118" s="355"/>
       <c r="B118" s="53"/>
       <c r="C118" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="D118" s="365"/>
+      <c r="D118" s="372"/>
       <c r="E118" s="117"/>
       <c r="F118" s="36"/>
       <c r="G118" s="36"/>
@@ -15696,12 +15710,12 @@
       <c r="AE118" s="201"/>
     </row>
     <row r="119" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="348"/>
+      <c r="A119" s="355"/>
       <c r="B119" s="53"/>
       <c r="C119" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D119" s="365"/>
+      <c r="D119" s="372"/>
       <c r="E119" s="117"/>
       <c r="F119" s="36"/>
       <c r="G119" s="36"/>
@@ -15773,12 +15787,12 @@
       </c>
     </row>
     <row r="120" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="348"/>
+      <c r="A120" s="355"/>
       <c r="B120" s="53"/>
       <c r="C120" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D120" s="365"/>
+      <c r="D120" s="372"/>
       <c r="E120" s="117"/>
       <c r="F120" s="36"/>
       <c r="G120" s="36"/>
@@ -15850,12 +15864,12 @@
       </c>
     </row>
     <row r="121" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="348"/>
+      <c r="A121" s="355"/>
       <c r="B121" s="53"/>
       <c r="C121" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D121" s="365"/>
+      <c r="D121" s="372"/>
       <c r="E121" s="117"/>
       <c r="F121" s="36"/>
       <c r="G121" s="36"/>
@@ -15927,12 +15941,12 @@
       </c>
     </row>
     <row r="122" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="348"/>
+      <c r="A122" s="355"/>
       <c r="B122" s="53"/>
       <c r="C122" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D122" s="365"/>
+      <c r="D122" s="372"/>
       <c r="E122" s="117"/>
       <c r="F122" s="36"/>
       <c r="G122" s="36"/>
@@ -16004,12 +16018,12 @@
       </c>
     </row>
     <row r="123" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="348"/>
+      <c r="A123" s="355"/>
       <c r="B123" s="53"/>
       <c r="C123" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D123" s="365"/>
+      <c r="D123" s="372"/>
       <c r="E123" s="117"/>
       <c r="F123" s="36"/>
       <c r="G123" s="36"/>
@@ -16081,12 +16095,12 @@
       </c>
     </row>
     <row r="124" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="348"/>
+      <c r="A124" s="355"/>
       <c r="B124" s="53"/>
       <c r="C124" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D124" s="365"/>
+      <c r="D124" s="372"/>
       <c r="E124" s="117"/>
       <c r="F124" s="36"/>
       <c r="G124" s="36"/>
@@ -16161,12 +16175,12 @@
       </c>
     </row>
     <row r="125" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="348"/>
+      <c r="A125" s="355"/>
       <c r="B125" s="53"/>
       <c r="C125" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D125" s="365"/>
+      <c r="D125" s="372"/>
       <c r="E125" s="117"/>
       <c r="F125" s="36"/>
       <c r="G125" s="36"/>
@@ -16238,12 +16252,12 @@
       </c>
     </row>
     <row r="126" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="348"/>
+      <c r="A126" s="355"/>
       <c r="B126" s="53"/>
       <c r="C126" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="D126" s="365"/>
+      <c r="D126" s="372"/>
       <c r="E126" s="117"/>
       <c r="F126" s="36"/>
       <c r="G126" s="36"/>
@@ -16289,12 +16303,12 @@
       <c r="AE126" s="201"/>
     </row>
     <row r="127" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="348"/>
+      <c r="A127" s="355"/>
       <c r="B127" s="53"/>
       <c r="C127" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D127" s="365"/>
+      <c r="D127" s="372"/>
       <c r="E127" s="117"/>
       <c r="F127" s="36"/>
       <c r="G127" s="36"/>
@@ -16340,12 +16354,12 @@
       <c r="AE127" s="201"/>
     </row>
     <row r="128" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="348"/>
+      <c r="A128" s="355"/>
       <c r="B128" s="53"/>
       <c r="C128" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D128" s="365"/>
+      <c r="D128" s="372"/>
       <c r="E128" s="117"/>
       <c r="F128" s="36"/>
       <c r="G128" s="36"/>
@@ -16391,12 +16405,12 @@
       <c r="AE128" s="201"/>
     </row>
     <row r="129" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="348"/>
+      <c r="A129" s="355"/>
       <c r="B129" s="53"/>
       <c r="C129" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D129" s="365"/>
+      <c r="D129" s="372"/>
       <c r="E129" s="117"/>
       <c r="F129" s="36"/>
       <c r="G129" s="36"/>
@@ -16442,12 +16456,12 @@
       <c r="AE129" s="201"/>
     </row>
     <row r="130" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="348"/>
+      <c r="A130" s="355"/>
       <c r="B130" s="53"/>
       <c r="C130" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D130" s="365"/>
+      <c r="D130" s="372"/>
       <c r="E130" s="117"/>
       <c r="F130" s="36"/>
       <c r="G130" s="36"/>
@@ -16493,12 +16507,12 @@
       <c r="AE130" s="201"/>
     </row>
     <row r="131" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="348"/>
+      <c r="A131" s="355"/>
       <c r="B131" s="53"/>
       <c r="C131" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D131" s="365"/>
+      <c r="D131" s="372"/>
       <c r="E131" s="117"/>
       <c r="F131" s="36"/>
       <c r="G131" s="36"/>
@@ -16544,12 +16558,12 @@
       <c r="AE131" s="201"/>
     </row>
     <row r="132" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="348"/>
+      <c r="A132" s="355"/>
       <c r="B132" s="53"/>
       <c r="C132" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D132" s="365"/>
+      <c r="D132" s="372"/>
       <c r="E132" s="117"/>
       <c r="F132" s="36"/>
       <c r="G132" s="36"/>
@@ -16595,12 +16609,12 @@
       <c r="AE132" s="201"/>
     </row>
     <row r="133" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="348"/>
+      <c r="A133" s="355"/>
       <c r="B133" s="53"/>
       <c r="C133" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D133" s="365"/>
+      <c r="D133" s="372"/>
       <c r="E133" s="117"/>
       <c r="F133" s="36"/>
       <c r="G133" s="36"/>
@@ -16646,12 +16660,12 @@
       <c r="AE133" s="201"/>
     </row>
     <row r="134" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="348"/>
+      <c r="A134" s="355"/>
       <c r="B134" s="53"/>
       <c r="C134" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D134" s="365"/>
+      <c r="D134" s="372"/>
       <c r="E134" s="117"/>
       <c r="F134" s="36"/>
       <c r="G134" s="36"/>
@@ -16697,12 +16711,12 @@
       <c r="AE134" s="201"/>
     </row>
     <row r="135" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="348"/>
+      <c r="A135" s="355"/>
       <c r="B135" s="53"/>
       <c r="C135" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D135" s="365"/>
+      <c r="D135" s="372"/>
       <c r="E135" s="117"/>
       <c r="F135" s="36"/>
       <c r="G135" s="36"/>
@@ -16748,12 +16762,12 @@
       <c r="AE135" s="201"/>
     </row>
     <row r="136" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="348"/>
+      <c r="A136" s="355"/>
       <c r="B136" s="53"/>
       <c r="C136" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D136" s="365"/>
+      <c r="D136" s="372"/>
       <c r="E136" s="117"/>
       <c r="F136" s="36"/>
       <c r="G136" s="36"/>
@@ -16799,12 +16813,12 @@
       <c r="AE136" s="201"/>
     </row>
     <row r="137" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="348"/>
+      <c r="A137" s="355"/>
       <c r="B137" s="53"/>
       <c r="C137" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D137" s="365"/>
+      <c r="D137" s="372"/>
       <c r="E137" s="117"/>
       <c r="F137" s="36"/>
       <c r="G137" s="36"/>
@@ -16862,12 +16876,12 @@
       </c>
     </row>
     <row r="138" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="348"/>
+      <c r="A138" s="355"/>
       <c r="B138" s="53"/>
       <c r="C138" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D138" s="365"/>
+      <c r="D138" s="372"/>
       <c r="E138" s="117"/>
       <c r="F138" s="36"/>
       <c r="G138" s="36"/>
@@ -16939,12 +16953,12 @@
       </c>
     </row>
     <row r="139" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="348"/>
+      <c r="A139" s="355"/>
       <c r="B139" s="53"/>
       <c r="C139" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D139" s="366"/>
+      <c r="D139" s="373"/>
       <c r="E139" s="131"/>
       <c r="F139" s="37"/>
       <c r="G139" s="37"/>
@@ -16974,12 +16988,12 @@
       <c r="AE139" s="201"/>
     </row>
     <row r="140" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="348"/>
+      <c r="A140" s="355"/>
       <c r="B140" s="53"/>
       <c r="C140" s="338" t="s">
         <v>69</v>
       </c>
-      <c r="D140" s="366"/>
+      <c r="D140" s="373"/>
       <c r="E140" s="131"/>
       <c r="F140" s="37"/>
       <c r="G140" s="37"/>
@@ -17051,12 +17065,12 @@
       </c>
     </row>
     <row r="141" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="348"/>
+      <c r="A141" s="355"/>
       <c r="B141" s="53"/>
       <c r="C141" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D141" s="366"/>
+      <c r="D141" s="373"/>
       <c r="E141" s="131"/>
       <c r="F141" s="37"/>
       <c r="G141" s="37"/>
@@ -17126,12 +17140,12 @@
       <c r="AE141" s="201"/>
     </row>
     <row r="142" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="348"/>
+      <c r="A142" s="355"/>
       <c r="B142" s="53"/>
       <c r="C142" s="339" t="s">
         <v>197</v>
       </c>
-      <c r="D142" s="366"/>
+      <c r="D142" s="373"/>
       <c r="E142" s="131"/>
       <c r="F142" s="37"/>
       <c r="G142" s="37"/>
@@ -17201,12 +17215,12 @@
       <c r="AE142" s="201"/>
     </row>
     <row r="143" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="348"/>
+      <c r="A143" s="355"/>
       <c r="B143" s="53"/>
       <c r="C143" s="339" t="s">
         <v>432</v>
       </c>
-      <c r="D143" s="366"/>
+      <c r="D143" s="373"/>
       <c r="E143" s="131"/>
       <c r="F143" s="37"/>
       <c r="G143" s="37"/>
@@ -17278,12 +17292,12 @@
       </c>
     </row>
     <row r="144" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="348"/>
+      <c r="A144" s="355"/>
       <c r="B144" s="53"/>
       <c r="C144" s="334" t="s">
         <v>411</v>
       </c>
-      <c r="D144" s="366"/>
+      <c r="D144" s="373"/>
       <c r="E144" s="131"/>
       <c r="F144" s="37"/>
       <c r="G144" s="37"/>
@@ -17355,12 +17369,12 @@
       </c>
     </row>
     <row r="145" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="348"/>
+      <c r="A145" s="355"/>
       <c r="B145" s="53"/>
       <c r="C145" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D145" s="366"/>
+      <c r="D145" s="373"/>
       <c r="E145" s="131"/>
       <c r="F145" s="37"/>
       <c r="G145" s="37"/>
@@ -17431,14 +17445,14 @@
         <v>426</v>
       </c>
     </row>
-    <row r="146" spans="1:31" s="392" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="348"/>
-      <c r="B146" s="386"/>
-      <c r="C146" s="387" t="s">
+    <row r="146" spans="1:31" s="351" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="355"/>
+      <c r="B146" s="345"/>
+      <c r="C146" s="346" t="s">
         <v>188</v>
       </c>
-      <c r="D146" s="366"/>
-      <c r="E146" s="390"/>
+      <c r="D146" s="373"/>
+      <c r="E146" s="349"/>
       <c r="F146" s="292"/>
       <c r="G146" s="292"/>
       <c r="H146" s="292"/>
@@ -17504,15 +17518,15 @@
       <c r="AD146" s="344" t="s">
         <v>445</v>
       </c>
-      <c r="AE146" s="391"/>
+      <c r="AE146" s="350"/>
     </row>
     <row r="147" spans="1:31" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="348"/>
+      <c r="A147" s="355"/>
       <c r="B147" s="55"/>
       <c r="C147" s="338" t="s">
         <v>68</v>
       </c>
-      <c r="D147" s="366"/>
+      <c r="D147" s="373"/>
       <c r="E147" s="131"/>
       <c r="F147" s="37"/>
       <c r="G147" s="37"/>
@@ -17582,12 +17596,12 @@
       <c r="AE147" s="201"/>
     </row>
     <row r="148" spans="1:31" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="353"/>
-      <c r="B148" s="389"/>
-      <c r="C148" s="388" t="s">
+      <c r="A148" s="360"/>
+      <c r="B148" s="348"/>
+      <c r="C148" s="347" t="s">
         <v>76</v>
       </c>
-      <c r="D148" s="366"/>
+      <c r="D148" s="373"/>
       <c r="E148" s="131"/>
       <c r="F148" s="37"/>
       <c r="G148" s="37"/>
@@ -17659,12 +17673,12 @@
       </c>
     </row>
     <row r="149" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="348"/>
+      <c r="A149" s="355"/>
       <c r="B149" s="54"/>
       <c r="C149" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="D149" s="366"/>
+      <c r="D149" s="373"/>
       <c r="E149" s="131"/>
       <c r="F149" s="37"/>
       <c r="G149" s="37"/>
@@ -17736,12 +17750,12 @@
       </c>
     </row>
     <row r="150" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="348"/>
+      <c r="A150" s="355"/>
       <c r="B150" s="53"/>
       <c r="C150" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="D150" s="366"/>
+      <c r="D150" s="373"/>
       <c r="E150" s="131"/>
       <c r="F150" s="37"/>
       <c r="G150" s="37"/>
@@ -17811,12 +17825,12 @@
       <c r="AE150" s="201"/>
     </row>
     <row r="151" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="348"/>
+      <c r="A151" s="355"/>
       <c r="B151" s="53"/>
       <c r="C151" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D151" s="366"/>
+      <c r="D151" s="373"/>
       <c r="E151" s="131"/>
       <c r="F151" s="37"/>
       <c r="G151" s="37"/>
@@ -17864,12 +17878,12 @@
       <c r="AE151" s="201"/>
     </row>
     <row r="152" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="348"/>
+      <c r="A152" s="355"/>
       <c r="B152" s="53"/>
       <c r="C152" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D152" s="366"/>
+      <c r="D152" s="373"/>
       <c r="E152" s="131"/>
       <c r="F152" s="37"/>
       <c r="G152" s="37"/>
@@ -17941,12 +17955,12 @@
       </c>
     </row>
     <row r="153" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="348"/>
+      <c r="A153" s="355"/>
       <c r="B153" s="53"/>
       <c r="C153" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D153" s="366"/>
+      <c r="D153" s="373"/>
       <c r="E153" s="131"/>
       <c r="F153" s="37"/>
       <c r="G153" s="37"/>
@@ -18016,12 +18030,12 @@
       <c r="AE153" s="201"/>
     </row>
     <row r="154" spans="1:31" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="348"/>
+      <c r="A154" s="355"/>
       <c r="B154" s="74"/>
       <c r="C154" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D154" s="366"/>
+      <c r="D154" s="373"/>
       <c r="E154" s="120"/>
       <c r="F154" s="80"/>
       <c r="G154" s="80"/>
@@ -18067,14 +18081,14 @@
       <c r="AE154" s="203"/>
     </row>
     <row r="155" spans="1:31" ht="26.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="348"/>
+      <c r="A155" s="355"/>
       <c r="B155" s="97" t="s">
         <v>78</v>
       </c>
       <c r="C155" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="D155" s="365"/>
+      <c r="D155" s="372"/>
       <c r="E155" s="132"/>
       <c r="F155" s="98"/>
       <c r="G155" s="98"/>
@@ -18146,12 +18160,12 @@
       </c>
     </row>
     <row r="156" spans="1:31" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A156" s="348"/>
+      <c r="A156" s="355"/>
       <c r="B156" s="53"/>
       <c r="C156" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D156" s="365"/>
+      <c r="D156" s="372"/>
       <c r="E156" s="131"/>
       <c r="F156" s="37"/>
       <c r="G156" s="37"/>
@@ -18223,12 +18237,12 @@
       </c>
     </row>
     <row r="157" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="348"/>
+      <c r="A157" s="355"/>
       <c r="B157" s="53"/>
       <c r="C157" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D157" s="365"/>
+      <c r="D157" s="372"/>
       <c r="E157" s="131"/>
       <c r="F157" s="37"/>
       <c r="G157" s="37"/>
@@ -18298,12 +18312,12 @@
       <c r="AE157" s="201"/>
     </row>
     <row r="158" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="348"/>
+      <c r="A158" s="355"/>
       <c r="B158" s="53"/>
       <c r="C158" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D158" s="365"/>
+      <c r="D158" s="372"/>
       <c r="E158" s="131"/>
       <c r="F158" s="37"/>
       <c r="G158" s="37"/>
@@ -18373,12 +18387,12 @@
       <c r="AE158" s="201"/>
     </row>
     <row r="159" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="348"/>
+      <c r="A159" s="355"/>
       <c r="B159" s="53"/>
       <c r="C159" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D159" s="365"/>
+      <c r="D159" s="372"/>
       <c r="E159" s="131"/>
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
@@ -18448,12 +18462,12 @@
       <c r="AE159" s="201"/>
     </row>
     <row r="160" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="348"/>
+      <c r="A160" s="355"/>
       <c r="B160" s="53"/>
       <c r="C160" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D160" s="365"/>
+      <c r="D160" s="372"/>
       <c r="E160" s="131"/>
       <c r="F160" s="37"/>
       <c r="G160" s="37"/>
@@ -18523,12 +18537,12 @@
       <c r="AE160" s="201"/>
     </row>
     <row r="161" spans="1:31" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A161" s="348"/>
+      <c r="A161" s="355"/>
       <c r="B161" s="53"/>
       <c r="C161" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D161" s="365"/>
+      <c r="D161" s="372"/>
       <c r="E161" s="131"/>
       <c r="F161" s="37"/>
       <c r="G161" s="37"/>
@@ -18600,12 +18614,12 @@
       </c>
     </row>
     <row r="162" spans="1:31" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A162" s="348"/>
+      <c r="A162" s="355"/>
       <c r="B162" s="53"/>
       <c r="C162" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D162" s="365"/>
+      <c r="D162" s="372"/>
       <c r="E162" s="131"/>
       <c r="F162" s="37"/>
       <c r="G162" s="37"/>
@@ -18675,12 +18689,12 @@
       <c r="AE162" s="209"/>
     </row>
     <row r="163" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="348"/>
+      <c r="A163" s="355"/>
       <c r="B163" s="53"/>
       <c r="C163" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D163" s="365"/>
+      <c r="D163" s="372"/>
       <c r="E163" s="131"/>
       <c r="F163" s="37"/>
       <c r="G163" s="37"/>
@@ -18750,12 +18764,12 @@
       <c r="AE163" s="209"/>
     </row>
     <row r="164" spans="1:31" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A164" s="348"/>
+      <c r="A164" s="355"/>
       <c r="B164" s="53"/>
       <c r="C164" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D164" s="365"/>
+      <c r="D164" s="372"/>
       <c r="E164" s="131"/>
       <c r="F164" s="37"/>
       <c r="G164" s="37"/>
@@ -18827,12 +18841,12 @@
       </c>
     </row>
     <row r="165" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A165" s="348"/>
+      <c r="A165" s="355"/>
       <c r="B165" s="53"/>
       <c r="C165" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D165" s="365"/>
+      <c r="D165" s="372"/>
       <c r="E165" s="131"/>
       <c r="F165" s="37"/>
       <c r="G165" s="37"/>
@@ -18904,12 +18918,12 @@
       </c>
     </row>
     <row r="166" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="348"/>
+      <c r="A166" s="355"/>
       <c r="B166" s="53"/>
       <c r="C166" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D166" s="365"/>
+      <c r="D166" s="372"/>
       <c r="E166" s="131"/>
       <c r="F166" s="37"/>
       <c r="G166" s="37"/>
@@ -18979,12 +18993,12 @@
       <c r="AE166" s="201"/>
     </row>
     <row r="167" spans="1:31" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A167" s="348"/>
+      <c r="A167" s="355"/>
       <c r="B167" s="53"/>
       <c r="C167" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D167" s="365"/>
+      <c r="D167" s="372"/>
       <c r="E167" s="131"/>
       <c r="F167" s="37"/>
       <c r="G167" s="37"/>
@@ -19056,12 +19070,12 @@
       </c>
     </row>
     <row r="168" spans="1:31" ht="51" x14ac:dyDescent="0.25">
-      <c r="A168" s="348"/>
+      <c r="A168" s="355"/>
       <c r="B168" s="53"/>
       <c r="C168" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D168" s="365"/>
+      <c r="D168" s="372"/>
       <c r="E168" s="131"/>
       <c r="F168" s="37"/>
       <c r="G168" s="37"/>
@@ -19131,12 +19145,12 @@
       <c r="AE168" s="201"/>
     </row>
     <row r="169" spans="1:31" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="348"/>
+      <c r="A169" s="355"/>
       <c r="B169" s="74"/>
       <c r="C169" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="D169" s="365"/>
+      <c r="D169" s="372"/>
       <c r="E169" s="120"/>
       <c r="F169" s="80"/>
       <c r="G169" s="80"/>
@@ -19192,14 +19206,14 @@
       <c r="AE169" s="203"/>
     </row>
     <row r="170" spans="1:31" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="348"/>
+      <c r="A170" s="355"/>
       <c r="B170" s="62" t="s">
         <v>138</v>
       </c>
       <c r="C170" s="63" t="s">
         <v>139</v>
       </c>
-      <c r="D170" s="365"/>
+      <c r="D170" s="372"/>
       <c r="E170" s="133"/>
       <c r="F170" s="64"/>
       <c r="G170" s="64"/>
@@ -19269,12 +19283,12 @@
       <c r="AE170" s="210"/>
     </row>
     <row r="171" spans="1:31" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="348"/>
+      <c r="A171" s="355"/>
       <c r="B171" s="66"/>
       <c r="C171" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D171" s="365"/>
+      <c r="D171" s="372"/>
       <c r="E171" s="134"/>
       <c r="F171" s="38"/>
       <c r="G171" s="38"/>
@@ -19344,12 +19358,12 @@
       <c r="AE171" s="211"/>
     </row>
     <row r="172" spans="1:31" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="348"/>
+      <c r="A172" s="355"/>
       <c r="B172" s="66"/>
       <c r="C172" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D172" s="365"/>
+      <c r="D172" s="372"/>
       <c r="E172" s="134"/>
       <c r="F172" s="38"/>
       <c r="G172" s="38"/>
@@ -19421,12 +19435,12 @@
       </c>
     </row>
     <row r="173" spans="1:31" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="348"/>
+      <c r="A173" s="355"/>
       <c r="B173" s="66"/>
       <c r="C173" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D173" s="365"/>
+      <c r="D173" s="372"/>
       <c r="E173" s="134"/>
       <c r="F173" s="38"/>
       <c r="G173" s="38"/>
@@ -19496,12 +19510,12 @@
       <c r="AE173" s="211"/>
     </row>
     <row r="174" spans="1:31" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="348"/>
+      <c r="A174" s="355"/>
       <c r="B174" s="66"/>
       <c r="C174" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D174" s="365"/>
+      <c r="D174" s="372"/>
       <c r="E174" s="134"/>
       <c r="F174" s="38"/>
       <c r="G174" s="38"/>
@@ -19571,12 +19585,12 @@
       <c r="AE174" s="211"/>
     </row>
     <row r="175" spans="1:31" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="348"/>
+      <c r="A175" s="355"/>
       <c r="B175" s="66"/>
       <c r="C175" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D175" s="365"/>
+      <c r="D175" s="372"/>
       <c r="E175" s="134"/>
       <c r="F175" s="38"/>
       <c r="G175" s="38"/>
@@ -19648,12 +19662,12 @@
       </c>
     </row>
     <row r="176" spans="1:31" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="348"/>
+      <c r="A176" s="355"/>
       <c r="B176" s="66"/>
       <c r="C176" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D176" s="365"/>
+      <c r="D176" s="372"/>
       <c r="E176" s="134"/>
       <c r="F176" s="38"/>
       <c r="G176" s="38"/>
@@ -19723,12 +19737,12 @@
       <c r="AE176" s="211"/>
     </row>
     <row r="177" spans="1:31" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="348"/>
+      <c r="A177" s="355"/>
       <c r="B177" s="66"/>
       <c r="C177" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D177" s="365"/>
+      <c r="D177" s="372"/>
       <c r="E177" s="134"/>
       <c r="F177" s="38"/>
       <c r="G177" s="38"/>
@@ -19798,12 +19812,12 @@
       <c r="AE177" s="211"/>
     </row>
     <row r="178" spans="1:31" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="348"/>
+      <c r="A178" s="355"/>
       <c r="B178" s="66"/>
       <c r="C178" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D178" s="365"/>
+      <c r="D178" s="372"/>
       <c r="E178" s="134"/>
       <c r="F178" s="38"/>
       <c r="G178" s="38"/>
@@ -19873,12 +19887,12 @@
       <c r="AE178" s="211"/>
     </row>
     <row r="179" spans="1:31" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="348"/>
+      <c r="A179" s="355"/>
       <c r="B179" s="66"/>
       <c r="C179" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="D179" s="365"/>
+      <c r="D179" s="372"/>
       <c r="E179" s="134"/>
       <c r="F179" s="38"/>
       <c r="G179" s="38"/>
@@ -19950,12 +19964,12 @@
       </c>
     </row>
     <row r="180" spans="1:31" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="348"/>
+      <c r="A180" s="355"/>
       <c r="B180" s="66"/>
       <c r="C180" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="D180" s="365"/>
+      <c r="D180" s="372"/>
       <c r="E180" s="134"/>
       <c r="F180" s="38"/>
       <c r="G180" s="38"/>
@@ -20025,12 +20039,12 @@
       <c r="AE180" s="211"/>
     </row>
     <row r="181" spans="1:31" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="348"/>
+      <c r="A181" s="355"/>
       <c r="B181" s="66"/>
       <c r="C181" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="D181" s="365"/>
+      <c r="D181" s="372"/>
       <c r="E181" s="134"/>
       <c r="F181" s="38"/>
       <c r="G181" s="38"/>
@@ -20100,12 +20114,12 @@
       <c r="AE181" s="211"/>
     </row>
     <row r="182" spans="1:31" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="348"/>
+      <c r="A182" s="355"/>
       <c r="B182" s="67"/>
       <c r="C182" s="68" t="s">
         <v>153</v>
       </c>
-      <c r="D182" s="367"/>
+      <c r="D182" s="374"/>
       <c r="E182" s="135"/>
       <c r="F182" s="69"/>
       <c r="G182" s="69"/>
@@ -20170,7 +20184,7 @@
         <v>141</v>
       </c>
       <c r="AD182" s="16" t="s">
-        <v>19</v>
+        <v>447</v>
       </c>
       <c r="AE182" s="213"/>
     </row>

</xml_diff>

<commit_message>
updated the cfg spreadsheet to remove PRTC
[git-p4: depot-paths = "//depot/projects/coe/CSME/": change = 760635]
</commit_message>
<xml_diff>
--- a/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
+++ b/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="105" windowWidth="10005" windowHeight="4665"/>
+    <workbookView xWindow="10470" yWindow="105" windowWidth="10005" windowHeight="4665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="2" r:id="rId1"/>
     <sheet name="CSE CSME IE OCS Features" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -7557,7 +7557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -8399,8 +8399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF184"/>
   <sheetViews>
-    <sheetView topLeftCell="A171" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="W1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="Y1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AD182" sqref="AD182"/>
     </sheetView>
   </sheetViews>
@@ -19957,7 +19957,7 @@
         <v>10</v>
       </c>
       <c r="AD179" s="322" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="AE179" s="212" t="s">
         <v>152</v>

</xml_diff>

<commit_message>
updated ATS configuration for OCS
[git-p4: depot-paths = "//depot/projects/coe/CSME/": change = 764516]
</commit_message>
<xml_diff>
--- a/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
+++ b/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="110" windowWidth="7800" windowHeight="4670" activeTab="1"/>
+    <workbookView xWindow="11400" yWindow="108" windowWidth="7800" windowHeight="4668"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="2" r:id="rId1"/>
@@ -3328,7 +3328,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3327" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3333" uniqueCount="494">
   <si>
     <t>CNP-LP</t>
   </si>
@@ -5154,6 +5154,21 @@
   </si>
   <si>
     <t>Added IPC Ch 3 for IUNIT IPU per PCR 2205532397</t>
+  </si>
+  <si>
+    <t>yes*</t>
+  </si>
+  <si>
+    <t>CTS and CCM cannot be disabled</t>
+  </si>
+  <si>
+    <t>*NA</t>
+  </si>
+  <si>
+    <t>There are no more knobs to choose between basic or advanced modes. SM4 is either included or excluded</t>
+  </si>
+  <si>
+    <t>Updated OCS configuration for ATS based on Designer feedback on knobs supported in design</t>
   </si>
 </sst>
 </file>
@@ -6364,7 +6379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="453">
+  <cellXfs count="454">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -7721,6 +7736,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8035,24 +8053,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E70" sqref="E70"/>
+      <selection pane="bottomRight" activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.453125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="207" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="78.81640625" style="262" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="23"/>
+    <col min="1" max="1" width="3.44140625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="207" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="23" customWidth="1"/>
+    <col min="5" max="5" width="78.77734375" style="262" customWidth="1"/>
+    <col min="6" max="16384" width="8.77734375" style="23"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="205" t="s">
         <v>311</v>
       </c>
@@ -8066,7 +8084,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="206">
         <v>1</v>
       </c>
@@ -8080,7 +8098,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B4" s="206">
         <v>2</v>
       </c>
@@ -8094,7 +8112,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="206">
         <v>3</v>
       </c>
@@ -8108,7 +8126,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="206">
         <v>4</v>
       </c>
@@ -8122,7 +8140,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="206">
         <v>5</v>
       </c>
@@ -8136,7 +8154,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B8" s="206">
         <v>6</v>
       </c>
@@ -8150,7 +8168,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="206">
         <v>7</v>
       </c>
@@ -8164,7 +8182,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="206">
         <v>8</v>
       </c>
@@ -8178,7 +8196,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="206">
         <v>9</v>
       </c>
@@ -8192,7 +8210,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="206">
         <v>10</v>
       </c>
@@ -8206,7 +8224,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="206">
         <v>11</v>
       </c>
@@ -8220,7 +8238,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="206">
         <v>12</v>
       </c>
@@ -8234,7 +8252,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="206">
         <v>13</v>
       </c>
@@ -8248,7 +8266,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B16" s="206">
         <v>14</v>
       </c>
@@ -8262,7 +8280,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="206">
         <v>15</v>
       </c>
@@ -8276,7 +8294,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="206">
         <v>16</v>
       </c>
@@ -8290,7 +8308,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="206">
         <v>17</v>
       </c>
@@ -8304,7 +8322,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="206">
         <v>18</v>
       </c>
@@ -8318,7 +8336,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="206">
         <v>19</v>
       </c>
@@ -8332,7 +8350,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="206">
         <v>20</v>
       </c>
@@ -8346,7 +8364,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="206">
         <v>21</v>
       </c>
@@ -8360,7 +8378,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B24" s="206">
         <v>22</v>
       </c>
@@ -8374,7 +8392,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="206">
         <v>23</v>
       </c>
@@ -8388,7 +8406,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="206">
         <v>24</v>
       </c>
@@ -8402,7 +8420,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B27" s="206">
         <v>25</v>
       </c>
@@ -8416,7 +8434,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B28" s="206">
         <v>26</v>
       </c>
@@ -8430,7 +8448,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="206">
         <v>27</v>
       </c>
@@ -8444,7 +8462,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B30" s="206">
         <v>28</v>
       </c>
@@ -8458,7 +8476,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="206">
         <v>29</v>
       </c>
@@ -8472,7 +8490,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B32" s="206">
         <v>30</v>
       </c>
@@ -8486,7 +8504,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="206">
         <v>31</v>
       </c>
@@ -8500,7 +8518,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B34" s="206">
         <v>32</v>
       </c>
@@ -8514,7 +8532,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="206">
         <v>33</v>
       </c>
@@ -8528,7 +8546,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B36" s="206">
         <v>34</v>
       </c>
@@ -8542,7 +8560,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="206">
         <v>35</v>
       </c>
@@ -8556,7 +8574,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="206">
         <v>36</v>
       </c>
@@ -8570,7 +8588,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B39" s="206">
         <v>37</v>
       </c>
@@ -8584,7 +8602,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B40" s="206">
         <v>28</v>
       </c>
@@ -8598,7 +8616,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="206">
         <v>29</v>
       </c>
@@ -8612,7 +8630,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="206">
         <v>30</v>
       </c>
@@ -8626,7 +8644,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="206">
         <v>31</v>
       </c>
@@ -8640,7 +8658,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B44" s="206">
         <v>32</v>
       </c>
@@ -8654,7 +8672,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B45" s="206">
         <v>33</v>
       </c>
@@ -8668,7 +8686,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B46" s="206">
         <v>34</v>
       </c>
@@ -8682,7 +8700,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="206">
         <v>35</v>
       </c>
@@ -8696,7 +8714,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="206">
         <v>36</v>
       </c>
@@ -8710,7 +8728,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="206">
         <v>37</v>
       </c>
@@ -8724,7 +8742,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="50" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B50" s="206">
         <v>38</v>
       </c>
@@ -8738,7 +8756,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" ht="72" x14ac:dyDescent="0.3">
       <c r="B51" s="206">
         <v>39</v>
       </c>
@@ -8752,7 +8770,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="206">
         <v>40</v>
       </c>
@@ -8766,7 +8784,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="206">
         <v>41</v>
       </c>
@@ -8780,7 +8798,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="206">
         <v>42</v>
       </c>
@@ -8794,7 +8812,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="206">
         <v>43</v>
       </c>
@@ -8808,7 +8826,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="56" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B56" s="206">
         <v>44</v>
       </c>
@@ -8822,7 +8840,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="57" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B57" s="206">
         <v>45</v>
       </c>
@@ -8836,7 +8854,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="206">
         <v>46</v>
       </c>
@@ -8850,7 +8868,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B59" s="206">
         <v>47</v>
       </c>
@@ -8864,7 +8882,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="206">
         <v>48</v>
       </c>
@@ -8878,7 +8896,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="61" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B61" s="206">
         <v>49</v>
       </c>
@@ -8892,7 +8910,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="62" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B62" s="206">
         <v>50</v>
       </c>
@@ -8906,7 +8924,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="206">
         <v>51</v>
       </c>
@@ -8920,7 +8938,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="64" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B64" s="206">
         <v>52</v>
       </c>
@@ -8934,7 +8952,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B65" s="206">
         <v>53</v>
       </c>
@@ -8948,7 +8966,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B66" s="206">
         <v>54</v>
       </c>
@@ -8962,7 +8980,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="67" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B67" s="206">
         <v>55</v>
       </c>
@@ -8976,7 +8994,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="206">
         <v>56</v>
       </c>
@@ -8990,7 +9008,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="206">
         <v>57</v>
       </c>
@@ -9004,199 +9022,207 @@
         <v>488</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B70" s="206"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="4"/>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B70" s="206">
+        <v>58</v>
+      </c>
+      <c r="C70" s="9">
+        <v>43374</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="206"/>
       <c r="C71" s="9"/>
       <c r="D71" s="10"/>
       <c r="E71" s="4"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="206"/>
       <c r="C72" s="9"/>
       <c r="D72" s="10"/>
       <c r="E72" s="4"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="206"/>
       <c r="C73" s="9"/>
       <c r="D73" s="10"/>
       <c r="E73" s="4"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74" s="206"/>
       <c r="C74" s="9"/>
       <c r="D74" s="10"/>
       <c r="E74" s="4"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B75" s="206"/>
       <c r="C75" s="9"/>
       <c r="D75" s="10"/>
       <c r="E75" s="4"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B76" s="206"/>
       <c r="C76" s="9"/>
       <c r="D76" s="10"/>
       <c r="E76" s="4"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77" s="206"/>
       <c r="C77" s="9"/>
       <c r="D77" s="10"/>
       <c r="E77" s="4"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B78" s="206"/>
       <c r="C78" s="9"/>
       <c r="D78" s="10"/>
       <c r="E78" s="4"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B79" s="206"/>
       <c r="C79" s="9"/>
       <c r="D79" s="10"/>
       <c r="E79" s="4"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B80" s="206"/>
       <c r="C80" s="9"/>
       <c r="D80" s="10"/>
       <c r="E80" s="4"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" s="206"/>
       <c r="C81" s="9"/>
       <c r="D81" s="10"/>
       <c r="E81" s="4"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82" s="206"/>
       <c r="C82" s="9"/>
       <c r="D82" s="10"/>
       <c r="E82" s="4"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B83" s="206"/>
       <c r="C83" s="9"/>
       <c r="D83" s="10"/>
       <c r="E83" s="4"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B84" s="206"/>
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
       <c r="E84" s="4"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B85" s="206"/>
       <c r="C85" s="9"/>
       <c r="D85" s="10"/>
       <c r="E85" s="4"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B86" s="206"/>
       <c r="C86" s="9"/>
       <c r="D86" s="10"/>
       <c r="E86" s="4"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87" s="206"/>
       <c r="C87" s="9"/>
       <c r="D87" s="10"/>
       <c r="E87" s="4"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B88" s="206"/>
       <c r="C88" s="9"/>
       <c r="D88" s="10"/>
       <c r="E88" s="4"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B89" s="206"/>
       <c r="C89" s="9"/>
       <c r="D89" s="10"/>
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B90" s="206"/>
       <c r="C90" s="9"/>
       <c r="D90" s="10"/>
       <c r="E90" s="4"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91" s="206"/>
       <c r="C91" s="9"/>
       <c r="D91" s="10"/>
       <c r="E91" s="4"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B92" s="206"/>
       <c r="C92" s="9"/>
       <c r="D92" s="10"/>
       <c r="E92" s="4"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B93" s="206"/>
       <c r="C93" s="9"/>
       <c r="D93" s="10"/>
       <c r="E93" s="4"/>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B94" s="206"/>
       <c r="C94" s="9"/>
       <c r="D94" s="10"/>
       <c r="E94" s="4"/>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B95" s="206"/>
       <c r="C95" s="9"/>
       <c r="D95" s="10"/>
       <c r="E95" s="4"/>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B96" s="206"/>
       <c r="C96" s="9"/>
       <c r="D96" s="10"/>
       <c r="E96" s="4"/>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B97" s="206"/>
       <c r="C97" s="9"/>
       <c r="D97" s="10"/>
       <c r="E97" s="4"/>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B98" s="206"/>
       <c r="C98" s="9"/>
       <c r="D98" s="10"/>
       <c r="E98" s="4"/>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B99" s="206"/>
       <c r="C99" s="9"/>
       <c r="D99" s="10"/>
       <c r="E99" s="4"/>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B100" s="206"/>
       <c r="C100" s="9"/>
       <c r="D100" s="10"/>
       <c r="E100" s="4"/>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B101" s="206"/>
       <c r="C101" s="9"/>
       <c r="D101" s="10"/>
       <c r="E101" s="4"/>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B102" s="206"/>
       <c r="C102" s="9"/>
       <c r="D102" s="10"/>
@@ -9213,37 +9239,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK190"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="AB106" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="AB38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AE118" sqref="AE118"/>
+      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" style="230" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.21875" style="230" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="12" customWidth="1"/>
-    <col min="3" max="3" width="43.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="15" width="10.453125" style="17" customWidth="1"/>
-    <col min="16" max="19" width="10.453125" style="24" customWidth="1"/>
-    <col min="20" max="22" width="10.453125" style="17" customWidth="1"/>
-    <col min="23" max="23" width="10.453125" style="231" customWidth="1"/>
-    <col min="24" max="32" width="10.453125" style="17" customWidth="1"/>
-    <col min="33" max="35" width="9.81640625" style="17" customWidth="1"/>
-    <col min="36" max="36" width="48.1796875" style="1" customWidth="1"/>
-    <col min="37" max="37" width="29.453125" style="1" customWidth="1"/>
-    <col min="38" max="16384" width="8.81640625" style="1"/>
+    <col min="3" max="3" width="43.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="15" width="10.44140625" style="17" customWidth="1"/>
+    <col min="16" max="19" width="10.44140625" style="24" customWidth="1"/>
+    <col min="20" max="22" width="10.44140625" style="17" customWidth="1"/>
+    <col min="23" max="23" width="10.44140625" style="231" customWidth="1"/>
+    <col min="24" max="32" width="10.44140625" style="17" customWidth="1"/>
+    <col min="33" max="35" width="9.77734375" style="17" customWidth="1"/>
+    <col min="36" max="36" width="48.21875" style="1" customWidth="1"/>
+    <col min="37" max="37" width="29.44140625" style="1" customWidth="1"/>
+    <col min="38" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="216"/>
       <c r="C1" s="333" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B2" s="422" t="s">
         <v>274</v>
       </c>
@@ -9322,7 +9348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="423"/>
       <c r="C3" s="318" t="s">
         <v>444</v>
@@ -9425,7 +9451,7 @@
       </c>
       <c r="AJ3" s="421"/>
     </row>
-    <row r="4" spans="1:36" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="430"/>
       <c r="B4" s="357" t="s">
         <v>303</v>
@@ -9473,7 +9499,7 @@
       <c r="AI4" s="443"/>
       <c r="AJ4" s="354"/>
     </row>
-    <row r="5" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="430"/>
       <c r="B5" s="360"/>
       <c r="C5" s="361" t="s">
@@ -9515,7 +9541,7 @@
       <c r="AI5" s="446"/>
       <c r="AJ5" s="355"/>
     </row>
-    <row r="6" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="430"/>
       <c r="B6" s="360"/>
       <c r="C6" s="361" t="s">
@@ -9557,7 +9583,7 @@
       <c r="AI6" s="446"/>
       <c r="AJ6" s="355"/>
     </row>
-    <row r="7" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="430"/>
       <c r="B7" s="360"/>
       <c r="C7" s="361" t="s">
@@ -9599,7 +9625,7 @@
       <c r="AI7" s="446"/>
       <c r="AJ7" s="355"/>
     </row>
-    <row r="8" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="430"/>
       <c r="B8" s="360"/>
       <c r="C8" s="361" t="s">
@@ -9641,7 +9667,7 @@
       <c r="AI8" s="446"/>
       <c r="AJ8" s="355"/>
     </row>
-    <row r="9" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="430"/>
       <c r="B9" s="360"/>
       <c r="C9" s="361" t="s">
@@ -9683,7 +9709,7 @@
       <c r="AI9" s="446"/>
       <c r="AJ9" s="355"/>
     </row>
-    <row r="10" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="430"/>
       <c r="B10" s="360"/>
       <c r="C10" s="361" t="s">
@@ -9725,7 +9751,7 @@
       <c r="AI10" s="446"/>
       <c r="AJ10" s="355"/>
     </row>
-    <row r="11" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="430"/>
       <c r="B11" s="360"/>
       <c r="C11" s="361" t="s">
@@ -9767,7 +9793,7 @@
       <c r="AI11" s="446"/>
       <c r="AJ11" s="355"/>
     </row>
-    <row r="12" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="430"/>
       <c r="B12" s="360"/>
       <c r="C12" s="361" t="s">
@@ -9809,7 +9835,7 @@
       <c r="AI12" s="446"/>
       <c r="AJ12" s="355"/>
     </row>
-    <row r="13" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="430"/>
       <c r="B13" s="360"/>
       <c r="C13" s="361" t="s">
@@ -9851,7 +9877,7 @@
       <c r="AI13" s="446"/>
       <c r="AJ13" s="355"/>
     </row>
-    <row r="14" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="430"/>
       <c r="B14" s="360"/>
       <c r="C14" s="361" t="s">
@@ -9893,7 +9919,7 @@
       <c r="AI14" s="446"/>
       <c r="AJ14" s="355"/>
     </row>
-    <row r="15" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="430"/>
       <c r="B15" s="360" t="s">
         <v>22</v>
@@ -9937,7 +9963,7 @@
       <c r="AI15" s="446"/>
       <c r="AJ15" s="355"/>
     </row>
-    <row r="16" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="430"/>
       <c r="B16" s="360"/>
       <c r="C16" s="361" t="s">
@@ -9979,7 +10005,7 @@
       <c r="AI16" s="446"/>
       <c r="AJ16" s="355"/>
     </row>
-    <row r="17" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="430"/>
       <c r="B17" s="360"/>
       <c r="C17" s="361" t="s">
@@ -10021,7 +10047,7 @@
       <c r="AI17" s="446"/>
       <c r="AJ17" s="355"/>
     </row>
-    <row r="18" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="430"/>
       <c r="B18" s="360"/>
       <c r="C18" s="361" t="s">
@@ -10063,7 +10089,7 @@
       <c r="AI18" s="446"/>
       <c r="AJ18" s="355"/>
     </row>
-    <row r="19" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="430"/>
       <c r="B19" s="360" t="s">
         <v>98</v>
@@ -10107,7 +10133,7 @@
       <c r="AI19" s="446"/>
       <c r="AJ19" s="355"/>
     </row>
-    <row r="20" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="430"/>
       <c r="B20" s="360" t="s">
         <v>45</v>
@@ -10151,7 +10177,7 @@
       <c r="AI20" s="446"/>
       <c r="AJ20" s="356"/>
     </row>
-    <row r="21" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="430"/>
       <c r="B21" s="360"/>
       <c r="C21" s="361" t="s">
@@ -10193,7 +10219,7 @@
       <c r="AI21" s="446"/>
       <c r="AJ21" s="356"/>
     </row>
-    <row r="22" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="430"/>
       <c r="B22" s="360"/>
       <c r="C22" s="361" t="s">
@@ -10235,7 +10261,7 @@
       <c r="AI22" s="446"/>
       <c r="AJ22" s="356"/>
     </row>
-    <row r="23" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="430"/>
       <c r="B23" s="360"/>
       <c r="C23" s="361" t="s">
@@ -10277,7 +10303,7 @@
       <c r="AI23" s="446"/>
       <c r="AJ23" s="356"/>
     </row>
-    <row r="24" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="430"/>
       <c r="B24" s="360"/>
       <c r="C24" s="361" t="s">
@@ -10319,7 +10345,7 @@
       <c r="AI24" s="446"/>
       <c r="AJ24" s="356"/>
     </row>
-    <row r="25" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="430"/>
       <c r="B25" s="360"/>
       <c r="C25" s="361" t="s">
@@ -10361,7 +10387,7 @@
       <c r="AI25" s="446"/>
       <c r="AJ25" s="356"/>
     </row>
-    <row r="26" spans="1:36" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:36" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="430"/>
       <c r="B26" s="364"/>
       <c r="C26" s="365" t="s">
@@ -10403,7 +10429,7 @@
       <c r="AI26" s="449"/>
       <c r="AJ26" s="356"/>
     </row>
-    <row r="27" spans="1:36" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:36" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A27" s="430"/>
       <c r="B27" s="41" t="s">
         <v>303</v>
@@ -10493,7 +10519,7 @@
       </c>
       <c r="AJ27" s="66"/>
     </row>
-    <row r="28" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="430"/>
       <c r="B28" s="47"/>
       <c r="C28" s="3" t="s">
@@ -10579,7 +10605,7 @@
       </c>
       <c r="AJ28" s="188"/>
     </row>
-    <row r="29" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="430"/>
       <c r="B29" s="47"/>
       <c r="C29" s="3" t="s">
@@ -10665,7 +10691,7 @@
       </c>
       <c r="AJ29" s="188"/>
     </row>
-    <row r="30" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="430"/>
       <c r="B30" s="47"/>
       <c r="C30" s="3" t="s">
@@ -10753,7 +10779,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="31" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="430"/>
       <c r="B31" s="47"/>
       <c r="C31" s="3" t="s">
@@ -10839,7 +10865,7 @@
       </c>
       <c r="AJ31" s="188"/>
     </row>
-    <row r="32" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="430"/>
       <c r="B32" s="47"/>
       <c r="C32" s="3" t="s">
@@ -10925,7 +10951,7 @@
       </c>
       <c r="AJ32" s="188"/>
     </row>
-    <row r="33" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="430"/>
       <c r="B33" s="47"/>
       <c r="C33" s="3" t="s">
@@ -11011,7 +11037,7 @@
       </c>
       <c r="AJ33" s="188"/>
     </row>
-    <row r="34" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="430"/>
       <c r="B34" s="47"/>
       <c r="C34" s="3" t="s">
@@ -11067,7 +11093,7 @@
       </c>
       <c r="AJ34" s="189"/>
     </row>
-    <row r="35" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="430"/>
       <c r="B35" s="47"/>
       <c r="C35" s="3" t="s">
@@ -11153,7 +11179,7 @@
       </c>
       <c r="AJ35" s="188"/>
     </row>
-    <row r="36" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="430"/>
       <c r="B36" s="47"/>
       <c r="C36" s="3" t="s">
@@ -11225,7 +11251,7 @@
       </c>
       <c r="AJ36" s="188"/>
     </row>
-    <row r="37" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="430"/>
       <c r="B37" s="47"/>
       <c r="C37" s="3" t="s">
@@ -11299,7 +11325,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="430"/>
       <c r="B38" s="47"/>
       <c r="C38" s="3" t="s">
@@ -11363,7 +11389,7 @@
       </c>
       <c r="AJ38" s="188"/>
     </row>
-    <row r="39" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="430"/>
       <c r="B39" s="49"/>
       <c r="C39" s="336" t="s">
@@ -11403,7 +11429,7 @@
       <c r="AI39" s="290"/>
       <c r="AJ39" s="194"/>
     </row>
-    <row r="40" spans="1:37" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:37" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="430"/>
       <c r="B40" s="67"/>
       <c r="C40" s="350" t="s">
@@ -11459,7 +11485,7 @@
       </c>
       <c r="AJ40" s="190"/>
     </row>
-    <row r="41" spans="1:37" ht="15.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:37" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A41" s="430"/>
       <c r="B41" s="48" t="s">
         <v>22</v>
@@ -11547,7 +11573,7 @@
       </c>
       <c r="AJ41" s="193"/>
     </row>
-    <row r="42" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="430"/>
       <c r="B42" s="47"/>
       <c r="C42" s="3" t="s">
@@ -11595,7 +11621,7 @@
       </c>
       <c r="AJ42" s="188"/>
     </row>
-    <row r="43" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="430"/>
       <c r="B43" s="47"/>
       <c r="C43" s="3" t="s">
@@ -11643,7 +11669,7 @@
       </c>
       <c r="AJ43" s="188"/>
     </row>
-    <row r="44" spans="1:37" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:37" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="430"/>
       <c r="B44" s="67"/>
       <c r="C44" s="68" t="s">
@@ -11699,7 +11725,7 @@
       </c>
       <c r="AJ44" s="190"/>
     </row>
-    <row r="45" spans="1:37" ht="15.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:37" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A45" s="430"/>
       <c r="B45" s="41" t="s">
         <v>98</v>
@@ -11789,7 +11815,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="430"/>
       <c r="B46" s="47"/>
       <c r="C46" s="3" t="s">
@@ -11880,7 +11906,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:37" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="430"/>
       <c r="B47" s="72"/>
       <c r="C47" s="68" t="s">
@@ -11936,7 +11962,7 @@
       </c>
       <c r="AJ47" s="191"/>
     </row>
-    <row r="48" spans="1:37" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:37" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="430"/>
       <c r="B48" s="410"/>
       <c r="C48" s="411" t="s">
@@ -12022,7 +12048,7 @@
       </c>
       <c r="AJ48" s="417"/>
     </row>
-    <row r="49" spans="1:36" s="38" customFormat="1" ht="15.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:36" s="38" customFormat="1" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="430"/>
       <c r="B49" s="74" t="s">
         <v>299</v>
@@ -12072,7 +12098,7 @@
       </c>
       <c r="AJ49" s="192"/>
     </row>
-    <row r="50" spans="1:36" ht="15.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:36" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A50" s="430"/>
       <c r="B50" s="41" t="s">
         <v>35</v>
@@ -12176,7 +12202,7 @@
       </c>
       <c r="AJ50" s="66"/>
     </row>
-    <row r="51" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="430"/>
       <c r="B51" s="48"/>
       <c r="C51" s="39" t="s">
@@ -12276,7 +12302,7 @@
       </c>
       <c r="AJ51" s="193"/>
     </row>
-    <row r="52" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="430"/>
       <c r="B52" s="48"/>
       <c r="C52" s="39" t="s">
@@ -12374,11 +12400,11 @@
         <v>9</v>
       </c>
       <c r="AI52" s="281" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AJ52" s="193"/>
     </row>
-    <row r="53" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="430"/>
       <c r="B53" s="47"/>
       <c r="C53" s="3" t="s">
@@ -12480,7 +12506,7 @@
       </c>
       <c r="AJ53" s="188"/>
     </row>
-    <row r="54" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="430"/>
       <c r="B54" s="47"/>
       <c r="C54" s="5" t="s">
@@ -12552,7 +12578,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="430"/>
       <c r="B55" s="47"/>
       <c r="C55" s="210" t="s">
@@ -12654,7 +12680,7 @@
       </c>
       <c r="AJ55" s="188"/>
     </row>
-    <row r="56" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="430"/>
       <c r="B56" s="47"/>
       <c r="C56" s="210" t="s">
@@ -12756,7 +12782,7 @@
       </c>
       <c r="AJ56" s="188"/>
     </row>
-    <row r="57" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="430"/>
       <c r="B57" s="47"/>
       <c r="C57" s="211" t="s">
@@ -12828,7 +12854,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="430"/>
       <c r="B58" s="47"/>
       <c r="C58" s="210" t="s">
@@ -12930,7 +12956,7 @@
       </c>
       <c r="AJ58" s="188"/>
     </row>
-    <row r="59" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="430"/>
       <c r="B59" s="47"/>
       <c r="C59" s="210" t="s">
@@ -13028,11 +13054,13 @@
         <v>9</v>
       </c>
       <c r="AI59" s="120" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ59" s="188"/>
-    </row>
-    <row r="60" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="AJ59" s="188" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="60" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="430"/>
       <c r="B60" s="47"/>
       <c r="C60" s="210" t="s">
@@ -13130,11 +13158,13 @@
         <v>9</v>
       </c>
       <c r="AI60" s="120" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ60" s="188"/>
-    </row>
-    <row r="61" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>489</v>
+      </c>
+      <c r="AJ60" s="188" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="61" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="430"/>
       <c r="B61" s="47"/>
       <c r="C61" s="210" t="s">
@@ -13236,7 +13266,7 @@
       </c>
       <c r="AJ61" s="188"/>
     </row>
-    <row r="62" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="430"/>
       <c r="B62" s="47"/>
       <c r="C62" s="386" t="s">
@@ -13276,7 +13306,7 @@
       <c r="AI62" s="120"/>
       <c r="AJ62" s="188"/>
     </row>
-    <row r="63" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="430"/>
       <c r="B63" s="47"/>
       <c r="C63" s="210" t="s">
@@ -13342,7 +13372,7 @@
       </c>
       <c r="AJ63" s="188"/>
     </row>
-    <row r="64" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="430"/>
       <c r="B64" s="47"/>
       <c r="C64" s="211" t="s">
@@ -13404,15 +13434,17 @@
       <c r="AG64" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="AH64" s="120" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI64" s="120" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ64" s="189"/>
-    </row>
-    <row r="65" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AH64" s="453" t="s">
+        <v>491</v>
+      </c>
+      <c r="AI64" s="453" t="s">
+        <v>491</v>
+      </c>
+      <c r="AJ64" s="189" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="65" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="430"/>
       <c r="B65" s="47"/>
       <c r="C65" s="211" t="s">
@@ -13474,15 +13506,17 @@
       <c r="AG65" s="120" t="s">
         <v>108</v>
       </c>
-      <c r="AH65" s="120" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI65" s="120" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ65" s="188"/>
-    </row>
-    <row r="66" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AH65" s="453" t="s">
+        <v>491</v>
+      </c>
+      <c r="AI65" s="453" t="s">
+        <v>491</v>
+      </c>
+      <c r="AJ65" s="188" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="66" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="430"/>
       <c r="B66" s="47"/>
       <c r="C66" s="210" t="s">
@@ -13584,7 +13618,7 @@
       </c>
       <c r="AJ66" s="188"/>
     </row>
-    <row r="67" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="430"/>
       <c r="B67" s="47"/>
       <c r="C67" s="210" t="s">
@@ -13686,7 +13720,7 @@
       </c>
       <c r="AJ67" s="188"/>
     </row>
-    <row r="68" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="430"/>
       <c r="B68" s="47"/>
       <c r="C68" s="210" t="s">
@@ -13788,7 +13822,7 @@
       </c>
       <c r="AJ68" s="188"/>
     </row>
-    <row r="69" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="430"/>
       <c r="B69" s="47"/>
       <c r="C69" s="210" t="s">
@@ -13890,7 +13924,7 @@
       </c>
       <c r="AJ69" s="188"/>
     </row>
-    <row r="70" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="430"/>
       <c r="B70" s="47"/>
       <c r="C70" s="386" t="s">
@@ -13930,7 +13964,7 @@
       <c r="AI70" s="120"/>
       <c r="AJ70" s="188"/>
     </row>
-    <row r="71" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="430"/>
       <c r="B71" s="47"/>
       <c r="C71" s="210" t="s">
@@ -14000,7 +14034,7 @@
       </c>
       <c r="AJ71" s="188"/>
     </row>
-    <row r="72" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="430"/>
       <c r="B72" s="47"/>
       <c r="C72" s="210" t="s">
@@ -14062,7 +14096,7 @@
       </c>
       <c r="AJ72" s="188"/>
     </row>
-    <row r="73" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="430"/>
       <c r="B73" s="47"/>
       <c r="C73" s="386" t="s">
@@ -14102,7 +14136,7 @@
       <c r="AI73" s="120"/>
       <c r="AJ73" s="188"/>
     </row>
-    <row r="74" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="430"/>
       <c r="B74" s="47"/>
       <c r="C74" s="210" t="s">
@@ -14168,7 +14202,7 @@
       </c>
       <c r="AJ74" s="188"/>
     </row>
-    <row r="75" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="430"/>
       <c r="B75" s="47"/>
       <c r="C75" s="210" t="s">
@@ -14224,7 +14258,7 @@
       </c>
       <c r="AJ75" s="188"/>
     </row>
-    <row r="76" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="430"/>
       <c r="B76" s="47"/>
       <c r="C76" s="210" t="s">
@@ -14326,7 +14360,7 @@
       </c>
       <c r="AJ76" s="188"/>
     </row>
-    <row r="77" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="430"/>
       <c r="B77" s="47"/>
       <c r="C77" s="210" t="s">
@@ -14428,7 +14462,7 @@
       </c>
       <c r="AJ77" s="188"/>
     </row>
-    <row r="78" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="430"/>
       <c r="B78" s="47"/>
       <c r="C78" s="210" t="s">
@@ -14490,7 +14524,7 @@
       </c>
       <c r="AJ78" s="188"/>
     </row>
-    <row r="79" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="430"/>
       <c r="B79" s="47"/>
       <c r="C79" s="386" t="s">
@@ -14530,7 +14564,7 @@
       <c r="AI79" s="120"/>
       <c r="AJ79" s="188"/>
     </row>
-    <row r="80" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="430"/>
       <c r="B80" s="47"/>
       <c r="C80" s="210" t="s">
@@ -14634,7 +14668,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="81" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="430"/>
       <c r="B81" s="47"/>
       <c r="C81" s="210" t="s">
@@ -14736,7 +14770,7 @@
       </c>
       <c r="AJ81" s="188"/>
     </row>
-    <row r="82" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="430"/>
       <c r="B82" s="47"/>
       <c r="C82" s="210" t="s">
@@ -14840,7 +14874,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="430"/>
       <c r="B83" s="47"/>
       <c r="C83" s="210" t="s">
@@ -14902,7 +14936,7 @@
       </c>
       <c r="AJ83" s="188"/>
     </row>
-    <row r="84" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="430"/>
       <c r="B84" s="268"/>
       <c r="C84" s="269" t="s">
@@ -15004,7 +15038,7 @@
       </c>
       <c r="AJ84" s="274"/>
     </row>
-    <row r="85" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="430"/>
       <c r="B85" s="268"/>
       <c r="C85" s="389" t="s">
@@ -15044,7 +15078,7 @@
       <c r="AI85" s="388"/>
       <c r="AJ85" s="274"/>
     </row>
-    <row r="86" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="430"/>
       <c r="B86" s="47"/>
       <c r="C86" s="210" t="s">
@@ -15090,7 +15124,7 @@
       <c r="AI86" s="289"/>
       <c r="AJ86" s="188"/>
     </row>
-    <row r="87" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="430"/>
       <c r="B87" s="47"/>
       <c r="C87" s="210" t="s">
@@ -15192,7 +15226,7 @@
       </c>
       <c r="AJ87" s="188"/>
     </row>
-    <row r="88" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="430"/>
       <c r="B88" s="47"/>
       <c r="C88" s="386" t="s">
@@ -15232,7 +15266,7 @@
       <c r="AI88" s="285"/>
       <c r="AJ88" s="188"/>
     </row>
-    <row r="89" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="430"/>
       <c r="B89" s="47"/>
       <c r="C89" s="210" t="s">
@@ -15306,7 +15340,7 @@
       </c>
       <c r="AJ89" s="188"/>
     </row>
-    <row r="90" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="430"/>
       <c r="B90" s="47"/>
       <c r="C90" s="210" t="s">
@@ -15376,7 +15410,7 @@
       </c>
       <c r="AJ90" s="188"/>
     </row>
-    <row r="91" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="430"/>
       <c r="B91" s="47"/>
       <c r="C91" s="210" t="s">
@@ -15442,7 +15476,7 @@
       </c>
       <c r="AJ91" s="188"/>
     </row>
-    <row r="92" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="430"/>
       <c r="B92" s="47"/>
       <c r="C92" s="210" t="s">
@@ -15512,7 +15546,7 @@
       </c>
       <c r="AJ92" s="188"/>
     </row>
-    <row r="93" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="430"/>
       <c r="B93" s="47"/>
       <c r="C93" s="386" t="s">
@@ -15552,7 +15586,7 @@
       <c r="AI93" s="120"/>
       <c r="AJ93" s="188"/>
     </row>
-    <row r="94" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="430"/>
       <c r="B94" s="47"/>
       <c r="C94" s="386" t="s">
@@ -15592,7 +15626,7 @@
       <c r="AI94" s="120"/>
       <c r="AJ94" s="188"/>
     </row>
-    <row r="95" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="430"/>
       <c r="B95" s="47"/>
       <c r="C95" s="210" t="s">
@@ -15662,7 +15696,7 @@
       </c>
       <c r="AJ95" s="188"/>
     </row>
-    <row r="96" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="430"/>
       <c r="B96" s="49"/>
       <c r="C96" s="386" t="s">
@@ -15702,7 +15736,7 @@
       <c r="AI96" s="385"/>
       <c r="AJ96" s="194"/>
     </row>
-    <row r="97" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="430"/>
       <c r="B97" s="49"/>
       <c r="C97" s="79" t="s">
@@ -15748,7 +15782,7 @@
       <c r="AI97" s="290"/>
       <c r="AJ97" s="194"/>
     </row>
-    <row r="98" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="430"/>
       <c r="B98" s="49"/>
       <c r="C98" s="79" t="s">
@@ -15850,7 +15884,7 @@
       </c>
       <c r="AJ98" s="194"/>
     </row>
-    <row r="99" spans="1:37" s="38" customFormat="1" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:37" s="38" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="430"/>
       <c r="B99" s="78"/>
       <c r="C99" s="79" t="s">
@@ -15955,7 +15989,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="100" spans="1:37" ht="15.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:37" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A100" s="430"/>
       <c r="B100" s="41" t="s">
         <v>45</v>
@@ -16045,7 +16079,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="101" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="430"/>
       <c r="B101" s="48"/>
       <c r="C101" s="39" t="s">
@@ -16101,7 +16135,7 @@
       </c>
       <c r="AJ101" s="193"/>
     </row>
-    <row r="102" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="430"/>
       <c r="B102" s="47"/>
       <c r="C102" s="3" t="s">
@@ -16187,7 +16221,7 @@
       </c>
       <c r="AJ102" s="188"/>
     </row>
-    <row r="103" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="430"/>
       <c r="B103" s="47"/>
       <c r="C103" s="3" t="s">
@@ -16273,7 +16307,7 @@
       </c>
       <c r="AJ103" s="188"/>
     </row>
-    <row r="104" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="430"/>
       <c r="B104" s="47"/>
       <c r="C104" s="3" t="s">
@@ -16359,7 +16393,7 @@
       </c>
       <c r="AJ104" s="188"/>
     </row>
-    <row r="105" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="430"/>
       <c r="B105" s="47"/>
       <c r="C105" s="3" t="s">
@@ -16450,7 +16484,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="106" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="430"/>
       <c r="B106" s="47"/>
       <c r="C106" s="3" t="s">
@@ -16539,7 +16573,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="107" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="430"/>
       <c r="B107" s="47"/>
       <c r="C107" s="3" t="s">
@@ -16630,7 +16664,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="108" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="430"/>
       <c r="B108" s="47"/>
       <c r="C108" s="3" t="s">
@@ -16718,7 +16752,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="430"/>
       <c r="B109" s="47"/>
       <c r="C109" s="3" t="s">
@@ -16806,7 +16840,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="430"/>
       <c r="B110" s="47"/>
       <c r="C110" s="3" t="s">
@@ -16894,7 +16928,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="111" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="430"/>
       <c r="B111" s="47"/>
       <c r="C111" s="3" t="s">
@@ -16950,7 +16984,7 @@
       </c>
       <c r="AJ111" s="188"/>
     </row>
-    <row r="112" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="430"/>
       <c r="B112" s="47"/>
       <c r="C112" s="3" t="s">
@@ -17014,7 +17048,7 @@
       </c>
       <c r="AJ112" s="188"/>
     </row>
-    <row r="113" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="430"/>
       <c r="B113" s="49"/>
       <c r="C113" s="210" t="s">
@@ -17070,7 +17104,7 @@
       </c>
       <c r="AJ113" s="188"/>
     </row>
-    <row r="114" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="430"/>
       <c r="B114" s="49"/>
       <c r="C114" s="3" t="s">
@@ -17156,7 +17190,7 @@
       </c>
       <c r="AJ114" s="188"/>
     </row>
-    <row r="115" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="433"/>
       <c r="B115" s="320"/>
       <c r="C115" s="298" t="s">
@@ -17242,7 +17276,7 @@
       </c>
       <c r="AJ115" s="188"/>
     </row>
-    <row r="116" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="430"/>
       <c r="B116" s="48"/>
       <c r="C116" s="3" t="s">
@@ -17316,7 +17350,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="117" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="430"/>
       <c r="B117" s="47"/>
       <c r="C117" s="3" t="s">
@@ -17402,7 +17436,7 @@
       </c>
       <c r="AJ117" s="196"/>
     </row>
-    <row r="118" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="430"/>
       <c r="B118" s="47"/>
       <c r="C118" s="3" t="s">
@@ -17488,7 +17522,7 @@
       </c>
       <c r="AJ118" s="188"/>
     </row>
-    <row r="119" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="430"/>
       <c r="B119" s="47"/>
       <c r="C119" s="3" t="s">
@@ -17574,7 +17608,7 @@
       </c>
       <c r="AJ119" s="188"/>
     </row>
-    <row r="120" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="430"/>
       <c r="B120" s="47"/>
       <c r="C120" s="3" t="s">
@@ -17660,7 +17694,7 @@
       </c>
       <c r="AJ120" s="196"/>
     </row>
-    <row r="121" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="430"/>
       <c r="B121" s="47"/>
       <c r="C121" s="3" t="s">
@@ -17746,7 +17780,7 @@
       </c>
       <c r="AJ121" s="188"/>
     </row>
-    <row r="122" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="430"/>
       <c r="B122" s="47"/>
       <c r="C122" s="3" t="s">
@@ -17832,7 +17866,7 @@
       </c>
       <c r="AJ122" s="196"/>
     </row>
-    <row r="123" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="430"/>
       <c r="B123" s="47"/>
       <c r="C123" s="3" t="s">
@@ -17918,7 +17952,7 @@
       </c>
       <c r="AJ123" s="188"/>
     </row>
-    <row r="124" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="430"/>
       <c r="B124" s="47"/>
       <c r="C124" s="3" t="s">
@@ -18004,7 +18038,7 @@
       </c>
       <c r="AJ124" s="188"/>
     </row>
-    <row r="125" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="430"/>
       <c r="B125" s="47"/>
       <c r="C125" s="3" t="s">
@@ -18092,7 +18126,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="126" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="430"/>
       <c r="B126" s="47"/>
       <c r="C126" s="3" t="s">
@@ -18180,7 +18214,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="127" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="430"/>
       <c r="B127" s="47"/>
       <c r="C127" s="3" t="s">
@@ -18268,7 +18302,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="128" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="430"/>
       <c r="B128" s="47"/>
       <c r="C128" s="3" t="s">
@@ -18356,7 +18390,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="129" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="430"/>
       <c r="B129" s="47"/>
       <c r="C129" s="3" t="s">
@@ -18444,7 +18478,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="130" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="430"/>
       <c r="B130" s="47"/>
       <c r="C130" s="3" t="s">
@@ -18535,7 +18569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="430"/>
       <c r="B131" s="47"/>
       <c r="C131" s="3" t="s">
@@ -18623,7 +18657,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="132" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="430"/>
       <c r="B132" s="47"/>
       <c r="C132" s="3" t="s">
@@ -18681,7 +18715,7 @@
       </c>
       <c r="AJ132" s="188"/>
     </row>
-    <row r="133" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="430"/>
       <c r="B133" s="47"/>
       <c r="C133" s="3" t="s">
@@ -18739,7 +18773,7 @@
       </c>
       <c r="AJ133" s="188"/>
     </row>
-    <row r="134" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="430"/>
       <c r="B134" s="47"/>
       <c r="C134" s="3" t="s">
@@ -18797,7 +18831,7 @@
       </c>
       <c r="AJ134" s="188"/>
     </row>
-    <row r="135" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="430"/>
       <c r="B135" s="47"/>
       <c r="C135" s="3" t="s">
@@ -18855,7 +18889,7 @@
       </c>
       <c r="AJ135" s="188"/>
     </row>
-    <row r="136" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="430"/>
       <c r="B136" s="47"/>
       <c r="C136" s="3" t="s">
@@ -18913,7 +18947,7 @@
       </c>
       <c r="AJ136" s="188"/>
     </row>
-    <row r="137" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="430"/>
       <c r="B137" s="47"/>
       <c r="C137" s="3" t="s">
@@ -18971,7 +19005,7 @@
       </c>
       <c r="AJ137" s="188"/>
     </row>
-    <row r="138" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="430"/>
       <c r="B138" s="47"/>
       <c r="C138" s="3" t="s">
@@ -19029,7 +19063,7 @@
       </c>
       <c r="AJ138" s="188"/>
     </row>
-    <row r="139" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="430"/>
       <c r="B139" s="47"/>
       <c r="C139" s="3" t="s">
@@ -19087,7 +19121,7 @@
       </c>
       <c r="AJ139" s="188"/>
     </row>
-    <row r="140" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="430"/>
       <c r="B140" s="47"/>
       <c r="C140" s="3" t="s">
@@ -19145,7 +19179,7 @@
       </c>
       <c r="AJ140" s="188"/>
     </row>
-    <row r="141" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="430"/>
       <c r="B141" s="47"/>
       <c r="C141" s="3" t="s">
@@ -19203,7 +19237,7 @@
       </c>
       <c r="AJ141" s="188"/>
     </row>
-    <row r="142" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="430"/>
       <c r="B142" s="47"/>
       <c r="C142" s="3" t="s">
@@ -19261,7 +19295,7 @@
       </c>
       <c r="AJ142" s="188"/>
     </row>
-    <row r="143" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="430"/>
       <c r="B143" s="47"/>
       <c r="C143" s="3" t="s">
@@ -19331,7 +19365,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="144" spans="1:37" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="430"/>
       <c r="B144" s="47"/>
       <c r="C144" s="3" t="s">
@@ -19419,7 +19453,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="145" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="430"/>
       <c r="B145" s="47"/>
       <c r="C145" s="308" t="s">
@@ -19459,7 +19493,7 @@
       <c r="AI145" s="289"/>
       <c r="AJ145" s="188"/>
     </row>
-    <row r="146" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="430"/>
       <c r="B146" s="47"/>
       <c r="C146" s="310" t="s">
@@ -19547,7 +19581,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="147" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="430"/>
       <c r="B147" s="47"/>
       <c r="C147" s="308" t="s">
@@ -19633,7 +19667,7 @@
       </c>
       <c r="AJ147" s="188"/>
     </row>
-    <row r="148" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="430"/>
       <c r="B148" s="47"/>
       <c r="C148" s="352" t="s">
@@ -19719,7 +19753,7 @@
       </c>
       <c r="AJ148" s="188"/>
     </row>
-    <row r="149" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="430"/>
       <c r="B149" s="47"/>
       <c r="C149" s="352" t="s">
@@ -19807,7 +19841,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="150" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="430"/>
       <c r="B150" s="47"/>
       <c r="C150" s="353" t="s">
@@ -19895,7 +19929,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="151" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="430"/>
       <c r="B151" s="47"/>
       <c r="C151" s="308" t="s">
@@ -19983,7 +20017,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="152" spans="1:36" s="302" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:36" s="302" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="430"/>
       <c r="B152" s="307"/>
       <c r="C152" s="309" t="s">
@@ -20069,7 +20103,7 @@
       </c>
       <c r="AJ152" s="301"/>
     </row>
-    <row r="153" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="430"/>
       <c r="B153" s="49"/>
       <c r="C153" s="310" t="s">
@@ -20155,7 +20189,7 @@
       </c>
       <c r="AJ153" s="188"/>
     </row>
-    <row r="154" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="433"/>
       <c r="B154" s="307"/>
       <c r="C154" s="310" t="s">
@@ -20243,7 +20277,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="155" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="430"/>
       <c r="B155" s="48"/>
       <c r="C155" s="308" t="s">
@@ -20331,7 +20365,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="156" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="430"/>
       <c r="B156" s="47"/>
       <c r="C156" s="308" t="s">
@@ -20417,7 +20451,7 @@
       </c>
       <c r="AJ156" s="188"/>
     </row>
-    <row r="157" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="430"/>
       <c r="B157" s="47"/>
       <c r="C157" s="308" t="s">
@@ -20477,7 +20511,7 @@
       </c>
       <c r="AJ157" s="188"/>
     </row>
-    <row r="158" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="430"/>
       <c r="B158" s="47"/>
       <c r="C158" s="308" t="s">
@@ -20565,7 +20599,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="159" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="430"/>
       <c r="B159" s="47"/>
       <c r="C159" s="308" t="s">
@@ -20651,7 +20685,7 @@
       </c>
       <c r="AJ159" s="188"/>
     </row>
-    <row r="160" spans="1:36" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:36" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="430"/>
       <c r="B160" s="67"/>
       <c r="C160" s="311" t="s">
@@ -20709,7 +20743,7 @@
       </c>
       <c r="AJ160" s="190"/>
     </row>
-    <row r="161" spans="1:36" ht="26.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:36" ht="28.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A161" s="430"/>
       <c r="B161" s="90" t="s">
         <v>76</v>
@@ -20799,7 +20833,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="162" spans="1:36" ht="26" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:36" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A162" s="430"/>
       <c r="B162" s="47"/>
       <c r="C162" s="3" t="s">
@@ -20887,7 +20921,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="163" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="430"/>
       <c r="B163" s="47"/>
       <c r="C163" s="3" t="s">
@@ -20973,7 +21007,7 @@
       </c>
       <c r="AJ163" s="188"/>
     </row>
-    <row r="164" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="430"/>
       <c r="B164" s="47"/>
       <c r="C164" s="3" t="s">
@@ -21059,7 +21093,7 @@
       </c>
       <c r="AJ164" s="188"/>
     </row>
-    <row r="165" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="430"/>
       <c r="B165" s="47"/>
       <c r="C165" s="3" t="s">
@@ -21145,7 +21179,7 @@
       </c>
       <c r="AJ165" s="188"/>
     </row>
-    <row r="166" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="430"/>
       <c r="B166" s="47"/>
       <c r="C166" s="3" t="s">
@@ -21231,7 +21265,7 @@
       </c>
       <c r="AJ166" s="188"/>
     </row>
-    <row r="167" spans="1:36" ht="39" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:36" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A167" s="430"/>
       <c r="B167" s="47"/>
       <c r="C167" s="3" t="s">
@@ -21319,7 +21353,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="168" spans="1:36" ht="39" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:36" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A168" s="430"/>
       <c r="B168" s="47"/>
       <c r="C168" s="2" t="s">
@@ -21405,7 +21439,7 @@
       </c>
       <c r="AJ168" s="196"/>
     </row>
-    <row r="169" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="430"/>
       <c r="B169" s="47"/>
       <c r="C169" s="2" t="s">
@@ -21491,7 +21525,7 @@
       </c>
       <c r="AJ169" s="196"/>
     </row>
-    <row r="170" spans="1:36" ht="39" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:36" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A170" s="430"/>
       <c r="B170" s="47"/>
       <c r="C170" s="2" t="s">
@@ -21579,7 +21613,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="171" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A171" s="430"/>
       <c r="B171" s="47"/>
       <c r="C171" s="2" t="s">
@@ -21667,7 +21701,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="172" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="430"/>
       <c r="B172" s="47"/>
       <c r="C172" s="3" t="s">
@@ -21753,7 +21787,7 @@
       </c>
       <c r="AJ172" s="188"/>
     </row>
-    <row r="173" spans="1:36" ht="26" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:36" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A173" s="430"/>
       <c r="B173" s="47"/>
       <c r="C173" s="3" t="s">
@@ -21841,7 +21875,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="174" spans="1:36" ht="52" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:36" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A174" s="430"/>
       <c r="B174" s="47"/>
       <c r="C174" s="3" t="s">
@@ -21927,7 +21961,7 @@
       </c>
       <c r="AJ174" s="188"/>
     </row>
-    <row r="175" spans="1:36" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:36" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A175" s="430"/>
       <c r="B175" s="67"/>
       <c r="C175" s="68" t="s">
@@ -21995,7 +22029,7 @@
       </c>
       <c r="AJ175" s="190"/>
     </row>
-    <row r="176" spans="1:36" ht="15.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:36" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A176" s="430"/>
       <c r="B176" s="55" t="s">
         <v>136</v>
@@ -22083,7 +22117,7 @@
       </c>
       <c r="AJ176" s="197"/>
     </row>
-    <row r="177" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="430"/>
       <c r="B177" s="59"/>
       <c r="C177" s="5" t="s">
@@ -22169,7 +22203,7 @@
       </c>
       <c r="AJ177" s="198"/>
     </row>
-    <row r="178" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="430"/>
       <c r="B178" s="59"/>
       <c r="C178" s="5" t="s">
@@ -22257,7 +22291,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="179" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="430"/>
       <c r="B179" s="59"/>
       <c r="C179" s="5" t="s">
@@ -22343,7 +22377,7 @@
       </c>
       <c r="AJ179" s="198"/>
     </row>
-    <row r="180" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="430"/>
       <c r="B180" s="59"/>
       <c r="C180" s="5" t="s">
@@ -22429,7 +22463,7 @@
       </c>
       <c r="AJ180" s="198"/>
     </row>
-    <row r="181" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="430"/>
       <c r="B181" s="59"/>
       <c r="C181" s="5" t="s">
@@ -22517,7 +22551,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="182" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="430"/>
       <c r="B182" s="59"/>
       <c r="C182" s="5" t="s">
@@ -22603,7 +22637,7 @@
       </c>
       <c r="AJ182" s="198"/>
     </row>
-    <row r="183" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="430"/>
       <c r="B183" s="59"/>
       <c r="C183" s="5" t="s">
@@ -22689,7 +22723,7 @@
       </c>
       <c r="AJ183" s="198"/>
     </row>
-    <row r="184" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="430"/>
       <c r="B184" s="59"/>
       <c r="C184" s="5" t="s">
@@ -22775,7 +22809,7 @@
       </c>
       <c r="AJ184" s="198"/>
     </row>
-    <row r="185" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="430"/>
       <c r="B185" s="59"/>
       <c r="C185" s="5" t="s">
@@ -22863,7 +22897,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="186" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="430"/>
       <c r="B186" s="59"/>
       <c r="C186" s="5" t="s">
@@ -22949,7 +22983,7 @@
       </c>
       <c r="AJ186" s="198"/>
     </row>
-    <row r="187" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="430"/>
       <c r="B187" s="59"/>
       <c r="C187" s="5" t="s">
@@ -23035,7 +23069,7 @@
       </c>
       <c r="AJ187" s="198"/>
     </row>
-    <row r="188" spans="1:36" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:36" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A188" s="430"/>
       <c r="B188" s="60"/>
       <c r="C188" s="61" t="s">
@@ -23121,7 +23155,7 @@
       </c>
       <c r="AJ188" s="200"/>
     </row>
-    <row r="189" spans="1:36" ht="13.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="189" spans="1:36" ht="14.4" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="190" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C190" s="294" t="s">
         <v>414</v>

</xml_diff>

<commit_message>
IP version number update for ADP-S
[git-p4: depot-paths = "//depot/projects/coe/CSME/": change = 767497]
</commit_message>
<xml_diff>
--- a/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
+++ b/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
@@ -4042,7 +4042,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3829" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3829" uniqueCount="524">
   <si>
     <t>CNP-LP</t>
   </si>
@@ -5985,6 +5985,9 @@
       </rPr>
       <t xml:space="preserve"> (11,20,15)</t>
     </r>
+  </si>
+  <si>
+    <t>CSME 4.51</t>
   </si>
 </sst>
 </file>
@@ -8366,6 +8369,54 @@
     <xf numFmtId="0" fontId="23" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -8428,54 +8479,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10017,10 +10020,10 @@
   <dimension ref="A1:AN199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="Z176" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="Z5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AG119" sqref="AG119"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10053,47 +10056,47 @@
       <c r="C2" s="423" t="s">
         <v>495</v>
       </c>
-      <c r="AK2" s="457" t="s">
+      <c r="AK2" s="438" t="s">
         <v>518</v>
       </c>
-      <c r="AL2" s="457"/>
+      <c r="AL2" s="438"/>
     </row>
     <row r="3" spans="1:39" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="438" t="s">
+      <c r="B3" s="454" t="s">
         <v>266</v>
       </c>
-      <c r="C3" s="443" t="s">
+      <c r="C3" s="459" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="444"/>
-      <c r="E3" s="452" t="s">
+      <c r="D3" s="460"/>
+      <c r="E3" s="468" t="s">
         <v>231</v>
       </c>
-      <c r="F3" s="453"/>
-      <c r="G3" s="453"/>
-      <c r="H3" s="453"/>
-      <c r="I3" s="453"/>
-      <c r="J3" s="453"/>
-      <c r="K3" s="453"/>
-      <c r="L3" s="454"/>
-      <c r="M3" s="449" t="s">
+      <c r="F3" s="469"/>
+      <c r="G3" s="469"/>
+      <c r="H3" s="469"/>
+      <c r="I3" s="469"/>
+      <c r="J3" s="469"/>
+      <c r="K3" s="469"/>
+      <c r="L3" s="470"/>
+      <c r="M3" s="465" t="s">
         <v>443</v>
       </c>
-      <c r="N3" s="450"/>
-      <c r="O3" s="451"/>
-      <c r="P3" s="445" t="s">
+      <c r="N3" s="466"/>
+      <c r="O3" s="467"/>
+      <c r="P3" s="461" t="s">
         <v>296</v>
       </c>
-      <c r="Q3" s="446"/>
-      <c r="R3" s="447" t="s">
+      <c r="Q3" s="462"/>
+      <c r="R3" s="463" t="s">
         <v>297</v>
       </c>
-      <c r="S3" s="448"/>
-      <c r="T3" s="440" t="s">
+      <c r="S3" s="464"/>
+      <c r="T3" s="456" t="s">
         <v>298</v>
       </c>
-      <c r="U3" s="441"/>
-      <c r="V3" s="442"/>
+      <c r="U3" s="457"/>
+      <c r="V3" s="458"/>
       <c r="W3" s="298" t="s">
         <v>434</v>
       </c>
@@ -10125,7 +10128,7 @@
         <v>310</v>
       </c>
       <c r="AG3" s="260" t="s">
-        <v>294</v>
+        <v>523</v>
       </c>
       <c r="AH3" s="214" t="s">
         <v>426</v>
@@ -10142,12 +10145,12 @@
       <c r="AL3" s="435" t="s">
         <v>494</v>
       </c>
-      <c r="AM3" s="436" t="s">
+      <c r="AM3" s="452" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="439"/>
+      <c r="B4" s="455"/>
       <c r="C4" s="295" t="s">
         <v>432</v>
       </c>
@@ -10250,14 +10253,14 @@
       <c r="AJ4" s="391" t="s">
         <v>431</v>
       </c>
-      <c r="AK4" s="455" t="s">
+      <c r="AK4" s="471" t="s">
         <v>520</v>
       </c>
-      <c r="AL4" s="456"/>
-      <c r="AM4" s="437"/>
+      <c r="AL4" s="472"/>
+      <c r="AM4" s="453"/>
     </row>
     <row r="5" spans="1:39" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="458"/>
+      <c r="A5" s="439"/>
       <c r="B5" s="326" t="s">
         <v>293</v>
       </c>
@@ -10267,48 +10270,48 @@
       <c r="D5" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="462" t="s">
+      <c r="E5" s="443" t="s">
         <v>333</v>
       </c>
-      <c r="F5" s="463"/>
-      <c r="G5" s="463"/>
-      <c r="H5" s="463"/>
-      <c r="I5" s="463"/>
-      <c r="J5" s="463"/>
-      <c r="K5" s="463"/>
-      <c r="L5" s="464"/>
-      <c r="M5" s="462" t="s">
+      <c r="F5" s="444"/>
+      <c r="G5" s="444"/>
+      <c r="H5" s="444"/>
+      <c r="I5" s="444"/>
+      <c r="J5" s="444"/>
+      <c r="K5" s="444"/>
+      <c r="L5" s="445"/>
+      <c r="M5" s="443" t="s">
         <v>334</v>
       </c>
-      <c r="N5" s="463"/>
-      <c r="O5" s="463"/>
-      <c r="P5" s="463"/>
-      <c r="Q5" s="463"/>
-      <c r="R5" s="463"/>
-      <c r="S5" s="463"/>
-      <c r="T5" s="463"/>
-      <c r="U5" s="463"/>
-      <c r="V5" s="463"/>
-      <c r="W5" s="463"/>
-      <c r="X5" s="463"/>
-      <c r="Y5" s="463"/>
-      <c r="Z5" s="463"/>
-      <c r="AA5" s="463"/>
-      <c r="AB5" s="463"/>
-      <c r="AC5" s="463"/>
-      <c r="AD5" s="463"/>
-      <c r="AE5" s="463"/>
-      <c r="AF5" s="463"/>
-      <c r="AG5" s="463"/>
-      <c r="AH5" s="463"/>
-      <c r="AI5" s="463"/>
-      <c r="AJ5" s="463"/>
-      <c r="AK5" s="466"/>
-      <c r="AL5" s="467"/>
+      <c r="N5" s="444"/>
+      <c r="O5" s="444"/>
+      <c r="P5" s="444"/>
+      <c r="Q5" s="444"/>
+      <c r="R5" s="444"/>
+      <c r="S5" s="444"/>
+      <c r="T5" s="444"/>
+      <c r="U5" s="444"/>
+      <c r="V5" s="444"/>
+      <c r="W5" s="444"/>
+      <c r="X5" s="444"/>
+      <c r="Y5" s="444"/>
+      <c r="Z5" s="444"/>
+      <c r="AA5" s="444"/>
+      <c r="AB5" s="444"/>
+      <c r="AC5" s="444"/>
+      <c r="AD5" s="444"/>
+      <c r="AE5" s="444"/>
+      <c r="AF5" s="444"/>
+      <c r="AG5" s="444"/>
+      <c r="AH5" s="444"/>
+      <c r="AI5" s="444"/>
+      <c r="AJ5" s="444"/>
+      <c r="AK5" s="447"/>
+      <c r="AL5" s="448"/>
       <c r="AM5" s="323"/>
     </row>
     <row r="6" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="458"/>
+      <c r="A6" s="439"/>
       <c r="B6" s="329"/>
       <c r="C6" s="330" t="s">
         <v>8</v>
@@ -10316,44 +10319,44 @@
       <c r="D6" s="331" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="465"/>
-      <c r="F6" s="466"/>
-      <c r="G6" s="466"/>
-      <c r="H6" s="466"/>
-      <c r="I6" s="466"/>
-      <c r="J6" s="466"/>
-      <c r="K6" s="466"/>
-      <c r="L6" s="467"/>
-      <c r="M6" s="465"/>
-      <c r="N6" s="466"/>
-      <c r="O6" s="466"/>
-      <c r="P6" s="466"/>
-      <c r="Q6" s="466"/>
-      <c r="R6" s="466"/>
-      <c r="S6" s="466"/>
-      <c r="T6" s="466"/>
-      <c r="U6" s="466"/>
-      <c r="V6" s="466"/>
-      <c r="W6" s="466"/>
-      <c r="X6" s="466"/>
-      <c r="Y6" s="466"/>
-      <c r="Z6" s="466"/>
-      <c r="AA6" s="466"/>
-      <c r="AB6" s="466"/>
-      <c r="AC6" s="466"/>
-      <c r="AD6" s="466"/>
-      <c r="AE6" s="466"/>
-      <c r="AF6" s="466"/>
-      <c r="AG6" s="466"/>
-      <c r="AH6" s="466"/>
-      <c r="AI6" s="466"/>
-      <c r="AJ6" s="466"/>
-      <c r="AK6" s="466"/>
-      <c r="AL6" s="467"/>
+      <c r="E6" s="446"/>
+      <c r="F6" s="447"/>
+      <c r="G6" s="447"/>
+      <c r="H6" s="447"/>
+      <c r="I6" s="447"/>
+      <c r="J6" s="447"/>
+      <c r="K6" s="447"/>
+      <c r="L6" s="448"/>
+      <c r="M6" s="446"/>
+      <c r="N6" s="447"/>
+      <c r="O6" s="447"/>
+      <c r="P6" s="447"/>
+      <c r="Q6" s="447"/>
+      <c r="R6" s="447"/>
+      <c r="S6" s="447"/>
+      <c r="T6" s="447"/>
+      <c r="U6" s="447"/>
+      <c r="V6" s="447"/>
+      <c r="W6" s="447"/>
+      <c r="X6" s="447"/>
+      <c r="Y6" s="447"/>
+      <c r="Z6" s="447"/>
+      <c r="AA6" s="447"/>
+      <c r="AB6" s="447"/>
+      <c r="AC6" s="447"/>
+      <c r="AD6" s="447"/>
+      <c r="AE6" s="447"/>
+      <c r="AF6" s="447"/>
+      <c r="AG6" s="447"/>
+      <c r="AH6" s="447"/>
+      <c r="AI6" s="447"/>
+      <c r="AJ6" s="447"/>
+      <c r="AK6" s="447"/>
+      <c r="AL6" s="448"/>
       <c r="AM6" s="324"/>
     </row>
     <row r="7" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="458"/>
+      <c r="A7" s="439"/>
       <c r="B7" s="329"/>
       <c r="C7" s="330" t="s">
         <v>11</v>
@@ -10361,44 +10364,44 @@
       <c r="D7" s="332" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="465"/>
-      <c r="F7" s="466"/>
-      <c r="G7" s="466"/>
-      <c r="H7" s="466"/>
-      <c r="I7" s="466"/>
-      <c r="J7" s="466"/>
-      <c r="K7" s="466"/>
-      <c r="L7" s="467"/>
-      <c r="M7" s="465"/>
-      <c r="N7" s="466"/>
-      <c r="O7" s="466"/>
-      <c r="P7" s="466"/>
-      <c r="Q7" s="466"/>
-      <c r="R7" s="466"/>
-      <c r="S7" s="466"/>
-      <c r="T7" s="466"/>
-      <c r="U7" s="466"/>
-      <c r="V7" s="466"/>
-      <c r="W7" s="466"/>
-      <c r="X7" s="466"/>
-      <c r="Y7" s="466"/>
-      <c r="Z7" s="466"/>
-      <c r="AA7" s="466"/>
-      <c r="AB7" s="466"/>
-      <c r="AC7" s="466"/>
-      <c r="AD7" s="466"/>
-      <c r="AE7" s="466"/>
-      <c r="AF7" s="466"/>
-      <c r="AG7" s="466"/>
-      <c r="AH7" s="466"/>
-      <c r="AI7" s="466"/>
-      <c r="AJ7" s="466"/>
-      <c r="AK7" s="466"/>
-      <c r="AL7" s="467"/>
+      <c r="E7" s="446"/>
+      <c r="F7" s="447"/>
+      <c r="G7" s="447"/>
+      <c r="H7" s="447"/>
+      <c r="I7" s="447"/>
+      <c r="J7" s="447"/>
+      <c r="K7" s="447"/>
+      <c r="L7" s="448"/>
+      <c r="M7" s="446"/>
+      <c r="N7" s="447"/>
+      <c r="O7" s="447"/>
+      <c r="P7" s="447"/>
+      <c r="Q7" s="447"/>
+      <c r="R7" s="447"/>
+      <c r="S7" s="447"/>
+      <c r="T7" s="447"/>
+      <c r="U7" s="447"/>
+      <c r="V7" s="447"/>
+      <c r="W7" s="447"/>
+      <c r="X7" s="447"/>
+      <c r="Y7" s="447"/>
+      <c r="Z7" s="447"/>
+      <c r="AA7" s="447"/>
+      <c r="AB7" s="447"/>
+      <c r="AC7" s="447"/>
+      <c r="AD7" s="447"/>
+      <c r="AE7" s="447"/>
+      <c r="AF7" s="447"/>
+      <c r="AG7" s="447"/>
+      <c r="AH7" s="447"/>
+      <c r="AI7" s="447"/>
+      <c r="AJ7" s="447"/>
+      <c r="AK7" s="447"/>
+      <c r="AL7" s="448"/>
       <c r="AM7" s="324"/>
     </row>
     <row r="8" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="458"/>
+      <c r="A8" s="439"/>
       <c r="B8" s="329"/>
       <c r="C8" s="330" t="s">
         <v>12</v>
@@ -10406,44 +10409,44 @@
       <c r="D8" s="332" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="465"/>
-      <c r="F8" s="466"/>
-      <c r="G8" s="466"/>
-      <c r="H8" s="466"/>
-      <c r="I8" s="466"/>
-      <c r="J8" s="466"/>
-      <c r="K8" s="466"/>
-      <c r="L8" s="467"/>
-      <c r="M8" s="465"/>
-      <c r="N8" s="466"/>
-      <c r="O8" s="466"/>
-      <c r="P8" s="466"/>
-      <c r="Q8" s="466"/>
-      <c r="R8" s="466"/>
-      <c r="S8" s="466"/>
-      <c r="T8" s="466"/>
-      <c r="U8" s="466"/>
-      <c r="V8" s="466"/>
-      <c r="W8" s="466"/>
-      <c r="X8" s="466"/>
-      <c r="Y8" s="466"/>
-      <c r="Z8" s="466"/>
-      <c r="AA8" s="466"/>
-      <c r="AB8" s="466"/>
-      <c r="AC8" s="466"/>
-      <c r="AD8" s="466"/>
-      <c r="AE8" s="466"/>
-      <c r="AF8" s="466"/>
-      <c r="AG8" s="466"/>
-      <c r="AH8" s="466"/>
-      <c r="AI8" s="466"/>
-      <c r="AJ8" s="466"/>
-      <c r="AK8" s="466"/>
-      <c r="AL8" s="467"/>
+      <c r="E8" s="446"/>
+      <c r="F8" s="447"/>
+      <c r="G8" s="447"/>
+      <c r="H8" s="447"/>
+      <c r="I8" s="447"/>
+      <c r="J8" s="447"/>
+      <c r="K8" s="447"/>
+      <c r="L8" s="448"/>
+      <c r="M8" s="446"/>
+      <c r="N8" s="447"/>
+      <c r="O8" s="447"/>
+      <c r="P8" s="447"/>
+      <c r="Q8" s="447"/>
+      <c r="R8" s="447"/>
+      <c r="S8" s="447"/>
+      <c r="T8" s="447"/>
+      <c r="U8" s="447"/>
+      <c r="V8" s="447"/>
+      <c r="W8" s="447"/>
+      <c r="X8" s="447"/>
+      <c r="Y8" s="447"/>
+      <c r="Z8" s="447"/>
+      <c r="AA8" s="447"/>
+      <c r="AB8" s="447"/>
+      <c r="AC8" s="447"/>
+      <c r="AD8" s="447"/>
+      <c r="AE8" s="447"/>
+      <c r="AF8" s="447"/>
+      <c r="AG8" s="447"/>
+      <c r="AH8" s="447"/>
+      <c r="AI8" s="447"/>
+      <c r="AJ8" s="447"/>
+      <c r="AK8" s="447"/>
+      <c r="AL8" s="448"/>
       <c r="AM8" s="324"/>
     </row>
     <row r="9" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="458"/>
+      <c r="A9" s="439"/>
       <c r="B9" s="329"/>
       <c r="C9" s="330" t="s">
         <v>319</v>
@@ -10451,44 +10454,44 @@
       <c r="D9" s="332" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="465"/>
-      <c r="F9" s="466"/>
-      <c r="G9" s="466"/>
-      <c r="H9" s="466"/>
-      <c r="I9" s="466"/>
-      <c r="J9" s="466"/>
-      <c r="K9" s="466"/>
-      <c r="L9" s="467"/>
-      <c r="M9" s="465"/>
-      <c r="N9" s="466"/>
-      <c r="O9" s="466"/>
-      <c r="P9" s="466"/>
-      <c r="Q9" s="466"/>
-      <c r="R9" s="466"/>
-      <c r="S9" s="466"/>
-      <c r="T9" s="466"/>
-      <c r="U9" s="466"/>
-      <c r="V9" s="466"/>
-      <c r="W9" s="466"/>
-      <c r="X9" s="466"/>
-      <c r="Y9" s="466"/>
-      <c r="Z9" s="466"/>
-      <c r="AA9" s="466"/>
-      <c r="AB9" s="466"/>
-      <c r="AC9" s="466"/>
-      <c r="AD9" s="466"/>
-      <c r="AE9" s="466"/>
-      <c r="AF9" s="466"/>
-      <c r="AG9" s="466"/>
-      <c r="AH9" s="466"/>
-      <c r="AI9" s="466"/>
-      <c r="AJ9" s="466"/>
-      <c r="AK9" s="466"/>
-      <c r="AL9" s="467"/>
+      <c r="E9" s="446"/>
+      <c r="F9" s="447"/>
+      <c r="G9" s="447"/>
+      <c r="H9" s="447"/>
+      <c r="I9" s="447"/>
+      <c r="J9" s="447"/>
+      <c r="K9" s="447"/>
+      <c r="L9" s="448"/>
+      <c r="M9" s="446"/>
+      <c r="N9" s="447"/>
+      <c r="O9" s="447"/>
+      <c r="P9" s="447"/>
+      <c r="Q9" s="447"/>
+      <c r="R9" s="447"/>
+      <c r="S9" s="447"/>
+      <c r="T9" s="447"/>
+      <c r="U9" s="447"/>
+      <c r="V9" s="447"/>
+      <c r="W9" s="447"/>
+      <c r="X9" s="447"/>
+      <c r="Y9" s="447"/>
+      <c r="Z9" s="447"/>
+      <c r="AA9" s="447"/>
+      <c r="AB9" s="447"/>
+      <c r="AC9" s="447"/>
+      <c r="AD9" s="447"/>
+      <c r="AE9" s="447"/>
+      <c r="AF9" s="447"/>
+      <c r="AG9" s="447"/>
+      <c r="AH9" s="447"/>
+      <c r="AI9" s="447"/>
+      <c r="AJ9" s="447"/>
+      <c r="AK9" s="447"/>
+      <c r="AL9" s="448"/>
       <c r="AM9" s="324"/>
     </row>
     <row r="10" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="458"/>
+      <c r="A10" s="439"/>
       <c r="B10" s="329"/>
       <c r="C10" s="330" t="s">
         <v>177</v>
@@ -10496,44 +10499,44 @@
       <c r="D10" s="332" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="465"/>
-      <c r="F10" s="466"/>
-      <c r="G10" s="466"/>
-      <c r="H10" s="466"/>
-      <c r="I10" s="466"/>
-      <c r="J10" s="466"/>
-      <c r="K10" s="466"/>
-      <c r="L10" s="467"/>
-      <c r="M10" s="465"/>
-      <c r="N10" s="466"/>
-      <c r="O10" s="466"/>
-      <c r="P10" s="466"/>
-      <c r="Q10" s="466"/>
-      <c r="R10" s="466"/>
-      <c r="S10" s="466"/>
-      <c r="T10" s="466"/>
-      <c r="U10" s="466"/>
-      <c r="V10" s="466"/>
-      <c r="W10" s="466"/>
-      <c r="X10" s="466"/>
-      <c r="Y10" s="466"/>
-      <c r="Z10" s="466"/>
-      <c r="AA10" s="466"/>
-      <c r="AB10" s="466"/>
-      <c r="AC10" s="466"/>
-      <c r="AD10" s="466"/>
-      <c r="AE10" s="466"/>
-      <c r="AF10" s="466"/>
-      <c r="AG10" s="466"/>
-      <c r="AH10" s="466"/>
-      <c r="AI10" s="466"/>
-      <c r="AJ10" s="466"/>
-      <c r="AK10" s="466"/>
-      <c r="AL10" s="467"/>
+      <c r="E10" s="446"/>
+      <c r="F10" s="447"/>
+      <c r="G10" s="447"/>
+      <c r="H10" s="447"/>
+      <c r="I10" s="447"/>
+      <c r="J10" s="447"/>
+      <c r="K10" s="447"/>
+      <c r="L10" s="448"/>
+      <c r="M10" s="446"/>
+      <c r="N10" s="447"/>
+      <c r="O10" s="447"/>
+      <c r="P10" s="447"/>
+      <c r="Q10" s="447"/>
+      <c r="R10" s="447"/>
+      <c r="S10" s="447"/>
+      <c r="T10" s="447"/>
+      <c r="U10" s="447"/>
+      <c r="V10" s="447"/>
+      <c r="W10" s="447"/>
+      <c r="X10" s="447"/>
+      <c r="Y10" s="447"/>
+      <c r="Z10" s="447"/>
+      <c r="AA10" s="447"/>
+      <c r="AB10" s="447"/>
+      <c r="AC10" s="447"/>
+      <c r="AD10" s="447"/>
+      <c r="AE10" s="447"/>
+      <c r="AF10" s="447"/>
+      <c r="AG10" s="447"/>
+      <c r="AH10" s="447"/>
+      <c r="AI10" s="447"/>
+      <c r="AJ10" s="447"/>
+      <c r="AK10" s="447"/>
+      <c r="AL10" s="448"/>
       <c r="AM10" s="324"/>
     </row>
     <row r="11" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="458"/>
+      <c r="A11" s="439"/>
       <c r="B11" s="329"/>
       <c r="C11" s="330" t="s">
         <v>16</v>
@@ -10541,44 +10544,44 @@
       <c r="D11" s="332" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="465"/>
-      <c r="F11" s="466"/>
-      <c r="G11" s="466"/>
-      <c r="H11" s="466"/>
-      <c r="I11" s="466"/>
-      <c r="J11" s="466"/>
-      <c r="K11" s="466"/>
-      <c r="L11" s="467"/>
-      <c r="M11" s="465"/>
-      <c r="N11" s="466"/>
-      <c r="O11" s="466"/>
-      <c r="P11" s="466"/>
-      <c r="Q11" s="466"/>
-      <c r="R11" s="466"/>
-      <c r="S11" s="466"/>
-      <c r="T11" s="466"/>
-      <c r="U11" s="466"/>
-      <c r="V11" s="466"/>
-      <c r="W11" s="466"/>
-      <c r="X11" s="466"/>
-      <c r="Y11" s="466"/>
-      <c r="Z11" s="466"/>
-      <c r="AA11" s="466"/>
-      <c r="AB11" s="466"/>
-      <c r="AC11" s="466"/>
-      <c r="AD11" s="466"/>
-      <c r="AE11" s="466"/>
-      <c r="AF11" s="466"/>
-      <c r="AG11" s="466"/>
-      <c r="AH11" s="466"/>
-      <c r="AI11" s="466"/>
-      <c r="AJ11" s="466"/>
-      <c r="AK11" s="466"/>
-      <c r="AL11" s="467"/>
+      <c r="E11" s="446"/>
+      <c r="F11" s="447"/>
+      <c r="G11" s="447"/>
+      <c r="H11" s="447"/>
+      <c r="I11" s="447"/>
+      <c r="J11" s="447"/>
+      <c r="K11" s="447"/>
+      <c r="L11" s="448"/>
+      <c r="M11" s="446"/>
+      <c r="N11" s="447"/>
+      <c r="O11" s="447"/>
+      <c r="P11" s="447"/>
+      <c r="Q11" s="447"/>
+      <c r="R11" s="447"/>
+      <c r="S11" s="447"/>
+      <c r="T11" s="447"/>
+      <c r="U11" s="447"/>
+      <c r="V11" s="447"/>
+      <c r="W11" s="447"/>
+      <c r="X11" s="447"/>
+      <c r="Y11" s="447"/>
+      <c r="Z11" s="447"/>
+      <c r="AA11" s="447"/>
+      <c r="AB11" s="447"/>
+      <c r="AC11" s="447"/>
+      <c r="AD11" s="447"/>
+      <c r="AE11" s="447"/>
+      <c r="AF11" s="447"/>
+      <c r="AG11" s="447"/>
+      <c r="AH11" s="447"/>
+      <c r="AI11" s="447"/>
+      <c r="AJ11" s="447"/>
+      <c r="AK11" s="447"/>
+      <c r="AL11" s="448"/>
       <c r="AM11" s="324"/>
     </row>
     <row r="12" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="458"/>
+      <c r="A12" s="439"/>
       <c r="B12" s="329"/>
       <c r="C12" s="330" t="s">
         <v>17</v>
@@ -10586,44 +10589,44 @@
       <c r="D12" s="332" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="465"/>
-      <c r="F12" s="466"/>
-      <c r="G12" s="466"/>
-      <c r="H12" s="466"/>
-      <c r="I12" s="466"/>
-      <c r="J12" s="466"/>
-      <c r="K12" s="466"/>
-      <c r="L12" s="467"/>
-      <c r="M12" s="465"/>
-      <c r="N12" s="466"/>
-      <c r="O12" s="466"/>
-      <c r="P12" s="466"/>
-      <c r="Q12" s="466"/>
-      <c r="R12" s="466"/>
-      <c r="S12" s="466"/>
-      <c r="T12" s="466"/>
-      <c r="U12" s="466"/>
-      <c r="V12" s="466"/>
-      <c r="W12" s="466"/>
-      <c r="X12" s="466"/>
-      <c r="Y12" s="466"/>
-      <c r="Z12" s="466"/>
-      <c r="AA12" s="466"/>
-      <c r="AB12" s="466"/>
-      <c r="AC12" s="466"/>
-      <c r="AD12" s="466"/>
-      <c r="AE12" s="466"/>
-      <c r="AF12" s="466"/>
-      <c r="AG12" s="466"/>
-      <c r="AH12" s="466"/>
-      <c r="AI12" s="466"/>
-      <c r="AJ12" s="466"/>
-      <c r="AK12" s="466"/>
-      <c r="AL12" s="467"/>
+      <c r="E12" s="446"/>
+      <c r="F12" s="447"/>
+      <c r="G12" s="447"/>
+      <c r="H12" s="447"/>
+      <c r="I12" s="447"/>
+      <c r="J12" s="447"/>
+      <c r="K12" s="447"/>
+      <c r="L12" s="448"/>
+      <c r="M12" s="446"/>
+      <c r="N12" s="447"/>
+      <c r="O12" s="447"/>
+      <c r="P12" s="447"/>
+      <c r="Q12" s="447"/>
+      <c r="R12" s="447"/>
+      <c r="S12" s="447"/>
+      <c r="T12" s="447"/>
+      <c r="U12" s="447"/>
+      <c r="V12" s="447"/>
+      <c r="W12" s="447"/>
+      <c r="X12" s="447"/>
+      <c r="Y12" s="447"/>
+      <c r="Z12" s="447"/>
+      <c r="AA12" s="447"/>
+      <c r="AB12" s="447"/>
+      <c r="AC12" s="447"/>
+      <c r="AD12" s="447"/>
+      <c r="AE12" s="447"/>
+      <c r="AF12" s="447"/>
+      <c r="AG12" s="447"/>
+      <c r="AH12" s="447"/>
+      <c r="AI12" s="447"/>
+      <c r="AJ12" s="447"/>
+      <c r="AK12" s="447"/>
+      <c r="AL12" s="448"/>
       <c r="AM12" s="324"/>
     </row>
     <row r="13" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="458"/>
+      <c r="A13" s="439"/>
       <c r="B13" s="329"/>
       <c r="C13" s="330" t="s">
         <v>19</v>
@@ -10631,44 +10634,44 @@
       <c r="D13" s="332">
         <v>32</v>
       </c>
-      <c r="E13" s="465"/>
-      <c r="F13" s="466"/>
-      <c r="G13" s="466"/>
-      <c r="H13" s="466"/>
-      <c r="I13" s="466"/>
-      <c r="J13" s="466"/>
-      <c r="K13" s="466"/>
-      <c r="L13" s="467"/>
-      <c r="M13" s="465"/>
-      <c r="N13" s="466"/>
-      <c r="O13" s="466"/>
-      <c r="P13" s="466"/>
-      <c r="Q13" s="466"/>
-      <c r="R13" s="466"/>
-      <c r="S13" s="466"/>
-      <c r="T13" s="466"/>
-      <c r="U13" s="466"/>
-      <c r="V13" s="466"/>
-      <c r="W13" s="466"/>
-      <c r="X13" s="466"/>
-      <c r="Y13" s="466"/>
-      <c r="Z13" s="466"/>
-      <c r="AA13" s="466"/>
-      <c r="AB13" s="466"/>
-      <c r="AC13" s="466"/>
-      <c r="AD13" s="466"/>
-      <c r="AE13" s="466"/>
-      <c r="AF13" s="466"/>
-      <c r="AG13" s="466"/>
-      <c r="AH13" s="466"/>
-      <c r="AI13" s="466"/>
-      <c r="AJ13" s="466"/>
-      <c r="AK13" s="466"/>
-      <c r="AL13" s="467"/>
+      <c r="E13" s="446"/>
+      <c r="F13" s="447"/>
+      <c r="G13" s="447"/>
+      <c r="H13" s="447"/>
+      <c r="I13" s="447"/>
+      <c r="J13" s="447"/>
+      <c r="K13" s="447"/>
+      <c r="L13" s="448"/>
+      <c r="M13" s="446"/>
+      <c r="N13" s="447"/>
+      <c r="O13" s="447"/>
+      <c r="P13" s="447"/>
+      <c r="Q13" s="447"/>
+      <c r="R13" s="447"/>
+      <c r="S13" s="447"/>
+      <c r="T13" s="447"/>
+      <c r="U13" s="447"/>
+      <c r="V13" s="447"/>
+      <c r="W13" s="447"/>
+      <c r="X13" s="447"/>
+      <c r="Y13" s="447"/>
+      <c r="Z13" s="447"/>
+      <c r="AA13" s="447"/>
+      <c r="AB13" s="447"/>
+      <c r="AC13" s="447"/>
+      <c r="AD13" s="447"/>
+      <c r="AE13" s="447"/>
+      <c r="AF13" s="447"/>
+      <c r="AG13" s="447"/>
+      <c r="AH13" s="447"/>
+      <c r="AI13" s="447"/>
+      <c r="AJ13" s="447"/>
+      <c r="AK13" s="447"/>
+      <c r="AL13" s="448"/>
       <c r="AM13" s="324"/>
     </row>
     <row r="14" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="458"/>
+      <c r="A14" s="439"/>
       <c r="B14" s="329"/>
       <c r="C14" s="330" t="s">
         <v>20</v>
@@ -10676,44 +10679,44 @@
       <c r="D14" s="332">
         <v>32</v>
       </c>
-      <c r="E14" s="465"/>
-      <c r="F14" s="466"/>
-      <c r="G14" s="466"/>
-      <c r="H14" s="466"/>
-      <c r="I14" s="466"/>
-      <c r="J14" s="466"/>
-      <c r="K14" s="466"/>
-      <c r="L14" s="467"/>
-      <c r="M14" s="465"/>
-      <c r="N14" s="466"/>
-      <c r="O14" s="466"/>
-      <c r="P14" s="466"/>
-      <c r="Q14" s="466"/>
-      <c r="R14" s="466"/>
-      <c r="S14" s="466"/>
-      <c r="T14" s="466"/>
-      <c r="U14" s="466"/>
-      <c r="V14" s="466"/>
-      <c r="W14" s="466"/>
-      <c r="X14" s="466"/>
-      <c r="Y14" s="466"/>
-      <c r="Z14" s="466"/>
-      <c r="AA14" s="466"/>
-      <c r="AB14" s="466"/>
-      <c r="AC14" s="466"/>
-      <c r="AD14" s="466"/>
-      <c r="AE14" s="466"/>
-      <c r="AF14" s="466"/>
-      <c r="AG14" s="466"/>
-      <c r="AH14" s="466"/>
-      <c r="AI14" s="466"/>
-      <c r="AJ14" s="466"/>
-      <c r="AK14" s="466"/>
-      <c r="AL14" s="467"/>
+      <c r="E14" s="446"/>
+      <c r="F14" s="447"/>
+      <c r="G14" s="447"/>
+      <c r="H14" s="447"/>
+      <c r="I14" s="447"/>
+      <c r="J14" s="447"/>
+      <c r="K14" s="447"/>
+      <c r="L14" s="448"/>
+      <c r="M14" s="446"/>
+      <c r="N14" s="447"/>
+      <c r="O14" s="447"/>
+      <c r="P14" s="447"/>
+      <c r="Q14" s="447"/>
+      <c r="R14" s="447"/>
+      <c r="S14" s="447"/>
+      <c r="T14" s="447"/>
+      <c r="U14" s="447"/>
+      <c r="V14" s="447"/>
+      <c r="W14" s="447"/>
+      <c r="X14" s="447"/>
+      <c r="Y14" s="447"/>
+      <c r="Z14" s="447"/>
+      <c r="AA14" s="447"/>
+      <c r="AB14" s="447"/>
+      <c r="AC14" s="447"/>
+      <c r="AD14" s="447"/>
+      <c r="AE14" s="447"/>
+      <c r="AF14" s="447"/>
+      <c r="AG14" s="447"/>
+      <c r="AH14" s="447"/>
+      <c r="AI14" s="447"/>
+      <c r="AJ14" s="447"/>
+      <c r="AK14" s="447"/>
+      <c r="AL14" s="448"/>
       <c r="AM14" s="324"/>
     </row>
     <row r="15" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="458"/>
+      <c r="A15" s="439"/>
       <c r="B15" s="329"/>
       <c r="C15" s="330" t="s">
         <v>21</v>
@@ -10721,44 +10724,44 @@
       <c r="D15" s="332" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="465"/>
-      <c r="F15" s="466"/>
-      <c r="G15" s="466"/>
-      <c r="H15" s="466"/>
-      <c r="I15" s="466"/>
-      <c r="J15" s="466"/>
-      <c r="K15" s="466"/>
-      <c r="L15" s="467"/>
-      <c r="M15" s="465"/>
-      <c r="N15" s="466"/>
-      <c r="O15" s="466"/>
-      <c r="P15" s="466"/>
-      <c r="Q15" s="466"/>
-      <c r="R15" s="466"/>
-      <c r="S15" s="466"/>
-      <c r="T15" s="466"/>
-      <c r="U15" s="466"/>
-      <c r="V15" s="466"/>
-      <c r="W15" s="466"/>
-      <c r="X15" s="466"/>
-      <c r="Y15" s="466"/>
-      <c r="Z15" s="466"/>
-      <c r="AA15" s="466"/>
-      <c r="AB15" s="466"/>
-      <c r="AC15" s="466"/>
-      <c r="AD15" s="466"/>
-      <c r="AE15" s="466"/>
-      <c r="AF15" s="466"/>
-      <c r="AG15" s="466"/>
-      <c r="AH15" s="466"/>
-      <c r="AI15" s="466"/>
-      <c r="AJ15" s="466"/>
-      <c r="AK15" s="466"/>
-      <c r="AL15" s="467"/>
+      <c r="E15" s="446"/>
+      <c r="F15" s="447"/>
+      <c r="G15" s="447"/>
+      <c r="H15" s="447"/>
+      <c r="I15" s="447"/>
+      <c r="J15" s="447"/>
+      <c r="K15" s="447"/>
+      <c r="L15" s="448"/>
+      <c r="M15" s="446"/>
+      <c r="N15" s="447"/>
+      <c r="O15" s="447"/>
+      <c r="P15" s="447"/>
+      <c r="Q15" s="447"/>
+      <c r="R15" s="447"/>
+      <c r="S15" s="447"/>
+      <c r="T15" s="447"/>
+      <c r="U15" s="447"/>
+      <c r="V15" s="447"/>
+      <c r="W15" s="447"/>
+      <c r="X15" s="447"/>
+      <c r="Y15" s="447"/>
+      <c r="Z15" s="447"/>
+      <c r="AA15" s="447"/>
+      <c r="AB15" s="447"/>
+      <c r="AC15" s="447"/>
+      <c r="AD15" s="447"/>
+      <c r="AE15" s="447"/>
+      <c r="AF15" s="447"/>
+      <c r="AG15" s="447"/>
+      <c r="AH15" s="447"/>
+      <c r="AI15" s="447"/>
+      <c r="AJ15" s="447"/>
+      <c r="AK15" s="447"/>
+      <c r="AL15" s="448"/>
       <c r="AM15" s="324"/>
     </row>
     <row r="16" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="458"/>
+      <c r="A16" s="439"/>
       <c r="B16" s="329" t="s">
         <v>22</v>
       </c>
@@ -10768,44 +10771,44 @@
       <c r="D16" s="331" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="465"/>
-      <c r="F16" s="466"/>
-      <c r="G16" s="466"/>
-      <c r="H16" s="466"/>
-      <c r="I16" s="466"/>
-      <c r="J16" s="466"/>
-      <c r="K16" s="466"/>
-      <c r="L16" s="467"/>
-      <c r="M16" s="465"/>
-      <c r="N16" s="466"/>
-      <c r="O16" s="466"/>
-      <c r="P16" s="466"/>
-      <c r="Q16" s="466"/>
-      <c r="R16" s="466"/>
-      <c r="S16" s="466"/>
-      <c r="T16" s="466"/>
-      <c r="U16" s="466"/>
-      <c r="V16" s="466"/>
-      <c r="W16" s="466"/>
-      <c r="X16" s="466"/>
-      <c r="Y16" s="466"/>
-      <c r="Z16" s="466"/>
-      <c r="AA16" s="466"/>
-      <c r="AB16" s="466"/>
-      <c r="AC16" s="466"/>
-      <c r="AD16" s="466"/>
-      <c r="AE16" s="466"/>
-      <c r="AF16" s="466"/>
-      <c r="AG16" s="466"/>
-      <c r="AH16" s="466"/>
-      <c r="AI16" s="466"/>
-      <c r="AJ16" s="466"/>
-      <c r="AK16" s="466"/>
-      <c r="AL16" s="467"/>
+      <c r="E16" s="446"/>
+      <c r="F16" s="447"/>
+      <c r="G16" s="447"/>
+      <c r="H16" s="447"/>
+      <c r="I16" s="447"/>
+      <c r="J16" s="447"/>
+      <c r="K16" s="447"/>
+      <c r="L16" s="448"/>
+      <c r="M16" s="446"/>
+      <c r="N16" s="447"/>
+      <c r="O16" s="447"/>
+      <c r="P16" s="447"/>
+      <c r="Q16" s="447"/>
+      <c r="R16" s="447"/>
+      <c r="S16" s="447"/>
+      <c r="T16" s="447"/>
+      <c r="U16" s="447"/>
+      <c r="V16" s="447"/>
+      <c r="W16" s="447"/>
+      <c r="X16" s="447"/>
+      <c r="Y16" s="447"/>
+      <c r="Z16" s="447"/>
+      <c r="AA16" s="447"/>
+      <c r="AB16" s="447"/>
+      <c r="AC16" s="447"/>
+      <c r="AD16" s="447"/>
+      <c r="AE16" s="447"/>
+      <c r="AF16" s="447"/>
+      <c r="AG16" s="447"/>
+      <c r="AH16" s="447"/>
+      <c r="AI16" s="447"/>
+      <c r="AJ16" s="447"/>
+      <c r="AK16" s="447"/>
+      <c r="AL16" s="448"/>
       <c r="AM16" s="324"/>
     </row>
     <row r="17" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="458"/>
+      <c r="A17" s="439"/>
       <c r="B17" s="329"/>
       <c r="C17" s="330" t="s">
         <v>26</v>
@@ -10813,44 +10816,44 @@
       <c r="D17" s="331">
         <v>128</v>
       </c>
-      <c r="E17" s="465"/>
-      <c r="F17" s="466"/>
-      <c r="G17" s="466"/>
-      <c r="H17" s="466"/>
-      <c r="I17" s="466"/>
-      <c r="J17" s="466"/>
-      <c r="K17" s="466"/>
-      <c r="L17" s="467"/>
-      <c r="M17" s="465"/>
-      <c r="N17" s="466"/>
-      <c r="O17" s="466"/>
-      <c r="P17" s="466"/>
-      <c r="Q17" s="466"/>
-      <c r="R17" s="466"/>
-      <c r="S17" s="466"/>
-      <c r="T17" s="466"/>
-      <c r="U17" s="466"/>
-      <c r="V17" s="466"/>
-      <c r="W17" s="466"/>
-      <c r="X17" s="466"/>
-      <c r="Y17" s="466"/>
-      <c r="Z17" s="466"/>
-      <c r="AA17" s="466"/>
-      <c r="AB17" s="466"/>
-      <c r="AC17" s="466"/>
-      <c r="AD17" s="466"/>
-      <c r="AE17" s="466"/>
-      <c r="AF17" s="466"/>
-      <c r="AG17" s="466"/>
-      <c r="AH17" s="466"/>
-      <c r="AI17" s="466"/>
-      <c r="AJ17" s="466"/>
-      <c r="AK17" s="466"/>
-      <c r="AL17" s="467"/>
+      <c r="E17" s="446"/>
+      <c r="F17" s="447"/>
+      <c r="G17" s="447"/>
+      <c r="H17" s="447"/>
+      <c r="I17" s="447"/>
+      <c r="J17" s="447"/>
+      <c r="K17" s="447"/>
+      <c r="L17" s="448"/>
+      <c r="M17" s="446"/>
+      <c r="N17" s="447"/>
+      <c r="O17" s="447"/>
+      <c r="P17" s="447"/>
+      <c r="Q17" s="447"/>
+      <c r="R17" s="447"/>
+      <c r="S17" s="447"/>
+      <c r="T17" s="447"/>
+      <c r="U17" s="447"/>
+      <c r="V17" s="447"/>
+      <c r="W17" s="447"/>
+      <c r="X17" s="447"/>
+      <c r="Y17" s="447"/>
+      <c r="Z17" s="447"/>
+      <c r="AA17" s="447"/>
+      <c r="AB17" s="447"/>
+      <c r="AC17" s="447"/>
+      <c r="AD17" s="447"/>
+      <c r="AE17" s="447"/>
+      <c r="AF17" s="447"/>
+      <c r="AG17" s="447"/>
+      <c r="AH17" s="447"/>
+      <c r="AI17" s="447"/>
+      <c r="AJ17" s="447"/>
+      <c r="AK17" s="447"/>
+      <c r="AL17" s="448"/>
       <c r="AM17" s="324"/>
     </row>
     <row r="18" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="458"/>
+      <c r="A18" s="439"/>
       <c r="B18" s="329"/>
       <c r="C18" s="330" t="s">
         <v>27</v>
@@ -10858,44 +10861,44 @@
       <c r="D18" s="331" t="s">
         <v>317</v>
       </c>
-      <c r="E18" s="465"/>
-      <c r="F18" s="466"/>
-      <c r="G18" s="466"/>
-      <c r="H18" s="466"/>
-      <c r="I18" s="466"/>
-      <c r="J18" s="466"/>
-      <c r="K18" s="466"/>
-      <c r="L18" s="467"/>
-      <c r="M18" s="465"/>
-      <c r="N18" s="466"/>
-      <c r="O18" s="466"/>
-      <c r="P18" s="466"/>
-      <c r="Q18" s="466"/>
-      <c r="R18" s="466"/>
-      <c r="S18" s="466"/>
-      <c r="T18" s="466"/>
-      <c r="U18" s="466"/>
-      <c r="V18" s="466"/>
-      <c r="W18" s="466"/>
-      <c r="X18" s="466"/>
-      <c r="Y18" s="466"/>
-      <c r="Z18" s="466"/>
-      <c r="AA18" s="466"/>
-      <c r="AB18" s="466"/>
-      <c r="AC18" s="466"/>
-      <c r="AD18" s="466"/>
-      <c r="AE18" s="466"/>
-      <c r="AF18" s="466"/>
-      <c r="AG18" s="466"/>
-      <c r="AH18" s="466"/>
-      <c r="AI18" s="466"/>
-      <c r="AJ18" s="466"/>
-      <c r="AK18" s="466"/>
-      <c r="AL18" s="467"/>
+      <c r="E18" s="446"/>
+      <c r="F18" s="447"/>
+      <c r="G18" s="447"/>
+      <c r="H18" s="447"/>
+      <c r="I18" s="447"/>
+      <c r="J18" s="447"/>
+      <c r="K18" s="447"/>
+      <c r="L18" s="448"/>
+      <c r="M18" s="446"/>
+      <c r="N18" s="447"/>
+      <c r="O18" s="447"/>
+      <c r="P18" s="447"/>
+      <c r="Q18" s="447"/>
+      <c r="R18" s="447"/>
+      <c r="S18" s="447"/>
+      <c r="T18" s="447"/>
+      <c r="U18" s="447"/>
+      <c r="V18" s="447"/>
+      <c r="W18" s="447"/>
+      <c r="X18" s="447"/>
+      <c r="Y18" s="447"/>
+      <c r="Z18" s="447"/>
+      <c r="AA18" s="447"/>
+      <c r="AB18" s="447"/>
+      <c r="AC18" s="447"/>
+      <c r="AD18" s="447"/>
+      <c r="AE18" s="447"/>
+      <c r="AF18" s="447"/>
+      <c r="AG18" s="447"/>
+      <c r="AH18" s="447"/>
+      <c r="AI18" s="447"/>
+      <c r="AJ18" s="447"/>
+      <c r="AK18" s="447"/>
+      <c r="AL18" s="448"/>
       <c r="AM18" s="324"/>
     </row>
     <row r="19" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="458"/>
+      <c r="A19" s="439"/>
       <c r="B19" s="329"/>
       <c r="C19" s="330" t="s">
         <v>28</v>
@@ -10903,44 +10906,44 @@
       <c r="D19" s="331" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="465"/>
-      <c r="F19" s="466"/>
-      <c r="G19" s="466"/>
-      <c r="H19" s="466"/>
-      <c r="I19" s="466"/>
-      <c r="J19" s="466"/>
-      <c r="K19" s="466"/>
-      <c r="L19" s="467"/>
-      <c r="M19" s="465"/>
-      <c r="N19" s="466"/>
-      <c r="O19" s="466"/>
-      <c r="P19" s="466"/>
-      <c r="Q19" s="466"/>
-      <c r="R19" s="466"/>
-      <c r="S19" s="466"/>
-      <c r="T19" s="466"/>
-      <c r="U19" s="466"/>
-      <c r="V19" s="466"/>
-      <c r="W19" s="466"/>
-      <c r="X19" s="466"/>
-      <c r="Y19" s="466"/>
-      <c r="Z19" s="466"/>
-      <c r="AA19" s="466"/>
-      <c r="AB19" s="466"/>
-      <c r="AC19" s="466"/>
-      <c r="AD19" s="466"/>
-      <c r="AE19" s="466"/>
-      <c r="AF19" s="466"/>
-      <c r="AG19" s="466"/>
-      <c r="AH19" s="466"/>
-      <c r="AI19" s="466"/>
-      <c r="AJ19" s="466"/>
-      <c r="AK19" s="466"/>
-      <c r="AL19" s="467"/>
+      <c r="E19" s="446"/>
+      <c r="F19" s="447"/>
+      <c r="G19" s="447"/>
+      <c r="H19" s="447"/>
+      <c r="I19" s="447"/>
+      <c r="J19" s="447"/>
+      <c r="K19" s="447"/>
+      <c r="L19" s="448"/>
+      <c r="M19" s="446"/>
+      <c r="N19" s="447"/>
+      <c r="O19" s="447"/>
+      <c r="P19" s="447"/>
+      <c r="Q19" s="447"/>
+      <c r="R19" s="447"/>
+      <c r="S19" s="447"/>
+      <c r="T19" s="447"/>
+      <c r="U19" s="447"/>
+      <c r="V19" s="447"/>
+      <c r="W19" s="447"/>
+      <c r="X19" s="447"/>
+      <c r="Y19" s="447"/>
+      <c r="Z19" s="447"/>
+      <c r="AA19" s="447"/>
+      <c r="AB19" s="447"/>
+      <c r="AC19" s="447"/>
+      <c r="AD19" s="447"/>
+      <c r="AE19" s="447"/>
+      <c r="AF19" s="447"/>
+      <c r="AG19" s="447"/>
+      <c r="AH19" s="447"/>
+      <c r="AI19" s="447"/>
+      <c r="AJ19" s="447"/>
+      <c r="AK19" s="447"/>
+      <c r="AL19" s="448"/>
       <c r="AM19" s="324"/>
     </row>
     <row r="20" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="458"/>
+      <c r="A20" s="439"/>
       <c r="B20" s="329" t="s">
         <v>97</v>
       </c>
@@ -10950,44 +10953,44 @@
       <c r="D20" s="331" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="465"/>
-      <c r="F20" s="466"/>
-      <c r="G20" s="466"/>
-      <c r="H20" s="466"/>
-      <c r="I20" s="466"/>
-      <c r="J20" s="466"/>
-      <c r="K20" s="466"/>
-      <c r="L20" s="467"/>
-      <c r="M20" s="465"/>
-      <c r="N20" s="466"/>
-      <c r="O20" s="466"/>
-      <c r="P20" s="466"/>
-      <c r="Q20" s="466"/>
-      <c r="R20" s="466"/>
-      <c r="S20" s="466"/>
-      <c r="T20" s="466"/>
-      <c r="U20" s="466"/>
-      <c r="V20" s="466"/>
-      <c r="W20" s="466"/>
-      <c r="X20" s="466"/>
-      <c r="Y20" s="466"/>
-      <c r="Z20" s="466"/>
-      <c r="AA20" s="466"/>
-      <c r="AB20" s="466"/>
-      <c r="AC20" s="466"/>
-      <c r="AD20" s="466"/>
-      <c r="AE20" s="466"/>
-      <c r="AF20" s="466"/>
-      <c r="AG20" s="466"/>
-      <c r="AH20" s="466"/>
-      <c r="AI20" s="466"/>
-      <c r="AJ20" s="466"/>
-      <c r="AK20" s="466"/>
-      <c r="AL20" s="467"/>
+      <c r="E20" s="446"/>
+      <c r="F20" s="447"/>
+      <c r="G20" s="447"/>
+      <c r="H20" s="447"/>
+      <c r="I20" s="447"/>
+      <c r="J20" s="447"/>
+      <c r="K20" s="447"/>
+      <c r="L20" s="448"/>
+      <c r="M20" s="446"/>
+      <c r="N20" s="447"/>
+      <c r="O20" s="447"/>
+      <c r="P20" s="447"/>
+      <c r="Q20" s="447"/>
+      <c r="R20" s="447"/>
+      <c r="S20" s="447"/>
+      <c r="T20" s="447"/>
+      <c r="U20" s="447"/>
+      <c r="V20" s="447"/>
+      <c r="W20" s="447"/>
+      <c r="X20" s="447"/>
+      <c r="Y20" s="447"/>
+      <c r="Z20" s="447"/>
+      <c r="AA20" s="447"/>
+      <c r="AB20" s="447"/>
+      <c r="AC20" s="447"/>
+      <c r="AD20" s="447"/>
+      <c r="AE20" s="447"/>
+      <c r="AF20" s="447"/>
+      <c r="AG20" s="447"/>
+      <c r="AH20" s="447"/>
+      <c r="AI20" s="447"/>
+      <c r="AJ20" s="447"/>
+      <c r="AK20" s="447"/>
+      <c r="AL20" s="448"/>
       <c r="AM20" s="324"/>
     </row>
     <row r="21" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="458"/>
+      <c r="A21" s="439"/>
       <c r="B21" s="329" t="s">
         <v>45</v>
       </c>
@@ -10997,44 +11000,44 @@
       <c r="D21" s="331" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="465"/>
-      <c r="F21" s="466"/>
-      <c r="G21" s="466"/>
-      <c r="H21" s="466"/>
-      <c r="I21" s="466"/>
-      <c r="J21" s="466"/>
-      <c r="K21" s="466"/>
-      <c r="L21" s="467"/>
-      <c r="M21" s="465"/>
-      <c r="N21" s="466"/>
-      <c r="O21" s="466"/>
-      <c r="P21" s="466"/>
-      <c r="Q21" s="466"/>
-      <c r="R21" s="466"/>
-      <c r="S21" s="466"/>
-      <c r="T21" s="466"/>
-      <c r="U21" s="466"/>
-      <c r="V21" s="466"/>
-      <c r="W21" s="466"/>
-      <c r="X21" s="466"/>
-      <c r="Y21" s="466"/>
-      <c r="Z21" s="466"/>
-      <c r="AA21" s="466"/>
-      <c r="AB21" s="466"/>
-      <c r="AC21" s="466"/>
-      <c r="AD21" s="466"/>
-      <c r="AE21" s="466"/>
-      <c r="AF21" s="466"/>
-      <c r="AG21" s="466"/>
-      <c r="AH21" s="466"/>
-      <c r="AI21" s="466"/>
-      <c r="AJ21" s="466"/>
-      <c r="AK21" s="466"/>
-      <c r="AL21" s="467"/>
+      <c r="E21" s="446"/>
+      <c r="F21" s="447"/>
+      <c r="G21" s="447"/>
+      <c r="H21" s="447"/>
+      <c r="I21" s="447"/>
+      <c r="J21" s="447"/>
+      <c r="K21" s="447"/>
+      <c r="L21" s="448"/>
+      <c r="M21" s="446"/>
+      <c r="N21" s="447"/>
+      <c r="O21" s="447"/>
+      <c r="P21" s="447"/>
+      <c r="Q21" s="447"/>
+      <c r="R21" s="447"/>
+      <c r="S21" s="447"/>
+      <c r="T21" s="447"/>
+      <c r="U21" s="447"/>
+      <c r="V21" s="447"/>
+      <c r="W21" s="447"/>
+      <c r="X21" s="447"/>
+      <c r="Y21" s="447"/>
+      <c r="Z21" s="447"/>
+      <c r="AA21" s="447"/>
+      <c r="AB21" s="447"/>
+      <c r="AC21" s="447"/>
+      <c r="AD21" s="447"/>
+      <c r="AE21" s="447"/>
+      <c r="AF21" s="447"/>
+      <c r="AG21" s="447"/>
+      <c r="AH21" s="447"/>
+      <c r="AI21" s="447"/>
+      <c r="AJ21" s="447"/>
+      <c r="AK21" s="447"/>
+      <c r="AL21" s="448"/>
       <c r="AM21" s="325"/>
     </row>
     <row r="22" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="458"/>
+      <c r="A22" s="439"/>
       <c r="B22" s="329"/>
       <c r="C22" s="330" t="s">
         <v>318</v>
@@ -11042,44 +11045,44 @@
       <c r="D22" s="331" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="465"/>
-      <c r="F22" s="466"/>
-      <c r="G22" s="466"/>
-      <c r="H22" s="466"/>
-      <c r="I22" s="466"/>
-      <c r="J22" s="466"/>
-      <c r="K22" s="466"/>
-      <c r="L22" s="467"/>
-      <c r="M22" s="465"/>
-      <c r="N22" s="466"/>
-      <c r="O22" s="466"/>
-      <c r="P22" s="466"/>
-      <c r="Q22" s="466"/>
-      <c r="R22" s="466"/>
-      <c r="S22" s="466"/>
-      <c r="T22" s="466"/>
-      <c r="U22" s="466"/>
-      <c r="V22" s="466"/>
-      <c r="W22" s="466"/>
-      <c r="X22" s="466"/>
-      <c r="Y22" s="466"/>
-      <c r="Z22" s="466"/>
-      <c r="AA22" s="466"/>
-      <c r="AB22" s="466"/>
-      <c r="AC22" s="466"/>
-      <c r="AD22" s="466"/>
-      <c r="AE22" s="466"/>
-      <c r="AF22" s="466"/>
-      <c r="AG22" s="466"/>
-      <c r="AH22" s="466"/>
-      <c r="AI22" s="466"/>
-      <c r="AJ22" s="466"/>
-      <c r="AK22" s="466"/>
-      <c r="AL22" s="467"/>
+      <c r="E22" s="446"/>
+      <c r="F22" s="447"/>
+      <c r="G22" s="447"/>
+      <c r="H22" s="447"/>
+      <c r="I22" s="447"/>
+      <c r="J22" s="447"/>
+      <c r="K22" s="447"/>
+      <c r="L22" s="448"/>
+      <c r="M22" s="446"/>
+      <c r="N22" s="447"/>
+      <c r="O22" s="447"/>
+      <c r="P22" s="447"/>
+      <c r="Q22" s="447"/>
+      <c r="R22" s="447"/>
+      <c r="S22" s="447"/>
+      <c r="T22" s="447"/>
+      <c r="U22" s="447"/>
+      <c r="V22" s="447"/>
+      <c r="W22" s="447"/>
+      <c r="X22" s="447"/>
+      <c r="Y22" s="447"/>
+      <c r="Z22" s="447"/>
+      <c r="AA22" s="447"/>
+      <c r="AB22" s="447"/>
+      <c r="AC22" s="447"/>
+      <c r="AD22" s="447"/>
+      <c r="AE22" s="447"/>
+      <c r="AF22" s="447"/>
+      <c r="AG22" s="447"/>
+      <c r="AH22" s="447"/>
+      <c r="AI22" s="447"/>
+      <c r="AJ22" s="447"/>
+      <c r="AK22" s="447"/>
+      <c r="AL22" s="448"/>
       <c r="AM22" s="325"/>
     </row>
     <row r="23" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="458"/>
+      <c r="A23" s="439"/>
       <c r="B23" s="329"/>
       <c r="C23" s="330" t="s">
         <v>290</v>
@@ -11087,44 +11090,44 @@
       <c r="D23" s="331" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="465"/>
-      <c r="F23" s="466"/>
-      <c r="G23" s="466"/>
-      <c r="H23" s="466"/>
-      <c r="I23" s="466"/>
-      <c r="J23" s="466"/>
-      <c r="K23" s="466"/>
-      <c r="L23" s="467"/>
-      <c r="M23" s="465"/>
-      <c r="N23" s="466"/>
-      <c r="O23" s="466"/>
-      <c r="P23" s="466"/>
-      <c r="Q23" s="466"/>
-      <c r="R23" s="466"/>
-      <c r="S23" s="466"/>
-      <c r="T23" s="466"/>
-      <c r="U23" s="466"/>
-      <c r="V23" s="466"/>
-      <c r="W23" s="466"/>
-      <c r="X23" s="466"/>
-      <c r="Y23" s="466"/>
-      <c r="Z23" s="466"/>
-      <c r="AA23" s="466"/>
-      <c r="AB23" s="466"/>
-      <c r="AC23" s="466"/>
-      <c r="AD23" s="466"/>
-      <c r="AE23" s="466"/>
-      <c r="AF23" s="466"/>
-      <c r="AG23" s="466"/>
-      <c r="AH23" s="466"/>
-      <c r="AI23" s="466"/>
-      <c r="AJ23" s="466"/>
-      <c r="AK23" s="466"/>
-      <c r="AL23" s="467"/>
+      <c r="E23" s="446"/>
+      <c r="F23" s="447"/>
+      <c r="G23" s="447"/>
+      <c r="H23" s="447"/>
+      <c r="I23" s="447"/>
+      <c r="J23" s="447"/>
+      <c r="K23" s="447"/>
+      <c r="L23" s="448"/>
+      <c r="M23" s="446"/>
+      <c r="N23" s="447"/>
+      <c r="O23" s="447"/>
+      <c r="P23" s="447"/>
+      <c r="Q23" s="447"/>
+      <c r="R23" s="447"/>
+      <c r="S23" s="447"/>
+      <c r="T23" s="447"/>
+      <c r="U23" s="447"/>
+      <c r="V23" s="447"/>
+      <c r="W23" s="447"/>
+      <c r="X23" s="447"/>
+      <c r="Y23" s="447"/>
+      <c r="Z23" s="447"/>
+      <c r="AA23" s="447"/>
+      <c r="AB23" s="447"/>
+      <c r="AC23" s="447"/>
+      <c r="AD23" s="447"/>
+      <c r="AE23" s="447"/>
+      <c r="AF23" s="447"/>
+      <c r="AG23" s="447"/>
+      <c r="AH23" s="447"/>
+      <c r="AI23" s="447"/>
+      <c r="AJ23" s="447"/>
+      <c r="AK23" s="447"/>
+      <c r="AL23" s="448"/>
       <c r="AM23" s="325"/>
     </row>
     <row r="24" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="458"/>
+      <c r="A24" s="439"/>
       <c r="B24" s="329"/>
       <c r="C24" s="330" t="s">
         <v>184</v>
@@ -11132,44 +11135,44 @@
       <c r="D24" s="331" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="465"/>
-      <c r="F24" s="466"/>
-      <c r="G24" s="466"/>
-      <c r="H24" s="466"/>
-      <c r="I24" s="466"/>
-      <c r="J24" s="466"/>
-      <c r="K24" s="466"/>
-      <c r="L24" s="467"/>
-      <c r="M24" s="465"/>
-      <c r="N24" s="466"/>
-      <c r="O24" s="466"/>
-      <c r="P24" s="466"/>
-      <c r="Q24" s="466"/>
-      <c r="R24" s="466"/>
-      <c r="S24" s="466"/>
-      <c r="T24" s="466"/>
-      <c r="U24" s="466"/>
-      <c r="V24" s="466"/>
-      <c r="W24" s="466"/>
-      <c r="X24" s="466"/>
-      <c r="Y24" s="466"/>
-      <c r="Z24" s="466"/>
-      <c r="AA24" s="466"/>
-      <c r="AB24" s="466"/>
-      <c r="AC24" s="466"/>
-      <c r="AD24" s="466"/>
-      <c r="AE24" s="466"/>
-      <c r="AF24" s="466"/>
-      <c r="AG24" s="466"/>
-      <c r="AH24" s="466"/>
-      <c r="AI24" s="466"/>
-      <c r="AJ24" s="466"/>
-      <c r="AK24" s="466"/>
-      <c r="AL24" s="467"/>
+      <c r="E24" s="446"/>
+      <c r="F24" s="447"/>
+      <c r="G24" s="447"/>
+      <c r="H24" s="447"/>
+      <c r="I24" s="447"/>
+      <c r="J24" s="447"/>
+      <c r="K24" s="447"/>
+      <c r="L24" s="448"/>
+      <c r="M24" s="446"/>
+      <c r="N24" s="447"/>
+      <c r="O24" s="447"/>
+      <c r="P24" s="447"/>
+      <c r="Q24" s="447"/>
+      <c r="R24" s="447"/>
+      <c r="S24" s="447"/>
+      <c r="T24" s="447"/>
+      <c r="U24" s="447"/>
+      <c r="V24" s="447"/>
+      <c r="W24" s="447"/>
+      <c r="X24" s="447"/>
+      <c r="Y24" s="447"/>
+      <c r="Z24" s="447"/>
+      <c r="AA24" s="447"/>
+      <c r="AB24" s="447"/>
+      <c r="AC24" s="447"/>
+      <c r="AD24" s="447"/>
+      <c r="AE24" s="447"/>
+      <c r="AF24" s="447"/>
+      <c r="AG24" s="447"/>
+      <c r="AH24" s="447"/>
+      <c r="AI24" s="447"/>
+      <c r="AJ24" s="447"/>
+      <c r="AK24" s="447"/>
+      <c r="AL24" s="448"/>
       <c r="AM24" s="325"/>
     </row>
     <row r="25" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="458"/>
+      <c r="A25" s="439"/>
       <c r="B25" s="329"/>
       <c r="C25" s="330" t="s">
         <v>72</v>
@@ -11177,44 +11180,44 @@
       <c r="D25" s="331" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="465"/>
-      <c r="F25" s="466"/>
-      <c r="G25" s="466"/>
-      <c r="H25" s="466"/>
-      <c r="I25" s="466"/>
-      <c r="J25" s="466"/>
-      <c r="K25" s="466"/>
-      <c r="L25" s="467"/>
-      <c r="M25" s="465"/>
-      <c r="N25" s="466"/>
-      <c r="O25" s="466"/>
-      <c r="P25" s="466"/>
-      <c r="Q25" s="466"/>
-      <c r="R25" s="466"/>
-      <c r="S25" s="466"/>
-      <c r="T25" s="466"/>
-      <c r="U25" s="466"/>
-      <c r="V25" s="466"/>
-      <c r="W25" s="466"/>
-      <c r="X25" s="466"/>
-      <c r="Y25" s="466"/>
-      <c r="Z25" s="466"/>
-      <c r="AA25" s="466"/>
-      <c r="AB25" s="466"/>
-      <c r="AC25" s="466"/>
-      <c r="AD25" s="466"/>
-      <c r="AE25" s="466"/>
-      <c r="AF25" s="466"/>
-      <c r="AG25" s="466"/>
-      <c r="AH25" s="466"/>
-      <c r="AI25" s="466"/>
-      <c r="AJ25" s="466"/>
-      <c r="AK25" s="466"/>
-      <c r="AL25" s="467"/>
+      <c r="E25" s="446"/>
+      <c r="F25" s="447"/>
+      <c r="G25" s="447"/>
+      <c r="H25" s="447"/>
+      <c r="I25" s="447"/>
+      <c r="J25" s="447"/>
+      <c r="K25" s="447"/>
+      <c r="L25" s="448"/>
+      <c r="M25" s="446"/>
+      <c r="N25" s="447"/>
+      <c r="O25" s="447"/>
+      <c r="P25" s="447"/>
+      <c r="Q25" s="447"/>
+      <c r="R25" s="447"/>
+      <c r="S25" s="447"/>
+      <c r="T25" s="447"/>
+      <c r="U25" s="447"/>
+      <c r="V25" s="447"/>
+      <c r="W25" s="447"/>
+      <c r="X25" s="447"/>
+      <c r="Y25" s="447"/>
+      <c r="Z25" s="447"/>
+      <c r="AA25" s="447"/>
+      <c r="AB25" s="447"/>
+      <c r="AC25" s="447"/>
+      <c r="AD25" s="447"/>
+      <c r="AE25" s="447"/>
+      <c r="AF25" s="447"/>
+      <c r="AG25" s="447"/>
+      <c r="AH25" s="447"/>
+      <c r="AI25" s="447"/>
+      <c r="AJ25" s="447"/>
+      <c r="AK25" s="447"/>
+      <c r="AL25" s="448"/>
       <c r="AM25" s="325"/>
     </row>
     <row r="26" spans="1:39" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="458"/>
+      <c r="A26" s="439"/>
       <c r="B26" s="333"/>
       <c r="C26" s="334" t="s">
         <v>74</v>
@@ -11222,51 +11225,51 @@
       <c r="D26" s="335" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="468"/>
-      <c r="F26" s="469"/>
-      <c r="G26" s="469"/>
-      <c r="H26" s="469"/>
-      <c r="I26" s="469"/>
-      <c r="J26" s="469"/>
-      <c r="K26" s="469"/>
-      <c r="L26" s="470"/>
-      <c r="M26" s="468"/>
-      <c r="N26" s="469"/>
-      <c r="O26" s="469"/>
-      <c r="P26" s="469"/>
-      <c r="Q26" s="469"/>
-      <c r="R26" s="469"/>
-      <c r="S26" s="469"/>
-      <c r="T26" s="469"/>
-      <c r="U26" s="469"/>
-      <c r="V26" s="469"/>
-      <c r="W26" s="469"/>
-      <c r="X26" s="469"/>
-      <c r="Y26" s="469"/>
-      <c r="Z26" s="469"/>
-      <c r="AA26" s="469"/>
-      <c r="AB26" s="469"/>
-      <c r="AC26" s="469"/>
-      <c r="AD26" s="469"/>
-      <c r="AE26" s="469"/>
-      <c r="AF26" s="469"/>
-      <c r="AG26" s="469"/>
-      <c r="AH26" s="469"/>
-      <c r="AI26" s="469"/>
-      <c r="AJ26" s="469"/>
-      <c r="AK26" s="466"/>
-      <c r="AL26" s="467"/>
+      <c r="E26" s="449"/>
+      <c r="F26" s="450"/>
+      <c r="G26" s="450"/>
+      <c r="H26" s="450"/>
+      <c r="I26" s="450"/>
+      <c r="J26" s="450"/>
+      <c r="K26" s="450"/>
+      <c r="L26" s="451"/>
+      <c r="M26" s="449"/>
+      <c r="N26" s="450"/>
+      <c r="O26" s="450"/>
+      <c r="P26" s="450"/>
+      <c r="Q26" s="450"/>
+      <c r="R26" s="450"/>
+      <c r="S26" s="450"/>
+      <c r="T26" s="450"/>
+      <c r="U26" s="450"/>
+      <c r="V26" s="450"/>
+      <c r="W26" s="450"/>
+      <c r="X26" s="450"/>
+      <c r="Y26" s="450"/>
+      <c r="Z26" s="450"/>
+      <c r="AA26" s="450"/>
+      <c r="AB26" s="450"/>
+      <c r="AC26" s="450"/>
+      <c r="AD26" s="450"/>
+      <c r="AE26" s="450"/>
+      <c r="AF26" s="450"/>
+      <c r="AG26" s="450"/>
+      <c r="AH26" s="450"/>
+      <c r="AI26" s="450"/>
+      <c r="AJ26" s="450"/>
+      <c r="AK26" s="447"/>
+      <c r="AL26" s="448"/>
       <c r="AM26" s="325"/>
     </row>
     <row r="27" spans="1:39" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="458"/>
+      <c r="A27" s="439"/>
       <c r="B27" s="41" t="s">
         <v>293</v>
       </c>
       <c r="C27" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="459" t="s">
+      <c r="D27" s="440" t="s">
         <v>363</v>
       </c>
       <c r="E27" s="102"/>
@@ -11358,12 +11361,12 @@
       <c r="AM27" s="66"/>
     </row>
     <row r="28" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="458"/>
+      <c r="A28" s="439"/>
       <c r="B28" s="47"/>
       <c r="C28" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="460"/>
+      <c r="D28" s="441"/>
       <c r="E28" s="103"/>
       <c r="F28" s="31"/>
       <c r="G28" s="31"/>
@@ -11453,12 +11456,12 @@
       <c r="AM28" s="179"/>
     </row>
     <row r="29" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="458"/>
+      <c r="A29" s="439"/>
       <c r="B29" s="47"/>
       <c r="C29" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D29" s="460"/>
+      <c r="D29" s="441"/>
       <c r="E29" s="103"/>
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
@@ -11548,12 +11551,12 @@
       <c r="AM29" s="179"/>
     </row>
     <row r="30" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="458"/>
+      <c r="A30" s="439"/>
       <c r="B30" s="47"/>
       <c r="C30" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D30" s="460"/>
+      <c r="D30" s="441"/>
       <c r="E30" s="103"/>
       <c r="F30" s="31"/>
       <c r="G30" s="31"/>
@@ -11645,12 +11648,12 @@
       </c>
     </row>
     <row r="31" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="458"/>
+      <c r="A31" s="439"/>
       <c r="B31" s="47"/>
       <c r="C31" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D31" s="460"/>
+      <c r="D31" s="441"/>
       <c r="E31" s="103"/>
       <c r="F31" s="31"/>
       <c r="G31" s="31"/>
@@ -11740,12 +11743,12 @@
       <c r="AM31" s="179"/>
     </row>
     <row r="32" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="458"/>
+      <c r="A32" s="439"/>
       <c r="B32" s="47"/>
       <c r="C32" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="D32" s="460"/>
+      <c r="D32" s="441"/>
       <c r="E32" s="103"/>
       <c r="F32" s="31"/>
       <c r="G32" s="31"/>
@@ -11835,12 +11838,12 @@
       <c r="AM32" s="179"/>
     </row>
     <row r="33" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="458"/>
+      <c r="A33" s="439"/>
       <c r="B33" s="47"/>
       <c r="C33" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="460"/>
+      <c r="D33" s="441"/>
       <c r="E33" s="103"/>
       <c r="F33" s="31"/>
       <c r="G33" s="31"/>
@@ -11930,12 +11933,12 @@
       <c r="AM33" s="179"/>
     </row>
     <row r="34" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="458"/>
+      <c r="A34" s="439"/>
       <c r="B34" s="47"/>
       <c r="C34" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D34" s="460"/>
+      <c r="D34" s="441"/>
       <c r="E34" s="103"/>
       <c r="F34" s="31"/>
       <c r="G34" s="31"/>
@@ -11995,12 +11998,12 @@
       <c r="AM34" s="180"/>
     </row>
     <row r="35" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="458"/>
+      <c r="A35" s="439"/>
       <c r="B35" s="47"/>
       <c r="C35" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="460"/>
+      <c r="D35" s="441"/>
       <c r="E35" s="103"/>
       <c r="F35" s="31"/>
       <c r="G35" s="31"/>
@@ -12090,12 +12093,12 @@
       <c r="AM35" s="179"/>
     </row>
     <row r="36" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="458"/>
+      <c r="A36" s="439"/>
       <c r="B36" s="47"/>
       <c r="C36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="460"/>
+      <c r="D36" s="441"/>
       <c r="E36" s="103"/>
       <c r="F36" s="31"/>
       <c r="G36" s="31"/>
@@ -12171,12 +12174,12 @@
       <c r="AM36" s="179"/>
     </row>
     <row r="37" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="458"/>
+      <c r="A37" s="439"/>
       <c r="B37" s="47"/>
       <c r="C37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="460"/>
+      <c r="D37" s="441"/>
       <c r="E37" s="103"/>
       <c r="F37" s="31"/>
       <c r="G37" s="31"/>
@@ -12254,12 +12257,12 @@
       </c>
     </row>
     <row r="38" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="458"/>
+      <c r="A38" s="439"/>
       <c r="B38" s="47"/>
       <c r="C38" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="D38" s="460"/>
+      <c r="D38" s="441"/>
       <c r="E38" s="103"/>
       <c r="F38" s="31"/>
       <c r="G38" s="31"/>
@@ -12327,12 +12330,12 @@
       <c r="AM38" s="179"/>
     </row>
     <row r="39" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="458"/>
+      <c r="A39" s="439"/>
       <c r="B39" s="49"/>
       <c r="C39" s="308" t="s">
         <v>272</v>
       </c>
-      <c r="D39" s="460"/>
+      <c r="D39" s="441"/>
       <c r="E39" s="309"/>
       <c r="F39" s="310"/>
       <c r="G39" s="310"/>
@@ -12370,12 +12373,12 @@
       <c r="AM39" s="183"/>
     </row>
     <row r="40" spans="1:40" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="458"/>
+      <c r="A40" s="439"/>
       <c r="B40" s="67"/>
       <c r="C40" s="427" t="s">
         <v>436</v>
       </c>
-      <c r="D40" s="460"/>
+      <c r="D40" s="441"/>
       <c r="E40" s="105"/>
       <c r="F40" s="69"/>
       <c r="G40" s="69"/>
@@ -12435,14 +12438,14 @@
       <c r="AM40" s="181"/>
     </row>
     <row r="41" spans="1:40" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="458"/>
+      <c r="A41" s="439"/>
       <c r="B41" s="48" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="D41" s="460"/>
+      <c r="D41" s="441"/>
       <c r="E41" s="109"/>
       <c r="F41" s="40"/>
       <c r="G41" s="40"/>
@@ -12532,12 +12535,12 @@
       <c r="AM41" s="182"/>
     </row>
     <row r="42" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="458"/>
+      <c r="A42" s="439"/>
       <c r="B42" s="47"/>
       <c r="C42" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="460"/>
+      <c r="D42" s="441"/>
       <c r="E42" s="103"/>
       <c r="F42" s="31"/>
       <c r="G42" s="31"/>
@@ -12587,12 +12590,12 @@
       <c r="AM42" s="179"/>
     </row>
     <row r="43" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="458"/>
+      <c r="A43" s="439"/>
       <c r="B43" s="47"/>
       <c r="C43" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="D43" s="460"/>
+      <c r="D43" s="441"/>
       <c r="E43" s="103"/>
       <c r="F43" s="31"/>
       <c r="G43" s="31"/>
@@ -12642,12 +12645,12 @@
       <c r="AM43" s="179"/>
     </row>
     <row r="44" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="458"/>
+      <c r="A44" s="439"/>
       <c r="B44" s="49"/>
       <c r="C44" s="425" t="s">
         <v>496</v>
       </c>
-      <c r="D44" s="460"/>
+      <c r="D44" s="441"/>
       <c r="E44" s="309"/>
       <c r="F44" s="310"/>
       <c r="G44" s="310"/>
@@ -12737,12 +12740,12 @@
       <c r="AM44" s="183"/>
     </row>
     <row r="45" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="458"/>
+      <c r="A45" s="439"/>
       <c r="B45" s="49"/>
       <c r="C45" s="425" t="s">
         <v>497</v>
       </c>
-      <c r="D45" s="460"/>
+      <c r="D45" s="441"/>
       <c r="E45" s="309"/>
       <c r="F45" s="310"/>
       <c r="G45" s="310"/>
@@ -12784,12 +12787,12 @@
       <c r="AM45" s="183"/>
     </row>
     <row r="46" spans="1:40" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="458"/>
+      <c r="A46" s="439"/>
       <c r="B46" s="67"/>
       <c r="C46" s="68" t="s">
         <v>275</v>
       </c>
-      <c r="D46" s="460"/>
+      <c r="D46" s="441"/>
       <c r="E46" s="105"/>
       <c r="F46" s="69"/>
       <c r="G46" s="69"/>
@@ -12849,14 +12852,14 @@
       <c r="AM46" s="181"/>
     </row>
     <row r="47" spans="1:40" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="458"/>
+      <c r="A47" s="439"/>
       <c r="B47" s="41" t="s">
         <v>97</v>
       </c>
       <c r="C47" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="D47" s="460"/>
+      <c r="D47" s="441"/>
       <c r="E47" s="102"/>
       <c r="F47" s="43"/>
       <c r="G47" s="43"/>
@@ -12948,12 +12951,12 @@
       </c>
     </row>
     <row r="48" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="458"/>
+      <c r="A48" s="439"/>
       <c r="B48" s="47"/>
       <c r="C48" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="460"/>
+      <c r="D48" s="441"/>
       <c r="E48" s="103"/>
       <c r="F48" s="31"/>
       <c r="G48" s="31"/>
@@ -13048,12 +13051,12 @@
       </c>
     </row>
     <row r="49" spans="1:39" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="458"/>
+      <c r="A49" s="439"/>
       <c r="B49" s="385"/>
       <c r="C49" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D49" s="460"/>
+      <c r="D49" s="441"/>
       <c r="E49" s="116"/>
       <c r="F49" s="32"/>
       <c r="G49" s="32"/>
@@ -13113,12 +13116,12 @@
       <c r="AM49" s="180"/>
     </row>
     <row r="50" spans="1:39" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="458"/>
+      <c r="A50" s="439"/>
       <c r="B50" s="371"/>
       <c r="C50" s="372" t="s">
         <v>458</v>
       </c>
-      <c r="D50" s="460"/>
+      <c r="D50" s="441"/>
       <c r="E50" s="373"/>
       <c r="F50" s="374"/>
       <c r="G50" s="374"/>
@@ -13208,14 +13211,14 @@
       <c r="AM50" s="377"/>
     </row>
     <row r="51" spans="1:39" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="458"/>
+      <c r="A51" s="439"/>
       <c r="B51" s="41" t="s">
         <v>35</v>
       </c>
       <c r="C51" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="460"/>
+      <c r="D51" s="441"/>
       <c r="E51" s="102" t="s">
         <v>18</v>
       </c>
@@ -13321,12 +13324,12 @@
       <c r="AM51" s="66"/>
     </row>
     <row r="52" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="458"/>
+      <c r="A52" s="439"/>
       <c r="B52" s="48"/>
       <c r="C52" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="D52" s="460"/>
+      <c r="D52" s="441"/>
       <c r="E52" s="107"/>
       <c r="F52" s="40" t="s">
         <v>9</v>
@@ -13430,12 +13433,12 @@
       <c r="AM52" s="182"/>
     </row>
     <row r="53" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="458"/>
+      <c r="A53" s="439"/>
       <c r="B53" s="48"/>
       <c r="C53" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="D53" s="460"/>
+      <c r="D53" s="441"/>
       <c r="E53" s="109" t="s">
         <v>9</v>
       </c>
@@ -13541,12 +13544,12 @@
       <c r="AM53" s="182"/>
     </row>
     <row r="54" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="458"/>
+      <c r="A54" s="439"/>
       <c r="B54" s="47"/>
       <c r="C54" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="D54" s="460"/>
+      <c r="D54" s="441"/>
       <c r="E54" s="103" t="s">
         <v>9</v>
       </c>
@@ -13652,12 +13655,12 @@
       <c r="AM54" s="179"/>
     </row>
     <row r="55" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="458"/>
+      <c r="A55" s="439"/>
       <c r="B55" s="47"/>
       <c r="C55" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="D55" s="460"/>
+      <c r="D55" s="441"/>
       <c r="E55" s="110"/>
       <c r="F55" s="35"/>
       <c r="G55" s="35"/>
@@ -13733,12 +13736,12 @@
       </c>
     </row>
     <row r="56" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="458"/>
+      <c r="A56" s="439"/>
       <c r="B56" s="47"/>
       <c r="C56" s="198" t="s">
         <v>271</v>
       </c>
-      <c r="D56" s="460"/>
+      <c r="D56" s="441"/>
       <c r="E56" s="103" t="s">
         <v>18</v>
       </c>
@@ -13844,12 +13847,12 @@
       <c r="AM56" s="179"/>
     </row>
     <row r="57" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="458"/>
+      <c r="A57" s="439"/>
       <c r="B57" s="47"/>
       <c r="C57" s="198" t="s">
         <v>454</v>
       </c>
-      <c r="D57" s="460"/>
+      <c r="D57" s="441"/>
       <c r="E57" s="103" t="s">
         <v>48</v>
       </c>
@@ -13955,12 +13958,12 @@
       <c r="AM57" s="179"/>
     </row>
     <row r="58" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="458"/>
+      <c r="A58" s="439"/>
       <c r="B58" s="47"/>
       <c r="C58" s="199" t="s">
         <v>474</v>
       </c>
-      <c r="D58" s="460"/>
+      <c r="D58" s="441"/>
       <c r="E58" s="110"/>
       <c r="F58" s="35"/>
       <c r="G58" s="35"/>
@@ -14036,12 +14039,12 @@
       </c>
     </row>
     <row r="59" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="458"/>
+      <c r="A59" s="439"/>
       <c r="B59" s="47"/>
       <c r="C59" s="198" t="s">
         <v>37</v>
       </c>
-      <c r="D59" s="460"/>
+      <c r="D59" s="441"/>
       <c r="E59" s="103" t="s">
         <v>9</v>
       </c>
@@ -14147,12 +14150,12 @@
       <c r="AM59" s="179"/>
     </row>
     <row r="60" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="458"/>
+      <c r="A60" s="439"/>
       <c r="B60" s="47"/>
       <c r="C60" s="198" t="s">
         <v>234</v>
       </c>
-      <c r="D60" s="460"/>
+      <c r="D60" s="441"/>
       <c r="E60" s="103" t="s">
         <v>9</v>
       </c>
@@ -14260,12 +14263,12 @@
       </c>
     </row>
     <row r="61" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="458"/>
+      <c r="A61" s="439"/>
       <c r="B61" s="47"/>
       <c r="C61" s="198" t="s">
         <v>235</v>
       </c>
-      <c r="D61" s="460"/>
+      <c r="D61" s="441"/>
       <c r="E61" s="103" t="s">
         <v>9</v>
       </c>
@@ -14373,12 +14376,12 @@
       </c>
     </row>
     <row r="62" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="458"/>
+      <c r="A62" s="439"/>
       <c r="B62" s="47"/>
       <c r="C62" s="198" t="s">
         <v>236</v>
       </c>
-      <c r="D62" s="460"/>
+      <c r="D62" s="441"/>
       <c r="E62" s="103" t="s">
         <v>9</v>
       </c>
@@ -14484,12 +14487,12 @@
       <c r="AM62" s="179"/>
     </row>
     <row r="63" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="458"/>
+      <c r="A63" s="439"/>
       <c r="B63" s="47"/>
       <c r="C63" s="430" t="s">
         <v>501</v>
       </c>
-      <c r="D63" s="460"/>
+      <c r="D63" s="441"/>
       <c r="E63" s="111"/>
       <c r="F63" s="34"/>
       <c r="G63" s="34"/>
@@ -14531,12 +14534,12 @@
       <c r="AM63" s="179"/>
     </row>
     <row r="64" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="458"/>
+      <c r="A64" s="439"/>
       <c r="B64" s="47"/>
       <c r="C64" s="198" t="s">
         <v>480</v>
       </c>
-      <c r="D64" s="460"/>
+      <c r="D64" s="441"/>
       <c r="E64" s="111"/>
       <c r="F64" s="34"/>
       <c r="G64" s="34"/>
@@ -14580,12 +14583,12 @@
       <c r="AM64" s="179"/>
     </row>
     <row r="65" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="458"/>
+      <c r="A65" s="439"/>
       <c r="B65" s="47"/>
       <c r="C65" s="198" t="s">
         <v>228</v>
       </c>
-      <c r="D65" s="460"/>
+      <c r="D65" s="441"/>
       <c r="E65" s="111"/>
       <c r="F65" s="34"/>
       <c r="G65" s="34"/>
@@ -14655,12 +14658,12 @@
       <c r="AM65" s="179"/>
     </row>
     <row r="66" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="458"/>
+      <c r="A66" s="439"/>
       <c r="B66" s="47"/>
       <c r="C66" s="199" t="s">
         <v>38</v>
       </c>
-      <c r="D66" s="460"/>
+      <c r="D66" s="441"/>
       <c r="E66" s="110"/>
       <c r="F66" s="35"/>
       <c r="G66" s="35"/>
@@ -14736,12 +14739,12 @@
       </c>
     </row>
     <row r="67" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="458"/>
+      <c r="A67" s="439"/>
       <c r="B67" s="47"/>
       <c r="C67" s="199" t="s">
         <v>39</v>
       </c>
-      <c r="D67" s="460"/>
+      <c r="D67" s="441"/>
       <c r="E67" s="110"/>
       <c r="F67" s="35"/>
       <c r="G67" s="35"/>
@@ -14817,12 +14820,12 @@
       </c>
     </row>
     <row r="68" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="458"/>
+      <c r="A68" s="439"/>
       <c r="B68" s="47"/>
       <c r="C68" s="198" t="s">
         <v>502</v>
       </c>
-      <c r="D68" s="460"/>
+      <c r="D68" s="441"/>
       <c r="E68" s="103" t="s">
         <v>9</v>
       </c>
@@ -14928,12 +14931,12 @@
       <c r="AM68" s="179"/>
     </row>
     <row r="69" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="458"/>
+      <c r="A69" s="439"/>
       <c r="B69" s="47"/>
       <c r="C69" s="198" t="s">
         <v>503</v>
       </c>
-      <c r="D69" s="460"/>
+      <c r="D69" s="441"/>
       <c r="E69" s="103" t="s">
         <v>9</v>
       </c>
@@ -15039,12 +15042,12 @@
       <c r="AM69" s="179"/>
     </row>
     <row r="70" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="458"/>
+      <c r="A70" s="439"/>
       <c r="B70" s="47"/>
       <c r="C70" s="198" t="s">
         <v>237</v>
       </c>
-      <c r="D70" s="460"/>
+      <c r="D70" s="441"/>
       <c r="E70" s="103" t="s">
         <v>9</v>
       </c>
@@ -15150,12 +15153,12 @@
       <c r="AM70" s="179"/>
     </row>
     <row r="71" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="458"/>
+      <c r="A71" s="439"/>
       <c r="B71" s="47"/>
       <c r="C71" s="430" t="s">
         <v>504</v>
       </c>
-      <c r="D71" s="460"/>
+      <c r="D71" s="441"/>
       <c r="E71" s="111"/>
       <c r="F71" s="34"/>
       <c r="G71" s="34"/>
@@ -15197,12 +15200,12 @@
       <c r="AM71" s="179"/>
     </row>
     <row r="72" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="458"/>
+      <c r="A72" s="439"/>
       <c r="B72" s="47"/>
       <c r="C72" s="198" t="s">
         <v>40</v>
       </c>
-      <c r="D72" s="460"/>
+      <c r="D72" s="441"/>
       <c r="E72" s="111"/>
       <c r="F72" s="34"/>
       <c r="G72" s="34"/>
@@ -15276,12 +15279,12 @@
       <c r="AM72" s="179"/>
     </row>
     <row r="73" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="458"/>
+      <c r="A73" s="439"/>
       <c r="B73" s="47"/>
       <c r="C73" s="198" t="s">
         <v>260</v>
       </c>
-      <c r="D73" s="460"/>
+      <c r="D73" s="441"/>
       <c r="E73" s="111"/>
       <c r="F73" s="34"/>
       <c r="G73" s="34"/>
@@ -15347,12 +15350,12 @@
       <c r="AM73" s="179"/>
     </row>
     <row r="74" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="458"/>
+      <c r="A74" s="439"/>
       <c r="B74" s="47"/>
       <c r="C74" s="430" t="s">
         <v>505</v>
       </c>
-      <c r="D74" s="460"/>
+      <c r="D74" s="441"/>
       <c r="E74" s="111"/>
       <c r="F74" s="34"/>
       <c r="G74" s="34"/>
@@ -15394,12 +15397,12 @@
       <c r="AM74" s="179"/>
     </row>
     <row r="75" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="458"/>
+      <c r="A75" s="439"/>
       <c r="B75" s="47"/>
       <c r="C75" s="198" t="s">
         <v>452</v>
       </c>
-      <c r="D75" s="460"/>
+      <c r="D75" s="441"/>
       <c r="E75" s="111"/>
       <c r="F75" s="34"/>
       <c r="G75" s="34"/>
@@ -15469,12 +15472,12 @@
       <c r="AM75" s="179"/>
     </row>
     <row r="76" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="458"/>
+      <c r="A76" s="439"/>
       <c r="B76" s="47"/>
       <c r="C76" s="198" t="s">
         <v>453</v>
       </c>
-      <c r="D76" s="460"/>
+      <c r="D76" s="441"/>
       <c r="E76" s="111"/>
       <c r="F76" s="34"/>
       <c r="G76" s="34"/>
@@ -15534,12 +15537,12 @@
       <c r="AM76" s="179"/>
     </row>
     <row r="77" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="458"/>
+      <c r="A77" s="439"/>
       <c r="B77" s="47"/>
       <c r="C77" s="198" t="s">
         <v>41</v>
       </c>
-      <c r="D77" s="460"/>
+      <c r="D77" s="441"/>
       <c r="E77" s="103" t="s">
         <v>18</v>
       </c>
@@ -15645,12 +15648,12 @@
       <c r="AM77" s="179"/>
     </row>
     <row r="78" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="458"/>
+      <c r="A78" s="439"/>
       <c r="B78" s="47"/>
       <c r="C78" s="198" t="s">
         <v>222</v>
       </c>
-      <c r="D78" s="460"/>
+      <c r="D78" s="441"/>
       <c r="E78" s="103" t="s">
         <v>9</v>
       </c>
@@ -15756,12 +15759,12 @@
       <c r="AM78" s="179"/>
     </row>
     <row r="79" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="458"/>
+      <c r="A79" s="439"/>
       <c r="B79" s="47"/>
       <c r="C79" s="198" t="s">
         <v>223</v>
       </c>
-      <c r="D79" s="460"/>
+      <c r="D79" s="441"/>
       <c r="E79" s="111"/>
       <c r="F79" s="34"/>
       <c r="G79" s="34"/>
@@ -15827,12 +15830,12 @@
       <c r="AM79" s="179"/>
     </row>
     <row r="80" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="458"/>
+      <c r="A80" s="439"/>
       <c r="B80" s="47"/>
       <c r="C80" s="430" t="s">
         <v>506</v>
       </c>
-      <c r="D80" s="460"/>
+      <c r="D80" s="441"/>
       <c r="E80" s="111"/>
       <c r="F80" s="34"/>
       <c r="G80" s="34"/>
@@ -15874,12 +15877,12 @@
       <c r="AM80" s="179"/>
     </row>
     <row r="81" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="458"/>
+      <c r="A81" s="439"/>
       <c r="B81" s="47"/>
       <c r="C81" s="198" t="s">
         <v>481</v>
       </c>
-      <c r="D81" s="460"/>
+      <c r="D81" s="441"/>
       <c r="E81" s="111"/>
       <c r="F81" s="34"/>
       <c r="G81" s="34"/>
@@ -15923,12 +15926,12 @@
       <c r="AM81" s="179"/>
     </row>
     <row r="82" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="458"/>
+      <c r="A82" s="439"/>
       <c r="B82" s="47"/>
       <c r="C82" s="198" t="s">
         <v>42</v>
       </c>
-      <c r="D82" s="460"/>
+      <c r="D82" s="441"/>
       <c r="E82" s="103" t="s">
         <v>18</v>
       </c>
@@ -16036,12 +16039,12 @@
       </c>
     </row>
     <row r="83" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="458"/>
+      <c r="A83" s="439"/>
       <c r="B83" s="47"/>
       <c r="C83" s="198" t="s">
         <v>109</v>
       </c>
-      <c r="D83" s="460"/>
+      <c r="D83" s="441"/>
       <c r="E83" s="103" t="s">
         <v>9</v>
       </c>
@@ -16147,12 +16150,12 @@
       <c r="AM83" s="179"/>
     </row>
     <row r="84" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="458"/>
+      <c r="A84" s="439"/>
       <c r="B84" s="47"/>
       <c r="C84" s="198" t="s">
         <v>43</v>
       </c>
-      <c r="D84" s="460"/>
+      <c r="D84" s="441"/>
       <c r="E84" s="103" t="s">
         <v>18</v>
       </c>
@@ -16260,12 +16263,12 @@
       </c>
     </row>
     <row r="85" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="458"/>
+      <c r="A85" s="439"/>
       <c r="B85" s="47"/>
       <c r="C85" s="198" t="s">
         <v>304</v>
       </c>
-      <c r="D85" s="460"/>
+      <c r="D85" s="441"/>
       <c r="E85" s="111"/>
       <c r="F85" s="34"/>
       <c r="G85" s="34"/>
@@ -16331,12 +16334,12 @@
       <c r="AM85" s="179"/>
     </row>
     <row r="86" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="458"/>
+      <c r="A86" s="439"/>
       <c r="B86" s="253"/>
       <c r="C86" s="254" t="s">
         <v>245</v>
       </c>
-      <c r="D86" s="460"/>
+      <c r="D86" s="441"/>
       <c r="E86" s="31" t="s">
         <v>361</v>
       </c>
@@ -16421,7 +16424,7 @@
       <c r="AF86" s="234" t="s">
         <v>359</v>
       </c>
-      <c r="AG86" s="472" t="s">
+      <c r="AG86" s="437" t="s">
         <v>522</v>
       </c>
       <c r="AH86" s="258" t="s">
@@ -16442,12 +16445,12 @@
       <c r="AM86" s="259"/>
     </row>
     <row r="87" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="458"/>
+      <c r="A87" s="439"/>
       <c r="B87" s="253"/>
       <c r="C87" s="431" t="s">
         <v>507</v>
       </c>
-      <c r="D87" s="460"/>
+      <c r="D87" s="441"/>
       <c r="E87" s="352"/>
       <c r="F87" s="34"/>
       <c r="G87" s="34"/>
@@ -16489,12 +16492,12 @@
       <c r="AM87" s="259"/>
     </row>
     <row r="88" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="458"/>
+      <c r="A88" s="439"/>
       <c r="B88" s="47"/>
       <c r="C88" s="198" t="s">
         <v>350</v>
       </c>
-      <c r="D88" s="460"/>
+      <c r="D88" s="441"/>
       <c r="E88" s="202"/>
       <c r="F88" s="34"/>
       <c r="G88" s="34"/>
@@ -16538,12 +16541,12 @@
       <c r="AM88" s="179"/>
     </row>
     <row r="89" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="458"/>
+      <c r="A89" s="439"/>
       <c r="B89" s="47"/>
       <c r="C89" s="198" t="s">
         <v>239</v>
       </c>
-      <c r="D89" s="460"/>
+      <c r="D89" s="441"/>
       <c r="E89" s="112" t="s">
         <v>18</v>
       </c>
@@ -16649,12 +16652,12 @@
       <c r="AM89" s="179"/>
     </row>
     <row r="90" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="458"/>
+      <c r="A90" s="439"/>
       <c r="B90" s="47"/>
       <c r="C90" s="198" t="s">
         <v>482</v>
       </c>
-      <c r="D90" s="460"/>
+      <c r="D90" s="441"/>
       <c r="E90" s="202"/>
       <c r="F90" s="34"/>
       <c r="G90" s="34"/>
@@ -16698,12 +16701,12 @@
       <c r="AM90" s="179"/>
     </row>
     <row r="91" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="458"/>
+      <c r="A91" s="439"/>
       <c r="B91" s="47"/>
       <c r="C91" s="430" t="s">
         <v>491</v>
       </c>
-      <c r="D91" s="460"/>
+      <c r="D91" s="441"/>
       <c r="E91" s="202"/>
       <c r="F91" s="34"/>
       <c r="G91" s="34"/>
@@ -16732,7 +16735,7 @@
       <c r="AD91" s="30"/>
       <c r="AE91" s="30"/>
       <c r="AF91" s="203"/>
-      <c r="AG91" s="471" t="s">
+      <c r="AG91" s="436" t="s">
         <v>9</v>
       </c>
       <c r="AH91" s="133"/>
@@ -16747,12 +16750,12 @@
       <c r="AM91" s="179"/>
     </row>
     <row r="92" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="458"/>
+      <c r="A92" s="439"/>
       <c r="B92" s="47"/>
       <c r="C92" s="198" t="s">
         <v>202</v>
       </c>
-      <c r="D92" s="460"/>
+      <c r="D92" s="441"/>
       <c r="E92" s="111"/>
       <c r="F92" s="34"/>
       <c r="G92" s="34"/>
@@ -16830,12 +16833,12 @@
       <c r="AM92" s="179"/>
     </row>
     <row r="93" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="458"/>
+      <c r="A93" s="439"/>
       <c r="B93" s="47"/>
       <c r="C93" s="198" t="s">
         <v>110</v>
       </c>
-      <c r="D93" s="460"/>
+      <c r="D93" s="441"/>
       <c r="E93" s="111"/>
       <c r="F93" s="34"/>
       <c r="G93" s="34"/>
@@ -16909,12 +16912,12 @@
       <c r="AM93" s="179"/>
     </row>
     <row r="94" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="458"/>
+      <c r="A94" s="439"/>
       <c r="B94" s="47"/>
       <c r="C94" s="198" t="s">
         <v>111</v>
       </c>
-      <c r="D94" s="460"/>
+      <c r="D94" s="441"/>
       <c r="E94" s="111"/>
       <c r="F94" s="34"/>
       <c r="G94" s="34"/>
@@ -16984,12 +16987,12 @@
       <c r="AM94" s="179"/>
     </row>
     <row r="95" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="458"/>
+      <c r="A95" s="439"/>
       <c r="B95" s="47"/>
       <c r="C95" s="198" t="s">
         <v>508</v>
       </c>
-      <c r="D95" s="460"/>
+      <c r="D95" s="441"/>
       <c r="E95" s="111"/>
       <c r="F95" s="34"/>
       <c r="G95" s="34"/>
@@ -17063,12 +17066,12 @@
       <c r="AM95" s="179"/>
     </row>
     <row r="96" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="458"/>
+      <c r="A96" s="439"/>
       <c r="B96" s="47"/>
       <c r="C96" s="430" t="s">
         <v>509</v>
       </c>
-      <c r="D96" s="460"/>
+      <c r="D96" s="441"/>
       <c r="E96" s="352"/>
       <c r="F96" s="34"/>
       <c r="G96" s="34"/>
@@ -17110,12 +17113,12 @@
       <c r="AM96" s="179"/>
     </row>
     <row r="97" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="458"/>
+      <c r="A97" s="439"/>
       <c r="B97" s="47"/>
       <c r="C97" s="430" t="s">
         <v>510</v>
       </c>
-      <c r="D97" s="460"/>
+      <c r="D97" s="441"/>
       <c r="E97" s="111"/>
       <c r="F97" s="34"/>
       <c r="G97" s="34"/>
@@ -17157,12 +17160,12 @@
       <c r="AM97" s="179"/>
     </row>
     <row r="98" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="458"/>
+      <c r="A98" s="439"/>
       <c r="B98" s="47"/>
       <c r="C98" s="430" t="s">
         <v>511</v>
       </c>
-      <c r="D98" s="460"/>
+      <c r="D98" s="441"/>
       <c r="E98" s="111"/>
       <c r="F98" s="34"/>
       <c r="G98" s="34"/>
@@ -17204,12 +17207,12 @@
       <c r="AM98" s="179"/>
     </row>
     <row r="99" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="458"/>
+      <c r="A99" s="439"/>
       <c r="B99" s="47"/>
       <c r="C99" s="430" t="s">
         <v>512</v>
       </c>
-      <c r="D99" s="460"/>
+      <c r="D99" s="441"/>
       <c r="E99" s="111"/>
       <c r="F99" s="34"/>
       <c r="G99" s="34"/>
@@ -17251,12 +17254,12 @@
       <c r="AM99" s="179"/>
     </row>
     <row r="100" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="458"/>
+      <c r="A100" s="439"/>
       <c r="B100" s="47"/>
       <c r="C100" s="198" t="s">
         <v>451</v>
       </c>
-      <c r="D100" s="460"/>
+      <c r="D100" s="441"/>
       <c r="E100" s="111"/>
       <c r="F100" s="34"/>
       <c r="G100" s="34"/>
@@ -17330,12 +17333,12 @@
       <c r="AM100" s="179"/>
     </row>
     <row r="101" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="458"/>
+      <c r="A101" s="439"/>
       <c r="B101" s="49"/>
       <c r="C101" s="430" t="s">
         <v>513</v>
       </c>
-      <c r="D101" s="460"/>
+      <c r="D101" s="441"/>
       <c r="E101" s="238"/>
       <c r="F101" s="239"/>
       <c r="G101" s="239"/>
@@ -17377,12 +17380,12 @@
       <c r="AM101" s="183"/>
     </row>
     <row r="102" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="458"/>
+      <c r="A102" s="439"/>
       <c r="B102" s="49"/>
       <c r="C102" s="74" t="s">
         <v>351</v>
       </c>
-      <c r="D102" s="460"/>
+      <c r="D102" s="441"/>
       <c r="E102" s="238"/>
       <c r="F102" s="239"/>
       <c r="G102" s="239"/>
@@ -17426,12 +17429,12 @@
       <c r="AM102" s="183"/>
     </row>
     <row r="103" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="458"/>
+      <c r="A103" s="439"/>
       <c r="B103" s="49"/>
       <c r="C103" s="425" t="s">
         <v>514</v>
       </c>
-      <c r="D103" s="460"/>
+      <c r="D103" s="441"/>
       <c r="E103" s="238"/>
       <c r="F103" s="239"/>
       <c r="G103" s="239"/>
@@ -17473,12 +17476,12 @@
       <c r="AM103" s="183"/>
     </row>
     <row r="104" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="458"/>
+      <c r="A104" s="439"/>
       <c r="B104" s="49"/>
       <c r="C104" s="425" t="s">
         <v>515</v>
       </c>
-      <c r="D104" s="460"/>
+      <c r="D104" s="441"/>
       <c r="E104" s="238"/>
       <c r="F104" s="239"/>
       <c r="G104" s="239"/>
@@ -17520,12 +17523,12 @@
       <c r="AM104" s="183"/>
     </row>
     <row r="105" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="458"/>
+      <c r="A105" s="439"/>
       <c r="B105" s="49"/>
       <c r="C105" s="74" t="s">
         <v>288</v>
       </c>
-      <c r="D105" s="460"/>
+      <c r="D105" s="441"/>
       <c r="E105" s="114" t="s">
         <v>243</v>
       </c>
@@ -17631,12 +17634,12 @@
       <c r="AM105" s="183"/>
     </row>
     <row r="106" spans="1:40" s="38" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="458"/>
+      <c r="A106" s="439"/>
       <c r="B106" s="73"/>
       <c r="C106" s="74" t="s">
         <v>229</v>
       </c>
-      <c r="D106" s="460"/>
+      <c r="D106" s="441"/>
       <c r="E106" s="114" t="s">
         <v>230</v>
       </c>
@@ -17745,14 +17748,14 @@
       </c>
     </row>
     <row r="107" spans="1:40" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="458"/>
+      <c r="A107" s="439"/>
       <c r="B107" s="41" t="s">
         <v>45</v>
       </c>
       <c r="C107" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="D107" s="460"/>
+      <c r="D107" s="441"/>
       <c r="E107" s="102"/>
       <c r="F107" s="43"/>
       <c r="G107" s="43"/>
@@ -17844,12 +17847,12 @@
       </c>
     </row>
     <row r="108" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="458"/>
+      <c r="A108" s="439"/>
       <c r="B108" s="48"/>
       <c r="C108" s="39" t="s">
         <v>305</v>
       </c>
-      <c r="D108" s="460"/>
+      <c r="D108" s="441"/>
       <c r="E108" s="109"/>
       <c r="F108" s="40"/>
       <c r="G108" s="40"/>
@@ -17909,12 +17912,12 @@
       <c r="AM108" s="182"/>
     </row>
     <row r="109" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="458"/>
+      <c r="A109" s="439"/>
       <c r="B109" s="47"/>
       <c r="C109" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D109" s="460"/>
+      <c r="D109" s="441"/>
       <c r="E109" s="103"/>
       <c r="F109" s="31"/>
       <c r="G109" s="31"/>
@@ -18004,12 +18007,12 @@
       <c r="AM109" s="179"/>
     </row>
     <row r="110" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="458"/>
+      <c r="A110" s="439"/>
       <c r="B110" s="47"/>
       <c r="C110" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D110" s="460"/>
+      <c r="D110" s="441"/>
       <c r="E110" s="103"/>
       <c r="F110" s="31"/>
       <c r="G110" s="31"/>
@@ -18099,12 +18102,12 @@
       <c r="AM110" s="179"/>
     </row>
     <row r="111" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="458"/>
+      <c r="A111" s="439"/>
       <c r="B111" s="47"/>
       <c r="C111" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D111" s="460"/>
+      <c r="D111" s="441"/>
       <c r="E111" s="103"/>
       <c r="F111" s="31"/>
       <c r="G111" s="31"/>
@@ -18194,12 +18197,12 @@
       <c r="AM111" s="179"/>
     </row>
     <row r="112" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="458"/>
+      <c r="A112" s="439"/>
       <c r="B112" s="47"/>
       <c r="C112" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D112" s="460"/>
+      <c r="D112" s="441"/>
       <c r="E112" s="103"/>
       <c r="F112" s="31"/>
       <c r="G112" s="31"/>
@@ -18294,12 +18297,12 @@
       </c>
     </row>
     <row r="113" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="458"/>
+      <c r="A113" s="439"/>
       <c r="B113" s="47"/>
       <c r="C113" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D113" s="460"/>
+      <c r="D113" s="441"/>
       <c r="E113" s="103"/>
       <c r="F113" s="31"/>
       <c r="G113" s="31"/>
@@ -18392,12 +18395,12 @@
       </c>
     </row>
     <row r="114" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="458"/>
+      <c r="A114" s="439"/>
       <c r="B114" s="47"/>
       <c r="C114" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D114" s="460"/>
+      <c r="D114" s="441"/>
       <c r="E114" s="103"/>
       <c r="F114" s="31"/>
       <c r="G114" s="31"/>
@@ -18492,12 +18495,12 @@
       </c>
     </row>
     <row r="115" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="458"/>
+      <c r="A115" s="439"/>
       <c r="B115" s="47"/>
       <c r="C115" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D115" s="460"/>
+      <c r="D115" s="441"/>
       <c r="E115" s="103"/>
       <c r="F115" s="31"/>
       <c r="G115" s="31"/>
@@ -18589,12 +18592,12 @@
       </c>
     </row>
     <row r="116" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="458"/>
+      <c r="A116" s="439"/>
       <c r="B116" s="47"/>
       <c r="C116" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D116" s="460"/>
+      <c r="D116" s="441"/>
       <c r="E116" s="103"/>
       <c r="F116" s="31"/>
       <c r="G116" s="31"/>
@@ -18686,12 +18689,12 @@
       </c>
     </row>
     <row r="117" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="458"/>
+      <c r="A117" s="439"/>
       <c r="B117" s="47"/>
       <c r="C117" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D117" s="460"/>
+      <c r="D117" s="441"/>
       <c r="E117" s="103"/>
       <c r="F117" s="31"/>
       <c r="G117" s="31"/>
@@ -18783,12 +18786,12 @@
       </c>
     </row>
     <row r="118" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="458"/>
+      <c r="A118" s="439"/>
       <c r="B118" s="47"/>
       <c r="C118" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="D118" s="460"/>
+      <c r="D118" s="441"/>
       <c r="E118" s="103"/>
       <c r="F118" s="31"/>
       <c r="G118" s="31"/>
@@ -18848,12 +18851,12 @@
       <c r="AM118" s="179"/>
     </row>
     <row r="119" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="458"/>
+      <c r="A119" s="439"/>
       <c r="B119" s="47"/>
       <c r="C119" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D119" s="460"/>
+      <c r="D119" s="441"/>
       <c r="E119" s="103"/>
       <c r="F119" s="31"/>
       <c r="G119" s="31"/>
@@ -18921,12 +18924,12 @@
       <c r="AM119" s="179"/>
     </row>
     <row r="120" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="458"/>
+      <c r="A120" s="439"/>
       <c r="B120" s="49"/>
       <c r="C120" s="198" t="s">
         <v>435</v>
       </c>
-      <c r="D120" s="460"/>
+      <c r="D120" s="441"/>
       <c r="E120" s="103"/>
       <c r="F120" s="31"/>
       <c r="G120" s="31"/>
@@ -18986,12 +18989,12 @@
       <c r="AM120" s="179"/>
     </row>
     <row r="121" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="458"/>
+      <c r="A121" s="439"/>
       <c r="B121" s="49"/>
       <c r="C121" s="381" t="s">
         <v>477</v>
       </c>
-      <c r="D121" s="460"/>
+      <c r="D121" s="441"/>
       <c r="E121" s="103"/>
       <c r="F121" s="31"/>
       <c r="G121" s="31"/>
@@ -19035,12 +19038,12 @@
       <c r="AM121" s="179"/>
     </row>
     <row r="122" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="458"/>
+      <c r="A122" s="439"/>
       <c r="B122" s="49"/>
       <c r="C122" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="D122" s="460"/>
+      <c r="D122" s="441"/>
       <c r="E122" s="103"/>
       <c r="F122" s="31"/>
       <c r="G122" s="31"/>
@@ -19130,12 +19133,12 @@
       <c r="AM122" s="179"/>
     </row>
     <row r="123" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="458"/>
+      <c r="A123" s="439"/>
       <c r="B123" s="297"/>
       <c r="C123" s="199" t="s">
         <v>181</v>
       </c>
-      <c r="D123" s="460"/>
+      <c r="D123" s="441"/>
       <c r="E123" s="103"/>
       <c r="F123" s="31"/>
       <c r="G123" s="31"/>
@@ -19225,12 +19228,12 @@
       <c r="AM123" s="179"/>
     </row>
     <row r="124" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="458"/>
+      <c r="A124" s="439"/>
       <c r="B124" s="48"/>
       <c r="C124" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D124" s="460"/>
+      <c r="D124" s="441"/>
       <c r="E124" s="103"/>
       <c r="F124" s="31"/>
       <c r="G124" s="31"/>
@@ -19308,12 +19311,12 @@
       </c>
     </row>
     <row r="125" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="458"/>
+      <c r="A125" s="439"/>
       <c r="B125" s="47"/>
       <c r="C125" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="D125" s="460"/>
+      <c r="D125" s="441"/>
       <c r="E125" s="103"/>
       <c r="F125" s="31"/>
       <c r="G125" s="31"/>
@@ -19403,12 +19406,12 @@
       <c r="AM125" s="185"/>
     </row>
     <row r="126" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="458"/>
+      <c r="A126" s="439"/>
       <c r="B126" s="47"/>
       <c r="C126" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="D126" s="460"/>
+      <c r="D126" s="441"/>
       <c r="E126" s="103"/>
       <c r="F126" s="31"/>
       <c r="G126" s="31"/>
@@ -19498,12 +19501,12 @@
       <c r="AM126" s="179"/>
     </row>
     <row r="127" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="458"/>
+      <c r="A127" s="439"/>
       <c r="B127" s="47"/>
       <c r="C127" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="D127" s="460"/>
+      <c r="D127" s="441"/>
       <c r="E127" s="103"/>
       <c r="F127" s="31"/>
       <c r="G127" s="31"/>
@@ -19593,12 +19596,12 @@
       <c r="AM127" s="179"/>
     </row>
     <row r="128" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="458"/>
+      <c r="A128" s="439"/>
       <c r="B128" s="47"/>
       <c r="C128" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D128" s="460"/>
+      <c r="D128" s="441"/>
       <c r="E128" s="103"/>
       <c r="F128" s="31"/>
       <c r="G128" s="31"/>
@@ -19688,12 +19691,12 @@
       <c r="AM128" s="185"/>
     </row>
     <row r="129" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="458"/>
+      <c r="A129" s="439"/>
       <c r="B129" s="47"/>
       <c r="C129" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="D129" s="460"/>
+      <c r="D129" s="441"/>
       <c r="E129" s="103"/>
       <c r="F129" s="31"/>
       <c r="G129" s="31"/>
@@ -19783,12 +19786,12 @@
       <c r="AM129" s="179"/>
     </row>
     <row r="130" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="458"/>
+      <c r="A130" s="439"/>
       <c r="B130" s="47"/>
       <c r="C130" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="D130" s="460"/>
+      <c r="D130" s="441"/>
       <c r="E130" s="103"/>
       <c r="F130" s="31"/>
       <c r="G130" s="31"/>
@@ -19878,12 +19881,12 @@
       <c r="AM130" s="185"/>
     </row>
     <row r="131" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="458"/>
+      <c r="A131" s="439"/>
       <c r="B131" s="47"/>
       <c r="C131" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="D131" s="460"/>
+      <c r="D131" s="441"/>
       <c r="E131" s="103"/>
       <c r="F131" s="31"/>
       <c r="G131" s="31"/>
@@ -19973,12 +19976,12 @@
       <c r="AM131" s="179"/>
     </row>
     <row r="132" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="458"/>
+      <c r="A132" s="439"/>
       <c r="B132" s="47"/>
       <c r="C132" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="D132" s="460"/>
+      <c r="D132" s="441"/>
       <c r="E132" s="103"/>
       <c r="F132" s="31"/>
       <c r="G132" s="31"/>
@@ -20068,12 +20071,12 @@
       <c r="AM132" s="179"/>
     </row>
     <row r="133" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="458"/>
+      <c r="A133" s="439"/>
       <c r="B133" s="47"/>
       <c r="C133" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D133" s="460"/>
+      <c r="D133" s="441"/>
       <c r="E133" s="103"/>
       <c r="F133" s="31"/>
       <c r="G133" s="31"/>
@@ -20165,12 +20168,12 @@
       </c>
     </row>
     <row r="134" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="458"/>
+      <c r="A134" s="439"/>
       <c r="B134" s="47"/>
       <c r="C134" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D134" s="460"/>
+      <c r="D134" s="441"/>
       <c r="E134" s="103"/>
       <c r="F134" s="31"/>
       <c r="G134" s="31"/>
@@ -20262,12 +20265,12 @@
       </c>
     </row>
     <row r="135" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="458"/>
+      <c r="A135" s="439"/>
       <c r="B135" s="47"/>
       <c r="C135" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D135" s="460"/>
+      <c r="D135" s="441"/>
       <c r="E135" s="103"/>
       <c r="F135" s="31"/>
       <c r="G135" s="31"/>
@@ -20359,12 +20362,12 @@
       </c>
     </row>
     <row r="136" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="458"/>
+      <c r="A136" s="439"/>
       <c r="B136" s="47"/>
       <c r="C136" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D136" s="460"/>
+      <c r="D136" s="441"/>
       <c r="E136" s="103"/>
       <c r="F136" s="31"/>
       <c r="G136" s="31"/>
@@ -20456,12 +20459,12 @@
       </c>
     </row>
     <row r="137" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="458"/>
+      <c r="A137" s="439"/>
       <c r="B137" s="47"/>
       <c r="C137" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D137" s="460"/>
+      <c r="D137" s="441"/>
       <c r="E137" s="103"/>
       <c r="F137" s="31"/>
       <c r="G137" s="31"/>
@@ -20553,12 +20556,12 @@
       </c>
     </row>
     <row r="138" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="458"/>
+      <c r="A138" s="439"/>
       <c r="B138" s="47"/>
       <c r="C138" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D138" s="460"/>
+      <c r="D138" s="441"/>
       <c r="E138" s="103"/>
       <c r="F138" s="31"/>
       <c r="G138" s="31"/>
@@ -20653,12 +20656,12 @@
       </c>
     </row>
     <row r="139" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="458"/>
+      <c r="A139" s="439"/>
       <c r="B139" s="47"/>
       <c r="C139" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D139" s="460"/>
+      <c r="D139" s="441"/>
       <c r="E139" s="103"/>
       <c r="F139" s="31"/>
       <c r="G139" s="31"/>
@@ -20750,12 +20753,12 @@
       </c>
     </row>
     <row r="140" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="458"/>
+      <c r="A140" s="439"/>
       <c r="B140" s="47"/>
       <c r="C140" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D140" s="460"/>
+      <c r="D140" s="441"/>
       <c r="E140" s="103"/>
       <c r="F140" s="31"/>
       <c r="G140" s="31"/>
@@ -20817,12 +20820,12 @@
       <c r="AM140" s="179"/>
     </row>
     <row r="141" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="458"/>
+      <c r="A141" s="439"/>
       <c r="B141" s="47"/>
       <c r="C141" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D141" s="460"/>
+      <c r="D141" s="441"/>
       <c r="E141" s="103"/>
       <c r="F141" s="31"/>
       <c r="G141" s="31"/>
@@ -20884,12 +20887,12 @@
       <c r="AM141" s="179"/>
     </row>
     <row r="142" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="458"/>
+      <c r="A142" s="439"/>
       <c r="B142" s="47"/>
       <c r="C142" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D142" s="460"/>
+      <c r="D142" s="441"/>
       <c r="E142" s="103"/>
       <c r="F142" s="31"/>
       <c r="G142" s="31"/>
@@ -20951,12 +20954,12 @@
       <c r="AM142" s="179"/>
     </row>
     <row r="143" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="458"/>
+      <c r="A143" s="439"/>
       <c r="B143" s="47"/>
       <c r="C143" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D143" s="460"/>
+      <c r="D143" s="441"/>
       <c r="E143" s="103"/>
       <c r="F143" s="31"/>
       <c r="G143" s="31"/>
@@ -21018,12 +21021,12 @@
       <c r="AM143" s="179"/>
     </row>
     <row r="144" spans="1:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="458"/>
+      <c r="A144" s="439"/>
       <c r="B144" s="47"/>
       <c r="C144" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D144" s="460"/>
+      <c r="D144" s="441"/>
       <c r="E144" s="103"/>
       <c r="F144" s="31"/>
       <c r="G144" s="31"/>
@@ -21085,12 +21088,12 @@
       <c r="AM144" s="179"/>
     </row>
     <row r="145" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="458"/>
+      <c r="A145" s="439"/>
       <c r="B145" s="47"/>
       <c r="C145" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D145" s="460"/>
+      <c r="D145" s="441"/>
       <c r="E145" s="103"/>
       <c r="F145" s="31"/>
       <c r="G145" s="31"/>
@@ -21152,12 +21155,12 @@
       <c r="AM145" s="179"/>
     </row>
     <row r="146" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="458"/>
+      <c r="A146" s="439"/>
       <c r="B146" s="47"/>
       <c r="C146" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D146" s="460"/>
+      <c r="D146" s="441"/>
       <c r="E146" s="103"/>
       <c r="F146" s="31"/>
       <c r="G146" s="31"/>
@@ -21219,12 +21222,12 @@
       <c r="AM146" s="179"/>
     </row>
     <row r="147" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="458"/>
+      <c r="A147" s="439"/>
       <c r="B147" s="47"/>
       <c r="C147" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D147" s="460"/>
+      <c r="D147" s="441"/>
       <c r="E147" s="103"/>
       <c r="F147" s="31"/>
       <c r="G147" s="31"/>
@@ -21286,12 +21289,12 @@
       <c r="AM147" s="179"/>
     </row>
     <row r="148" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="458"/>
+      <c r="A148" s="439"/>
       <c r="B148" s="47"/>
       <c r="C148" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D148" s="460"/>
+      <c r="D148" s="441"/>
       <c r="E148" s="103"/>
       <c r="F148" s="31"/>
       <c r="G148" s="31"/>
@@ -21353,12 +21356,12 @@
       <c r="AM148" s="179"/>
     </row>
     <row r="149" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="458"/>
+      <c r="A149" s="439"/>
       <c r="B149" s="47"/>
       <c r="C149" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D149" s="460"/>
+      <c r="D149" s="441"/>
       <c r="E149" s="103"/>
       <c r="F149" s="31"/>
       <c r="G149" s="31"/>
@@ -21420,12 +21423,12 @@
       <c r="AM149" s="179"/>
     </row>
     <row r="150" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="458"/>
+      <c r="A150" s="439"/>
       <c r="B150" s="47"/>
       <c r="C150" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D150" s="460"/>
+      <c r="D150" s="441"/>
       <c r="E150" s="103"/>
       <c r="F150" s="31"/>
       <c r="G150" s="31"/>
@@ -21487,12 +21490,12 @@
       <c r="AM150" s="179"/>
     </row>
     <row r="151" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="458"/>
+      <c r="A151" s="439"/>
       <c r="B151" s="47"/>
       <c r="C151" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D151" s="460"/>
+      <c r="D151" s="441"/>
       <c r="E151" s="103"/>
       <c r="F151" s="31"/>
       <c r="G151" s="31"/>
@@ -21566,12 +21569,12 @@
       </c>
     </row>
     <row r="152" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="458"/>
+      <c r="A152" s="439"/>
       <c r="B152" s="47"/>
       <c r="C152" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D152" s="460"/>
+      <c r="D152" s="441"/>
       <c r="E152" s="103"/>
       <c r="F152" s="31"/>
       <c r="G152" s="31"/>
@@ -21663,12 +21666,12 @@
       </c>
     </row>
     <row r="153" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="458"/>
+      <c r="A153" s="439"/>
       <c r="B153" s="47"/>
       <c r="C153" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D153" s="460"/>
+      <c r="D153" s="441"/>
       <c r="E153" s="116"/>
       <c r="F153" s="32"/>
       <c r="G153" s="32"/>
@@ -21706,12 +21709,12 @@
       <c r="AM153" s="179"/>
     </row>
     <row r="154" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="458"/>
+      <c r="A154" s="439"/>
       <c r="B154" s="47"/>
       <c r="C154" s="199" t="s">
         <v>67</v>
       </c>
-      <c r="D154" s="460"/>
+      <c r="D154" s="441"/>
       <c r="E154" s="116"/>
       <c r="F154" s="32"/>
       <c r="G154" s="32"/>
@@ -21803,12 +21806,12 @@
       </c>
     </row>
     <row r="155" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="458"/>
+      <c r="A155" s="439"/>
       <c r="B155" s="47"/>
       <c r="C155" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="D155" s="460"/>
+      <c r="D155" s="441"/>
       <c r="E155" s="116"/>
       <c r="F155" s="32"/>
       <c r="G155" s="32"/>
@@ -21898,12 +21901,12 @@
       <c r="AM155" s="179"/>
     </row>
     <row r="156" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="458"/>
+      <c r="A156" s="439"/>
       <c r="B156" s="47"/>
       <c r="C156" s="428" t="s">
         <v>192</v>
       </c>
-      <c r="D156" s="460"/>
+      <c r="D156" s="441"/>
       <c r="E156" s="116"/>
       <c r="F156" s="32"/>
       <c r="G156" s="32"/>
@@ -21993,12 +21996,12 @@
       <c r="AM156" s="179"/>
     </row>
     <row r="157" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="458"/>
+      <c r="A157" s="439"/>
       <c r="B157" s="47"/>
       <c r="C157" s="428" t="s">
         <v>408</v>
       </c>
-      <c r="D157" s="460"/>
+      <c r="D157" s="441"/>
       <c r="E157" s="116"/>
       <c r="F157" s="32"/>
       <c r="G157" s="32"/>
@@ -22090,12 +22093,12 @@
       </c>
     </row>
     <row r="158" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="458"/>
+      <c r="A158" s="439"/>
       <c r="B158" s="47"/>
       <c r="C158" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="D158" s="460"/>
+      <c r="D158" s="441"/>
       <c r="E158" s="116"/>
       <c r="F158" s="32"/>
       <c r="G158" s="32"/>
@@ -22187,12 +22190,12 @@
       </c>
     </row>
     <row r="159" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="458"/>
+      <c r="A159" s="439"/>
       <c r="B159" s="47"/>
       <c r="C159" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D159" s="460"/>
+      <c r="D159" s="441"/>
       <c r="E159" s="116"/>
       <c r="F159" s="32"/>
       <c r="G159" s="32"/>
@@ -22284,12 +22287,12 @@
       </c>
     </row>
     <row r="160" spans="1:39" s="284" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="458"/>
+      <c r="A160" s="439"/>
       <c r="B160" s="288"/>
       <c r="C160" s="429" t="s">
         <v>183</v>
       </c>
-      <c r="D160" s="460"/>
+      <c r="D160" s="441"/>
       <c r="E160" s="282"/>
       <c r="F160" s="255"/>
       <c r="G160" s="255"/>
@@ -22379,12 +22382,12 @@
       <c r="AM160" s="283"/>
     </row>
     <row r="161" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="458"/>
+      <c r="A161" s="439"/>
       <c r="B161" s="49"/>
       <c r="C161" s="199" t="s">
         <v>66</v>
       </c>
-      <c r="D161" s="460"/>
+      <c r="D161" s="441"/>
       <c r="E161" s="116"/>
       <c r="F161" s="32"/>
       <c r="G161" s="32"/>
@@ -22474,12 +22477,12 @@
       <c r="AM161" s="179"/>
     </row>
     <row r="162" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="458"/>
+      <c r="A162" s="439"/>
       <c r="B162" s="288"/>
       <c r="C162" s="199" t="s">
         <v>73</v>
       </c>
-      <c r="D162" s="460"/>
+      <c r="D162" s="441"/>
       <c r="E162" s="116"/>
       <c r="F162" s="32"/>
       <c r="G162" s="32"/>
@@ -22571,12 +22574,12 @@
       </c>
     </row>
     <row r="163" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="458"/>
+      <c r="A163" s="439"/>
       <c r="B163" s="48"/>
       <c r="C163" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="D163" s="460"/>
+      <c r="D163" s="441"/>
       <c r="E163" s="116"/>
       <c r="F163" s="32"/>
       <c r="G163" s="32"/>
@@ -22668,12 +22671,12 @@
       </c>
     </row>
     <row r="164" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="458"/>
+      <c r="A164" s="439"/>
       <c r="B164" s="47"/>
       <c r="C164" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D164" s="460"/>
+      <c r="D164" s="441"/>
       <c r="E164" s="116"/>
       <c r="F164" s="32"/>
       <c r="G164" s="32"/>
@@ -22763,12 +22766,12 @@
       <c r="AM164" s="179"/>
     </row>
     <row r="165" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="458"/>
+      <c r="A165" s="439"/>
       <c r="B165" s="47"/>
       <c r="C165" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D165" s="460"/>
+      <c r="D165" s="441"/>
       <c r="E165" s="116"/>
       <c r="F165" s="32"/>
       <c r="G165" s="32"/>
@@ -22832,12 +22835,12 @@
       <c r="AM165" s="179"/>
     </row>
     <row r="166" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="458"/>
+      <c r="A166" s="439"/>
       <c r="B166" s="47"/>
       <c r="C166" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D166" s="460"/>
+      <c r="D166" s="441"/>
       <c r="E166" s="116"/>
       <c r="F166" s="32"/>
       <c r="G166" s="32"/>
@@ -22929,12 +22932,12 @@
       </c>
     </row>
     <row r="167" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="458"/>
+      <c r="A167" s="439"/>
       <c r="B167" s="47"/>
       <c r="C167" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D167" s="460"/>
+      <c r="D167" s="441"/>
       <c r="E167" s="116"/>
       <c r="F167" s="32"/>
       <c r="G167" s="32"/>
@@ -23024,12 +23027,12 @@
       <c r="AM167" s="179"/>
     </row>
     <row r="168" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="458"/>
+      <c r="A168" s="439"/>
       <c r="B168" s="49"/>
       <c r="C168" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="D168" s="460"/>
+      <c r="D168" s="441"/>
       <c r="E168" s="421"/>
       <c r="F168" s="362"/>
       <c r="G168" s="362"/>
@@ -23119,12 +23122,12 @@
       <c r="AM168" s="183"/>
     </row>
     <row r="169" spans="1:39" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="458"/>
+      <c r="A169" s="439"/>
       <c r="B169" s="67"/>
       <c r="C169" s="68" t="s">
         <v>226</v>
       </c>
-      <c r="D169" s="460"/>
+      <c r="D169" s="441"/>
       <c r="E169" s="106"/>
       <c r="F169" s="72"/>
       <c r="G169" s="72"/>
@@ -23186,14 +23189,14 @@
       <c r="AM169" s="181"/>
     </row>
     <row r="170" spans="1:39" ht="26.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="458"/>
+      <c r="A170" s="439"/>
       <c r="B170" s="85" t="s">
         <v>75</v>
       </c>
       <c r="C170" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="D170" s="460"/>
+      <c r="D170" s="441"/>
       <c r="E170" s="117"/>
       <c r="F170" s="86"/>
       <c r="G170" s="86"/>
@@ -23285,12 +23288,12 @@
       </c>
     </row>
     <row r="171" spans="1:39" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A171" s="458"/>
+      <c r="A171" s="439"/>
       <c r="B171" s="47"/>
       <c r="C171" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D171" s="460"/>
+      <c r="D171" s="441"/>
       <c r="E171" s="116"/>
       <c r="F171" s="32"/>
       <c r="G171" s="32"/>
@@ -23382,12 +23385,12 @@
       </c>
     </row>
     <row r="172" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="458"/>
+      <c r="A172" s="439"/>
       <c r="B172" s="47"/>
       <c r="C172" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D172" s="460"/>
+      <c r="D172" s="441"/>
       <c r="E172" s="116"/>
       <c r="F172" s="32"/>
       <c r="G172" s="32"/>
@@ -23477,12 +23480,12 @@
       <c r="AM172" s="179"/>
     </row>
     <row r="173" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="458"/>
+      <c r="A173" s="439"/>
       <c r="B173" s="47"/>
       <c r="C173" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D173" s="460"/>
+      <c r="D173" s="441"/>
       <c r="E173" s="116"/>
       <c r="F173" s="32"/>
       <c r="G173" s="32"/>
@@ -23572,12 +23575,12 @@
       <c r="AM173" s="179"/>
     </row>
     <row r="174" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="458"/>
+      <c r="A174" s="439"/>
       <c r="B174" s="47"/>
       <c r="C174" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D174" s="460"/>
+      <c r="D174" s="441"/>
       <c r="E174" s="116"/>
       <c r="F174" s="32"/>
       <c r="G174" s="32"/>
@@ -23667,12 +23670,12 @@
       <c r="AM174" s="179"/>
     </row>
     <row r="175" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="458"/>
+      <c r="A175" s="439"/>
       <c r="B175" s="47"/>
       <c r="C175" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D175" s="460"/>
+      <c r="D175" s="441"/>
       <c r="E175" s="116"/>
       <c r="F175" s="32"/>
       <c r="G175" s="32"/>
@@ -23762,12 +23765,12 @@
       <c r="AM175" s="179"/>
     </row>
     <row r="176" spans="1:39" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A176" s="458"/>
+      <c r="A176" s="439"/>
       <c r="B176" s="47"/>
       <c r="C176" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D176" s="460"/>
+      <c r="D176" s="441"/>
       <c r="E176" s="116"/>
       <c r="F176" s="32"/>
       <c r="G176" s="32"/>
@@ -23859,12 +23862,12 @@
       </c>
     </row>
     <row r="177" spans="1:39" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A177" s="458"/>
+      <c r="A177" s="439"/>
       <c r="B177" s="47"/>
       <c r="C177" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D177" s="460"/>
+      <c r="D177" s="441"/>
       <c r="E177" s="116"/>
       <c r="F177" s="32"/>
       <c r="G177" s="32"/>
@@ -23954,12 +23957,12 @@
       <c r="AM177" s="185"/>
     </row>
     <row r="178" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="458"/>
+      <c r="A178" s="439"/>
       <c r="B178" s="47"/>
       <c r="C178" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D178" s="460"/>
+      <c r="D178" s="441"/>
       <c r="E178" s="116"/>
       <c r="F178" s="32"/>
       <c r="G178" s="32"/>
@@ -24049,12 +24052,12 @@
       <c r="AM178" s="185"/>
     </row>
     <row r="179" spans="1:39" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A179" s="458"/>
+      <c r="A179" s="439"/>
       <c r="B179" s="47"/>
       <c r="C179" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D179" s="460"/>
+      <c r="D179" s="441"/>
       <c r="E179" s="116"/>
       <c r="F179" s="32"/>
       <c r="G179" s="32"/>
@@ -24146,12 +24149,12 @@
       </c>
     </row>
     <row r="180" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A180" s="458"/>
+      <c r="A180" s="439"/>
       <c r="B180" s="47"/>
       <c r="C180" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D180" s="460"/>
+      <c r="D180" s="441"/>
       <c r="E180" s="116"/>
       <c r="F180" s="32"/>
       <c r="G180" s="32"/>
@@ -24243,12 +24246,12 @@
       </c>
     </row>
     <row r="181" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="458"/>
+      <c r="A181" s="439"/>
       <c r="B181" s="47"/>
       <c r="C181" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D181" s="460"/>
+      <c r="D181" s="441"/>
       <c r="E181" s="116"/>
       <c r="F181" s="32"/>
       <c r="G181" s="32"/>
@@ -24338,12 +24341,12 @@
       <c r="AM181" s="179"/>
     </row>
     <row r="182" spans="1:39" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A182" s="458"/>
+      <c r="A182" s="439"/>
       <c r="B182" s="47"/>
       <c r="C182" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D182" s="460"/>
+      <c r="D182" s="441"/>
       <c r="E182" s="116"/>
       <c r="F182" s="32"/>
       <c r="G182" s="32"/>
@@ -24435,12 +24438,12 @@
       </c>
     </row>
     <row r="183" spans="1:39" ht="51" x14ac:dyDescent="0.25">
-      <c r="A183" s="458"/>
+      <c r="A183" s="439"/>
       <c r="B183" s="47"/>
       <c r="C183" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D183" s="460"/>
+      <c r="D183" s="441"/>
       <c r="E183" s="116"/>
       <c r="F183" s="32"/>
       <c r="G183" s="32"/>
@@ -24530,12 +24533,12 @@
       <c r="AM183" s="179"/>
     </row>
     <row r="184" spans="1:39" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="458"/>
+      <c r="A184" s="439"/>
       <c r="B184" s="67"/>
       <c r="C184" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="D184" s="460"/>
+      <c r="D184" s="441"/>
       <c r="E184" s="106"/>
       <c r="F184" s="72"/>
       <c r="G184" s="72"/>
@@ -24607,14 +24610,14 @@
       <c r="AM184" s="181"/>
     </row>
     <row r="185" spans="1:39" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="458"/>
+      <c r="A185" s="439"/>
       <c r="B185" s="55" t="s">
         <v>135</v>
       </c>
       <c r="C185" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="D185" s="460"/>
+      <c r="D185" s="441"/>
       <c r="E185" s="118"/>
       <c r="F185" s="57"/>
       <c r="G185" s="57"/>
@@ -24704,12 +24707,12 @@
       <c r="AM185" s="186"/>
     </row>
     <row r="186" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A186" s="458"/>
+      <c r="A186" s="439"/>
       <c r="B186" s="59"/>
       <c r="C186" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D186" s="460"/>
+      <c r="D186" s="441"/>
       <c r="E186" s="119"/>
       <c r="F186" s="33"/>
       <c r="G186" s="33"/>
@@ -24799,12 +24802,12 @@
       <c r="AM186" s="187"/>
     </row>
     <row r="187" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="458"/>
+      <c r="A187" s="439"/>
       <c r="B187" s="59"/>
       <c r="C187" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D187" s="460"/>
+      <c r="D187" s="441"/>
       <c r="E187" s="119"/>
       <c r="F187" s="33"/>
       <c r="G187" s="33"/>
@@ -24896,12 +24899,12 @@
       </c>
     </row>
     <row r="188" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="458"/>
+      <c r="A188" s="439"/>
       <c r="B188" s="59"/>
       <c r="C188" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D188" s="460"/>
+      <c r="D188" s="441"/>
       <c r="E188" s="119"/>
       <c r="F188" s="33"/>
       <c r="G188" s="33"/>
@@ -24991,12 +24994,12 @@
       <c r="AM188" s="187"/>
     </row>
     <row r="189" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="458"/>
+      <c r="A189" s="439"/>
       <c r="B189" s="59"/>
       <c r="C189" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D189" s="460"/>
+      <c r="D189" s="441"/>
       <c r="E189" s="119"/>
       <c r="F189" s="33"/>
       <c r="G189" s="33"/>
@@ -25086,12 +25089,12 @@
       <c r="AM189" s="187"/>
     </row>
     <row r="190" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="458"/>
+      <c r="A190" s="439"/>
       <c r="B190" s="59"/>
       <c r="C190" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D190" s="460"/>
+      <c r="D190" s="441"/>
       <c r="E190" s="119"/>
       <c r="F190" s="33"/>
       <c r="G190" s="33"/>
@@ -25183,12 +25186,12 @@
       </c>
     </row>
     <row r="191" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="458"/>
+      <c r="A191" s="439"/>
       <c r="B191" s="59"/>
       <c r="C191" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D191" s="460"/>
+      <c r="D191" s="441"/>
       <c r="E191" s="119"/>
       <c r="F191" s="33"/>
       <c r="G191" s="33"/>
@@ -25278,12 +25281,12 @@
       <c r="AM191" s="187"/>
     </row>
     <row r="192" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="458"/>
+      <c r="A192" s="439"/>
       <c r="B192" s="59"/>
       <c r="C192" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D192" s="460"/>
+      <c r="D192" s="441"/>
       <c r="E192" s="119"/>
       <c r="F192" s="33"/>
       <c r="G192" s="33"/>
@@ -25373,12 +25376,12 @@
       <c r="AM192" s="187"/>
     </row>
     <row r="193" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="458"/>
+      <c r="A193" s="439"/>
       <c r="B193" s="59"/>
       <c r="C193" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D193" s="460"/>
+      <c r="D193" s="441"/>
       <c r="E193" s="119"/>
       <c r="F193" s="33"/>
       <c r="G193" s="33"/>
@@ -25468,12 +25471,12 @@
       <c r="AM193" s="187"/>
     </row>
     <row r="194" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="458"/>
+      <c r="A194" s="439"/>
       <c r="B194" s="59"/>
       <c r="C194" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="D194" s="460"/>
+      <c r="D194" s="441"/>
       <c r="E194" s="119"/>
       <c r="F194" s="33"/>
       <c r="G194" s="33"/>
@@ -25565,12 +25568,12 @@
       </c>
     </row>
     <row r="195" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="458"/>
+      <c r="A195" s="439"/>
       <c r="B195" s="59"/>
       <c r="C195" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D195" s="460"/>
+      <c r="D195" s="441"/>
       <c r="E195" s="119"/>
       <c r="F195" s="33"/>
       <c r="G195" s="33"/>
@@ -25660,12 +25663,12 @@
       <c r="AM195" s="187"/>
     </row>
     <row r="196" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="458"/>
+      <c r="A196" s="439"/>
       <c r="B196" s="59"/>
       <c r="C196" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="D196" s="460"/>
+      <c r="D196" s="441"/>
       <c r="E196" s="119"/>
       <c r="F196" s="33"/>
       <c r="G196" s="33"/>
@@ -25755,12 +25758,12 @@
       <c r="AM196" s="187"/>
     </row>
     <row r="197" spans="1:39" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="458"/>
+      <c r="A197" s="439"/>
       <c r="B197" s="60"/>
       <c r="C197" s="61" t="s">
         <v>150</v>
       </c>
-      <c r="D197" s="461"/>
+      <c r="D197" s="442"/>
       <c r="E197" s="120"/>
       <c r="F197" s="62"/>
       <c r="G197" s="62"/>
@@ -25853,12 +25856,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="A27:A197"/>
-    <mergeCell ref="D27:D197"/>
-    <mergeCell ref="E5:L26"/>
-    <mergeCell ref="M5:AL26"/>
-    <mergeCell ref="A5:A26"/>
     <mergeCell ref="AM3:AM4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="T3:V3"/>
@@ -25868,6 +25865,12 @@
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="A27:A197"/>
+    <mergeCell ref="D27:D197"/>
+    <mergeCell ref="E5:L26"/>
+    <mergeCell ref="M5:AL26"/>
+    <mergeCell ref="A5:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
--- IOMMU Translation Table entry size chage from 64 to 128 for both engines.
[git-p4: depot-paths = "//depot/projects/coe/CSME/": change = 772680]
</commit_message>
<xml_diff>
--- a/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
+++ b/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12330" yWindow="105" windowWidth="3210" windowHeight="4665" activeTab="1"/>
+    <workbookView xWindow="12330" yWindow="105" windowWidth="3210" windowHeight="4665"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="2" r:id="rId1"/>
@@ -996,7 +996,7 @@
           <t xml:space="preserve">
 Boot from* usage.
 Michael N will provide data for 128 KB.
-keep 64 KB until data is released.
+keep 64 entry until data is released.
 Arch: data how to use IOMMU table for it.
 Michael B added new mechanism to use DMA for UFS.
 There is a risk where legacy flow is needed in case of bug.
@@ -4341,7 +4341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4150" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4152" uniqueCount="544">
   <si>
     <t>CNP-LP</t>
   </si>
@@ -6361,6 +6361,9 @@
   </si>
   <si>
     <t>Updated configuration for ME - PRTC since it's not placed in CSE</t>
+  </si>
+  <si>
+    <t>Updated IOMMU Translation Table  (128 Entry) size for both engines.</t>
   </si>
 </sst>
 </file>
@@ -8928,6 +8931,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -8990,48 +9035,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9346,11 +9349,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E86" sqref="E86"/>
+      <selection pane="bottomRight" activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10540,10 +10543,18 @@
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="194"/>
-      <c r="C86" s="9"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="4"/>
+      <c r="B86" s="194">
+        <v>74</v>
+      </c>
+      <c r="C86" s="9">
+        <v>43592</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="194"/>
@@ -10652,11 +10663,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="AC188" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="AC38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AM196" sqref="AM196"/>
+      <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10689,48 +10700,48 @@
       <c r="C2" s="418" t="s">
         <v>494</v>
       </c>
-      <c r="AL2" s="511" t="s">
+      <c r="AL2" s="490" t="s">
         <v>515</v>
       </c>
-      <c r="AM2" s="511"/>
+      <c r="AM2" s="490"/>
       <c r="AN2" s="474"/>
     </row>
     <row r="3" spans="1:41" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="492" t="s">
+      <c r="B3" s="506" t="s">
         <v>266</v>
       </c>
-      <c r="C3" s="497" t="s">
+      <c r="C3" s="511" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="498"/>
-      <c r="E3" s="506" t="s">
+      <c r="D3" s="512"/>
+      <c r="E3" s="520" t="s">
         <v>231</v>
       </c>
-      <c r="F3" s="507"/>
-      <c r="G3" s="507"/>
-      <c r="H3" s="507"/>
-      <c r="I3" s="507"/>
-      <c r="J3" s="507"/>
-      <c r="K3" s="507"/>
-      <c r="L3" s="508"/>
-      <c r="M3" s="503" t="s">
+      <c r="F3" s="521"/>
+      <c r="G3" s="521"/>
+      <c r="H3" s="521"/>
+      <c r="I3" s="521"/>
+      <c r="J3" s="521"/>
+      <c r="K3" s="521"/>
+      <c r="L3" s="522"/>
+      <c r="M3" s="517" t="s">
         <v>443</v>
       </c>
-      <c r="N3" s="504"/>
-      <c r="O3" s="505"/>
-      <c r="P3" s="499" t="s">
+      <c r="N3" s="518"/>
+      <c r="O3" s="519"/>
+      <c r="P3" s="513" t="s">
         <v>296</v>
       </c>
-      <c r="Q3" s="500"/>
-      <c r="R3" s="501" t="s">
+      <c r="Q3" s="514"/>
+      <c r="R3" s="515" t="s">
         <v>297</v>
       </c>
-      <c r="S3" s="502"/>
-      <c r="T3" s="494" t="s">
+      <c r="S3" s="516"/>
+      <c r="T3" s="508" t="s">
         <v>298</v>
       </c>
-      <c r="U3" s="495"/>
-      <c r="V3" s="496"/>
+      <c r="U3" s="509"/>
+      <c r="V3" s="510"/>
       <c r="W3" s="296" t="s">
         <v>434</v>
       </c>
@@ -10783,12 +10794,12 @@
         <v>493</v>
       </c>
       <c r="AN3" s="475"/>
-      <c r="AO3" s="490" t="s">
+      <c r="AO3" s="504" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:41" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="493"/>
+      <c r="B4" s="507"/>
       <c r="C4" s="293" t="s">
         <v>432</v>
       </c>
@@ -10894,17 +10905,17 @@
       <c r="AK4" s="387" t="s">
         <v>431</v>
       </c>
-      <c r="AL4" s="509" t="s">
+      <c r="AL4" s="523" t="s">
         <v>517</v>
       </c>
-      <c r="AM4" s="510"/>
+      <c r="AM4" s="524"/>
       <c r="AN4" s="476" t="s">
         <v>535</v>
       </c>
-      <c r="AO4" s="491"/>
+      <c r="AO4" s="505"/>
     </row>
     <row r="5" spans="1:41" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="512"/>
+      <c r="A5" s="491"/>
       <c r="B5" s="323" t="s">
         <v>293</v>
       </c>
@@ -10914,50 +10925,50 @@
       <c r="D5" s="325" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="516" t="s">
+      <c r="E5" s="495" t="s">
         <v>333</v>
       </c>
-      <c r="F5" s="517"/>
-      <c r="G5" s="517"/>
-      <c r="H5" s="517"/>
-      <c r="I5" s="517"/>
-      <c r="J5" s="517"/>
-      <c r="K5" s="517"/>
-      <c r="L5" s="518"/>
-      <c r="M5" s="516" t="s">
+      <c r="F5" s="496"/>
+      <c r="G5" s="496"/>
+      <c r="H5" s="496"/>
+      <c r="I5" s="496"/>
+      <c r="J5" s="496"/>
+      <c r="K5" s="496"/>
+      <c r="L5" s="497"/>
+      <c r="M5" s="495" t="s">
         <v>334</v>
       </c>
-      <c r="N5" s="517"/>
-      <c r="O5" s="517"/>
-      <c r="P5" s="517"/>
-      <c r="Q5" s="517"/>
-      <c r="R5" s="517"/>
-      <c r="S5" s="517"/>
-      <c r="T5" s="517"/>
-      <c r="U5" s="517"/>
-      <c r="V5" s="517"/>
-      <c r="W5" s="517"/>
-      <c r="X5" s="517"/>
-      <c r="Y5" s="517"/>
-      <c r="Z5" s="517"/>
-      <c r="AA5" s="517"/>
-      <c r="AB5" s="517"/>
-      <c r="AC5" s="517"/>
-      <c r="AD5" s="517"/>
-      <c r="AE5" s="517"/>
-      <c r="AF5" s="517"/>
-      <c r="AG5" s="517"/>
-      <c r="AH5" s="517"/>
-      <c r="AI5" s="517"/>
-      <c r="AJ5" s="517"/>
-      <c r="AK5" s="517"/>
-      <c r="AL5" s="520"/>
-      <c r="AM5" s="521"/>
+      <c r="N5" s="496"/>
+      <c r="O5" s="496"/>
+      <c r="P5" s="496"/>
+      <c r="Q5" s="496"/>
+      <c r="R5" s="496"/>
+      <c r="S5" s="496"/>
+      <c r="T5" s="496"/>
+      <c r="U5" s="496"/>
+      <c r="V5" s="496"/>
+      <c r="W5" s="496"/>
+      <c r="X5" s="496"/>
+      <c r="Y5" s="496"/>
+      <c r="Z5" s="496"/>
+      <c r="AA5" s="496"/>
+      <c r="AB5" s="496"/>
+      <c r="AC5" s="496"/>
+      <c r="AD5" s="496"/>
+      <c r="AE5" s="496"/>
+      <c r="AF5" s="496"/>
+      <c r="AG5" s="496"/>
+      <c r="AH5" s="496"/>
+      <c r="AI5" s="496"/>
+      <c r="AJ5" s="496"/>
+      <c r="AK5" s="496"/>
+      <c r="AL5" s="499"/>
+      <c r="AM5" s="500"/>
       <c r="AN5" s="473"/>
       <c r="AO5" s="320"/>
     </row>
     <row r="6" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="512"/>
+      <c r="A6" s="491"/>
       <c r="B6" s="326"/>
       <c r="C6" s="327" t="s">
         <v>8</v>
@@ -10965,46 +10976,46 @@
       <c r="D6" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="519"/>
-      <c r="F6" s="520"/>
-      <c r="G6" s="520"/>
-      <c r="H6" s="520"/>
-      <c r="I6" s="520"/>
-      <c r="J6" s="520"/>
-      <c r="K6" s="520"/>
-      <c r="L6" s="521"/>
-      <c r="M6" s="519"/>
-      <c r="N6" s="520"/>
-      <c r="O6" s="520"/>
-      <c r="P6" s="520"/>
-      <c r="Q6" s="520"/>
-      <c r="R6" s="520"/>
-      <c r="S6" s="520"/>
-      <c r="T6" s="520"/>
-      <c r="U6" s="520"/>
-      <c r="V6" s="520"/>
-      <c r="W6" s="520"/>
-      <c r="X6" s="520"/>
-      <c r="Y6" s="520"/>
-      <c r="Z6" s="520"/>
-      <c r="AA6" s="520"/>
-      <c r="AB6" s="520"/>
-      <c r="AC6" s="520"/>
-      <c r="AD6" s="520"/>
-      <c r="AE6" s="520"/>
-      <c r="AF6" s="520"/>
-      <c r="AG6" s="520"/>
-      <c r="AH6" s="520"/>
-      <c r="AI6" s="520"/>
-      <c r="AJ6" s="520"/>
-      <c r="AK6" s="520"/>
-      <c r="AL6" s="520"/>
-      <c r="AM6" s="521"/>
+      <c r="E6" s="498"/>
+      <c r="F6" s="499"/>
+      <c r="G6" s="499"/>
+      <c r="H6" s="499"/>
+      <c r="I6" s="499"/>
+      <c r="J6" s="499"/>
+      <c r="K6" s="499"/>
+      <c r="L6" s="500"/>
+      <c r="M6" s="498"/>
+      <c r="N6" s="499"/>
+      <c r="O6" s="499"/>
+      <c r="P6" s="499"/>
+      <c r="Q6" s="499"/>
+      <c r="R6" s="499"/>
+      <c r="S6" s="499"/>
+      <c r="T6" s="499"/>
+      <c r="U6" s="499"/>
+      <c r="V6" s="499"/>
+      <c r="W6" s="499"/>
+      <c r="X6" s="499"/>
+      <c r="Y6" s="499"/>
+      <c r="Z6" s="499"/>
+      <c r="AA6" s="499"/>
+      <c r="AB6" s="499"/>
+      <c r="AC6" s="499"/>
+      <c r="AD6" s="499"/>
+      <c r="AE6" s="499"/>
+      <c r="AF6" s="499"/>
+      <c r="AG6" s="499"/>
+      <c r="AH6" s="499"/>
+      <c r="AI6" s="499"/>
+      <c r="AJ6" s="499"/>
+      <c r="AK6" s="499"/>
+      <c r="AL6" s="499"/>
+      <c r="AM6" s="500"/>
       <c r="AN6" s="473"/>
       <c r="AO6" s="321"/>
     </row>
     <row r="7" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="512"/>
+      <c r="A7" s="491"/>
       <c r="B7" s="326"/>
       <c r="C7" s="327" t="s">
         <v>11</v>
@@ -11012,46 +11023,46 @@
       <c r="D7" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="519"/>
-      <c r="F7" s="520"/>
-      <c r="G7" s="520"/>
-      <c r="H7" s="520"/>
-      <c r="I7" s="520"/>
-      <c r="J7" s="520"/>
-      <c r="K7" s="520"/>
-      <c r="L7" s="521"/>
-      <c r="M7" s="519"/>
-      <c r="N7" s="520"/>
-      <c r="O7" s="520"/>
-      <c r="P7" s="520"/>
-      <c r="Q7" s="520"/>
-      <c r="R7" s="520"/>
-      <c r="S7" s="520"/>
-      <c r="T7" s="520"/>
-      <c r="U7" s="520"/>
-      <c r="V7" s="520"/>
-      <c r="W7" s="520"/>
-      <c r="X7" s="520"/>
-      <c r="Y7" s="520"/>
-      <c r="Z7" s="520"/>
-      <c r="AA7" s="520"/>
-      <c r="AB7" s="520"/>
-      <c r="AC7" s="520"/>
-      <c r="AD7" s="520"/>
-      <c r="AE7" s="520"/>
-      <c r="AF7" s="520"/>
-      <c r="AG7" s="520"/>
-      <c r="AH7" s="520"/>
-      <c r="AI7" s="520"/>
-      <c r="AJ7" s="520"/>
-      <c r="AK7" s="520"/>
-      <c r="AL7" s="520"/>
-      <c r="AM7" s="521"/>
+      <c r="E7" s="498"/>
+      <c r="F7" s="499"/>
+      <c r="G7" s="499"/>
+      <c r="H7" s="499"/>
+      <c r="I7" s="499"/>
+      <c r="J7" s="499"/>
+      <c r="K7" s="499"/>
+      <c r="L7" s="500"/>
+      <c r="M7" s="498"/>
+      <c r="N7" s="499"/>
+      <c r="O7" s="499"/>
+      <c r="P7" s="499"/>
+      <c r="Q7" s="499"/>
+      <c r="R7" s="499"/>
+      <c r="S7" s="499"/>
+      <c r="T7" s="499"/>
+      <c r="U7" s="499"/>
+      <c r="V7" s="499"/>
+      <c r="W7" s="499"/>
+      <c r="X7" s="499"/>
+      <c r="Y7" s="499"/>
+      <c r="Z7" s="499"/>
+      <c r="AA7" s="499"/>
+      <c r="AB7" s="499"/>
+      <c r="AC7" s="499"/>
+      <c r="AD7" s="499"/>
+      <c r="AE7" s="499"/>
+      <c r="AF7" s="499"/>
+      <c r="AG7" s="499"/>
+      <c r="AH7" s="499"/>
+      <c r="AI7" s="499"/>
+      <c r="AJ7" s="499"/>
+      <c r="AK7" s="499"/>
+      <c r="AL7" s="499"/>
+      <c r="AM7" s="500"/>
       <c r="AN7" s="473"/>
       <c r="AO7" s="321"/>
     </row>
     <row r="8" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="512"/>
+      <c r="A8" s="491"/>
       <c r="B8" s="326"/>
       <c r="C8" s="327" t="s">
         <v>12</v>
@@ -11059,46 +11070,46 @@
       <c r="D8" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="519"/>
-      <c r="F8" s="520"/>
-      <c r="G8" s="520"/>
-      <c r="H8" s="520"/>
-      <c r="I8" s="520"/>
-      <c r="J8" s="520"/>
-      <c r="K8" s="520"/>
-      <c r="L8" s="521"/>
-      <c r="M8" s="519"/>
-      <c r="N8" s="520"/>
-      <c r="O8" s="520"/>
-      <c r="P8" s="520"/>
-      <c r="Q8" s="520"/>
-      <c r="R8" s="520"/>
-      <c r="S8" s="520"/>
-      <c r="T8" s="520"/>
-      <c r="U8" s="520"/>
-      <c r="V8" s="520"/>
-      <c r="W8" s="520"/>
-      <c r="X8" s="520"/>
-      <c r="Y8" s="520"/>
-      <c r="Z8" s="520"/>
-      <c r="AA8" s="520"/>
-      <c r="AB8" s="520"/>
-      <c r="AC8" s="520"/>
-      <c r="AD8" s="520"/>
-      <c r="AE8" s="520"/>
-      <c r="AF8" s="520"/>
-      <c r="AG8" s="520"/>
-      <c r="AH8" s="520"/>
-      <c r="AI8" s="520"/>
-      <c r="AJ8" s="520"/>
-      <c r="AK8" s="520"/>
-      <c r="AL8" s="520"/>
-      <c r="AM8" s="521"/>
+      <c r="E8" s="498"/>
+      <c r="F8" s="499"/>
+      <c r="G8" s="499"/>
+      <c r="H8" s="499"/>
+      <c r="I8" s="499"/>
+      <c r="J8" s="499"/>
+      <c r="K8" s="499"/>
+      <c r="L8" s="500"/>
+      <c r="M8" s="498"/>
+      <c r="N8" s="499"/>
+      <c r="O8" s="499"/>
+      <c r="P8" s="499"/>
+      <c r="Q8" s="499"/>
+      <c r="R8" s="499"/>
+      <c r="S8" s="499"/>
+      <c r="T8" s="499"/>
+      <c r="U8" s="499"/>
+      <c r="V8" s="499"/>
+      <c r="W8" s="499"/>
+      <c r="X8" s="499"/>
+      <c r="Y8" s="499"/>
+      <c r="Z8" s="499"/>
+      <c r="AA8" s="499"/>
+      <c r="AB8" s="499"/>
+      <c r="AC8" s="499"/>
+      <c r="AD8" s="499"/>
+      <c r="AE8" s="499"/>
+      <c r="AF8" s="499"/>
+      <c r="AG8" s="499"/>
+      <c r="AH8" s="499"/>
+      <c r="AI8" s="499"/>
+      <c r="AJ8" s="499"/>
+      <c r="AK8" s="499"/>
+      <c r="AL8" s="499"/>
+      <c r="AM8" s="500"/>
       <c r="AN8" s="473"/>
       <c r="AO8" s="321"/>
     </row>
     <row r="9" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="512"/>
+      <c r="A9" s="491"/>
       <c r="B9" s="326"/>
       <c r="C9" s="327" t="s">
         <v>319</v>
@@ -11106,46 +11117,46 @@
       <c r="D9" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="519"/>
-      <c r="F9" s="520"/>
-      <c r="G9" s="520"/>
-      <c r="H9" s="520"/>
-      <c r="I9" s="520"/>
-      <c r="J9" s="520"/>
-      <c r="K9" s="520"/>
-      <c r="L9" s="521"/>
-      <c r="M9" s="519"/>
-      <c r="N9" s="520"/>
-      <c r="O9" s="520"/>
-      <c r="P9" s="520"/>
-      <c r="Q9" s="520"/>
-      <c r="R9" s="520"/>
-      <c r="S9" s="520"/>
-      <c r="T9" s="520"/>
-      <c r="U9" s="520"/>
-      <c r="V9" s="520"/>
-      <c r="W9" s="520"/>
-      <c r="X9" s="520"/>
-      <c r="Y9" s="520"/>
-      <c r="Z9" s="520"/>
-      <c r="AA9" s="520"/>
-      <c r="AB9" s="520"/>
-      <c r="AC9" s="520"/>
-      <c r="AD9" s="520"/>
-      <c r="AE9" s="520"/>
-      <c r="AF9" s="520"/>
-      <c r="AG9" s="520"/>
-      <c r="AH9" s="520"/>
-      <c r="AI9" s="520"/>
-      <c r="AJ9" s="520"/>
-      <c r="AK9" s="520"/>
-      <c r="AL9" s="520"/>
-      <c r="AM9" s="521"/>
+      <c r="E9" s="498"/>
+      <c r="F9" s="499"/>
+      <c r="G9" s="499"/>
+      <c r="H9" s="499"/>
+      <c r="I9" s="499"/>
+      <c r="J9" s="499"/>
+      <c r="K9" s="499"/>
+      <c r="L9" s="500"/>
+      <c r="M9" s="498"/>
+      <c r="N9" s="499"/>
+      <c r="O9" s="499"/>
+      <c r="P9" s="499"/>
+      <c r="Q9" s="499"/>
+      <c r="R9" s="499"/>
+      <c r="S9" s="499"/>
+      <c r="T9" s="499"/>
+      <c r="U9" s="499"/>
+      <c r="V9" s="499"/>
+      <c r="W9" s="499"/>
+      <c r="X9" s="499"/>
+      <c r="Y9" s="499"/>
+      <c r="Z9" s="499"/>
+      <c r="AA9" s="499"/>
+      <c r="AB9" s="499"/>
+      <c r="AC9" s="499"/>
+      <c r="AD9" s="499"/>
+      <c r="AE9" s="499"/>
+      <c r="AF9" s="499"/>
+      <c r="AG9" s="499"/>
+      <c r="AH9" s="499"/>
+      <c r="AI9" s="499"/>
+      <c r="AJ9" s="499"/>
+      <c r="AK9" s="499"/>
+      <c r="AL9" s="499"/>
+      <c r="AM9" s="500"/>
       <c r="AN9" s="473"/>
       <c r="AO9" s="321"/>
     </row>
     <row r="10" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="512"/>
+      <c r="A10" s="491"/>
       <c r="B10" s="326"/>
       <c r="C10" s="327" t="s">
         <v>177</v>
@@ -11153,46 +11164,46 @@
       <c r="D10" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="519"/>
-      <c r="F10" s="520"/>
-      <c r="G10" s="520"/>
-      <c r="H10" s="520"/>
-      <c r="I10" s="520"/>
-      <c r="J10" s="520"/>
-      <c r="K10" s="520"/>
-      <c r="L10" s="521"/>
-      <c r="M10" s="519"/>
-      <c r="N10" s="520"/>
-      <c r="O10" s="520"/>
-      <c r="P10" s="520"/>
-      <c r="Q10" s="520"/>
-      <c r="R10" s="520"/>
-      <c r="S10" s="520"/>
-      <c r="T10" s="520"/>
-      <c r="U10" s="520"/>
-      <c r="V10" s="520"/>
-      <c r="W10" s="520"/>
-      <c r="X10" s="520"/>
-      <c r="Y10" s="520"/>
-      <c r="Z10" s="520"/>
-      <c r="AA10" s="520"/>
-      <c r="AB10" s="520"/>
-      <c r="AC10" s="520"/>
-      <c r="AD10" s="520"/>
-      <c r="AE10" s="520"/>
-      <c r="AF10" s="520"/>
-      <c r="AG10" s="520"/>
-      <c r="AH10" s="520"/>
-      <c r="AI10" s="520"/>
-      <c r="AJ10" s="520"/>
-      <c r="AK10" s="520"/>
-      <c r="AL10" s="520"/>
-      <c r="AM10" s="521"/>
+      <c r="E10" s="498"/>
+      <c r="F10" s="499"/>
+      <c r="G10" s="499"/>
+      <c r="H10" s="499"/>
+      <c r="I10" s="499"/>
+      <c r="J10" s="499"/>
+      <c r="K10" s="499"/>
+      <c r="L10" s="500"/>
+      <c r="M10" s="498"/>
+      <c r="N10" s="499"/>
+      <c r="O10" s="499"/>
+      <c r="P10" s="499"/>
+      <c r="Q10" s="499"/>
+      <c r="R10" s="499"/>
+      <c r="S10" s="499"/>
+      <c r="T10" s="499"/>
+      <c r="U10" s="499"/>
+      <c r="V10" s="499"/>
+      <c r="W10" s="499"/>
+      <c r="X10" s="499"/>
+      <c r="Y10" s="499"/>
+      <c r="Z10" s="499"/>
+      <c r="AA10" s="499"/>
+      <c r="AB10" s="499"/>
+      <c r="AC10" s="499"/>
+      <c r="AD10" s="499"/>
+      <c r="AE10" s="499"/>
+      <c r="AF10" s="499"/>
+      <c r="AG10" s="499"/>
+      <c r="AH10" s="499"/>
+      <c r="AI10" s="499"/>
+      <c r="AJ10" s="499"/>
+      <c r="AK10" s="499"/>
+      <c r="AL10" s="499"/>
+      <c r="AM10" s="500"/>
       <c r="AN10" s="473"/>
       <c r="AO10" s="321"/>
     </row>
     <row r="11" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="512"/>
+      <c r="A11" s="491"/>
       <c r="B11" s="326"/>
       <c r="C11" s="327" t="s">
         <v>16</v>
@@ -11200,46 +11211,46 @@
       <c r="D11" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="519"/>
-      <c r="F11" s="520"/>
-      <c r="G11" s="520"/>
-      <c r="H11" s="520"/>
-      <c r="I11" s="520"/>
-      <c r="J11" s="520"/>
-      <c r="K11" s="520"/>
-      <c r="L11" s="521"/>
-      <c r="M11" s="519"/>
-      <c r="N11" s="520"/>
-      <c r="O11" s="520"/>
-      <c r="P11" s="520"/>
-      <c r="Q11" s="520"/>
-      <c r="R11" s="520"/>
-      <c r="S11" s="520"/>
-      <c r="T11" s="520"/>
-      <c r="U11" s="520"/>
-      <c r="V11" s="520"/>
-      <c r="W11" s="520"/>
-      <c r="X11" s="520"/>
-      <c r="Y11" s="520"/>
-      <c r="Z11" s="520"/>
-      <c r="AA11" s="520"/>
-      <c r="AB11" s="520"/>
-      <c r="AC11" s="520"/>
-      <c r="AD11" s="520"/>
-      <c r="AE11" s="520"/>
-      <c r="AF11" s="520"/>
-      <c r="AG11" s="520"/>
-      <c r="AH11" s="520"/>
-      <c r="AI11" s="520"/>
-      <c r="AJ11" s="520"/>
-      <c r="AK11" s="520"/>
-      <c r="AL11" s="520"/>
-      <c r="AM11" s="521"/>
+      <c r="E11" s="498"/>
+      <c r="F11" s="499"/>
+      <c r="G11" s="499"/>
+      <c r="H11" s="499"/>
+      <c r="I11" s="499"/>
+      <c r="J11" s="499"/>
+      <c r="K11" s="499"/>
+      <c r="L11" s="500"/>
+      <c r="M11" s="498"/>
+      <c r="N11" s="499"/>
+      <c r="O11" s="499"/>
+      <c r="P11" s="499"/>
+      <c r="Q11" s="499"/>
+      <c r="R11" s="499"/>
+      <c r="S11" s="499"/>
+      <c r="T11" s="499"/>
+      <c r="U11" s="499"/>
+      <c r="V11" s="499"/>
+      <c r="W11" s="499"/>
+      <c r="X11" s="499"/>
+      <c r="Y11" s="499"/>
+      <c r="Z11" s="499"/>
+      <c r="AA11" s="499"/>
+      <c r="AB11" s="499"/>
+      <c r="AC11" s="499"/>
+      <c r="AD11" s="499"/>
+      <c r="AE11" s="499"/>
+      <c r="AF11" s="499"/>
+      <c r="AG11" s="499"/>
+      <c r="AH11" s="499"/>
+      <c r="AI11" s="499"/>
+      <c r="AJ11" s="499"/>
+      <c r="AK11" s="499"/>
+      <c r="AL11" s="499"/>
+      <c r="AM11" s="500"/>
       <c r="AN11" s="473"/>
       <c r="AO11" s="321"/>
     </row>
     <row r="12" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="512"/>
+      <c r="A12" s="491"/>
       <c r="B12" s="326"/>
       <c r="C12" s="327" t="s">
         <v>17</v>
@@ -11247,46 +11258,46 @@
       <c r="D12" s="329" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="519"/>
-      <c r="F12" s="520"/>
-      <c r="G12" s="520"/>
-      <c r="H12" s="520"/>
-      <c r="I12" s="520"/>
-      <c r="J12" s="520"/>
-      <c r="K12" s="520"/>
-      <c r="L12" s="521"/>
-      <c r="M12" s="519"/>
-      <c r="N12" s="520"/>
-      <c r="O12" s="520"/>
-      <c r="P12" s="520"/>
-      <c r="Q12" s="520"/>
-      <c r="R12" s="520"/>
-      <c r="S12" s="520"/>
-      <c r="T12" s="520"/>
-      <c r="U12" s="520"/>
-      <c r="V12" s="520"/>
-      <c r="W12" s="520"/>
-      <c r="X12" s="520"/>
-      <c r="Y12" s="520"/>
-      <c r="Z12" s="520"/>
-      <c r="AA12" s="520"/>
-      <c r="AB12" s="520"/>
-      <c r="AC12" s="520"/>
-      <c r="AD12" s="520"/>
-      <c r="AE12" s="520"/>
-      <c r="AF12" s="520"/>
-      <c r="AG12" s="520"/>
-      <c r="AH12" s="520"/>
-      <c r="AI12" s="520"/>
-      <c r="AJ12" s="520"/>
-      <c r="AK12" s="520"/>
-      <c r="AL12" s="520"/>
-      <c r="AM12" s="521"/>
+      <c r="E12" s="498"/>
+      <c r="F12" s="499"/>
+      <c r="G12" s="499"/>
+      <c r="H12" s="499"/>
+      <c r="I12" s="499"/>
+      <c r="J12" s="499"/>
+      <c r="K12" s="499"/>
+      <c r="L12" s="500"/>
+      <c r="M12" s="498"/>
+      <c r="N12" s="499"/>
+      <c r="O12" s="499"/>
+      <c r="P12" s="499"/>
+      <c r="Q12" s="499"/>
+      <c r="R12" s="499"/>
+      <c r="S12" s="499"/>
+      <c r="T12" s="499"/>
+      <c r="U12" s="499"/>
+      <c r="V12" s="499"/>
+      <c r="W12" s="499"/>
+      <c r="X12" s="499"/>
+      <c r="Y12" s="499"/>
+      <c r="Z12" s="499"/>
+      <c r="AA12" s="499"/>
+      <c r="AB12" s="499"/>
+      <c r="AC12" s="499"/>
+      <c r="AD12" s="499"/>
+      <c r="AE12" s="499"/>
+      <c r="AF12" s="499"/>
+      <c r="AG12" s="499"/>
+      <c r="AH12" s="499"/>
+      <c r="AI12" s="499"/>
+      <c r="AJ12" s="499"/>
+      <c r="AK12" s="499"/>
+      <c r="AL12" s="499"/>
+      <c r="AM12" s="500"/>
       <c r="AN12" s="473"/>
       <c r="AO12" s="321"/>
     </row>
     <row r="13" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="512"/>
+      <c r="A13" s="491"/>
       <c r="B13" s="326"/>
       <c r="C13" s="327" t="s">
         <v>19</v>
@@ -11294,46 +11305,46 @@
       <c r="D13" s="329">
         <v>32</v>
       </c>
-      <c r="E13" s="519"/>
-      <c r="F13" s="520"/>
-      <c r="G13" s="520"/>
-      <c r="H13" s="520"/>
-      <c r="I13" s="520"/>
-      <c r="J13" s="520"/>
-      <c r="K13" s="520"/>
-      <c r="L13" s="521"/>
-      <c r="M13" s="519"/>
-      <c r="N13" s="520"/>
-      <c r="O13" s="520"/>
-      <c r="P13" s="520"/>
-      <c r="Q13" s="520"/>
-      <c r="R13" s="520"/>
-      <c r="S13" s="520"/>
-      <c r="T13" s="520"/>
-      <c r="U13" s="520"/>
-      <c r="V13" s="520"/>
-      <c r="W13" s="520"/>
-      <c r="X13" s="520"/>
-      <c r="Y13" s="520"/>
-      <c r="Z13" s="520"/>
-      <c r="AA13" s="520"/>
-      <c r="AB13" s="520"/>
-      <c r="AC13" s="520"/>
-      <c r="AD13" s="520"/>
-      <c r="AE13" s="520"/>
-      <c r="AF13" s="520"/>
-      <c r="AG13" s="520"/>
-      <c r="AH13" s="520"/>
-      <c r="AI13" s="520"/>
-      <c r="AJ13" s="520"/>
-      <c r="AK13" s="520"/>
-      <c r="AL13" s="520"/>
-      <c r="AM13" s="521"/>
+      <c r="E13" s="498"/>
+      <c r="F13" s="499"/>
+      <c r="G13" s="499"/>
+      <c r="H13" s="499"/>
+      <c r="I13" s="499"/>
+      <c r="J13" s="499"/>
+      <c r="K13" s="499"/>
+      <c r="L13" s="500"/>
+      <c r="M13" s="498"/>
+      <c r="N13" s="499"/>
+      <c r="O13" s="499"/>
+      <c r="P13" s="499"/>
+      <c r="Q13" s="499"/>
+      <c r="R13" s="499"/>
+      <c r="S13" s="499"/>
+      <c r="T13" s="499"/>
+      <c r="U13" s="499"/>
+      <c r="V13" s="499"/>
+      <c r="W13" s="499"/>
+      <c r="X13" s="499"/>
+      <c r="Y13" s="499"/>
+      <c r="Z13" s="499"/>
+      <c r="AA13" s="499"/>
+      <c r="AB13" s="499"/>
+      <c r="AC13" s="499"/>
+      <c r="AD13" s="499"/>
+      <c r="AE13" s="499"/>
+      <c r="AF13" s="499"/>
+      <c r="AG13" s="499"/>
+      <c r="AH13" s="499"/>
+      <c r="AI13" s="499"/>
+      <c r="AJ13" s="499"/>
+      <c r="AK13" s="499"/>
+      <c r="AL13" s="499"/>
+      <c r="AM13" s="500"/>
       <c r="AN13" s="473"/>
       <c r="AO13" s="321"/>
     </row>
     <row r="14" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="512"/>
+      <c r="A14" s="491"/>
       <c r="B14" s="326"/>
       <c r="C14" s="327" t="s">
         <v>20</v>
@@ -11341,46 +11352,46 @@
       <c r="D14" s="329">
         <v>32</v>
       </c>
-      <c r="E14" s="519"/>
-      <c r="F14" s="520"/>
-      <c r="G14" s="520"/>
-      <c r="H14" s="520"/>
-      <c r="I14" s="520"/>
-      <c r="J14" s="520"/>
-      <c r="K14" s="520"/>
-      <c r="L14" s="521"/>
-      <c r="M14" s="519"/>
-      <c r="N14" s="520"/>
-      <c r="O14" s="520"/>
-      <c r="P14" s="520"/>
-      <c r="Q14" s="520"/>
-      <c r="R14" s="520"/>
-      <c r="S14" s="520"/>
-      <c r="T14" s="520"/>
-      <c r="U14" s="520"/>
-      <c r="V14" s="520"/>
-      <c r="W14" s="520"/>
-      <c r="X14" s="520"/>
-      <c r="Y14" s="520"/>
-      <c r="Z14" s="520"/>
-      <c r="AA14" s="520"/>
-      <c r="AB14" s="520"/>
-      <c r="AC14" s="520"/>
-      <c r="AD14" s="520"/>
-      <c r="AE14" s="520"/>
-      <c r="AF14" s="520"/>
-      <c r="AG14" s="520"/>
-      <c r="AH14" s="520"/>
-      <c r="AI14" s="520"/>
-      <c r="AJ14" s="520"/>
-      <c r="AK14" s="520"/>
-      <c r="AL14" s="520"/>
-      <c r="AM14" s="521"/>
+      <c r="E14" s="498"/>
+      <c r="F14" s="499"/>
+      <c r="G14" s="499"/>
+      <c r="H14" s="499"/>
+      <c r="I14" s="499"/>
+      <c r="J14" s="499"/>
+      <c r="K14" s="499"/>
+      <c r="L14" s="500"/>
+      <c r="M14" s="498"/>
+      <c r="N14" s="499"/>
+      <c r="O14" s="499"/>
+      <c r="P14" s="499"/>
+      <c r="Q14" s="499"/>
+      <c r="R14" s="499"/>
+      <c r="S14" s="499"/>
+      <c r="T14" s="499"/>
+      <c r="U14" s="499"/>
+      <c r="V14" s="499"/>
+      <c r="W14" s="499"/>
+      <c r="X14" s="499"/>
+      <c r="Y14" s="499"/>
+      <c r="Z14" s="499"/>
+      <c r="AA14" s="499"/>
+      <c r="AB14" s="499"/>
+      <c r="AC14" s="499"/>
+      <c r="AD14" s="499"/>
+      <c r="AE14" s="499"/>
+      <c r="AF14" s="499"/>
+      <c r="AG14" s="499"/>
+      <c r="AH14" s="499"/>
+      <c r="AI14" s="499"/>
+      <c r="AJ14" s="499"/>
+      <c r="AK14" s="499"/>
+      <c r="AL14" s="499"/>
+      <c r="AM14" s="500"/>
       <c r="AN14" s="473"/>
       <c r="AO14" s="321"/>
     </row>
     <row r="15" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="512"/>
+      <c r="A15" s="491"/>
       <c r="B15" s="326"/>
       <c r="C15" s="327" t="s">
         <v>21</v>
@@ -11388,46 +11399,46 @@
       <c r="D15" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="519"/>
-      <c r="F15" s="520"/>
-      <c r="G15" s="520"/>
-      <c r="H15" s="520"/>
-      <c r="I15" s="520"/>
-      <c r="J15" s="520"/>
-      <c r="K15" s="520"/>
-      <c r="L15" s="521"/>
-      <c r="M15" s="519"/>
-      <c r="N15" s="520"/>
-      <c r="O15" s="520"/>
-      <c r="P15" s="520"/>
-      <c r="Q15" s="520"/>
-      <c r="R15" s="520"/>
-      <c r="S15" s="520"/>
-      <c r="T15" s="520"/>
-      <c r="U15" s="520"/>
-      <c r="V15" s="520"/>
-      <c r="W15" s="520"/>
-      <c r="X15" s="520"/>
-      <c r="Y15" s="520"/>
-      <c r="Z15" s="520"/>
-      <c r="AA15" s="520"/>
-      <c r="AB15" s="520"/>
-      <c r="AC15" s="520"/>
-      <c r="AD15" s="520"/>
-      <c r="AE15" s="520"/>
-      <c r="AF15" s="520"/>
-      <c r="AG15" s="520"/>
-      <c r="AH15" s="520"/>
-      <c r="AI15" s="520"/>
-      <c r="AJ15" s="520"/>
-      <c r="AK15" s="520"/>
-      <c r="AL15" s="520"/>
-      <c r="AM15" s="521"/>
+      <c r="E15" s="498"/>
+      <c r="F15" s="499"/>
+      <c r="G15" s="499"/>
+      <c r="H15" s="499"/>
+      <c r="I15" s="499"/>
+      <c r="J15" s="499"/>
+      <c r="K15" s="499"/>
+      <c r="L15" s="500"/>
+      <c r="M15" s="498"/>
+      <c r="N15" s="499"/>
+      <c r="O15" s="499"/>
+      <c r="P15" s="499"/>
+      <c r="Q15" s="499"/>
+      <c r="R15" s="499"/>
+      <c r="S15" s="499"/>
+      <c r="T15" s="499"/>
+      <c r="U15" s="499"/>
+      <c r="V15" s="499"/>
+      <c r="W15" s="499"/>
+      <c r="X15" s="499"/>
+      <c r="Y15" s="499"/>
+      <c r="Z15" s="499"/>
+      <c r="AA15" s="499"/>
+      <c r="AB15" s="499"/>
+      <c r="AC15" s="499"/>
+      <c r="AD15" s="499"/>
+      <c r="AE15" s="499"/>
+      <c r="AF15" s="499"/>
+      <c r="AG15" s="499"/>
+      <c r="AH15" s="499"/>
+      <c r="AI15" s="499"/>
+      <c r="AJ15" s="499"/>
+      <c r="AK15" s="499"/>
+      <c r="AL15" s="499"/>
+      <c r="AM15" s="500"/>
       <c r="AN15" s="473"/>
       <c r="AO15" s="321"/>
     </row>
     <row r="16" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="512"/>
+      <c r="A16" s="491"/>
       <c r="B16" s="326" t="s">
         <v>22</v>
       </c>
@@ -11437,46 +11448,46 @@
       <c r="D16" s="328" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="519"/>
-      <c r="F16" s="520"/>
-      <c r="G16" s="520"/>
-      <c r="H16" s="520"/>
-      <c r="I16" s="520"/>
-      <c r="J16" s="520"/>
-      <c r="K16" s="520"/>
-      <c r="L16" s="521"/>
-      <c r="M16" s="519"/>
-      <c r="N16" s="520"/>
-      <c r="O16" s="520"/>
-      <c r="P16" s="520"/>
-      <c r="Q16" s="520"/>
-      <c r="R16" s="520"/>
-      <c r="S16" s="520"/>
-      <c r="T16" s="520"/>
-      <c r="U16" s="520"/>
-      <c r="V16" s="520"/>
-      <c r="W16" s="520"/>
-      <c r="X16" s="520"/>
-      <c r="Y16" s="520"/>
-      <c r="Z16" s="520"/>
-      <c r="AA16" s="520"/>
-      <c r="AB16" s="520"/>
-      <c r="AC16" s="520"/>
-      <c r="AD16" s="520"/>
-      <c r="AE16" s="520"/>
-      <c r="AF16" s="520"/>
-      <c r="AG16" s="520"/>
-      <c r="AH16" s="520"/>
-      <c r="AI16" s="520"/>
-      <c r="AJ16" s="520"/>
-      <c r="AK16" s="520"/>
-      <c r="AL16" s="520"/>
-      <c r="AM16" s="521"/>
+      <c r="E16" s="498"/>
+      <c r="F16" s="499"/>
+      <c r="G16" s="499"/>
+      <c r="H16" s="499"/>
+      <c r="I16" s="499"/>
+      <c r="J16" s="499"/>
+      <c r="K16" s="499"/>
+      <c r="L16" s="500"/>
+      <c r="M16" s="498"/>
+      <c r="N16" s="499"/>
+      <c r="O16" s="499"/>
+      <c r="P16" s="499"/>
+      <c r="Q16" s="499"/>
+      <c r="R16" s="499"/>
+      <c r="S16" s="499"/>
+      <c r="T16" s="499"/>
+      <c r="U16" s="499"/>
+      <c r="V16" s="499"/>
+      <c r="W16" s="499"/>
+      <c r="X16" s="499"/>
+      <c r="Y16" s="499"/>
+      <c r="Z16" s="499"/>
+      <c r="AA16" s="499"/>
+      <c r="AB16" s="499"/>
+      <c r="AC16" s="499"/>
+      <c r="AD16" s="499"/>
+      <c r="AE16" s="499"/>
+      <c r="AF16" s="499"/>
+      <c r="AG16" s="499"/>
+      <c r="AH16" s="499"/>
+      <c r="AI16" s="499"/>
+      <c r="AJ16" s="499"/>
+      <c r="AK16" s="499"/>
+      <c r="AL16" s="499"/>
+      <c r="AM16" s="500"/>
       <c r="AN16" s="473"/>
       <c r="AO16" s="321"/>
     </row>
     <row r="17" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="512"/>
+      <c r="A17" s="491"/>
       <c r="B17" s="326"/>
       <c r="C17" s="327" t="s">
         <v>26</v>
@@ -11484,46 +11495,46 @@
       <c r="D17" s="328">
         <v>128</v>
       </c>
-      <c r="E17" s="519"/>
-      <c r="F17" s="520"/>
-      <c r="G17" s="520"/>
-      <c r="H17" s="520"/>
-      <c r="I17" s="520"/>
-      <c r="J17" s="520"/>
-      <c r="K17" s="520"/>
-      <c r="L17" s="521"/>
-      <c r="M17" s="519"/>
-      <c r="N17" s="520"/>
-      <c r="O17" s="520"/>
-      <c r="P17" s="520"/>
-      <c r="Q17" s="520"/>
-      <c r="R17" s="520"/>
-      <c r="S17" s="520"/>
-      <c r="T17" s="520"/>
-      <c r="U17" s="520"/>
-      <c r="V17" s="520"/>
-      <c r="W17" s="520"/>
-      <c r="X17" s="520"/>
-      <c r="Y17" s="520"/>
-      <c r="Z17" s="520"/>
-      <c r="AA17" s="520"/>
-      <c r="AB17" s="520"/>
-      <c r="AC17" s="520"/>
-      <c r="AD17" s="520"/>
-      <c r="AE17" s="520"/>
-      <c r="AF17" s="520"/>
-      <c r="AG17" s="520"/>
-      <c r="AH17" s="520"/>
-      <c r="AI17" s="520"/>
-      <c r="AJ17" s="520"/>
-      <c r="AK17" s="520"/>
-      <c r="AL17" s="520"/>
-      <c r="AM17" s="521"/>
+      <c r="E17" s="498"/>
+      <c r="F17" s="499"/>
+      <c r="G17" s="499"/>
+      <c r="H17" s="499"/>
+      <c r="I17" s="499"/>
+      <c r="J17" s="499"/>
+      <c r="K17" s="499"/>
+      <c r="L17" s="500"/>
+      <c r="M17" s="498"/>
+      <c r="N17" s="499"/>
+      <c r="O17" s="499"/>
+      <c r="P17" s="499"/>
+      <c r="Q17" s="499"/>
+      <c r="R17" s="499"/>
+      <c r="S17" s="499"/>
+      <c r="T17" s="499"/>
+      <c r="U17" s="499"/>
+      <c r="V17" s="499"/>
+      <c r="W17" s="499"/>
+      <c r="X17" s="499"/>
+      <c r="Y17" s="499"/>
+      <c r="Z17" s="499"/>
+      <c r="AA17" s="499"/>
+      <c r="AB17" s="499"/>
+      <c r="AC17" s="499"/>
+      <c r="AD17" s="499"/>
+      <c r="AE17" s="499"/>
+      <c r="AF17" s="499"/>
+      <c r="AG17" s="499"/>
+      <c r="AH17" s="499"/>
+      <c r="AI17" s="499"/>
+      <c r="AJ17" s="499"/>
+      <c r="AK17" s="499"/>
+      <c r="AL17" s="499"/>
+      <c r="AM17" s="500"/>
       <c r="AN17" s="473"/>
       <c r="AO17" s="321"/>
     </row>
     <row r="18" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="512"/>
+      <c r="A18" s="491"/>
       <c r="B18" s="326"/>
       <c r="C18" s="327" t="s">
         <v>27</v>
@@ -11531,46 +11542,46 @@
       <c r="D18" s="328" t="s">
         <v>317</v>
       </c>
-      <c r="E18" s="519"/>
-      <c r="F18" s="520"/>
-      <c r="G18" s="520"/>
-      <c r="H18" s="520"/>
-      <c r="I18" s="520"/>
-      <c r="J18" s="520"/>
-      <c r="K18" s="520"/>
-      <c r="L18" s="521"/>
-      <c r="M18" s="519"/>
-      <c r="N18" s="520"/>
-      <c r="O18" s="520"/>
-      <c r="P18" s="520"/>
-      <c r="Q18" s="520"/>
-      <c r="R18" s="520"/>
-      <c r="S18" s="520"/>
-      <c r="T18" s="520"/>
-      <c r="U18" s="520"/>
-      <c r="V18" s="520"/>
-      <c r="W18" s="520"/>
-      <c r="X18" s="520"/>
-      <c r="Y18" s="520"/>
-      <c r="Z18" s="520"/>
-      <c r="AA18" s="520"/>
-      <c r="AB18" s="520"/>
-      <c r="AC18" s="520"/>
-      <c r="AD18" s="520"/>
-      <c r="AE18" s="520"/>
-      <c r="AF18" s="520"/>
-      <c r="AG18" s="520"/>
-      <c r="AH18" s="520"/>
-      <c r="AI18" s="520"/>
-      <c r="AJ18" s="520"/>
-      <c r="AK18" s="520"/>
-      <c r="AL18" s="520"/>
-      <c r="AM18" s="521"/>
+      <c r="E18" s="498"/>
+      <c r="F18" s="499"/>
+      <c r="G18" s="499"/>
+      <c r="H18" s="499"/>
+      <c r="I18" s="499"/>
+      <c r="J18" s="499"/>
+      <c r="K18" s="499"/>
+      <c r="L18" s="500"/>
+      <c r="M18" s="498"/>
+      <c r="N18" s="499"/>
+      <c r="O18" s="499"/>
+      <c r="P18" s="499"/>
+      <c r="Q18" s="499"/>
+      <c r="R18" s="499"/>
+      <c r="S18" s="499"/>
+      <c r="T18" s="499"/>
+      <c r="U18" s="499"/>
+      <c r="V18" s="499"/>
+      <c r="W18" s="499"/>
+      <c r="X18" s="499"/>
+      <c r="Y18" s="499"/>
+      <c r="Z18" s="499"/>
+      <c r="AA18" s="499"/>
+      <c r="AB18" s="499"/>
+      <c r="AC18" s="499"/>
+      <c r="AD18" s="499"/>
+      <c r="AE18" s="499"/>
+      <c r="AF18" s="499"/>
+      <c r="AG18" s="499"/>
+      <c r="AH18" s="499"/>
+      <c r="AI18" s="499"/>
+      <c r="AJ18" s="499"/>
+      <c r="AK18" s="499"/>
+      <c r="AL18" s="499"/>
+      <c r="AM18" s="500"/>
       <c r="AN18" s="473"/>
       <c r="AO18" s="321"/>
     </row>
     <row r="19" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="512"/>
+      <c r="A19" s="491"/>
       <c r="B19" s="326"/>
       <c r="C19" s="327" t="s">
         <v>28</v>
@@ -11578,46 +11589,46 @@
       <c r="D19" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="519"/>
-      <c r="F19" s="520"/>
-      <c r="G19" s="520"/>
-      <c r="H19" s="520"/>
-      <c r="I19" s="520"/>
-      <c r="J19" s="520"/>
-      <c r="K19" s="520"/>
-      <c r="L19" s="521"/>
-      <c r="M19" s="519"/>
-      <c r="N19" s="520"/>
-      <c r="O19" s="520"/>
-      <c r="P19" s="520"/>
-      <c r="Q19" s="520"/>
-      <c r="R19" s="520"/>
-      <c r="S19" s="520"/>
-      <c r="T19" s="520"/>
-      <c r="U19" s="520"/>
-      <c r="V19" s="520"/>
-      <c r="W19" s="520"/>
-      <c r="X19" s="520"/>
-      <c r="Y19" s="520"/>
-      <c r="Z19" s="520"/>
-      <c r="AA19" s="520"/>
-      <c r="AB19" s="520"/>
-      <c r="AC19" s="520"/>
-      <c r="AD19" s="520"/>
-      <c r="AE19" s="520"/>
-      <c r="AF19" s="520"/>
-      <c r="AG19" s="520"/>
-      <c r="AH19" s="520"/>
-      <c r="AI19" s="520"/>
-      <c r="AJ19" s="520"/>
-      <c r="AK19" s="520"/>
-      <c r="AL19" s="520"/>
-      <c r="AM19" s="521"/>
+      <c r="E19" s="498"/>
+      <c r="F19" s="499"/>
+      <c r="G19" s="499"/>
+      <c r="H19" s="499"/>
+      <c r="I19" s="499"/>
+      <c r="J19" s="499"/>
+      <c r="K19" s="499"/>
+      <c r="L19" s="500"/>
+      <c r="M19" s="498"/>
+      <c r="N19" s="499"/>
+      <c r="O19" s="499"/>
+      <c r="P19" s="499"/>
+      <c r="Q19" s="499"/>
+      <c r="R19" s="499"/>
+      <c r="S19" s="499"/>
+      <c r="T19" s="499"/>
+      <c r="U19" s="499"/>
+      <c r="V19" s="499"/>
+      <c r="W19" s="499"/>
+      <c r="X19" s="499"/>
+      <c r="Y19" s="499"/>
+      <c r="Z19" s="499"/>
+      <c r="AA19" s="499"/>
+      <c r="AB19" s="499"/>
+      <c r="AC19" s="499"/>
+      <c r="AD19" s="499"/>
+      <c r="AE19" s="499"/>
+      <c r="AF19" s="499"/>
+      <c r="AG19" s="499"/>
+      <c r="AH19" s="499"/>
+      <c r="AI19" s="499"/>
+      <c r="AJ19" s="499"/>
+      <c r="AK19" s="499"/>
+      <c r="AL19" s="499"/>
+      <c r="AM19" s="500"/>
       <c r="AN19" s="473"/>
       <c r="AO19" s="321"/>
     </row>
     <row r="20" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="512"/>
+      <c r="A20" s="491"/>
       <c r="B20" s="326" t="s">
         <v>97</v>
       </c>
@@ -11627,46 +11638,46 @@
       <c r="D20" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="519"/>
-      <c r="F20" s="520"/>
-      <c r="G20" s="520"/>
-      <c r="H20" s="520"/>
-      <c r="I20" s="520"/>
-      <c r="J20" s="520"/>
-      <c r="K20" s="520"/>
-      <c r="L20" s="521"/>
-      <c r="M20" s="519"/>
-      <c r="N20" s="520"/>
-      <c r="O20" s="520"/>
-      <c r="P20" s="520"/>
-      <c r="Q20" s="520"/>
-      <c r="R20" s="520"/>
-      <c r="S20" s="520"/>
-      <c r="T20" s="520"/>
-      <c r="U20" s="520"/>
-      <c r="V20" s="520"/>
-      <c r="W20" s="520"/>
-      <c r="X20" s="520"/>
-      <c r="Y20" s="520"/>
-      <c r="Z20" s="520"/>
-      <c r="AA20" s="520"/>
-      <c r="AB20" s="520"/>
-      <c r="AC20" s="520"/>
-      <c r="AD20" s="520"/>
-      <c r="AE20" s="520"/>
-      <c r="AF20" s="520"/>
-      <c r="AG20" s="520"/>
-      <c r="AH20" s="520"/>
-      <c r="AI20" s="520"/>
-      <c r="AJ20" s="520"/>
-      <c r="AK20" s="520"/>
-      <c r="AL20" s="520"/>
-      <c r="AM20" s="521"/>
+      <c r="E20" s="498"/>
+      <c r="F20" s="499"/>
+      <c r="G20" s="499"/>
+      <c r="H20" s="499"/>
+      <c r="I20" s="499"/>
+      <c r="J20" s="499"/>
+      <c r="K20" s="499"/>
+      <c r="L20" s="500"/>
+      <c r="M20" s="498"/>
+      <c r="N20" s="499"/>
+      <c r="O20" s="499"/>
+      <c r="P20" s="499"/>
+      <c r="Q20" s="499"/>
+      <c r="R20" s="499"/>
+      <c r="S20" s="499"/>
+      <c r="T20" s="499"/>
+      <c r="U20" s="499"/>
+      <c r="V20" s="499"/>
+      <c r="W20" s="499"/>
+      <c r="X20" s="499"/>
+      <c r="Y20" s="499"/>
+      <c r="Z20" s="499"/>
+      <c r="AA20" s="499"/>
+      <c r="AB20" s="499"/>
+      <c r="AC20" s="499"/>
+      <c r="AD20" s="499"/>
+      <c r="AE20" s="499"/>
+      <c r="AF20" s="499"/>
+      <c r="AG20" s="499"/>
+      <c r="AH20" s="499"/>
+      <c r="AI20" s="499"/>
+      <c r="AJ20" s="499"/>
+      <c r="AK20" s="499"/>
+      <c r="AL20" s="499"/>
+      <c r="AM20" s="500"/>
       <c r="AN20" s="473"/>
       <c r="AO20" s="321"/>
     </row>
     <row r="21" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="512"/>
+      <c r="A21" s="491"/>
       <c r="B21" s="326" t="s">
         <v>45</v>
       </c>
@@ -11676,46 +11687,46 @@
       <c r="D21" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="519"/>
-      <c r="F21" s="520"/>
-      <c r="G21" s="520"/>
-      <c r="H21" s="520"/>
-      <c r="I21" s="520"/>
-      <c r="J21" s="520"/>
-      <c r="K21" s="520"/>
-      <c r="L21" s="521"/>
-      <c r="M21" s="519"/>
-      <c r="N21" s="520"/>
-      <c r="O21" s="520"/>
-      <c r="P21" s="520"/>
-      <c r="Q21" s="520"/>
-      <c r="R21" s="520"/>
-      <c r="S21" s="520"/>
-      <c r="T21" s="520"/>
-      <c r="U21" s="520"/>
-      <c r="V21" s="520"/>
-      <c r="W21" s="520"/>
-      <c r="X21" s="520"/>
-      <c r="Y21" s="520"/>
-      <c r="Z21" s="520"/>
-      <c r="AA21" s="520"/>
-      <c r="AB21" s="520"/>
-      <c r="AC21" s="520"/>
-      <c r="AD21" s="520"/>
-      <c r="AE21" s="520"/>
-      <c r="AF21" s="520"/>
-      <c r="AG21" s="520"/>
-      <c r="AH21" s="520"/>
-      <c r="AI21" s="520"/>
-      <c r="AJ21" s="520"/>
-      <c r="AK21" s="520"/>
-      <c r="AL21" s="520"/>
-      <c r="AM21" s="521"/>
+      <c r="E21" s="498"/>
+      <c r="F21" s="499"/>
+      <c r="G21" s="499"/>
+      <c r="H21" s="499"/>
+      <c r="I21" s="499"/>
+      <c r="J21" s="499"/>
+      <c r="K21" s="499"/>
+      <c r="L21" s="500"/>
+      <c r="M21" s="498"/>
+      <c r="N21" s="499"/>
+      <c r="O21" s="499"/>
+      <c r="P21" s="499"/>
+      <c r="Q21" s="499"/>
+      <c r="R21" s="499"/>
+      <c r="S21" s="499"/>
+      <c r="T21" s="499"/>
+      <c r="U21" s="499"/>
+      <c r="V21" s="499"/>
+      <c r="W21" s="499"/>
+      <c r="X21" s="499"/>
+      <c r="Y21" s="499"/>
+      <c r="Z21" s="499"/>
+      <c r="AA21" s="499"/>
+      <c r="AB21" s="499"/>
+      <c r="AC21" s="499"/>
+      <c r="AD21" s="499"/>
+      <c r="AE21" s="499"/>
+      <c r="AF21" s="499"/>
+      <c r="AG21" s="499"/>
+      <c r="AH21" s="499"/>
+      <c r="AI21" s="499"/>
+      <c r="AJ21" s="499"/>
+      <c r="AK21" s="499"/>
+      <c r="AL21" s="499"/>
+      <c r="AM21" s="500"/>
       <c r="AN21" s="473"/>
       <c r="AO21" s="322"/>
     </row>
     <row r="22" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="512"/>
+      <c r="A22" s="491"/>
       <c r="B22" s="326"/>
       <c r="C22" s="327" t="s">
         <v>318</v>
@@ -11723,46 +11734,46 @@
       <c r="D22" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="519"/>
-      <c r="F22" s="520"/>
-      <c r="G22" s="520"/>
-      <c r="H22" s="520"/>
-      <c r="I22" s="520"/>
-      <c r="J22" s="520"/>
-      <c r="K22" s="520"/>
-      <c r="L22" s="521"/>
-      <c r="M22" s="519"/>
-      <c r="N22" s="520"/>
-      <c r="O22" s="520"/>
-      <c r="P22" s="520"/>
-      <c r="Q22" s="520"/>
-      <c r="R22" s="520"/>
-      <c r="S22" s="520"/>
-      <c r="T22" s="520"/>
-      <c r="U22" s="520"/>
-      <c r="V22" s="520"/>
-      <c r="W22" s="520"/>
-      <c r="X22" s="520"/>
-      <c r="Y22" s="520"/>
-      <c r="Z22" s="520"/>
-      <c r="AA22" s="520"/>
-      <c r="AB22" s="520"/>
-      <c r="AC22" s="520"/>
-      <c r="AD22" s="520"/>
-      <c r="AE22" s="520"/>
-      <c r="AF22" s="520"/>
-      <c r="AG22" s="520"/>
-      <c r="AH22" s="520"/>
-      <c r="AI22" s="520"/>
-      <c r="AJ22" s="520"/>
-      <c r="AK22" s="520"/>
-      <c r="AL22" s="520"/>
-      <c r="AM22" s="521"/>
+      <c r="E22" s="498"/>
+      <c r="F22" s="499"/>
+      <c r="G22" s="499"/>
+      <c r="H22" s="499"/>
+      <c r="I22" s="499"/>
+      <c r="J22" s="499"/>
+      <c r="K22" s="499"/>
+      <c r="L22" s="500"/>
+      <c r="M22" s="498"/>
+      <c r="N22" s="499"/>
+      <c r="O22" s="499"/>
+      <c r="P22" s="499"/>
+      <c r="Q22" s="499"/>
+      <c r="R22" s="499"/>
+      <c r="S22" s="499"/>
+      <c r="T22" s="499"/>
+      <c r="U22" s="499"/>
+      <c r="V22" s="499"/>
+      <c r="W22" s="499"/>
+      <c r="X22" s="499"/>
+      <c r="Y22" s="499"/>
+      <c r="Z22" s="499"/>
+      <c r="AA22" s="499"/>
+      <c r="AB22" s="499"/>
+      <c r="AC22" s="499"/>
+      <c r="AD22" s="499"/>
+      <c r="AE22" s="499"/>
+      <c r="AF22" s="499"/>
+      <c r="AG22" s="499"/>
+      <c r="AH22" s="499"/>
+      <c r="AI22" s="499"/>
+      <c r="AJ22" s="499"/>
+      <c r="AK22" s="499"/>
+      <c r="AL22" s="499"/>
+      <c r="AM22" s="500"/>
       <c r="AN22" s="473"/>
       <c r="AO22" s="322"/>
     </row>
     <row r="23" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="512"/>
+      <c r="A23" s="491"/>
       <c r="B23" s="326"/>
       <c r="C23" s="327" t="s">
         <v>290</v>
@@ -11770,46 +11781,46 @@
       <c r="D23" s="328" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="519"/>
-      <c r="F23" s="520"/>
-      <c r="G23" s="520"/>
-      <c r="H23" s="520"/>
-      <c r="I23" s="520"/>
-      <c r="J23" s="520"/>
-      <c r="K23" s="520"/>
-      <c r="L23" s="521"/>
-      <c r="M23" s="519"/>
-      <c r="N23" s="520"/>
-      <c r="O23" s="520"/>
-      <c r="P23" s="520"/>
-      <c r="Q23" s="520"/>
-      <c r="R23" s="520"/>
-      <c r="S23" s="520"/>
-      <c r="T23" s="520"/>
-      <c r="U23" s="520"/>
-      <c r="V23" s="520"/>
-      <c r="W23" s="520"/>
-      <c r="X23" s="520"/>
-      <c r="Y23" s="520"/>
-      <c r="Z23" s="520"/>
-      <c r="AA23" s="520"/>
-      <c r="AB23" s="520"/>
-      <c r="AC23" s="520"/>
-      <c r="AD23" s="520"/>
-      <c r="AE23" s="520"/>
-      <c r="AF23" s="520"/>
-      <c r="AG23" s="520"/>
-      <c r="AH23" s="520"/>
-      <c r="AI23" s="520"/>
-      <c r="AJ23" s="520"/>
-      <c r="AK23" s="520"/>
-      <c r="AL23" s="520"/>
-      <c r="AM23" s="521"/>
+      <c r="E23" s="498"/>
+      <c r="F23" s="499"/>
+      <c r="G23" s="499"/>
+      <c r="H23" s="499"/>
+      <c r="I23" s="499"/>
+      <c r="J23" s="499"/>
+      <c r="K23" s="499"/>
+      <c r="L23" s="500"/>
+      <c r="M23" s="498"/>
+      <c r="N23" s="499"/>
+      <c r="O23" s="499"/>
+      <c r="P23" s="499"/>
+      <c r="Q23" s="499"/>
+      <c r="R23" s="499"/>
+      <c r="S23" s="499"/>
+      <c r="T23" s="499"/>
+      <c r="U23" s="499"/>
+      <c r="V23" s="499"/>
+      <c r="W23" s="499"/>
+      <c r="X23" s="499"/>
+      <c r="Y23" s="499"/>
+      <c r="Z23" s="499"/>
+      <c r="AA23" s="499"/>
+      <c r="AB23" s="499"/>
+      <c r="AC23" s="499"/>
+      <c r="AD23" s="499"/>
+      <c r="AE23" s="499"/>
+      <c r="AF23" s="499"/>
+      <c r="AG23" s="499"/>
+      <c r="AH23" s="499"/>
+      <c r="AI23" s="499"/>
+      <c r="AJ23" s="499"/>
+      <c r="AK23" s="499"/>
+      <c r="AL23" s="499"/>
+      <c r="AM23" s="500"/>
       <c r="AN23" s="473"/>
       <c r="AO23" s="322"/>
     </row>
     <row r="24" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="512"/>
+      <c r="A24" s="491"/>
       <c r="B24" s="326"/>
       <c r="C24" s="327" t="s">
         <v>184</v>
@@ -11817,46 +11828,46 @@
       <c r="D24" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="519"/>
-      <c r="F24" s="520"/>
-      <c r="G24" s="520"/>
-      <c r="H24" s="520"/>
-      <c r="I24" s="520"/>
-      <c r="J24" s="520"/>
-      <c r="K24" s="520"/>
-      <c r="L24" s="521"/>
-      <c r="M24" s="519"/>
-      <c r="N24" s="520"/>
-      <c r="O24" s="520"/>
-      <c r="P24" s="520"/>
-      <c r="Q24" s="520"/>
-      <c r="R24" s="520"/>
-      <c r="S24" s="520"/>
-      <c r="T24" s="520"/>
-      <c r="U24" s="520"/>
-      <c r="V24" s="520"/>
-      <c r="W24" s="520"/>
-      <c r="X24" s="520"/>
-      <c r="Y24" s="520"/>
-      <c r="Z24" s="520"/>
-      <c r="AA24" s="520"/>
-      <c r="AB24" s="520"/>
-      <c r="AC24" s="520"/>
-      <c r="AD24" s="520"/>
-      <c r="AE24" s="520"/>
-      <c r="AF24" s="520"/>
-      <c r="AG24" s="520"/>
-      <c r="AH24" s="520"/>
-      <c r="AI24" s="520"/>
-      <c r="AJ24" s="520"/>
-      <c r="AK24" s="520"/>
-      <c r="AL24" s="520"/>
-      <c r="AM24" s="521"/>
+      <c r="E24" s="498"/>
+      <c r="F24" s="499"/>
+      <c r="G24" s="499"/>
+      <c r="H24" s="499"/>
+      <c r="I24" s="499"/>
+      <c r="J24" s="499"/>
+      <c r="K24" s="499"/>
+      <c r="L24" s="500"/>
+      <c r="M24" s="498"/>
+      <c r="N24" s="499"/>
+      <c r="O24" s="499"/>
+      <c r="P24" s="499"/>
+      <c r="Q24" s="499"/>
+      <c r="R24" s="499"/>
+      <c r="S24" s="499"/>
+      <c r="T24" s="499"/>
+      <c r="U24" s="499"/>
+      <c r="V24" s="499"/>
+      <c r="W24" s="499"/>
+      <c r="X24" s="499"/>
+      <c r="Y24" s="499"/>
+      <c r="Z24" s="499"/>
+      <c r="AA24" s="499"/>
+      <c r="AB24" s="499"/>
+      <c r="AC24" s="499"/>
+      <c r="AD24" s="499"/>
+      <c r="AE24" s="499"/>
+      <c r="AF24" s="499"/>
+      <c r="AG24" s="499"/>
+      <c r="AH24" s="499"/>
+      <c r="AI24" s="499"/>
+      <c r="AJ24" s="499"/>
+      <c r="AK24" s="499"/>
+      <c r="AL24" s="499"/>
+      <c r="AM24" s="500"/>
       <c r="AN24" s="473"/>
       <c r="AO24" s="322"/>
     </row>
     <row r="25" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="512"/>
+      <c r="A25" s="491"/>
       <c r="B25" s="326"/>
       <c r="C25" s="327" t="s">
         <v>72</v>
@@ -11864,46 +11875,46 @@
       <c r="D25" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="519"/>
-      <c r="F25" s="520"/>
-      <c r="G25" s="520"/>
-      <c r="H25" s="520"/>
-      <c r="I25" s="520"/>
-      <c r="J25" s="520"/>
-      <c r="K25" s="520"/>
-      <c r="L25" s="521"/>
-      <c r="M25" s="519"/>
-      <c r="N25" s="520"/>
-      <c r="O25" s="520"/>
-      <c r="P25" s="520"/>
-      <c r="Q25" s="520"/>
-      <c r="R25" s="520"/>
-      <c r="S25" s="520"/>
-      <c r="T25" s="520"/>
-      <c r="U25" s="520"/>
-      <c r="V25" s="520"/>
-      <c r="W25" s="520"/>
-      <c r="X25" s="520"/>
-      <c r="Y25" s="520"/>
-      <c r="Z25" s="520"/>
-      <c r="AA25" s="520"/>
-      <c r="AB25" s="520"/>
-      <c r="AC25" s="520"/>
-      <c r="AD25" s="520"/>
-      <c r="AE25" s="520"/>
-      <c r="AF25" s="520"/>
-      <c r="AG25" s="520"/>
-      <c r="AH25" s="520"/>
-      <c r="AI25" s="520"/>
-      <c r="AJ25" s="520"/>
-      <c r="AK25" s="520"/>
-      <c r="AL25" s="520"/>
-      <c r="AM25" s="521"/>
+      <c r="E25" s="498"/>
+      <c r="F25" s="499"/>
+      <c r="G25" s="499"/>
+      <c r="H25" s="499"/>
+      <c r="I25" s="499"/>
+      <c r="J25" s="499"/>
+      <c r="K25" s="499"/>
+      <c r="L25" s="500"/>
+      <c r="M25" s="498"/>
+      <c r="N25" s="499"/>
+      <c r="O25" s="499"/>
+      <c r="P25" s="499"/>
+      <c r="Q25" s="499"/>
+      <c r="R25" s="499"/>
+      <c r="S25" s="499"/>
+      <c r="T25" s="499"/>
+      <c r="U25" s="499"/>
+      <c r="V25" s="499"/>
+      <c r="W25" s="499"/>
+      <c r="X25" s="499"/>
+      <c r="Y25" s="499"/>
+      <c r="Z25" s="499"/>
+      <c r="AA25" s="499"/>
+      <c r="AB25" s="499"/>
+      <c r="AC25" s="499"/>
+      <c r="AD25" s="499"/>
+      <c r="AE25" s="499"/>
+      <c r="AF25" s="499"/>
+      <c r="AG25" s="499"/>
+      <c r="AH25" s="499"/>
+      <c r="AI25" s="499"/>
+      <c r="AJ25" s="499"/>
+      <c r="AK25" s="499"/>
+      <c r="AL25" s="499"/>
+      <c r="AM25" s="500"/>
       <c r="AN25" s="473"/>
       <c r="AO25" s="322"/>
     </row>
     <row r="26" spans="1:41" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="512"/>
+      <c r="A26" s="491"/>
       <c r="B26" s="330"/>
       <c r="C26" s="331" t="s">
         <v>74</v>
@@ -11911,53 +11922,53 @@
       <c r="D26" s="332" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="522"/>
-      <c r="F26" s="523"/>
-      <c r="G26" s="523"/>
-      <c r="H26" s="523"/>
-      <c r="I26" s="523"/>
-      <c r="J26" s="523"/>
-      <c r="K26" s="523"/>
-      <c r="L26" s="524"/>
-      <c r="M26" s="522"/>
-      <c r="N26" s="523"/>
-      <c r="O26" s="523"/>
-      <c r="P26" s="523"/>
-      <c r="Q26" s="523"/>
-      <c r="R26" s="523"/>
-      <c r="S26" s="523"/>
-      <c r="T26" s="523"/>
-      <c r="U26" s="523"/>
-      <c r="V26" s="523"/>
-      <c r="W26" s="523"/>
-      <c r="X26" s="523"/>
-      <c r="Y26" s="523"/>
-      <c r="Z26" s="523"/>
-      <c r="AA26" s="523"/>
-      <c r="AB26" s="523"/>
-      <c r="AC26" s="523"/>
-      <c r="AD26" s="523"/>
-      <c r="AE26" s="523"/>
-      <c r="AF26" s="523"/>
-      <c r="AG26" s="523"/>
-      <c r="AH26" s="523"/>
-      <c r="AI26" s="523"/>
-      <c r="AJ26" s="523"/>
-      <c r="AK26" s="523"/>
-      <c r="AL26" s="520"/>
-      <c r="AM26" s="521"/>
+      <c r="E26" s="501"/>
+      <c r="F26" s="502"/>
+      <c r="G26" s="502"/>
+      <c r="H26" s="502"/>
+      <c r="I26" s="502"/>
+      <c r="J26" s="502"/>
+      <c r="K26" s="502"/>
+      <c r="L26" s="503"/>
+      <c r="M26" s="501"/>
+      <c r="N26" s="502"/>
+      <c r="O26" s="502"/>
+      <c r="P26" s="502"/>
+      <c r="Q26" s="502"/>
+      <c r="R26" s="502"/>
+      <c r="S26" s="502"/>
+      <c r="T26" s="502"/>
+      <c r="U26" s="502"/>
+      <c r="V26" s="502"/>
+      <c r="W26" s="502"/>
+      <c r="X26" s="502"/>
+      <c r="Y26" s="502"/>
+      <c r="Z26" s="502"/>
+      <c r="AA26" s="502"/>
+      <c r="AB26" s="502"/>
+      <c r="AC26" s="502"/>
+      <c r="AD26" s="502"/>
+      <c r="AE26" s="502"/>
+      <c r="AF26" s="502"/>
+      <c r="AG26" s="502"/>
+      <c r="AH26" s="502"/>
+      <c r="AI26" s="502"/>
+      <c r="AJ26" s="502"/>
+      <c r="AK26" s="502"/>
+      <c r="AL26" s="499"/>
+      <c r="AM26" s="500"/>
       <c r="AN26" s="473"/>
       <c r="AO26" s="322"/>
     </row>
     <row r="27" spans="1:41" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="512"/>
+      <c r="A27" s="491"/>
       <c r="B27" s="41" t="s">
         <v>293</v>
       </c>
       <c r="C27" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="513" t="s">
+      <c r="D27" s="492" t="s">
         <v>363</v>
       </c>
       <c r="E27" s="102"/>
@@ -12055,12 +12066,12 @@
       <c r="AO27" s="66"/>
     </row>
     <row r="28" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="512"/>
+      <c r="A28" s="491"/>
       <c r="B28" s="47"/>
       <c r="C28" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="514"/>
+      <c r="D28" s="493"/>
       <c r="E28" s="103"/>
       <c r="F28" s="31"/>
       <c r="G28" s="31"/>
@@ -12156,12 +12167,12 @@
       <c r="AO28" s="179"/>
     </row>
     <row r="29" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="512"/>
+      <c r="A29" s="491"/>
       <c r="B29" s="47"/>
       <c r="C29" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D29" s="514"/>
+      <c r="D29" s="493"/>
       <c r="E29" s="103"/>
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
@@ -12257,12 +12268,12 @@
       <c r="AO29" s="179"/>
     </row>
     <row r="30" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="512"/>
+      <c r="A30" s="491"/>
       <c r="B30" s="47"/>
       <c r="C30" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D30" s="514"/>
+      <c r="D30" s="493"/>
       <c r="E30" s="103"/>
       <c r="F30" s="31"/>
       <c r="G30" s="31"/>
@@ -12360,12 +12371,12 @@
       </c>
     </row>
     <row r="31" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="512"/>
+      <c r="A31" s="491"/>
       <c r="B31" s="47"/>
       <c r="C31" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D31" s="514"/>
+      <c r="D31" s="493"/>
       <c r="E31" s="103"/>
       <c r="F31" s="31"/>
       <c r="G31" s="31"/>
@@ -12461,12 +12472,12 @@
       <c r="AO31" s="179"/>
     </row>
     <row r="32" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="512"/>
+      <c r="A32" s="491"/>
       <c r="B32" s="47"/>
       <c r="C32" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="D32" s="514"/>
+      <c r="D32" s="493"/>
       <c r="E32" s="103"/>
       <c r="F32" s="31"/>
       <c r="G32" s="31"/>
@@ -12562,12 +12573,12 @@
       <c r="AO32" s="179"/>
     </row>
     <row r="33" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="512"/>
+      <c r="A33" s="491"/>
       <c r="B33" s="47"/>
       <c r="C33" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="514"/>
+      <c r="D33" s="493"/>
       <c r="E33" s="103"/>
       <c r="F33" s="31"/>
       <c r="G33" s="31"/>
@@ -12663,12 +12674,12 @@
       <c r="AO33" s="179"/>
     </row>
     <row r="34" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="512"/>
+      <c r="A34" s="491"/>
       <c r="B34" s="47"/>
       <c r="C34" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D34" s="514"/>
+      <c r="D34" s="493"/>
       <c r="E34" s="103"/>
       <c r="F34" s="31"/>
       <c r="G34" s="31"/>
@@ -12734,12 +12745,12 @@
       <c r="AO34" s="180"/>
     </row>
     <row r="35" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="512"/>
+      <c r="A35" s="491"/>
       <c r="B35" s="47"/>
       <c r="C35" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="514"/>
+      <c r="D35" s="493"/>
       <c r="E35" s="103"/>
       <c r="F35" s="31"/>
       <c r="G35" s="31"/>
@@ -12835,12 +12846,12 @@
       <c r="AO35" s="179"/>
     </row>
     <row r="36" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="512"/>
+      <c r="A36" s="491"/>
       <c r="B36" s="47"/>
       <c r="C36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="514"/>
+      <c r="D36" s="493"/>
       <c r="E36" s="103"/>
       <c r="F36" s="31"/>
       <c r="G36" s="31"/>
@@ -12922,12 +12933,12 @@
       <c r="AO36" s="179"/>
     </row>
     <row r="37" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="512"/>
+      <c r="A37" s="491"/>
       <c r="B37" s="47"/>
       <c r="C37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="514"/>
+      <c r="D37" s="493"/>
       <c r="E37" s="103"/>
       <c r="F37" s="31"/>
       <c r="G37" s="31"/>
@@ -13011,12 +13022,12 @@
       </c>
     </row>
     <row r="38" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="512"/>
+      <c r="A38" s="491"/>
       <c r="B38" s="47"/>
       <c r="C38" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="D38" s="514"/>
+      <c r="D38" s="493"/>
       <c r="E38" s="103"/>
       <c r="F38" s="31"/>
       <c r="G38" s="31"/>
@@ -13090,12 +13101,12 @@
       <c r="AO38" s="179"/>
     </row>
     <row r="39" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="512"/>
+      <c r="A39" s="491"/>
       <c r="B39" s="49"/>
       <c r="C39" s="305" t="s">
         <v>272</v>
       </c>
-      <c r="D39" s="514"/>
+      <c r="D39" s="493"/>
       <c r="E39" s="306"/>
       <c r="F39" s="307"/>
       <c r="G39" s="307"/>
@@ -13135,12 +13146,12 @@
       <c r="AO39" s="183"/>
     </row>
     <row r="40" spans="1:42" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="512"/>
+      <c r="A40" s="491"/>
       <c r="B40" s="67"/>
       <c r="C40" s="421" t="s">
         <v>436</v>
       </c>
-      <c r="D40" s="514"/>
+      <c r="D40" s="493"/>
       <c r="E40" s="105"/>
       <c r="F40" s="69"/>
       <c r="G40" s="69"/>
@@ -13206,14 +13217,14 @@
       <c r="AO40" s="181"/>
     </row>
     <row r="41" spans="1:42" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="512"/>
+      <c r="A41" s="491"/>
       <c r="B41" s="48" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="D41" s="514"/>
+      <c r="D41" s="493"/>
       <c r="E41" s="109"/>
       <c r="F41" s="40"/>
       <c r="G41" s="40"/>
@@ -13298,10 +13309,10 @@
         <v>25</v>
       </c>
       <c r="AL41" s="411" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AM41" s="376" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AN41" s="486" t="s">
         <v>24</v>
@@ -13309,12 +13320,12 @@
       <c r="AO41" s="182"/>
     </row>
     <row r="42" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="512"/>
+      <c r="A42" s="491"/>
       <c r="B42" s="47"/>
       <c r="C42" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="514"/>
+      <c r="D42" s="493"/>
       <c r="E42" s="103"/>
       <c r="F42" s="31"/>
       <c r="G42" s="31"/>
@@ -13370,12 +13381,12 @@
       <c r="AO42" s="179"/>
     </row>
     <row r="43" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="512"/>
+      <c r="A43" s="491"/>
       <c r="B43" s="47"/>
       <c r="C43" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="D43" s="514"/>
+      <c r="D43" s="493"/>
       <c r="E43" s="103"/>
       <c r="F43" s="31"/>
       <c r="G43" s="31"/>
@@ -13431,12 +13442,12 @@
       <c r="AO43" s="179"/>
     </row>
     <row r="44" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="512"/>
+      <c r="A44" s="491"/>
       <c r="B44" s="49"/>
       <c r="C44" s="420" t="s">
         <v>495</v>
       </c>
-      <c r="D44" s="514"/>
+      <c r="D44" s="493"/>
       <c r="E44" s="306"/>
       <c r="F44" s="307"/>
       <c r="G44" s="307"/>
@@ -13532,12 +13543,12 @@
       <c r="AO44" s="183"/>
     </row>
     <row r="45" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="512"/>
+      <c r="A45" s="491"/>
       <c r="B45" s="49"/>
       <c r="C45" s="420" t="s">
         <v>496</v>
       </c>
-      <c r="D45" s="514"/>
+      <c r="D45" s="493"/>
       <c r="E45" s="306"/>
       <c r="F45" s="307"/>
       <c r="G45" s="307"/>
@@ -13577,12 +13588,12 @@
       <c r="AO45" s="183"/>
     </row>
     <row r="46" spans="1:42" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="512"/>
+      <c r="A46" s="491"/>
       <c r="B46" s="67"/>
       <c r="C46" s="68" t="s">
         <v>275</v>
       </c>
-      <c r="D46" s="514"/>
+      <c r="D46" s="493"/>
       <c r="E46" s="105"/>
       <c r="F46" s="69"/>
       <c r="G46" s="69"/>
@@ -13648,14 +13659,14 @@
       <c r="AO46" s="181"/>
     </row>
     <row r="47" spans="1:42" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="512"/>
+      <c r="A47" s="491"/>
       <c r="B47" s="41" t="s">
         <v>97</v>
       </c>
       <c r="C47" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="D47" s="514"/>
+      <c r="D47" s="493"/>
       <c r="E47" s="102"/>
       <c r="F47" s="43"/>
       <c r="G47" s="43"/>
@@ -13753,12 +13764,12 @@
       </c>
     </row>
     <row r="48" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="512"/>
+      <c r="A48" s="491"/>
       <c r="B48" s="47"/>
       <c r="C48" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="514"/>
+      <c r="D48" s="493"/>
       <c r="E48" s="103"/>
       <c r="F48" s="31"/>
       <c r="G48" s="31"/>
@@ -13859,12 +13870,12 @@
       </c>
     </row>
     <row r="49" spans="1:41" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="512"/>
+      <c r="A49" s="491"/>
       <c r="B49" s="381"/>
       <c r="C49" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D49" s="514"/>
+      <c r="D49" s="493"/>
       <c r="E49" s="116"/>
       <c r="F49" s="32"/>
       <c r="G49" s="32"/>
@@ -13930,12 +13941,12 @@
       <c r="AO49" s="180"/>
     </row>
     <row r="50" spans="1:41" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="512"/>
+      <c r="A50" s="491"/>
       <c r="B50" s="368"/>
       <c r="C50" s="369" t="s">
         <v>458</v>
       </c>
-      <c r="D50" s="514"/>
+      <c r="D50" s="493"/>
       <c r="E50" s="370"/>
       <c r="F50" s="371"/>
       <c r="G50" s="371"/>
@@ -14031,14 +14042,14 @@
       <c r="AO50" s="374"/>
     </row>
     <row r="51" spans="1:41" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="512"/>
+      <c r="A51" s="491"/>
       <c r="B51" s="41" t="s">
         <v>35</v>
       </c>
       <c r="C51" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="514"/>
+      <c r="D51" s="493"/>
       <c r="E51" s="102" t="s">
         <v>18</v>
       </c>
@@ -14150,12 +14161,12 @@
       <c r="AO51" s="66"/>
     </row>
     <row r="52" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="512"/>
+      <c r="A52" s="491"/>
       <c r="B52" s="48"/>
       <c r="C52" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="D52" s="514"/>
+      <c r="D52" s="493"/>
       <c r="E52" s="107"/>
       <c r="F52" s="40" t="s">
         <v>9</v>
@@ -14265,12 +14276,12 @@
       <c r="AO52" s="182"/>
     </row>
     <row r="53" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="512"/>
+      <c r="A53" s="491"/>
       <c r="B53" s="48"/>
       <c r="C53" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="D53" s="514"/>
+      <c r="D53" s="493"/>
       <c r="E53" s="109" t="s">
         <v>9</v>
       </c>
@@ -14382,12 +14393,12 @@
       <c r="AO53" s="182"/>
     </row>
     <row r="54" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="512"/>
+      <c r="A54" s="491"/>
       <c r="B54" s="47"/>
       <c r="C54" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="D54" s="514"/>
+      <c r="D54" s="493"/>
       <c r="E54" s="103" t="s">
         <v>9</v>
       </c>
@@ -14499,12 +14510,12 @@
       <c r="AO54" s="179"/>
     </row>
     <row r="55" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="512"/>
+      <c r="A55" s="491"/>
       <c r="B55" s="47"/>
       <c r="C55" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="D55" s="514"/>
+      <c r="D55" s="493"/>
       <c r="E55" s="110"/>
       <c r="F55" s="35"/>
       <c r="G55" s="35"/>
@@ -14586,12 +14597,12 @@
       </c>
     </row>
     <row r="56" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="512"/>
+      <c r="A56" s="491"/>
       <c r="B56" s="47"/>
       <c r="C56" s="198" t="s">
         <v>271</v>
       </c>
-      <c r="D56" s="514"/>
+      <c r="D56" s="493"/>
       <c r="E56" s="103" t="s">
         <v>18</v>
       </c>
@@ -14703,12 +14714,12 @@
       <c r="AO56" s="179"/>
     </row>
     <row r="57" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="512"/>
+      <c r="A57" s="491"/>
       <c r="B57" s="47"/>
       <c r="C57" s="198" t="s">
         <v>454</v>
       </c>
-      <c r="D57" s="514"/>
+      <c r="D57" s="493"/>
       <c r="E57" s="103" t="s">
         <v>48</v>
       </c>
@@ -14820,12 +14831,12 @@
       <c r="AO57" s="179"/>
     </row>
     <row r="58" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="512"/>
+      <c r="A58" s="491"/>
       <c r="B58" s="47"/>
       <c r="C58" s="199" t="s">
         <v>474</v>
       </c>
-      <c r="D58" s="514"/>
+      <c r="D58" s="493"/>
       <c r="E58" s="110"/>
       <c r="F58" s="35"/>
       <c r="G58" s="35"/>
@@ -14907,12 +14918,12 @@
       </c>
     </row>
     <row r="59" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="512"/>
+      <c r="A59" s="491"/>
       <c r="B59" s="47"/>
       <c r="C59" s="198" t="s">
         <v>37</v>
       </c>
-      <c r="D59" s="514"/>
+      <c r="D59" s="493"/>
       <c r="E59" s="103" t="s">
         <v>9</v>
       </c>
@@ -15024,12 +15035,12 @@
       <c r="AO59" s="179"/>
     </row>
     <row r="60" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="512"/>
+      <c r="A60" s="491"/>
       <c r="B60" s="47"/>
       <c r="C60" s="198" t="s">
         <v>234</v>
       </c>
-      <c r="D60" s="514"/>
+      <c r="D60" s="493"/>
       <c r="E60" s="103" t="s">
         <v>9</v>
       </c>
@@ -15143,12 +15154,12 @@
       </c>
     </row>
     <row r="61" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="512"/>
+      <c r="A61" s="491"/>
       <c r="B61" s="47"/>
       <c r="C61" s="198" t="s">
         <v>235</v>
       </c>
-      <c r="D61" s="514"/>
+      <c r="D61" s="493"/>
       <c r="E61" s="103" t="s">
         <v>9</v>
       </c>
@@ -15262,12 +15273,12 @@
       </c>
     </row>
     <row r="62" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="512"/>
+      <c r="A62" s="491"/>
       <c r="B62" s="47"/>
       <c r="C62" s="198" t="s">
         <v>236</v>
       </c>
-      <c r="D62" s="514"/>
+      <c r="D62" s="493"/>
       <c r="E62" s="103" t="s">
         <v>9</v>
       </c>
@@ -15379,12 +15390,12 @@
       <c r="AO62" s="179"/>
     </row>
     <row r="63" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="512"/>
+      <c r="A63" s="491"/>
       <c r="B63" s="47"/>
       <c r="C63" s="424" t="s">
         <v>498</v>
       </c>
-      <c r="D63" s="514"/>
+      <c r="D63" s="493"/>
       <c r="E63" s="111"/>
       <c r="F63" s="34"/>
       <c r="G63" s="34"/>
@@ -15428,12 +15439,12 @@
       <c r="AO63" s="179"/>
     </row>
     <row r="64" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="512"/>
+      <c r="A64" s="491"/>
       <c r="B64" s="47"/>
       <c r="C64" s="198" t="s">
         <v>480</v>
       </c>
-      <c r="D64" s="514"/>
+      <c r="D64" s="493"/>
       <c r="E64" s="111"/>
       <c r="F64" s="34"/>
       <c r="G64" s="34"/>
@@ -15479,12 +15490,12 @@
       <c r="AO64" s="179"/>
     </row>
     <row r="65" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="512"/>
+      <c r="A65" s="491"/>
       <c r="B65" s="47"/>
       <c r="C65" s="198" t="s">
         <v>228</v>
       </c>
-      <c r="D65" s="514"/>
+      <c r="D65" s="493"/>
       <c r="E65" s="111"/>
       <c r="F65" s="34"/>
       <c r="G65" s="34"/>
@@ -15560,12 +15571,12 @@
       <c r="AO65" s="179"/>
     </row>
     <row r="66" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="512"/>
+      <c r="A66" s="491"/>
       <c r="B66" s="47"/>
       <c r="C66" s="199" t="s">
         <v>38</v>
       </c>
-      <c r="D66" s="514"/>
+      <c r="D66" s="493"/>
       <c r="E66" s="110"/>
       <c r="F66" s="35"/>
       <c r="G66" s="35"/>
@@ -15647,12 +15658,12 @@
       </c>
     </row>
     <row r="67" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="512"/>
+      <c r="A67" s="491"/>
       <c r="B67" s="47"/>
       <c r="C67" s="199" t="s">
         <v>39</v>
       </c>
-      <c r="D67" s="514"/>
+      <c r="D67" s="493"/>
       <c r="E67" s="110"/>
       <c r="F67" s="35"/>
       <c r="G67" s="35"/>
@@ -15734,12 +15745,12 @@
       </c>
     </row>
     <row r="68" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="512"/>
+      <c r="A68" s="491"/>
       <c r="B68" s="47"/>
       <c r="C68" s="198" t="s">
         <v>499</v>
       </c>
-      <c r="D68" s="514"/>
+      <c r="D68" s="493"/>
       <c r="E68" s="103" t="s">
         <v>9</v>
       </c>
@@ -15851,12 +15862,12 @@
       <c r="AO68" s="179"/>
     </row>
     <row r="69" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="512"/>
+      <c r="A69" s="491"/>
       <c r="B69" s="47"/>
       <c r="C69" s="198" t="s">
         <v>500</v>
       </c>
-      <c r="D69" s="514"/>
+      <c r="D69" s="493"/>
       <c r="E69" s="103" t="s">
         <v>9</v>
       </c>
@@ -15968,12 +15979,12 @@
       <c r="AO69" s="179"/>
     </row>
     <row r="70" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="512"/>
+      <c r="A70" s="491"/>
       <c r="B70" s="47"/>
       <c r="C70" s="198" t="s">
         <v>237</v>
       </c>
-      <c r="D70" s="514"/>
+      <c r="D70" s="493"/>
       <c r="E70" s="103" t="s">
         <v>9</v>
       </c>
@@ -16085,12 +16096,12 @@
       <c r="AO70" s="179"/>
     </row>
     <row r="71" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="512"/>
+      <c r="A71" s="491"/>
       <c r="B71" s="47"/>
       <c r="C71" s="424" t="s">
         <v>501</v>
       </c>
-      <c r="D71" s="514"/>
+      <c r="D71" s="493"/>
       <c r="E71" s="111"/>
       <c r="F71" s="34"/>
       <c r="G71" s="34"/>
@@ -16134,12 +16145,12 @@
       <c r="AO71" s="179"/>
     </row>
     <row r="72" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="512"/>
+      <c r="A72" s="491"/>
       <c r="B72" s="47"/>
       <c r="C72" s="198" t="s">
         <v>40</v>
       </c>
-      <c r="D72" s="514"/>
+      <c r="D72" s="493"/>
       <c r="E72" s="111"/>
       <c r="F72" s="34"/>
       <c r="G72" s="34"/>
@@ -16219,12 +16230,12 @@
       <c r="AO72" s="179"/>
     </row>
     <row r="73" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="512"/>
+      <c r="A73" s="491"/>
       <c r="B73" s="47"/>
       <c r="C73" s="198" t="s">
         <v>260</v>
       </c>
-      <c r="D73" s="514"/>
+      <c r="D73" s="493"/>
       <c r="E73" s="111"/>
       <c r="F73" s="34"/>
       <c r="G73" s="34"/>
@@ -16296,12 +16307,12 @@
       <c r="AO73" s="179"/>
     </row>
     <row r="74" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="512"/>
+      <c r="A74" s="491"/>
       <c r="B74" s="47"/>
       <c r="C74" s="424" t="s">
         <v>502</v>
       </c>
-      <c r="D74" s="514"/>
+      <c r="D74" s="493"/>
       <c r="E74" s="111"/>
       <c r="F74" s="34"/>
       <c r="G74" s="34"/>
@@ -16345,12 +16356,12 @@
       <c r="AO74" s="179"/>
     </row>
     <row r="75" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="512"/>
+      <c r="A75" s="491"/>
       <c r="B75" s="47"/>
       <c r="C75" s="198" t="s">
         <v>452</v>
       </c>
-      <c r="D75" s="514"/>
+      <c r="D75" s="493"/>
       <c r="E75" s="111"/>
       <c r="F75" s="34"/>
       <c r="G75" s="34"/>
@@ -16426,12 +16437,12 @@
       <c r="AO75" s="179"/>
     </row>
     <row r="76" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="512"/>
+      <c r="A76" s="491"/>
       <c r="B76" s="47"/>
       <c r="C76" s="198" t="s">
         <v>453</v>
       </c>
-      <c r="D76" s="514"/>
+      <c r="D76" s="493"/>
       <c r="E76" s="111"/>
       <c r="F76" s="34"/>
       <c r="G76" s="34"/>
@@ -16497,12 +16508,12 @@
       <c r="AO76" s="179"/>
     </row>
     <row r="77" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="512"/>
+      <c r="A77" s="491"/>
       <c r="B77" s="47"/>
       <c r="C77" s="198" t="s">
         <v>41</v>
       </c>
-      <c r="D77" s="514"/>
+      <c r="D77" s="493"/>
       <c r="E77" s="103" t="s">
         <v>18</v>
       </c>
@@ -16614,12 +16625,12 @@
       <c r="AO77" s="179"/>
     </row>
     <row r="78" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="512"/>
+      <c r="A78" s="491"/>
       <c r="B78" s="47"/>
       <c r="C78" s="198" t="s">
         <v>222</v>
       </c>
-      <c r="D78" s="514"/>
+      <c r="D78" s="493"/>
       <c r="E78" s="103" t="s">
         <v>9</v>
       </c>
@@ -16731,12 +16742,12 @@
       <c r="AO78" s="179"/>
     </row>
     <row r="79" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="512"/>
+      <c r="A79" s="491"/>
       <c r="B79" s="47"/>
       <c r="C79" s="198" t="s">
         <v>223</v>
       </c>
-      <c r="D79" s="514"/>
+      <c r="D79" s="493"/>
       <c r="E79" s="111"/>
       <c r="F79" s="34"/>
       <c r="G79" s="34"/>
@@ -16808,12 +16819,12 @@
       <c r="AO79" s="179"/>
     </row>
     <row r="80" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="512"/>
+      <c r="A80" s="491"/>
       <c r="B80" s="47"/>
       <c r="C80" s="424" t="s">
         <v>503</v>
       </c>
-      <c r="D80" s="514"/>
+      <c r="D80" s="493"/>
       <c r="E80" s="111"/>
       <c r="F80" s="34"/>
       <c r="G80" s="34"/>
@@ -16857,12 +16868,12 @@
       <c r="AO80" s="179"/>
     </row>
     <row r="81" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="512"/>
+      <c r="A81" s="491"/>
       <c r="B81" s="47"/>
       <c r="C81" s="198" t="s">
         <v>481</v>
       </c>
-      <c r="D81" s="514"/>
+      <c r="D81" s="493"/>
       <c r="E81" s="111"/>
       <c r="F81" s="34"/>
       <c r="G81" s="34"/>
@@ -16910,12 +16921,12 @@
       <c r="AO81" s="179"/>
     </row>
     <row r="82" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="512"/>
+      <c r="A82" s="491"/>
       <c r="B82" s="47"/>
       <c r="C82" s="198" t="s">
         <v>42</v>
       </c>
-      <c r="D82" s="514"/>
+      <c r="D82" s="493"/>
       <c r="E82" s="103" t="s">
         <v>18</v>
       </c>
@@ -17029,12 +17040,12 @@
       </c>
     </row>
     <row r="83" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="512"/>
+      <c r="A83" s="491"/>
       <c r="B83" s="47"/>
       <c r="C83" s="198" t="s">
         <v>109</v>
       </c>
-      <c r="D83" s="514"/>
+      <c r="D83" s="493"/>
       <c r="E83" s="103" t="s">
         <v>9</v>
       </c>
@@ -17146,12 +17157,12 @@
       <c r="AO83" s="179"/>
     </row>
     <row r="84" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="512"/>
+      <c r="A84" s="491"/>
       <c r="B84" s="47"/>
       <c r="C84" s="198" t="s">
         <v>43</v>
       </c>
-      <c r="D84" s="514"/>
+      <c r="D84" s="493"/>
       <c r="E84" s="103" t="s">
         <v>18</v>
       </c>
@@ -17265,12 +17276,12 @@
       </c>
     </row>
     <row r="85" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="512"/>
+      <c r="A85" s="491"/>
       <c r="B85" s="47"/>
       <c r="C85" s="198" t="s">
         <v>304</v>
       </c>
-      <c r="D85" s="514"/>
+      <c r="D85" s="493"/>
       <c r="E85" s="111"/>
       <c r="F85" s="34"/>
       <c r="G85" s="34"/>
@@ -17342,12 +17353,12 @@
       <c r="AO85" s="179"/>
     </row>
     <row r="86" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="512"/>
+      <c r="A86" s="491"/>
       <c r="B86" s="253"/>
       <c r="C86" s="254" t="s">
         <v>245</v>
       </c>
-      <c r="D86" s="514"/>
+      <c r="D86" s="493"/>
       <c r="E86" s="31" t="s">
         <v>361</v>
       </c>
@@ -17459,12 +17470,12 @@
       <c r="AO86" s="259"/>
     </row>
     <row r="87" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="512"/>
+      <c r="A87" s="491"/>
       <c r="B87" s="253"/>
       <c r="C87" s="425" t="s">
         <v>504</v>
       </c>
-      <c r="D87" s="514"/>
+      <c r="D87" s="493"/>
       <c r="E87" s="349"/>
       <c r="F87" s="34"/>
       <c r="G87" s="34"/>
@@ -17508,12 +17519,12 @@
       <c r="AO87" s="259"/>
     </row>
     <row r="88" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="512"/>
+      <c r="A88" s="491"/>
       <c r="B88" s="47"/>
       <c r="C88" s="198" t="s">
         <v>350</v>
       </c>
-      <c r="D88" s="514"/>
+      <c r="D88" s="493"/>
       <c r="E88" s="202"/>
       <c r="F88" s="34"/>
       <c r="G88" s="34"/>
@@ -17559,12 +17570,12 @@
       <c r="AO88" s="179"/>
     </row>
     <row r="89" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="512"/>
+      <c r="A89" s="491"/>
       <c r="B89" s="47"/>
       <c r="C89" s="198" t="s">
         <v>239</v>
       </c>
-      <c r="D89" s="514"/>
+      <c r="D89" s="493"/>
       <c r="E89" s="112" t="s">
         <v>18</v>
       </c>
@@ -17676,12 +17687,12 @@
       <c r="AO89" s="179"/>
     </row>
     <row r="90" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="512"/>
+      <c r="A90" s="491"/>
       <c r="B90" s="47"/>
       <c r="C90" s="198" t="s">
         <v>482</v>
       </c>
-      <c r="D90" s="514"/>
+      <c r="D90" s="493"/>
       <c r="E90" s="202"/>
       <c r="F90" s="34"/>
       <c r="G90" s="34"/>
@@ -17729,12 +17740,12 @@
       <c r="AO90" s="179"/>
     </row>
     <row r="91" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="512"/>
+      <c r="A91" s="491"/>
       <c r="B91" s="47"/>
       <c r="C91" s="424" t="s">
         <v>490</v>
       </c>
-      <c r="D91" s="514"/>
+      <c r="D91" s="493"/>
       <c r="E91" s="202"/>
       <c r="F91" s="34"/>
       <c r="G91" s="34"/>
@@ -17780,12 +17791,12 @@
       <c r="AO91" s="179"/>
     </row>
     <row r="92" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="512"/>
+      <c r="A92" s="491"/>
       <c r="B92" s="47"/>
       <c r="C92" s="198" t="s">
         <v>202</v>
       </c>
-      <c r="D92" s="514"/>
+      <c r="D92" s="493"/>
       <c r="E92" s="111"/>
       <c r="F92" s="34"/>
       <c r="G92" s="34"/>
@@ -17869,12 +17880,12 @@
       <c r="AO92" s="179"/>
     </row>
     <row r="93" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="512"/>
+      <c r="A93" s="491"/>
       <c r="B93" s="47"/>
       <c r="C93" s="198" t="s">
         <v>110</v>
       </c>
-      <c r="D93" s="514"/>
+      <c r="D93" s="493"/>
       <c r="E93" s="111"/>
       <c r="F93" s="34"/>
       <c r="G93" s="34"/>
@@ -17954,12 +17965,12 @@
       <c r="AO93" s="179"/>
     </row>
     <row r="94" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="512"/>
+      <c r="A94" s="491"/>
       <c r="B94" s="47"/>
       <c r="C94" s="198" t="s">
         <v>111</v>
       </c>
-      <c r="D94" s="514"/>
+      <c r="D94" s="493"/>
       <c r="E94" s="111"/>
       <c r="F94" s="34"/>
       <c r="G94" s="34"/>
@@ -18035,12 +18046,12 @@
       <c r="AO94" s="179"/>
     </row>
     <row r="95" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="512"/>
+      <c r="A95" s="491"/>
       <c r="B95" s="47"/>
       <c r="C95" s="198" t="s">
         <v>505</v>
       </c>
-      <c r="D95" s="514"/>
+      <c r="D95" s="493"/>
       <c r="E95" s="111"/>
       <c r="F95" s="34"/>
       <c r="G95" s="34"/>
@@ -18120,12 +18131,12 @@
       <c r="AO95" s="179"/>
     </row>
     <row r="96" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="512"/>
+      <c r="A96" s="491"/>
       <c r="B96" s="47"/>
       <c r="C96" s="424" t="s">
         <v>506</v>
       </c>
-      <c r="D96" s="514"/>
+      <c r="D96" s="493"/>
       <c r="E96" s="349"/>
       <c r="F96" s="34"/>
       <c r="G96" s="34"/>
@@ -18169,12 +18180,12 @@
       <c r="AO96" s="179"/>
     </row>
     <row r="97" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="512"/>
+      <c r="A97" s="491"/>
       <c r="B97" s="47"/>
       <c r="C97" s="424" t="s">
         <v>507</v>
       </c>
-      <c r="D97" s="514"/>
+      <c r="D97" s="493"/>
       <c r="E97" s="111"/>
       <c r="F97" s="34"/>
       <c r="G97" s="34"/>
@@ -18218,12 +18229,12 @@
       <c r="AO97" s="179"/>
     </row>
     <row r="98" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="512"/>
+      <c r="A98" s="491"/>
       <c r="B98" s="47"/>
       <c r="C98" s="424" t="s">
         <v>508</v>
       </c>
-      <c r="D98" s="514"/>
+      <c r="D98" s="493"/>
       <c r="E98" s="111"/>
       <c r="F98" s="34"/>
       <c r="G98" s="34"/>
@@ -18267,12 +18278,12 @@
       <c r="AO98" s="179"/>
     </row>
     <row r="99" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="512"/>
+      <c r="A99" s="491"/>
       <c r="B99" s="47"/>
       <c r="C99" s="424" t="s">
         <v>509</v>
       </c>
-      <c r="D99" s="514"/>
+      <c r="D99" s="493"/>
       <c r="E99" s="111"/>
       <c r="F99" s="34"/>
       <c r="G99" s="34"/>
@@ -18316,12 +18327,12 @@
       <c r="AO99" s="179"/>
     </row>
     <row r="100" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="512"/>
+      <c r="A100" s="491"/>
       <c r="B100" s="47"/>
       <c r="C100" s="198" t="s">
         <v>451</v>
       </c>
-      <c r="D100" s="514"/>
+      <c r="D100" s="493"/>
       <c r="E100" s="111"/>
       <c r="F100" s="34"/>
       <c r="G100" s="34"/>
@@ -18401,12 +18412,12 @@
       <c r="AO100" s="179"/>
     </row>
     <row r="101" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="512"/>
+      <c r="A101" s="491"/>
       <c r="B101" s="49"/>
       <c r="C101" s="424" t="s">
         <v>510</v>
       </c>
-      <c r="D101" s="514"/>
+      <c r="D101" s="493"/>
       <c r="E101" s="238"/>
       <c r="F101" s="239"/>
       <c r="G101" s="239"/>
@@ -18450,12 +18461,12 @@
       <c r="AO101" s="183"/>
     </row>
     <row r="102" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="512"/>
+      <c r="A102" s="491"/>
       <c r="B102" s="49"/>
       <c r="C102" s="74" t="s">
         <v>351</v>
       </c>
-      <c r="D102" s="514"/>
+      <c r="D102" s="493"/>
       <c r="E102" s="238"/>
       <c r="F102" s="239"/>
       <c r="G102" s="239"/>
@@ -18501,12 +18512,12 @@
       <c r="AO102" s="183"/>
     </row>
     <row r="103" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="512"/>
+      <c r="A103" s="491"/>
       <c r="B103" s="49"/>
       <c r="C103" s="420" t="s">
         <v>511</v>
       </c>
-      <c r="D103" s="514"/>
+      <c r="D103" s="493"/>
       <c r="E103" s="238"/>
       <c r="F103" s="239"/>
       <c r="G103" s="239"/>
@@ -18550,12 +18561,12 @@
       <c r="AO103" s="183"/>
     </row>
     <row r="104" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="512"/>
+      <c r="A104" s="491"/>
       <c r="B104" s="49"/>
       <c r="C104" s="420" t="s">
         <v>512</v>
       </c>
-      <c r="D104" s="514"/>
+      <c r="D104" s="493"/>
       <c r="E104" s="238"/>
       <c r="F104" s="239"/>
       <c r="G104" s="239"/>
@@ -18599,12 +18610,12 @@
       <c r="AO104" s="183"/>
     </row>
     <row r="105" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="512"/>
+      <c r="A105" s="491"/>
       <c r="B105" s="49"/>
       <c r="C105" s="74" t="s">
         <v>288</v>
       </c>
-      <c r="D105" s="514"/>
+      <c r="D105" s="493"/>
       <c r="E105" s="114" t="s">
         <v>243</v>
       </c>
@@ -18716,12 +18727,12 @@
       <c r="AO105" s="183"/>
     </row>
     <row r="106" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="512"/>
+      <c r="A106" s="491"/>
       <c r="B106" s="49"/>
       <c r="C106" s="74" t="s">
         <v>536</v>
       </c>
-      <c r="D106" s="514"/>
+      <c r="D106" s="493"/>
       <c r="E106" s="483"/>
       <c r="F106" s="477"/>
       <c r="G106" s="477"/>
@@ -18763,12 +18774,12 @@
       <c r="AO106" s="183"/>
     </row>
     <row r="107" spans="1:42" s="38" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="512"/>
+      <c r="A107" s="491"/>
       <c r="B107" s="73"/>
       <c r="C107" s="74" t="s">
         <v>229</v>
       </c>
-      <c r="D107" s="514"/>
+      <c r="D107" s="493"/>
       <c r="E107" s="114" t="s">
         <v>230</v>
       </c>
@@ -18883,14 +18894,14 @@
       </c>
     </row>
     <row r="108" spans="1:42" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="512"/>
+      <c r="A108" s="491"/>
       <c r="B108" s="41" t="s">
         <v>45</v>
       </c>
       <c r="C108" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="D108" s="514"/>
+      <c r="D108" s="493"/>
       <c r="E108" s="102"/>
       <c r="F108" s="43"/>
       <c r="G108" s="43"/>
@@ -18988,12 +18999,12 @@
       </c>
     </row>
     <row r="109" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="512"/>
+      <c r="A109" s="491"/>
       <c r="B109" s="48"/>
       <c r="C109" s="39" t="s">
         <v>305</v>
       </c>
-      <c r="D109" s="514"/>
+      <c r="D109" s="493"/>
       <c r="E109" s="109"/>
       <c r="F109" s="40"/>
       <c r="G109" s="40"/>
@@ -19059,12 +19070,12 @@
       <c r="AO109" s="182"/>
     </row>
     <row r="110" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="512"/>
+      <c r="A110" s="491"/>
       <c r="B110" s="47"/>
       <c r="C110" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D110" s="514"/>
+      <c r="D110" s="493"/>
       <c r="E110" s="103"/>
       <c r="F110" s="31"/>
       <c r="G110" s="31"/>
@@ -19160,12 +19171,12 @@
       <c r="AO110" s="179"/>
     </row>
     <row r="111" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="512"/>
+      <c r="A111" s="491"/>
       <c r="B111" s="47"/>
       <c r="C111" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D111" s="514"/>
+      <c r="D111" s="493"/>
       <c r="E111" s="103"/>
       <c r="F111" s="31"/>
       <c r="G111" s="31"/>
@@ -19261,12 +19272,12 @@
       <c r="AO111" s="179"/>
     </row>
     <row r="112" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="512"/>
+      <c r="A112" s="491"/>
       <c r="B112" s="47"/>
       <c r="C112" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D112" s="514"/>
+      <c r="D112" s="493"/>
       <c r="E112" s="103"/>
       <c r="F112" s="31"/>
       <c r="G112" s="31"/>
@@ -19362,12 +19373,12 @@
       <c r="AO112" s="179"/>
     </row>
     <row r="113" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="512"/>
+      <c r="A113" s="491"/>
       <c r="B113" s="47"/>
       <c r="C113" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D113" s="514"/>
+      <c r="D113" s="493"/>
       <c r="E113" s="103"/>
       <c r="F113" s="31"/>
       <c r="G113" s="31"/>
@@ -19468,12 +19479,12 @@
       </c>
     </row>
     <row r="114" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="512"/>
+      <c r="A114" s="491"/>
       <c r="B114" s="47"/>
       <c r="C114" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D114" s="514"/>
+      <c r="D114" s="493"/>
       <c r="E114" s="103"/>
       <c r="F114" s="31"/>
       <c r="G114" s="31"/>
@@ -19572,12 +19583,12 @@
       </c>
     </row>
     <row r="115" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="512"/>
+      <c r="A115" s="491"/>
       <c r="B115" s="47"/>
       <c r="C115" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D115" s="514"/>
+      <c r="D115" s="493"/>
       <c r="E115" s="103"/>
       <c r="F115" s="31"/>
       <c r="G115" s="31"/>
@@ -19678,12 +19689,12 @@
       </c>
     </row>
     <row r="116" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="512"/>
+      <c r="A116" s="491"/>
       <c r="B116" s="47"/>
       <c r="C116" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D116" s="514"/>
+      <c r="D116" s="493"/>
       <c r="E116" s="103"/>
       <c r="F116" s="31"/>
       <c r="G116" s="31"/>
@@ -19781,12 +19792,12 @@
       </c>
     </row>
     <row r="117" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="512"/>
+      <c r="A117" s="491"/>
       <c r="B117" s="47"/>
       <c r="C117" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D117" s="514"/>
+      <c r="D117" s="493"/>
       <c r="E117" s="103"/>
       <c r="F117" s="31"/>
       <c r="G117" s="31"/>
@@ -19884,12 +19895,12 @@
       </c>
     </row>
     <row r="118" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="512"/>
+      <c r="A118" s="491"/>
       <c r="B118" s="47"/>
       <c r="C118" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D118" s="514"/>
+      <c r="D118" s="493"/>
       <c r="E118" s="103"/>
       <c r="F118" s="31"/>
       <c r="G118" s="31"/>
@@ -19987,12 +19998,12 @@
       </c>
     </row>
     <row r="119" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="512"/>
+      <c r="A119" s="491"/>
       <c r="B119" s="47"/>
       <c r="C119" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="D119" s="514"/>
+      <c r="D119" s="493"/>
       <c r="E119" s="103"/>
       <c r="F119" s="31"/>
       <c r="G119" s="31"/>
@@ -20058,12 +20069,12 @@
       <c r="AO119" s="179"/>
     </row>
     <row r="120" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="512"/>
+      <c r="A120" s="491"/>
       <c r="B120" s="47"/>
       <c r="C120" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D120" s="514"/>
+      <c r="D120" s="493"/>
       <c r="E120" s="103"/>
       <c r="F120" s="31"/>
       <c r="G120" s="31"/>
@@ -20137,12 +20148,12 @@
       <c r="AO120" s="179"/>
     </row>
     <row r="121" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="512"/>
+      <c r="A121" s="491"/>
       <c r="B121" s="49"/>
       <c r="C121" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="D121" s="514"/>
+      <c r="D121" s="493"/>
       <c r="E121" s="103"/>
       <c r="F121" s="31"/>
       <c r="G121" s="31"/>
@@ -20202,12 +20213,12 @@
       <c r="AO121" s="179"/>
     </row>
     <row r="122" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="512"/>
+      <c r="A122" s="491"/>
       <c r="B122" s="49"/>
       <c r="C122" s="198" t="s">
         <v>435</v>
       </c>
-      <c r="D122" s="514"/>
+      <c r="D122" s="493"/>
       <c r="E122" s="103"/>
       <c r="F122" s="31"/>
       <c r="G122" s="31"/>
@@ -20273,12 +20284,12 @@
       <c r="AO122" s="179"/>
     </row>
     <row r="123" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="512"/>
+      <c r="A123" s="491"/>
       <c r="B123" s="49"/>
       <c r="C123" s="377" t="s">
         <v>477</v>
       </c>
-      <c r="D123" s="514"/>
+      <c r="D123" s="493"/>
       <c r="E123" s="103"/>
       <c r="F123" s="31"/>
       <c r="G123" s="31"/>
@@ -20324,12 +20335,12 @@
       <c r="AO123" s="179"/>
     </row>
     <row r="124" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="512"/>
+      <c r="A124" s="491"/>
       <c r="B124" s="49"/>
       <c r="C124" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="D124" s="514"/>
+      <c r="D124" s="493"/>
       <c r="E124" s="103"/>
       <c r="F124" s="31"/>
       <c r="G124" s="31"/>
@@ -20425,12 +20436,12 @@
       <c r="AO124" s="179"/>
     </row>
     <row r="125" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="512"/>
+      <c r="A125" s="491"/>
       <c r="B125" s="295"/>
       <c r="C125" s="199" t="s">
         <v>181</v>
       </c>
-      <c r="D125" s="514"/>
+      <c r="D125" s="493"/>
       <c r="E125" s="103"/>
       <c r="F125" s="31"/>
       <c r="G125" s="31"/>
@@ -20526,12 +20537,12 @@
       <c r="AO125" s="179"/>
     </row>
     <row r="126" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="512"/>
+      <c r="A126" s="491"/>
       <c r="B126" s="48"/>
       <c r="C126" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D126" s="514"/>
+      <c r="D126" s="493"/>
       <c r="E126" s="103"/>
       <c r="F126" s="31"/>
       <c r="G126" s="31"/>
@@ -20615,12 +20626,12 @@
       </c>
     </row>
     <row r="127" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="512"/>
+      <c r="A127" s="491"/>
       <c r="B127" s="47"/>
       <c r="C127" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="D127" s="514"/>
+      <c r="D127" s="493"/>
       <c r="E127" s="103"/>
       <c r="F127" s="31"/>
       <c r="G127" s="31"/>
@@ -20716,12 +20727,12 @@
       <c r="AO127" s="185"/>
     </row>
     <row r="128" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="512"/>
+      <c r="A128" s="491"/>
       <c r="B128" s="47"/>
       <c r="C128" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="D128" s="514"/>
+      <c r="D128" s="493"/>
       <c r="E128" s="103"/>
       <c r="F128" s="31"/>
       <c r="G128" s="31"/>
@@ -20817,12 +20828,12 @@
       <c r="AO128" s="179"/>
     </row>
     <row r="129" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="512"/>
+      <c r="A129" s="491"/>
       <c r="B129" s="47"/>
       <c r="C129" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="D129" s="514"/>
+      <c r="D129" s="493"/>
       <c r="E129" s="103"/>
       <c r="F129" s="31"/>
       <c r="G129" s="31"/>
@@ -20918,12 +20929,12 @@
       <c r="AO129" s="179"/>
     </row>
     <row r="130" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="512"/>
+      <c r="A130" s="491"/>
       <c r="B130" s="47"/>
       <c r="C130" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D130" s="514"/>
+      <c r="D130" s="493"/>
       <c r="E130" s="103"/>
       <c r="F130" s="31"/>
       <c r="G130" s="31"/>
@@ -21019,12 +21030,12 @@
       <c r="AO130" s="185"/>
     </row>
     <row r="131" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="512"/>
+      <c r="A131" s="491"/>
       <c r="B131" s="47"/>
       <c r="C131" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="D131" s="514"/>
+      <c r="D131" s="493"/>
       <c r="E131" s="103"/>
       <c r="F131" s="31"/>
       <c r="G131" s="31"/>
@@ -21120,12 +21131,12 @@
       <c r="AO131" s="179"/>
     </row>
     <row r="132" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="512"/>
+      <c r="A132" s="491"/>
       <c r="B132" s="47"/>
       <c r="C132" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="D132" s="514"/>
+      <c r="D132" s="493"/>
       <c r="E132" s="103"/>
       <c r="F132" s="31"/>
       <c r="G132" s="31"/>
@@ -21221,12 +21232,12 @@
       <c r="AO132" s="185"/>
     </row>
     <row r="133" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="512"/>
+      <c r="A133" s="491"/>
       <c r="B133" s="47"/>
       <c r="C133" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="D133" s="514"/>
+      <c r="D133" s="493"/>
       <c r="E133" s="103"/>
       <c r="F133" s="31"/>
       <c r="G133" s="31"/>
@@ -21322,12 +21333,12 @@
       <c r="AO133" s="179"/>
     </row>
     <row r="134" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="512"/>
+      <c r="A134" s="491"/>
       <c r="B134" s="47"/>
       <c r="C134" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="D134" s="514"/>
+      <c r="D134" s="493"/>
       <c r="E134" s="103"/>
       <c r="F134" s="31"/>
       <c r="G134" s="31"/>
@@ -21423,12 +21434,12 @@
       <c r="AO134" s="179"/>
     </row>
     <row r="135" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="512"/>
+      <c r="A135" s="491"/>
       <c r="B135" s="47"/>
       <c r="C135" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D135" s="514"/>
+      <c r="D135" s="493"/>
       <c r="E135" s="103"/>
       <c r="F135" s="31"/>
       <c r="G135" s="31"/>
@@ -21526,12 +21537,12 @@
       </c>
     </row>
     <row r="136" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="512"/>
+      <c r="A136" s="491"/>
       <c r="B136" s="47"/>
       <c r="C136" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D136" s="514"/>
+      <c r="D136" s="493"/>
       <c r="E136" s="103"/>
       <c r="F136" s="31"/>
       <c r="G136" s="31"/>
@@ -21629,12 +21640,12 @@
       </c>
     </row>
     <row r="137" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="512"/>
+      <c r="A137" s="491"/>
       <c r="B137" s="47"/>
       <c r="C137" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D137" s="514"/>
+      <c r="D137" s="493"/>
       <c r="E137" s="103"/>
       <c r="F137" s="31"/>
       <c r="G137" s="31"/>
@@ -21732,12 +21743,12 @@
       </c>
     </row>
     <row r="138" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="512"/>
+      <c r="A138" s="491"/>
       <c r="B138" s="47"/>
       <c r="C138" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D138" s="514"/>
+      <c r="D138" s="493"/>
       <c r="E138" s="103"/>
       <c r="F138" s="31"/>
       <c r="G138" s="31"/>
@@ -21835,12 +21846,12 @@
       </c>
     </row>
     <row r="139" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="512"/>
+      <c r="A139" s="491"/>
       <c r="B139" s="47"/>
       <c r="C139" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D139" s="514"/>
+      <c r="D139" s="493"/>
       <c r="E139" s="103"/>
       <c r="F139" s="31"/>
       <c r="G139" s="31"/>
@@ -21938,12 +21949,12 @@
       </c>
     </row>
     <row r="140" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="512"/>
+      <c r="A140" s="491"/>
       <c r="B140" s="47"/>
       <c r="C140" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D140" s="514"/>
+      <c r="D140" s="493"/>
       <c r="E140" s="103"/>
       <c r="F140" s="31"/>
       <c r="G140" s="31"/>
@@ -22044,12 +22055,12 @@
       </c>
     </row>
     <row r="141" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="512"/>
+      <c r="A141" s="491"/>
       <c r="B141" s="47"/>
       <c r="C141" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D141" s="514"/>
+      <c r="D141" s="493"/>
       <c r="E141" s="103"/>
       <c r="F141" s="31"/>
       <c r="G141" s="31"/>
@@ -22147,12 +22158,12 @@
       </c>
     </row>
     <row r="142" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="512"/>
+      <c r="A142" s="491"/>
       <c r="B142" s="47"/>
       <c r="C142" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D142" s="514"/>
+      <c r="D142" s="493"/>
       <c r="E142" s="103"/>
       <c r="F142" s="31"/>
       <c r="G142" s="31"/>
@@ -22220,12 +22231,12 @@
       <c r="AO142" s="179"/>
     </row>
     <row r="143" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="512"/>
+      <c r="A143" s="491"/>
       <c r="B143" s="47"/>
       <c r="C143" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D143" s="514"/>
+      <c r="D143" s="493"/>
       <c r="E143" s="103"/>
       <c r="F143" s="31"/>
       <c r="G143" s="31"/>
@@ -22293,12 +22304,12 @@
       <c r="AO143" s="179"/>
     </row>
     <row r="144" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="512"/>
+      <c r="A144" s="491"/>
       <c r="B144" s="47"/>
       <c r="C144" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D144" s="514"/>
+      <c r="D144" s="493"/>
       <c r="E144" s="103"/>
       <c r="F144" s="31"/>
       <c r="G144" s="31"/>
@@ -22366,12 +22377,12 @@
       <c r="AO144" s="179"/>
     </row>
     <row r="145" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="512"/>
+      <c r="A145" s="491"/>
       <c r="B145" s="47"/>
       <c r="C145" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D145" s="514"/>
+      <c r="D145" s="493"/>
       <c r="E145" s="103"/>
       <c r="F145" s="31"/>
       <c r="G145" s="31"/>
@@ -22439,12 +22450,12 @@
       <c r="AO145" s="179"/>
     </row>
     <row r="146" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="512"/>
+      <c r="A146" s="491"/>
       <c r="B146" s="47"/>
       <c r="C146" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D146" s="514"/>
+      <c r="D146" s="493"/>
       <c r="E146" s="103"/>
       <c r="F146" s="31"/>
       <c r="G146" s="31"/>
@@ -22512,12 +22523,12 @@
       <c r="AO146" s="179"/>
     </row>
     <row r="147" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="512"/>
+      <c r="A147" s="491"/>
       <c r="B147" s="47"/>
       <c r="C147" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D147" s="514"/>
+      <c r="D147" s="493"/>
       <c r="E147" s="103"/>
       <c r="F147" s="31"/>
       <c r="G147" s="31"/>
@@ -22585,12 +22596,12 @@
       <c r="AO147" s="179"/>
     </row>
     <row r="148" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="512"/>
+      <c r="A148" s="491"/>
       <c r="B148" s="47"/>
       <c r="C148" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D148" s="514"/>
+      <c r="D148" s="493"/>
       <c r="E148" s="103"/>
       <c r="F148" s="31"/>
       <c r="G148" s="31"/>
@@ -22658,12 +22669,12 @@
       <c r="AO148" s="179"/>
     </row>
     <row r="149" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="512"/>
+      <c r="A149" s="491"/>
       <c r="B149" s="47"/>
       <c r="C149" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D149" s="514"/>
+      <c r="D149" s="493"/>
       <c r="E149" s="103"/>
       <c r="F149" s="31"/>
       <c r="G149" s="31"/>
@@ -22731,12 +22742,12 @@
       <c r="AO149" s="179"/>
     </row>
     <row r="150" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="512"/>
+      <c r="A150" s="491"/>
       <c r="B150" s="47"/>
       <c r="C150" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D150" s="514"/>
+      <c r="D150" s="493"/>
       <c r="E150" s="103"/>
       <c r="F150" s="31"/>
       <c r="G150" s="31"/>
@@ -22804,12 +22815,12 @@
       <c r="AO150" s="179"/>
     </row>
     <row r="151" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="512"/>
+      <c r="A151" s="491"/>
       <c r="B151" s="47"/>
       <c r="C151" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D151" s="514"/>
+      <c r="D151" s="493"/>
       <c r="E151" s="103"/>
       <c r="F151" s="31"/>
       <c r="G151" s="31"/>
@@ -22877,12 +22888,12 @@
       <c r="AO151" s="179"/>
     </row>
     <row r="152" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="512"/>
+      <c r="A152" s="491"/>
       <c r="B152" s="47"/>
       <c r="C152" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D152" s="514"/>
+      <c r="D152" s="493"/>
       <c r="E152" s="103"/>
       <c r="F152" s="31"/>
       <c r="G152" s="31"/>
@@ -22950,12 +22961,12 @@
       <c r="AO152" s="179"/>
     </row>
     <row r="153" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="512"/>
+      <c r="A153" s="491"/>
       <c r="B153" s="47"/>
       <c r="C153" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D153" s="514"/>
+      <c r="D153" s="493"/>
       <c r="E153" s="103"/>
       <c r="F153" s="31"/>
       <c r="G153" s="31"/>
@@ -23035,12 +23046,12 @@
       </c>
     </row>
     <row r="154" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="512"/>
+      <c r="A154" s="491"/>
       <c r="B154" s="47"/>
       <c r="C154" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D154" s="514"/>
+      <c r="D154" s="493"/>
       <c r="E154" s="103"/>
       <c r="F154" s="31"/>
       <c r="G154" s="31"/>
@@ -23138,12 +23149,12 @@
       </c>
     </row>
     <row r="155" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="512"/>
+      <c r="A155" s="491"/>
       <c r="B155" s="47"/>
       <c r="C155" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D155" s="514"/>
+      <c r="D155" s="493"/>
       <c r="E155" s="116"/>
       <c r="F155" s="32"/>
       <c r="G155" s="32"/>
@@ -23183,12 +23194,12 @@
       <c r="AO155" s="179"/>
     </row>
     <row r="156" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="512"/>
+      <c r="A156" s="491"/>
       <c r="B156" s="47"/>
       <c r="C156" s="199" t="s">
         <v>67</v>
       </c>
-      <c r="D156" s="514"/>
+      <c r="D156" s="493"/>
       <c r="E156" s="116"/>
       <c r="F156" s="32"/>
       <c r="G156" s="32"/>
@@ -23286,12 +23297,12 @@
       </c>
     </row>
     <row r="157" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="512"/>
+      <c r="A157" s="491"/>
       <c r="B157" s="47"/>
       <c r="C157" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="D157" s="514"/>
+      <c r="D157" s="493"/>
       <c r="E157" s="116"/>
       <c r="F157" s="32"/>
       <c r="G157" s="32"/>
@@ -23387,12 +23398,12 @@
       <c r="AO157" s="179"/>
     </row>
     <row r="158" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="512"/>
+      <c r="A158" s="491"/>
       <c r="B158" s="47"/>
       <c r="C158" s="422" t="s">
         <v>192</v>
       </c>
-      <c r="D158" s="514"/>
+      <c r="D158" s="493"/>
       <c r="E158" s="116"/>
       <c r="F158" s="32"/>
       <c r="G158" s="32"/>
@@ -23488,12 +23499,12 @@
       <c r="AO158" s="179"/>
     </row>
     <row r="159" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="512"/>
+      <c r="A159" s="491"/>
       <c r="B159" s="47"/>
       <c r="C159" s="422" t="s">
         <v>408</v>
       </c>
-      <c r="D159" s="514"/>
+      <c r="D159" s="493"/>
       <c r="E159" s="116"/>
       <c r="F159" s="32"/>
       <c r="G159" s="32"/>
@@ -23591,12 +23602,12 @@
       </c>
     </row>
     <row r="160" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="512"/>
+      <c r="A160" s="491"/>
       <c r="B160" s="47"/>
       <c r="C160" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="D160" s="514"/>
+      <c r="D160" s="493"/>
       <c r="E160" s="116"/>
       <c r="F160" s="32"/>
       <c r="G160" s="32"/>
@@ -23694,12 +23705,12 @@
       </c>
     </row>
     <row r="161" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="512"/>
+      <c r="A161" s="491"/>
       <c r="B161" s="47"/>
       <c r="C161" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D161" s="514"/>
+      <c r="D161" s="493"/>
       <c r="E161" s="116"/>
       <c r="F161" s="32"/>
       <c r="G161" s="32"/>
@@ -23797,12 +23808,12 @@
       </c>
     </row>
     <row r="162" spans="1:41" s="283" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="512"/>
+      <c r="A162" s="491"/>
       <c r="B162" s="286"/>
       <c r="C162" s="423" t="s">
         <v>183</v>
       </c>
-      <c r="D162" s="514"/>
+      <c r="D162" s="493"/>
       <c r="E162" s="281"/>
       <c r="F162" s="255"/>
       <c r="G162" s="255"/>
@@ -23898,12 +23909,12 @@
       <c r="AO162" s="282"/>
     </row>
     <row r="163" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="512"/>
+      <c r="A163" s="491"/>
       <c r="B163" s="49"/>
       <c r="C163" s="199" t="s">
         <v>66</v>
       </c>
-      <c r="D163" s="514"/>
+      <c r="D163" s="493"/>
       <c r="E163" s="116"/>
       <c r="F163" s="32"/>
       <c r="G163" s="32"/>
@@ -23999,12 +24010,12 @@
       <c r="AO163" s="179"/>
     </row>
     <row r="164" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="512"/>
+      <c r="A164" s="491"/>
       <c r="B164" s="286"/>
       <c r="C164" s="199" t="s">
         <v>73</v>
       </c>
-      <c r="D164" s="514"/>
+      <c r="D164" s="493"/>
       <c r="E164" s="116"/>
       <c r="F164" s="32"/>
       <c r="G164" s="32"/>
@@ -24102,12 +24113,12 @@
       </c>
     </row>
     <row r="165" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="512"/>
+      <c r="A165" s="491"/>
       <c r="B165" s="48"/>
       <c r="C165" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="D165" s="514"/>
+      <c r="D165" s="493"/>
       <c r="E165" s="116"/>
       <c r="F165" s="32"/>
       <c r="G165" s="32"/>
@@ -24205,12 +24216,12 @@
       </c>
     </row>
     <row r="166" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="512"/>
+      <c r="A166" s="491"/>
       <c r="B166" s="47"/>
       <c r="C166" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D166" s="514"/>
+      <c r="D166" s="493"/>
       <c r="E166" s="116"/>
       <c r="F166" s="32"/>
       <c r="G166" s="32"/>
@@ -24306,12 +24317,12 @@
       <c r="AO166" s="179"/>
     </row>
     <row r="167" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="512"/>
+      <c r="A167" s="491"/>
       <c r="B167" s="47"/>
       <c r="C167" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D167" s="514"/>
+      <c r="D167" s="493"/>
       <c r="E167" s="116"/>
       <c r="F167" s="32"/>
       <c r="G167" s="32"/>
@@ -24381,12 +24392,12 @@
       <c r="AO167" s="179"/>
     </row>
     <row r="168" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="512"/>
+      <c r="A168" s="491"/>
       <c r="B168" s="47"/>
       <c r="C168" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D168" s="514"/>
+      <c r="D168" s="493"/>
       <c r="E168" s="116"/>
       <c r="F168" s="32"/>
       <c r="G168" s="32"/>
@@ -24484,12 +24495,12 @@
       </c>
     </row>
     <row r="169" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="512"/>
+      <c r="A169" s="491"/>
       <c r="B169" s="47"/>
       <c r="C169" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D169" s="514"/>
+      <c r="D169" s="493"/>
       <c r="E169" s="116"/>
       <c r="F169" s="32"/>
       <c r="G169" s="32"/>
@@ -24585,12 +24596,12 @@
       <c r="AO169" s="179"/>
     </row>
     <row r="170" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="512"/>
+      <c r="A170" s="491"/>
       <c r="B170" s="49"/>
       <c r="C170" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="D170" s="514"/>
+      <c r="D170" s="493"/>
       <c r="E170" s="417"/>
       <c r="F170" s="359"/>
       <c r="G170" s="359"/>
@@ -24686,12 +24697,12 @@
       <c r="AO170" s="183"/>
     </row>
     <row r="171" spans="1:41" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="512"/>
+      <c r="A171" s="491"/>
       <c r="B171" s="67"/>
       <c r="C171" s="68" t="s">
         <v>226</v>
       </c>
-      <c r="D171" s="514"/>
+      <c r="D171" s="493"/>
       <c r="E171" s="106"/>
       <c r="F171" s="72"/>
       <c r="G171" s="72"/>
@@ -24759,14 +24770,14 @@
       <c r="AO171" s="181"/>
     </row>
     <row r="172" spans="1:41" ht="26.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="512"/>
+      <c r="A172" s="491"/>
       <c r="B172" s="85" t="s">
         <v>75</v>
       </c>
       <c r="C172" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="D172" s="514"/>
+      <c r="D172" s="493"/>
       <c r="E172" s="117"/>
       <c r="F172" s="86"/>
       <c r="G172" s="86"/>
@@ -24864,12 +24875,12 @@
       </c>
     </row>
     <row r="173" spans="1:41" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A173" s="512"/>
+      <c r="A173" s="491"/>
       <c r="B173" s="47"/>
       <c r="C173" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D173" s="514"/>
+      <c r="D173" s="493"/>
       <c r="E173" s="116"/>
       <c r="F173" s="32"/>
       <c r="G173" s="32"/>
@@ -24967,12 +24978,12 @@
       </c>
     </row>
     <row r="174" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="512"/>
+      <c r="A174" s="491"/>
       <c r="B174" s="47"/>
       <c r="C174" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D174" s="514"/>
+      <c r="D174" s="493"/>
       <c r="E174" s="116"/>
       <c r="F174" s="32"/>
       <c r="G174" s="32"/>
@@ -25068,12 +25079,12 @@
       <c r="AO174" s="179"/>
     </row>
     <row r="175" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="512"/>
+      <c r="A175" s="491"/>
       <c r="B175" s="47"/>
       <c r="C175" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D175" s="514"/>
+      <c r="D175" s="493"/>
       <c r="E175" s="116"/>
       <c r="F175" s="32"/>
       <c r="G175" s="32"/>
@@ -25169,12 +25180,12 @@
       <c r="AO175" s="179"/>
     </row>
     <row r="176" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="512"/>
+      <c r="A176" s="491"/>
       <c r="B176" s="47"/>
       <c r="C176" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D176" s="514"/>
+      <c r="D176" s="493"/>
       <c r="E176" s="116"/>
       <c r="F176" s="32"/>
       <c r="G176" s="32"/>
@@ -25270,12 +25281,12 @@
       <c r="AO176" s="179"/>
     </row>
     <row r="177" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="512"/>
+      <c r="A177" s="491"/>
       <c r="B177" s="47"/>
       <c r="C177" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D177" s="514"/>
+      <c r="D177" s="493"/>
       <c r="E177" s="116"/>
       <c r="F177" s="32"/>
       <c r="G177" s="32"/>
@@ -25371,12 +25382,12 @@
       <c r="AO177" s="179"/>
     </row>
     <row r="178" spans="1:41" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A178" s="512"/>
+      <c r="A178" s="491"/>
       <c r="B178" s="47"/>
       <c r="C178" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D178" s="514"/>
+      <c r="D178" s="493"/>
       <c r="E178" s="116"/>
       <c r="F178" s="32"/>
       <c r="G178" s="32"/>
@@ -25474,12 +25485,12 @@
       </c>
     </row>
     <row r="179" spans="1:41" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A179" s="512"/>
+      <c r="A179" s="491"/>
       <c r="B179" s="47"/>
       <c r="C179" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D179" s="514"/>
+      <c r="D179" s="493"/>
       <c r="E179" s="116"/>
       <c r="F179" s="32"/>
       <c r="G179" s="32"/>
@@ -25575,12 +25586,12 @@
       <c r="AO179" s="185"/>
     </row>
     <row r="180" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="512"/>
+      <c r="A180" s="491"/>
       <c r="B180" s="47"/>
       <c r="C180" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D180" s="514"/>
+      <c r="D180" s="493"/>
       <c r="E180" s="116"/>
       <c r="F180" s="32"/>
       <c r="G180" s="32"/>
@@ -25676,12 +25687,12 @@
       <c r="AO180" s="185"/>
     </row>
     <row r="181" spans="1:41" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A181" s="512"/>
+      <c r="A181" s="491"/>
       <c r="B181" s="47"/>
       <c r="C181" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D181" s="514"/>
+      <c r="D181" s="493"/>
       <c r="E181" s="116"/>
       <c r="F181" s="32"/>
       <c r="G181" s="32"/>
@@ -25779,12 +25790,12 @@
       </c>
     </row>
     <row r="182" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A182" s="512"/>
+      <c r="A182" s="491"/>
       <c r="B182" s="47"/>
       <c r="C182" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D182" s="514"/>
+      <c r="D182" s="493"/>
       <c r="E182" s="116"/>
       <c r="F182" s="32"/>
       <c r="G182" s="32"/>
@@ -25882,12 +25893,12 @@
       </c>
     </row>
     <row r="183" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="512"/>
+      <c r="A183" s="491"/>
       <c r="B183" s="47"/>
       <c r="C183" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D183" s="514"/>
+      <c r="D183" s="493"/>
       <c r="E183" s="116"/>
       <c r="F183" s="32"/>
       <c r="G183" s="32"/>
@@ -25983,12 +25994,12 @@
       <c r="AO183" s="179"/>
     </row>
     <row r="184" spans="1:41" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A184" s="512"/>
+      <c r="A184" s="491"/>
       <c r="B184" s="47"/>
       <c r="C184" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D184" s="514"/>
+      <c r="D184" s="493"/>
       <c r="E184" s="116"/>
       <c r="F184" s="32"/>
       <c r="G184" s="32"/>
@@ -26086,12 +26097,12 @@
       </c>
     </row>
     <row r="185" spans="1:41" ht="51" x14ac:dyDescent="0.25">
-      <c r="A185" s="512"/>
+      <c r="A185" s="491"/>
       <c r="B185" s="47"/>
       <c r="C185" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D185" s="514"/>
+      <c r="D185" s="493"/>
       <c r="E185" s="116"/>
       <c r="F185" s="32"/>
       <c r="G185" s="32"/>
@@ -26187,12 +26198,12 @@
       <c r="AO185" s="179"/>
     </row>
     <row r="186" spans="1:41" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="512"/>
+      <c r="A186" s="491"/>
       <c r="B186" s="67"/>
       <c r="C186" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="D186" s="514"/>
+      <c r="D186" s="493"/>
       <c r="E186" s="106"/>
       <c r="F186" s="72"/>
       <c r="G186" s="72"/>
@@ -26270,14 +26281,14 @@
       <c r="AO186" s="181"/>
     </row>
     <row r="187" spans="1:41" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="512"/>
+      <c r="A187" s="491"/>
       <c r="B187" s="55" t="s">
         <v>135</v>
       </c>
       <c r="C187" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="D187" s="514"/>
+      <c r="D187" s="493"/>
       <c r="E187" s="118"/>
       <c r="F187" s="57"/>
       <c r="G187" s="57"/>
@@ -26373,12 +26384,12 @@
       <c r="AO187" s="186"/>
     </row>
     <row r="188" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="512"/>
+      <c r="A188" s="491"/>
       <c r="B188" s="59"/>
       <c r="C188" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D188" s="514"/>
+      <c r="D188" s="493"/>
       <c r="E188" s="119"/>
       <c r="F188" s="33"/>
       <c r="G188" s="33"/>
@@ -26474,12 +26485,12 @@
       <c r="AO188" s="187"/>
     </row>
     <row r="189" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="512"/>
+      <c r="A189" s="491"/>
       <c r="B189" s="59"/>
       <c r="C189" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D189" s="514"/>
+      <c r="D189" s="493"/>
       <c r="E189" s="119"/>
       <c r="F189" s="33"/>
       <c r="G189" s="33"/>
@@ -26577,12 +26588,12 @@
       </c>
     </row>
     <row r="190" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="512"/>
+      <c r="A190" s="491"/>
       <c r="B190" s="59"/>
       <c r="C190" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D190" s="514"/>
+      <c r="D190" s="493"/>
       <c r="E190" s="119"/>
       <c r="F190" s="33"/>
       <c r="G190" s="33"/>
@@ -26678,12 +26689,12 @@
       <c r="AO190" s="187"/>
     </row>
     <row r="191" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="512"/>
+      <c r="A191" s="491"/>
       <c r="B191" s="59"/>
       <c r="C191" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D191" s="514"/>
+      <c r="D191" s="493"/>
       <c r="E191" s="119"/>
       <c r="F191" s="33"/>
       <c r="G191" s="33"/>
@@ -26779,12 +26790,12 @@
       <c r="AO191" s="187"/>
     </row>
     <row r="192" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="512"/>
+      <c r="A192" s="491"/>
       <c r="B192" s="59"/>
       <c r="C192" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D192" s="514"/>
+      <c r="D192" s="493"/>
       <c r="E192" s="119"/>
       <c r="F192" s="33"/>
       <c r="G192" s="33"/>
@@ -26882,12 +26893,12 @@
       </c>
     </row>
     <row r="193" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="512"/>
+      <c r="A193" s="491"/>
       <c r="B193" s="59"/>
       <c r="C193" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D193" s="514"/>
+      <c r="D193" s="493"/>
       <c r="E193" s="119"/>
       <c r="F193" s="33"/>
       <c r="G193" s="33"/>
@@ -26983,12 +26994,12 @@
       <c r="AO193" s="187"/>
     </row>
     <row r="194" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="512"/>
+      <c r="A194" s="491"/>
       <c r="B194" s="59"/>
       <c r="C194" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D194" s="514"/>
+      <c r="D194" s="493"/>
       <c r="E194" s="119"/>
       <c r="F194" s="33"/>
       <c r="G194" s="33"/>
@@ -27084,12 +27095,12 @@
       <c r="AO194" s="187"/>
     </row>
     <row r="195" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="512"/>
+      <c r="A195" s="491"/>
       <c r="B195" s="59"/>
       <c r="C195" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D195" s="514"/>
+      <c r="D195" s="493"/>
       <c r="E195" s="119"/>
       <c r="F195" s="33"/>
       <c r="G195" s="33"/>
@@ -27185,12 +27196,12 @@
       <c r="AO195" s="187"/>
     </row>
     <row r="196" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="512"/>
+      <c r="A196" s="491"/>
       <c r="B196" s="59"/>
       <c r="C196" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="D196" s="514"/>
+      <c r="D196" s="493"/>
       <c r="E196" s="119"/>
       <c r="F196" s="33"/>
       <c r="G196" s="33"/>
@@ -27288,12 +27299,12 @@
       </c>
     </row>
     <row r="197" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A197" s="512"/>
+      <c r="A197" s="491"/>
       <c r="B197" s="59"/>
       <c r="C197" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D197" s="514"/>
+      <c r="D197" s="493"/>
       <c r="E197" s="119"/>
       <c r="F197" s="33"/>
       <c r="G197" s="33"/>
@@ -27389,12 +27400,12 @@
       <c r="AO197" s="187"/>
     </row>
     <row r="198" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="512"/>
+      <c r="A198" s="491"/>
       <c r="B198" s="59"/>
       <c r="C198" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="D198" s="514"/>
+      <c r="D198" s="493"/>
       <c r="E198" s="119"/>
       <c r="F198" s="33"/>
       <c r="G198" s="33"/>
@@ -27490,12 +27501,12 @@
       <c r="AO198" s="187"/>
     </row>
     <row r="199" spans="1:41" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="512"/>
+      <c r="A199" s="491"/>
       <c r="B199" s="60"/>
       <c r="C199" s="61" t="s">
         <v>150</v>
       </c>
-      <c r="D199" s="515"/>
+      <c r="D199" s="494"/>
       <c r="E199" s="120"/>
       <c r="F199" s="62"/>
       <c r="G199" s="62"/>
@@ -27594,12 +27605,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="A27:A199"/>
-    <mergeCell ref="D27:D199"/>
-    <mergeCell ref="E5:L26"/>
-    <mergeCell ref="M5:AM26"/>
-    <mergeCell ref="A5:A26"/>
     <mergeCell ref="AO3:AO4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="T3:V3"/>
@@ -27609,6 +27614,12 @@
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="A27:A199"/>
+    <mergeCell ref="D27:D199"/>
+    <mergeCell ref="E5:L26"/>
+    <mergeCell ref="M5:AM26"/>
+    <mergeCell ref="A5:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
IOMMU Translation Table entry size chage from 64 to 128 for both engines.
[git-p4: depot-paths = "//depot/projects/coe/CSME/": change = 772681]
</commit_message>
<xml_diff>
--- a/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
+++ b/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
@@ -9353,7 +9353,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E87" sqref="E87"/>
+      <selection pane="bottomRight" activeCell="B86" sqref="B86:E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10664,10 +10664,10 @@
   <dimension ref="A1:AP201"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="AC38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="AC20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
+      <selection pane="bottomRight" activeCell="AL41" sqref="AL41:AM41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
75 - Update ECDSA configuration for Soteria-ME to release HAS 0.21
[git-p4: depot-paths = "//depot/projects/coe/CSME/": change = 772809]
</commit_message>
<xml_diff>
--- a/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
+++ b/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12330" yWindow="105" windowWidth="3210" windowHeight="4665"/>
+    <workbookView xWindow="12330" yWindow="105" windowWidth="3210" windowHeight="4665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="2" r:id="rId1"/>
@@ -1954,33 +1954,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM90" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-DRNG is required for Data Protection Key in AMT - Blob.
-However, Soterial-ME uses the PCH shared DRNG in fuse controller.
-Integrated DRNG - No.
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="AD94" authorId="0" shapeId="0">
       <text>
         <r>
@@ -2002,55 +1975,6 @@
           </rPr>
           <t xml:space="preserve">
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AM95" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-New PCR:
-OCS will have ability to configure randam value input from either HW or FW.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AM96" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Soterial-ME doesn't have Internal DRNG. Hence, only supports FW assisted ECDSA.</t>
         </r>
       </text>
     </comment>
@@ -4341,7 +4265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4152" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4154" uniqueCount="545">
   <si>
     <t>CNP-LP</t>
   </si>
@@ -6364,6 +6288,9 @@
   </si>
   <si>
     <t>Updated IOMMU Translation Table  (128 Entry) size for both engines.</t>
+  </si>
+  <si>
+    <t>Updated ECDSA and internal DRNG support configuration for Soteria-ME.</t>
   </si>
 </sst>
 </file>
@@ -6543,7 +6470,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6625,6 +6552,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7462,7 +7395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="525">
+  <cellXfs count="526">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -8931,6 +8864,69 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -8973,67 +8969,7 @@
     <xf numFmtId="0" fontId="10" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9045,6 +8981,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF99"/>
       <color rgb="FF00FF00"/>
       <color rgb="FFFFFFCC"/>
     </mruColors>
@@ -9349,11 +9286,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B86" sqref="B86:E86"/>
+      <selection pane="bottomRight" activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10557,10 +10494,18 @@
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="194"/>
-      <c r="C87" s="9"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="4"/>
+      <c r="B87" s="194">
+        <v>75</v>
+      </c>
+      <c r="C87" s="9">
+        <v>43592</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="194"/>
@@ -10663,11 +10608,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP201"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="AC20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="AC80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AL41" sqref="AL41:AM41"/>
+      <selection pane="bottomRight" activeCell="AO84" sqref="AO84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10700,48 +10645,48 @@
       <c r="C2" s="418" t="s">
         <v>494</v>
       </c>
-      <c r="AL2" s="490" t="s">
+      <c r="AL2" s="511" t="s">
         <v>515</v>
       </c>
-      <c r="AM2" s="490"/>
+      <c r="AM2" s="511"/>
       <c r="AN2" s="474"/>
     </row>
     <row r="3" spans="1:41" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="506" t="s">
+      <c r="B3" s="492" t="s">
         <v>266</v>
       </c>
-      <c r="C3" s="511" t="s">
+      <c r="C3" s="497" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="512"/>
-      <c r="E3" s="520" t="s">
+      <c r="D3" s="498"/>
+      <c r="E3" s="506" t="s">
         <v>231</v>
       </c>
-      <c r="F3" s="521"/>
-      <c r="G3" s="521"/>
-      <c r="H3" s="521"/>
-      <c r="I3" s="521"/>
-      <c r="J3" s="521"/>
-      <c r="K3" s="521"/>
-      <c r="L3" s="522"/>
-      <c r="M3" s="517" t="s">
+      <c r="F3" s="507"/>
+      <c r="G3" s="507"/>
+      <c r="H3" s="507"/>
+      <c r="I3" s="507"/>
+      <c r="J3" s="507"/>
+      <c r="K3" s="507"/>
+      <c r="L3" s="508"/>
+      <c r="M3" s="503" t="s">
         <v>443</v>
       </c>
-      <c r="N3" s="518"/>
-      <c r="O3" s="519"/>
-      <c r="P3" s="513" t="s">
+      <c r="N3" s="504"/>
+      <c r="O3" s="505"/>
+      <c r="P3" s="499" t="s">
         <v>296</v>
       </c>
-      <c r="Q3" s="514"/>
-      <c r="R3" s="515" t="s">
+      <c r="Q3" s="500"/>
+      <c r="R3" s="501" t="s">
         <v>297</v>
       </c>
-      <c r="S3" s="516"/>
-      <c r="T3" s="508" t="s">
+      <c r="S3" s="502"/>
+      <c r="T3" s="494" t="s">
         <v>298</v>
       </c>
-      <c r="U3" s="509"/>
-      <c r="V3" s="510"/>
+      <c r="U3" s="495"/>
+      <c r="V3" s="496"/>
       <c r="W3" s="296" t="s">
         <v>434</v>
       </c>
@@ -10794,12 +10739,12 @@
         <v>493</v>
       </c>
       <c r="AN3" s="475"/>
-      <c r="AO3" s="504" t="s">
+      <c r="AO3" s="490" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:41" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="507"/>
+      <c r="B4" s="493"/>
       <c r="C4" s="293" t="s">
         <v>432</v>
       </c>
@@ -10905,17 +10850,17 @@
       <c r="AK4" s="387" t="s">
         <v>431</v>
       </c>
-      <c r="AL4" s="523" t="s">
+      <c r="AL4" s="509" t="s">
         <v>517</v>
       </c>
-      <c r="AM4" s="524"/>
+      <c r="AM4" s="510"/>
       <c r="AN4" s="476" t="s">
         <v>535</v>
       </c>
-      <c r="AO4" s="505"/>
+      <c r="AO4" s="491"/>
     </row>
     <row r="5" spans="1:41" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="491"/>
+      <c r="A5" s="512"/>
       <c r="B5" s="323" t="s">
         <v>293</v>
       </c>
@@ -10925,50 +10870,50 @@
       <c r="D5" s="325" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="495" t="s">
+      <c r="E5" s="516" t="s">
         <v>333</v>
       </c>
-      <c r="F5" s="496"/>
-      <c r="G5" s="496"/>
-      <c r="H5" s="496"/>
-      <c r="I5" s="496"/>
-      <c r="J5" s="496"/>
-      <c r="K5" s="496"/>
-      <c r="L5" s="497"/>
-      <c r="M5" s="495" t="s">
+      <c r="F5" s="517"/>
+      <c r="G5" s="517"/>
+      <c r="H5" s="517"/>
+      <c r="I5" s="517"/>
+      <c r="J5" s="517"/>
+      <c r="K5" s="517"/>
+      <c r="L5" s="518"/>
+      <c r="M5" s="516" t="s">
         <v>334</v>
       </c>
-      <c r="N5" s="496"/>
-      <c r="O5" s="496"/>
-      <c r="P5" s="496"/>
-      <c r="Q5" s="496"/>
-      <c r="R5" s="496"/>
-      <c r="S5" s="496"/>
-      <c r="T5" s="496"/>
-      <c r="U5" s="496"/>
-      <c r="V5" s="496"/>
-      <c r="W5" s="496"/>
-      <c r="X5" s="496"/>
-      <c r="Y5" s="496"/>
-      <c r="Z5" s="496"/>
-      <c r="AA5" s="496"/>
-      <c r="AB5" s="496"/>
-      <c r="AC5" s="496"/>
-      <c r="AD5" s="496"/>
-      <c r="AE5" s="496"/>
-      <c r="AF5" s="496"/>
-      <c r="AG5" s="496"/>
-      <c r="AH5" s="496"/>
-      <c r="AI5" s="496"/>
-      <c r="AJ5" s="496"/>
-      <c r="AK5" s="496"/>
-      <c r="AL5" s="499"/>
-      <c r="AM5" s="500"/>
+      <c r="N5" s="517"/>
+      <c r="O5" s="517"/>
+      <c r="P5" s="517"/>
+      <c r="Q5" s="517"/>
+      <c r="R5" s="517"/>
+      <c r="S5" s="517"/>
+      <c r="T5" s="517"/>
+      <c r="U5" s="517"/>
+      <c r="V5" s="517"/>
+      <c r="W5" s="517"/>
+      <c r="X5" s="517"/>
+      <c r="Y5" s="517"/>
+      <c r="Z5" s="517"/>
+      <c r="AA5" s="517"/>
+      <c r="AB5" s="517"/>
+      <c r="AC5" s="517"/>
+      <c r="AD5" s="517"/>
+      <c r="AE5" s="517"/>
+      <c r="AF5" s="517"/>
+      <c r="AG5" s="517"/>
+      <c r="AH5" s="517"/>
+      <c r="AI5" s="517"/>
+      <c r="AJ5" s="517"/>
+      <c r="AK5" s="517"/>
+      <c r="AL5" s="520"/>
+      <c r="AM5" s="521"/>
       <c r="AN5" s="473"/>
       <c r="AO5" s="320"/>
     </row>
     <row r="6" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="491"/>
+      <c r="A6" s="512"/>
       <c r="B6" s="326"/>
       <c r="C6" s="327" t="s">
         <v>8</v>
@@ -10976,46 +10921,46 @@
       <c r="D6" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="498"/>
-      <c r="F6" s="499"/>
-      <c r="G6" s="499"/>
-      <c r="H6" s="499"/>
-      <c r="I6" s="499"/>
-      <c r="J6" s="499"/>
-      <c r="K6" s="499"/>
-      <c r="L6" s="500"/>
-      <c r="M6" s="498"/>
-      <c r="N6" s="499"/>
-      <c r="O6" s="499"/>
-      <c r="P6" s="499"/>
-      <c r="Q6" s="499"/>
-      <c r="R6" s="499"/>
-      <c r="S6" s="499"/>
-      <c r="T6" s="499"/>
-      <c r="U6" s="499"/>
-      <c r="V6" s="499"/>
-      <c r="W6" s="499"/>
-      <c r="X6" s="499"/>
-      <c r="Y6" s="499"/>
-      <c r="Z6" s="499"/>
-      <c r="AA6" s="499"/>
-      <c r="AB6" s="499"/>
-      <c r="AC6" s="499"/>
-      <c r="AD6" s="499"/>
-      <c r="AE6" s="499"/>
-      <c r="AF6" s="499"/>
-      <c r="AG6" s="499"/>
-      <c r="AH6" s="499"/>
-      <c r="AI6" s="499"/>
-      <c r="AJ6" s="499"/>
-      <c r="AK6" s="499"/>
-      <c r="AL6" s="499"/>
-      <c r="AM6" s="500"/>
+      <c r="E6" s="519"/>
+      <c r="F6" s="520"/>
+      <c r="G6" s="520"/>
+      <c r="H6" s="520"/>
+      <c r="I6" s="520"/>
+      <c r="J6" s="520"/>
+      <c r="K6" s="520"/>
+      <c r="L6" s="521"/>
+      <c r="M6" s="519"/>
+      <c r="N6" s="520"/>
+      <c r="O6" s="520"/>
+      <c r="P6" s="520"/>
+      <c r="Q6" s="520"/>
+      <c r="R6" s="520"/>
+      <c r="S6" s="520"/>
+      <c r="T6" s="520"/>
+      <c r="U6" s="520"/>
+      <c r="V6" s="520"/>
+      <c r="W6" s="520"/>
+      <c r="X6" s="520"/>
+      <c r="Y6" s="520"/>
+      <c r="Z6" s="520"/>
+      <c r="AA6" s="520"/>
+      <c r="AB6" s="520"/>
+      <c r="AC6" s="520"/>
+      <c r="AD6" s="520"/>
+      <c r="AE6" s="520"/>
+      <c r="AF6" s="520"/>
+      <c r="AG6" s="520"/>
+      <c r="AH6" s="520"/>
+      <c r="AI6" s="520"/>
+      <c r="AJ6" s="520"/>
+      <c r="AK6" s="520"/>
+      <c r="AL6" s="520"/>
+      <c r="AM6" s="521"/>
       <c r="AN6" s="473"/>
       <c r="AO6" s="321"/>
     </row>
     <row r="7" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="491"/>
+      <c r="A7" s="512"/>
       <c r="B7" s="326"/>
       <c r="C7" s="327" t="s">
         <v>11</v>
@@ -11023,46 +10968,46 @@
       <c r="D7" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="498"/>
-      <c r="F7" s="499"/>
-      <c r="G7" s="499"/>
-      <c r="H7" s="499"/>
-      <c r="I7" s="499"/>
-      <c r="J7" s="499"/>
-      <c r="K7" s="499"/>
-      <c r="L7" s="500"/>
-      <c r="M7" s="498"/>
-      <c r="N7" s="499"/>
-      <c r="O7" s="499"/>
-      <c r="P7" s="499"/>
-      <c r="Q7" s="499"/>
-      <c r="R7" s="499"/>
-      <c r="S7" s="499"/>
-      <c r="T7" s="499"/>
-      <c r="U7" s="499"/>
-      <c r="V7" s="499"/>
-      <c r="W7" s="499"/>
-      <c r="X7" s="499"/>
-      <c r="Y7" s="499"/>
-      <c r="Z7" s="499"/>
-      <c r="AA7" s="499"/>
-      <c r="AB7" s="499"/>
-      <c r="AC7" s="499"/>
-      <c r="AD7" s="499"/>
-      <c r="AE7" s="499"/>
-      <c r="AF7" s="499"/>
-      <c r="AG7" s="499"/>
-      <c r="AH7" s="499"/>
-      <c r="AI7" s="499"/>
-      <c r="AJ7" s="499"/>
-      <c r="AK7" s="499"/>
-      <c r="AL7" s="499"/>
-      <c r="AM7" s="500"/>
+      <c r="E7" s="519"/>
+      <c r="F7" s="520"/>
+      <c r="G7" s="520"/>
+      <c r="H7" s="520"/>
+      <c r="I7" s="520"/>
+      <c r="J7" s="520"/>
+      <c r="K7" s="520"/>
+      <c r="L7" s="521"/>
+      <c r="M7" s="519"/>
+      <c r="N7" s="520"/>
+      <c r="O7" s="520"/>
+      <c r="P7" s="520"/>
+      <c r="Q7" s="520"/>
+      <c r="R7" s="520"/>
+      <c r="S7" s="520"/>
+      <c r="T7" s="520"/>
+      <c r="U7" s="520"/>
+      <c r="V7" s="520"/>
+      <c r="W7" s="520"/>
+      <c r="X7" s="520"/>
+      <c r="Y7" s="520"/>
+      <c r="Z7" s="520"/>
+      <c r="AA7" s="520"/>
+      <c r="AB7" s="520"/>
+      <c r="AC7" s="520"/>
+      <c r="AD7" s="520"/>
+      <c r="AE7" s="520"/>
+      <c r="AF7" s="520"/>
+      <c r="AG7" s="520"/>
+      <c r="AH7" s="520"/>
+      <c r="AI7" s="520"/>
+      <c r="AJ7" s="520"/>
+      <c r="AK7" s="520"/>
+      <c r="AL7" s="520"/>
+      <c r="AM7" s="521"/>
       <c r="AN7" s="473"/>
       <c r="AO7" s="321"/>
     </row>
     <row r="8" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="491"/>
+      <c r="A8" s="512"/>
       <c r="B8" s="326"/>
       <c r="C8" s="327" t="s">
         <v>12</v>
@@ -11070,46 +11015,46 @@
       <c r="D8" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="498"/>
-      <c r="F8" s="499"/>
-      <c r="G8" s="499"/>
-      <c r="H8" s="499"/>
-      <c r="I8" s="499"/>
-      <c r="J8" s="499"/>
-      <c r="K8" s="499"/>
-      <c r="L8" s="500"/>
-      <c r="M8" s="498"/>
-      <c r="N8" s="499"/>
-      <c r="O8" s="499"/>
-      <c r="P8" s="499"/>
-      <c r="Q8" s="499"/>
-      <c r="R8" s="499"/>
-      <c r="S8" s="499"/>
-      <c r="T8" s="499"/>
-      <c r="U8" s="499"/>
-      <c r="V8" s="499"/>
-      <c r="W8" s="499"/>
-      <c r="X8" s="499"/>
-      <c r="Y8" s="499"/>
-      <c r="Z8" s="499"/>
-      <c r="AA8" s="499"/>
-      <c r="AB8" s="499"/>
-      <c r="AC8" s="499"/>
-      <c r="AD8" s="499"/>
-      <c r="AE8" s="499"/>
-      <c r="AF8" s="499"/>
-      <c r="AG8" s="499"/>
-      <c r="AH8" s="499"/>
-      <c r="AI8" s="499"/>
-      <c r="AJ8" s="499"/>
-      <c r="AK8" s="499"/>
-      <c r="AL8" s="499"/>
-      <c r="AM8" s="500"/>
+      <c r="E8" s="519"/>
+      <c r="F8" s="520"/>
+      <c r="G8" s="520"/>
+      <c r="H8" s="520"/>
+      <c r="I8" s="520"/>
+      <c r="J8" s="520"/>
+      <c r="K8" s="520"/>
+      <c r="L8" s="521"/>
+      <c r="M8" s="519"/>
+      <c r="N8" s="520"/>
+      <c r="O8" s="520"/>
+      <c r="P8" s="520"/>
+      <c r="Q8" s="520"/>
+      <c r="R8" s="520"/>
+      <c r="S8" s="520"/>
+      <c r="T8" s="520"/>
+      <c r="U8" s="520"/>
+      <c r="V8" s="520"/>
+      <c r="W8" s="520"/>
+      <c r="X8" s="520"/>
+      <c r="Y8" s="520"/>
+      <c r="Z8" s="520"/>
+      <c r="AA8" s="520"/>
+      <c r="AB8" s="520"/>
+      <c r="AC8" s="520"/>
+      <c r="AD8" s="520"/>
+      <c r="AE8" s="520"/>
+      <c r="AF8" s="520"/>
+      <c r="AG8" s="520"/>
+      <c r="AH8" s="520"/>
+      <c r="AI8" s="520"/>
+      <c r="AJ8" s="520"/>
+      <c r="AK8" s="520"/>
+      <c r="AL8" s="520"/>
+      <c r="AM8" s="521"/>
       <c r="AN8" s="473"/>
       <c r="AO8" s="321"/>
     </row>
     <row r="9" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="491"/>
+      <c r="A9" s="512"/>
       <c r="B9" s="326"/>
       <c r="C9" s="327" t="s">
         <v>319</v>
@@ -11117,46 +11062,46 @@
       <c r="D9" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="498"/>
-      <c r="F9" s="499"/>
-      <c r="G9" s="499"/>
-      <c r="H9" s="499"/>
-      <c r="I9" s="499"/>
-      <c r="J9" s="499"/>
-      <c r="K9" s="499"/>
-      <c r="L9" s="500"/>
-      <c r="M9" s="498"/>
-      <c r="N9" s="499"/>
-      <c r="O9" s="499"/>
-      <c r="P9" s="499"/>
-      <c r="Q9" s="499"/>
-      <c r="R9" s="499"/>
-      <c r="S9" s="499"/>
-      <c r="T9" s="499"/>
-      <c r="U9" s="499"/>
-      <c r="V9" s="499"/>
-      <c r="W9" s="499"/>
-      <c r="X9" s="499"/>
-      <c r="Y9" s="499"/>
-      <c r="Z9" s="499"/>
-      <c r="AA9" s="499"/>
-      <c r="AB9" s="499"/>
-      <c r="AC9" s="499"/>
-      <c r="AD9" s="499"/>
-      <c r="AE9" s="499"/>
-      <c r="AF9" s="499"/>
-      <c r="AG9" s="499"/>
-      <c r="AH9" s="499"/>
-      <c r="AI9" s="499"/>
-      <c r="AJ9" s="499"/>
-      <c r="AK9" s="499"/>
-      <c r="AL9" s="499"/>
-      <c r="AM9" s="500"/>
+      <c r="E9" s="519"/>
+      <c r="F9" s="520"/>
+      <c r="G9" s="520"/>
+      <c r="H9" s="520"/>
+      <c r="I9" s="520"/>
+      <c r="J9" s="520"/>
+      <c r="K9" s="520"/>
+      <c r="L9" s="521"/>
+      <c r="M9" s="519"/>
+      <c r="N9" s="520"/>
+      <c r="O9" s="520"/>
+      <c r="P9" s="520"/>
+      <c r="Q9" s="520"/>
+      <c r="R9" s="520"/>
+      <c r="S9" s="520"/>
+      <c r="T9" s="520"/>
+      <c r="U9" s="520"/>
+      <c r="V9" s="520"/>
+      <c r="W9" s="520"/>
+      <c r="X9" s="520"/>
+      <c r="Y9" s="520"/>
+      <c r="Z9" s="520"/>
+      <c r="AA9" s="520"/>
+      <c r="AB9" s="520"/>
+      <c r="AC9" s="520"/>
+      <c r="AD9" s="520"/>
+      <c r="AE9" s="520"/>
+      <c r="AF9" s="520"/>
+      <c r="AG9" s="520"/>
+      <c r="AH9" s="520"/>
+      <c r="AI9" s="520"/>
+      <c r="AJ9" s="520"/>
+      <c r="AK9" s="520"/>
+      <c r="AL9" s="520"/>
+      <c r="AM9" s="521"/>
       <c r="AN9" s="473"/>
       <c r="AO9" s="321"/>
     </row>
     <row r="10" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="491"/>
+      <c r="A10" s="512"/>
       <c r="B10" s="326"/>
       <c r="C10" s="327" t="s">
         <v>177</v>
@@ -11164,46 +11109,46 @@
       <c r="D10" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="498"/>
-      <c r="F10" s="499"/>
-      <c r="G10" s="499"/>
-      <c r="H10" s="499"/>
-      <c r="I10" s="499"/>
-      <c r="J10" s="499"/>
-      <c r="K10" s="499"/>
-      <c r="L10" s="500"/>
-      <c r="M10" s="498"/>
-      <c r="N10" s="499"/>
-      <c r="O10" s="499"/>
-      <c r="P10" s="499"/>
-      <c r="Q10" s="499"/>
-      <c r="R10" s="499"/>
-      <c r="S10" s="499"/>
-      <c r="T10" s="499"/>
-      <c r="U10" s="499"/>
-      <c r="V10" s="499"/>
-      <c r="W10" s="499"/>
-      <c r="X10" s="499"/>
-      <c r="Y10" s="499"/>
-      <c r="Z10" s="499"/>
-      <c r="AA10" s="499"/>
-      <c r="AB10" s="499"/>
-      <c r="AC10" s="499"/>
-      <c r="AD10" s="499"/>
-      <c r="AE10" s="499"/>
-      <c r="AF10" s="499"/>
-      <c r="AG10" s="499"/>
-      <c r="AH10" s="499"/>
-      <c r="AI10" s="499"/>
-      <c r="AJ10" s="499"/>
-      <c r="AK10" s="499"/>
-      <c r="AL10" s="499"/>
-      <c r="AM10" s="500"/>
+      <c r="E10" s="519"/>
+      <c r="F10" s="520"/>
+      <c r="G10" s="520"/>
+      <c r="H10" s="520"/>
+      <c r="I10" s="520"/>
+      <c r="J10" s="520"/>
+      <c r="K10" s="520"/>
+      <c r="L10" s="521"/>
+      <c r="M10" s="519"/>
+      <c r="N10" s="520"/>
+      <c r="O10" s="520"/>
+      <c r="P10" s="520"/>
+      <c r="Q10" s="520"/>
+      <c r="R10" s="520"/>
+      <c r="S10" s="520"/>
+      <c r="T10" s="520"/>
+      <c r="U10" s="520"/>
+      <c r="V10" s="520"/>
+      <c r="W10" s="520"/>
+      <c r="X10" s="520"/>
+      <c r="Y10" s="520"/>
+      <c r="Z10" s="520"/>
+      <c r="AA10" s="520"/>
+      <c r="AB10" s="520"/>
+      <c r="AC10" s="520"/>
+      <c r="AD10" s="520"/>
+      <c r="AE10" s="520"/>
+      <c r="AF10" s="520"/>
+      <c r="AG10" s="520"/>
+      <c r="AH10" s="520"/>
+      <c r="AI10" s="520"/>
+      <c r="AJ10" s="520"/>
+      <c r="AK10" s="520"/>
+      <c r="AL10" s="520"/>
+      <c r="AM10" s="521"/>
       <c r="AN10" s="473"/>
       <c r="AO10" s="321"/>
     </row>
     <row r="11" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="491"/>
+      <c r="A11" s="512"/>
       <c r="B11" s="326"/>
       <c r="C11" s="327" t="s">
         <v>16</v>
@@ -11211,46 +11156,46 @@
       <c r="D11" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="498"/>
-      <c r="F11" s="499"/>
-      <c r="G11" s="499"/>
-      <c r="H11" s="499"/>
-      <c r="I11" s="499"/>
-      <c r="J11" s="499"/>
-      <c r="K11" s="499"/>
-      <c r="L11" s="500"/>
-      <c r="M11" s="498"/>
-      <c r="N11" s="499"/>
-      <c r="O11" s="499"/>
-      <c r="P11" s="499"/>
-      <c r="Q11" s="499"/>
-      <c r="R11" s="499"/>
-      <c r="S11" s="499"/>
-      <c r="T11" s="499"/>
-      <c r="U11" s="499"/>
-      <c r="V11" s="499"/>
-      <c r="W11" s="499"/>
-      <c r="X11" s="499"/>
-      <c r="Y11" s="499"/>
-      <c r="Z11" s="499"/>
-      <c r="AA11" s="499"/>
-      <c r="AB11" s="499"/>
-      <c r="AC11" s="499"/>
-      <c r="AD11" s="499"/>
-      <c r="AE11" s="499"/>
-      <c r="AF11" s="499"/>
-      <c r="AG11" s="499"/>
-      <c r="AH11" s="499"/>
-      <c r="AI11" s="499"/>
-      <c r="AJ11" s="499"/>
-      <c r="AK11" s="499"/>
-      <c r="AL11" s="499"/>
-      <c r="AM11" s="500"/>
+      <c r="E11" s="519"/>
+      <c r="F11" s="520"/>
+      <c r="G11" s="520"/>
+      <c r="H11" s="520"/>
+      <c r="I11" s="520"/>
+      <c r="J11" s="520"/>
+      <c r="K11" s="520"/>
+      <c r="L11" s="521"/>
+      <c r="M11" s="519"/>
+      <c r="N11" s="520"/>
+      <c r="O11" s="520"/>
+      <c r="P11" s="520"/>
+      <c r="Q11" s="520"/>
+      <c r="R11" s="520"/>
+      <c r="S11" s="520"/>
+      <c r="T11" s="520"/>
+      <c r="U11" s="520"/>
+      <c r="V11" s="520"/>
+      <c r="W11" s="520"/>
+      <c r="X11" s="520"/>
+      <c r="Y11" s="520"/>
+      <c r="Z11" s="520"/>
+      <c r="AA11" s="520"/>
+      <c r="AB11" s="520"/>
+      <c r="AC11" s="520"/>
+      <c r="AD11" s="520"/>
+      <c r="AE11" s="520"/>
+      <c r="AF11" s="520"/>
+      <c r="AG11" s="520"/>
+      <c r="AH11" s="520"/>
+      <c r="AI11" s="520"/>
+      <c r="AJ11" s="520"/>
+      <c r="AK11" s="520"/>
+      <c r="AL11" s="520"/>
+      <c r="AM11" s="521"/>
       <c r="AN11" s="473"/>
       <c r="AO11" s="321"/>
     </row>
     <row r="12" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="491"/>
+      <c r="A12" s="512"/>
       <c r="B12" s="326"/>
       <c r="C12" s="327" t="s">
         <v>17</v>
@@ -11258,46 +11203,46 @@
       <c r="D12" s="329" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="498"/>
-      <c r="F12" s="499"/>
-      <c r="G12" s="499"/>
-      <c r="H12" s="499"/>
-      <c r="I12" s="499"/>
-      <c r="J12" s="499"/>
-      <c r="K12" s="499"/>
-      <c r="L12" s="500"/>
-      <c r="M12" s="498"/>
-      <c r="N12" s="499"/>
-      <c r="O12" s="499"/>
-      <c r="P12" s="499"/>
-      <c r="Q12" s="499"/>
-      <c r="R12" s="499"/>
-      <c r="S12" s="499"/>
-      <c r="T12" s="499"/>
-      <c r="U12" s="499"/>
-      <c r="V12" s="499"/>
-      <c r="W12" s="499"/>
-      <c r="X12" s="499"/>
-      <c r="Y12" s="499"/>
-      <c r="Z12" s="499"/>
-      <c r="AA12" s="499"/>
-      <c r="AB12" s="499"/>
-      <c r="AC12" s="499"/>
-      <c r="AD12" s="499"/>
-      <c r="AE12" s="499"/>
-      <c r="AF12" s="499"/>
-      <c r="AG12" s="499"/>
-      <c r="AH12" s="499"/>
-      <c r="AI12" s="499"/>
-      <c r="AJ12" s="499"/>
-      <c r="AK12" s="499"/>
-      <c r="AL12" s="499"/>
-      <c r="AM12" s="500"/>
+      <c r="E12" s="519"/>
+      <c r="F12" s="520"/>
+      <c r="G12" s="520"/>
+      <c r="H12" s="520"/>
+      <c r="I12" s="520"/>
+      <c r="J12" s="520"/>
+      <c r="K12" s="520"/>
+      <c r="L12" s="521"/>
+      <c r="M12" s="519"/>
+      <c r="N12" s="520"/>
+      <c r="O12" s="520"/>
+      <c r="P12" s="520"/>
+      <c r="Q12" s="520"/>
+      <c r="R12" s="520"/>
+      <c r="S12" s="520"/>
+      <c r="T12" s="520"/>
+      <c r="U12" s="520"/>
+      <c r="V12" s="520"/>
+      <c r="W12" s="520"/>
+      <c r="X12" s="520"/>
+      <c r="Y12" s="520"/>
+      <c r="Z12" s="520"/>
+      <c r="AA12" s="520"/>
+      <c r="AB12" s="520"/>
+      <c r="AC12" s="520"/>
+      <c r="AD12" s="520"/>
+      <c r="AE12" s="520"/>
+      <c r="AF12" s="520"/>
+      <c r="AG12" s="520"/>
+      <c r="AH12" s="520"/>
+      <c r="AI12" s="520"/>
+      <c r="AJ12" s="520"/>
+      <c r="AK12" s="520"/>
+      <c r="AL12" s="520"/>
+      <c r="AM12" s="521"/>
       <c r="AN12" s="473"/>
       <c r="AO12" s="321"/>
     </row>
     <row r="13" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="491"/>
+      <c r="A13" s="512"/>
       <c r="B13" s="326"/>
       <c r="C13" s="327" t="s">
         <v>19</v>
@@ -11305,46 +11250,46 @@
       <c r="D13" s="329">
         <v>32</v>
       </c>
-      <c r="E13" s="498"/>
-      <c r="F13" s="499"/>
-      <c r="G13" s="499"/>
-      <c r="H13" s="499"/>
-      <c r="I13" s="499"/>
-      <c r="J13" s="499"/>
-      <c r="K13" s="499"/>
-      <c r="L13" s="500"/>
-      <c r="M13" s="498"/>
-      <c r="N13" s="499"/>
-      <c r="O13" s="499"/>
-      <c r="P13" s="499"/>
-      <c r="Q13" s="499"/>
-      <c r="R13" s="499"/>
-      <c r="S13" s="499"/>
-      <c r="T13" s="499"/>
-      <c r="U13" s="499"/>
-      <c r="V13" s="499"/>
-      <c r="W13" s="499"/>
-      <c r="X13" s="499"/>
-      <c r="Y13" s="499"/>
-      <c r="Z13" s="499"/>
-      <c r="AA13" s="499"/>
-      <c r="AB13" s="499"/>
-      <c r="AC13" s="499"/>
-      <c r="AD13" s="499"/>
-      <c r="AE13" s="499"/>
-      <c r="AF13" s="499"/>
-      <c r="AG13" s="499"/>
-      <c r="AH13" s="499"/>
-      <c r="AI13" s="499"/>
-      <c r="AJ13" s="499"/>
-      <c r="AK13" s="499"/>
-      <c r="AL13" s="499"/>
-      <c r="AM13" s="500"/>
+      <c r="E13" s="519"/>
+      <c r="F13" s="520"/>
+      <c r="G13" s="520"/>
+      <c r="H13" s="520"/>
+      <c r="I13" s="520"/>
+      <c r="J13" s="520"/>
+      <c r="K13" s="520"/>
+      <c r="L13" s="521"/>
+      <c r="M13" s="519"/>
+      <c r="N13" s="520"/>
+      <c r="O13" s="520"/>
+      <c r="P13" s="520"/>
+      <c r="Q13" s="520"/>
+      <c r="R13" s="520"/>
+      <c r="S13" s="520"/>
+      <c r="T13" s="520"/>
+      <c r="U13" s="520"/>
+      <c r="V13" s="520"/>
+      <c r="W13" s="520"/>
+      <c r="X13" s="520"/>
+      <c r="Y13" s="520"/>
+      <c r="Z13" s="520"/>
+      <c r="AA13" s="520"/>
+      <c r="AB13" s="520"/>
+      <c r="AC13" s="520"/>
+      <c r="AD13" s="520"/>
+      <c r="AE13" s="520"/>
+      <c r="AF13" s="520"/>
+      <c r="AG13" s="520"/>
+      <c r="AH13" s="520"/>
+      <c r="AI13" s="520"/>
+      <c r="AJ13" s="520"/>
+      <c r="AK13" s="520"/>
+      <c r="AL13" s="520"/>
+      <c r="AM13" s="521"/>
       <c r="AN13" s="473"/>
       <c r="AO13" s="321"/>
     </row>
     <row r="14" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="491"/>
+      <c r="A14" s="512"/>
       <c r="B14" s="326"/>
       <c r="C14" s="327" t="s">
         <v>20</v>
@@ -11352,46 +11297,46 @@
       <c r="D14" s="329">
         <v>32</v>
       </c>
-      <c r="E14" s="498"/>
-      <c r="F14" s="499"/>
-      <c r="G14" s="499"/>
-      <c r="H14" s="499"/>
-      <c r="I14" s="499"/>
-      <c r="J14" s="499"/>
-      <c r="K14" s="499"/>
-      <c r="L14" s="500"/>
-      <c r="M14" s="498"/>
-      <c r="N14" s="499"/>
-      <c r="O14" s="499"/>
-      <c r="P14" s="499"/>
-      <c r="Q14" s="499"/>
-      <c r="R14" s="499"/>
-      <c r="S14" s="499"/>
-      <c r="T14" s="499"/>
-      <c r="U14" s="499"/>
-      <c r="V14" s="499"/>
-      <c r="W14" s="499"/>
-      <c r="X14" s="499"/>
-      <c r="Y14" s="499"/>
-      <c r="Z14" s="499"/>
-      <c r="AA14" s="499"/>
-      <c r="AB14" s="499"/>
-      <c r="AC14" s="499"/>
-      <c r="AD14" s="499"/>
-      <c r="AE14" s="499"/>
-      <c r="AF14" s="499"/>
-      <c r="AG14" s="499"/>
-      <c r="AH14" s="499"/>
-      <c r="AI14" s="499"/>
-      <c r="AJ14" s="499"/>
-      <c r="AK14" s="499"/>
-      <c r="AL14" s="499"/>
-      <c r="AM14" s="500"/>
+      <c r="E14" s="519"/>
+      <c r="F14" s="520"/>
+      <c r="G14" s="520"/>
+      <c r="H14" s="520"/>
+      <c r="I14" s="520"/>
+      <c r="J14" s="520"/>
+      <c r="K14" s="520"/>
+      <c r="L14" s="521"/>
+      <c r="M14" s="519"/>
+      <c r="N14" s="520"/>
+      <c r="O14" s="520"/>
+      <c r="P14" s="520"/>
+      <c r="Q14" s="520"/>
+      <c r="R14" s="520"/>
+      <c r="S14" s="520"/>
+      <c r="T14" s="520"/>
+      <c r="U14" s="520"/>
+      <c r="V14" s="520"/>
+      <c r="W14" s="520"/>
+      <c r="X14" s="520"/>
+      <c r="Y14" s="520"/>
+      <c r="Z14" s="520"/>
+      <c r="AA14" s="520"/>
+      <c r="AB14" s="520"/>
+      <c r="AC14" s="520"/>
+      <c r="AD14" s="520"/>
+      <c r="AE14" s="520"/>
+      <c r="AF14" s="520"/>
+      <c r="AG14" s="520"/>
+      <c r="AH14" s="520"/>
+      <c r="AI14" s="520"/>
+      <c r="AJ14" s="520"/>
+      <c r="AK14" s="520"/>
+      <c r="AL14" s="520"/>
+      <c r="AM14" s="521"/>
       <c r="AN14" s="473"/>
       <c r="AO14" s="321"/>
     </row>
     <row r="15" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="491"/>
+      <c r="A15" s="512"/>
       <c r="B15" s="326"/>
       <c r="C15" s="327" t="s">
         <v>21</v>
@@ -11399,46 +11344,46 @@
       <c r="D15" s="329" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="498"/>
-      <c r="F15" s="499"/>
-      <c r="G15" s="499"/>
-      <c r="H15" s="499"/>
-      <c r="I15" s="499"/>
-      <c r="J15" s="499"/>
-      <c r="K15" s="499"/>
-      <c r="L15" s="500"/>
-      <c r="M15" s="498"/>
-      <c r="N15" s="499"/>
-      <c r="O15" s="499"/>
-      <c r="P15" s="499"/>
-      <c r="Q15" s="499"/>
-      <c r="R15" s="499"/>
-      <c r="S15" s="499"/>
-      <c r="T15" s="499"/>
-      <c r="U15" s="499"/>
-      <c r="V15" s="499"/>
-      <c r="W15" s="499"/>
-      <c r="X15" s="499"/>
-      <c r="Y15" s="499"/>
-      <c r="Z15" s="499"/>
-      <c r="AA15" s="499"/>
-      <c r="AB15" s="499"/>
-      <c r="AC15" s="499"/>
-      <c r="AD15" s="499"/>
-      <c r="AE15" s="499"/>
-      <c r="AF15" s="499"/>
-      <c r="AG15" s="499"/>
-      <c r="AH15" s="499"/>
-      <c r="AI15" s="499"/>
-      <c r="AJ15" s="499"/>
-      <c r="AK15" s="499"/>
-      <c r="AL15" s="499"/>
-      <c r="AM15" s="500"/>
+      <c r="E15" s="519"/>
+      <c r="F15" s="520"/>
+      <c r="G15" s="520"/>
+      <c r="H15" s="520"/>
+      <c r="I15" s="520"/>
+      <c r="J15" s="520"/>
+      <c r="K15" s="520"/>
+      <c r="L15" s="521"/>
+      <c r="M15" s="519"/>
+      <c r="N15" s="520"/>
+      <c r="O15" s="520"/>
+      <c r="P15" s="520"/>
+      <c r="Q15" s="520"/>
+      <c r="R15" s="520"/>
+      <c r="S15" s="520"/>
+      <c r="T15" s="520"/>
+      <c r="U15" s="520"/>
+      <c r="V15" s="520"/>
+      <c r="W15" s="520"/>
+      <c r="X15" s="520"/>
+      <c r="Y15" s="520"/>
+      <c r="Z15" s="520"/>
+      <c r="AA15" s="520"/>
+      <c r="AB15" s="520"/>
+      <c r="AC15" s="520"/>
+      <c r="AD15" s="520"/>
+      <c r="AE15" s="520"/>
+      <c r="AF15" s="520"/>
+      <c r="AG15" s="520"/>
+      <c r="AH15" s="520"/>
+      <c r="AI15" s="520"/>
+      <c r="AJ15" s="520"/>
+      <c r="AK15" s="520"/>
+      <c r="AL15" s="520"/>
+      <c r="AM15" s="521"/>
       <c r="AN15" s="473"/>
       <c r="AO15" s="321"/>
     </row>
     <row r="16" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="491"/>
+      <c r="A16" s="512"/>
       <c r="B16" s="326" t="s">
         <v>22</v>
       </c>
@@ -11448,46 +11393,46 @@
       <c r="D16" s="328" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="498"/>
-      <c r="F16" s="499"/>
-      <c r="G16" s="499"/>
-      <c r="H16" s="499"/>
-      <c r="I16" s="499"/>
-      <c r="J16" s="499"/>
-      <c r="K16" s="499"/>
-      <c r="L16" s="500"/>
-      <c r="M16" s="498"/>
-      <c r="N16" s="499"/>
-      <c r="O16" s="499"/>
-      <c r="P16" s="499"/>
-      <c r="Q16" s="499"/>
-      <c r="R16" s="499"/>
-      <c r="S16" s="499"/>
-      <c r="T16" s="499"/>
-      <c r="U16" s="499"/>
-      <c r="V16" s="499"/>
-      <c r="W16" s="499"/>
-      <c r="X16" s="499"/>
-      <c r="Y16" s="499"/>
-      <c r="Z16" s="499"/>
-      <c r="AA16" s="499"/>
-      <c r="AB16" s="499"/>
-      <c r="AC16" s="499"/>
-      <c r="AD16" s="499"/>
-      <c r="AE16" s="499"/>
-      <c r="AF16" s="499"/>
-      <c r="AG16" s="499"/>
-      <c r="AH16" s="499"/>
-      <c r="AI16" s="499"/>
-      <c r="AJ16" s="499"/>
-      <c r="AK16" s="499"/>
-      <c r="AL16" s="499"/>
-      <c r="AM16" s="500"/>
+      <c r="E16" s="519"/>
+      <c r="F16" s="520"/>
+      <c r="G16" s="520"/>
+      <c r="H16" s="520"/>
+      <c r="I16" s="520"/>
+      <c r="J16" s="520"/>
+      <c r="K16" s="520"/>
+      <c r="L16" s="521"/>
+      <c r="M16" s="519"/>
+      <c r="N16" s="520"/>
+      <c r="O16" s="520"/>
+      <c r="P16" s="520"/>
+      <c r="Q16" s="520"/>
+      <c r="R16" s="520"/>
+      <c r="S16" s="520"/>
+      <c r="T16" s="520"/>
+      <c r="U16" s="520"/>
+      <c r="V16" s="520"/>
+      <c r="W16" s="520"/>
+      <c r="X16" s="520"/>
+      <c r="Y16" s="520"/>
+      <c r="Z16" s="520"/>
+      <c r="AA16" s="520"/>
+      <c r="AB16" s="520"/>
+      <c r="AC16" s="520"/>
+      <c r="AD16" s="520"/>
+      <c r="AE16" s="520"/>
+      <c r="AF16" s="520"/>
+      <c r="AG16" s="520"/>
+      <c r="AH16" s="520"/>
+      <c r="AI16" s="520"/>
+      <c r="AJ16" s="520"/>
+      <c r="AK16" s="520"/>
+      <c r="AL16" s="520"/>
+      <c r="AM16" s="521"/>
       <c r="AN16" s="473"/>
       <c r="AO16" s="321"/>
     </row>
     <row r="17" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="491"/>
+      <c r="A17" s="512"/>
       <c r="B17" s="326"/>
       <c r="C17" s="327" t="s">
         <v>26</v>
@@ -11495,46 +11440,46 @@
       <c r="D17" s="328">
         <v>128</v>
       </c>
-      <c r="E17" s="498"/>
-      <c r="F17" s="499"/>
-      <c r="G17" s="499"/>
-      <c r="H17" s="499"/>
-      <c r="I17" s="499"/>
-      <c r="J17" s="499"/>
-      <c r="K17" s="499"/>
-      <c r="L17" s="500"/>
-      <c r="M17" s="498"/>
-      <c r="N17" s="499"/>
-      <c r="O17" s="499"/>
-      <c r="P17" s="499"/>
-      <c r="Q17" s="499"/>
-      <c r="R17" s="499"/>
-      <c r="S17" s="499"/>
-      <c r="T17" s="499"/>
-      <c r="U17" s="499"/>
-      <c r="V17" s="499"/>
-      <c r="W17" s="499"/>
-      <c r="X17" s="499"/>
-      <c r="Y17" s="499"/>
-      <c r="Z17" s="499"/>
-      <c r="AA17" s="499"/>
-      <c r="AB17" s="499"/>
-      <c r="AC17" s="499"/>
-      <c r="AD17" s="499"/>
-      <c r="AE17" s="499"/>
-      <c r="AF17" s="499"/>
-      <c r="AG17" s="499"/>
-      <c r="AH17" s="499"/>
-      <c r="AI17" s="499"/>
-      <c r="AJ17" s="499"/>
-      <c r="AK17" s="499"/>
-      <c r="AL17" s="499"/>
-      <c r="AM17" s="500"/>
+      <c r="E17" s="519"/>
+      <c r="F17" s="520"/>
+      <c r="G17" s="520"/>
+      <c r="H17" s="520"/>
+      <c r="I17" s="520"/>
+      <c r="J17" s="520"/>
+      <c r="K17" s="520"/>
+      <c r="L17" s="521"/>
+      <c r="M17" s="519"/>
+      <c r="N17" s="520"/>
+      <c r="O17" s="520"/>
+      <c r="P17" s="520"/>
+      <c r="Q17" s="520"/>
+      <c r="R17" s="520"/>
+      <c r="S17" s="520"/>
+      <c r="T17" s="520"/>
+      <c r="U17" s="520"/>
+      <c r="V17" s="520"/>
+      <c r="W17" s="520"/>
+      <c r="X17" s="520"/>
+      <c r="Y17" s="520"/>
+      <c r="Z17" s="520"/>
+      <c r="AA17" s="520"/>
+      <c r="AB17" s="520"/>
+      <c r="AC17" s="520"/>
+      <c r="AD17" s="520"/>
+      <c r="AE17" s="520"/>
+      <c r="AF17" s="520"/>
+      <c r="AG17" s="520"/>
+      <c r="AH17" s="520"/>
+      <c r="AI17" s="520"/>
+      <c r="AJ17" s="520"/>
+      <c r="AK17" s="520"/>
+      <c r="AL17" s="520"/>
+      <c r="AM17" s="521"/>
       <c r="AN17" s="473"/>
       <c r="AO17" s="321"/>
     </row>
     <row r="18" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="491"/>
+      <c r="A18" s="512"/>
       <c r="B18" s="326"/>
       <c r="C18" s="327" t="s">
         <v>27</v>
@@ -11542,46 +11487,46 @@
       <c r="D18" s="328" t="s">
         <v>317</v>
       </c>
-      <c r="E18" s="498"/>
-      <c r="F18" s="499"/>
-      <c r="G18" s="499"/>
-      <c r="H18" s="499"/>
-      <c r="I18" s="499"/>
-      <c r="J18" s="499"/>
-      <c r="K18" s="499"/>
-      <c r="L18" s="500"/>
-      <c r="M18" s="498"/>
-      <c r="N18" s="499"/>
-      <c r="O18" s="499"/>
-      <c r="P18" s="499"/>
-      <c r="Q18" s="499"/>
-      <c r="R18" s="499"/>
-      <c r="S18" s="499"/>
-      <c r="T18" s="499"/>
-      <c r="U18" s="499"/>
-      <c r="V18" s="499"/>
-      <c r="W18" s="499"/>
-      <c r="X18" s="499"/>
-      <c r="Y18" s="499"/>
-      <c r="Z18" s="499"/>
-      <c r="AA18" s="499"/>
-      <c r="AB18" s="499"/>
-      <c r="AC18" s="499"/>
-      <c r="AD18" s="499"/>
-      <c r="AE18" s="499"/>
-      <c r="AF18" s="499"/>
-      <c r="AG18" s="499"/>
-      <c r="AH18" s="499"/>
-      <c r="AI18" s="499"/>
-      <c r="AJ18" s="499"/>
-      <c r="AK18" s="499"/>
-      <c r="AL18" s="499"/>
-      <c r="AM18" s="500"/>
+      <c r="E18" s="519"/>
+      <c r="F18" s="520"/>
+      <c r="G18" s="520"/>
+      <c r="H18" s="520"/>
+      <c r="I18" s="520"/>
+      <c r="J18" s="520"/>
+      <c r="K18" s="520"/>
+      <c r="L18" s="521"/>
+      <c r="M18" s="519"/>
+      <c r="N18" s="520"/>
+      <c r="O18" s="520"/>
+      <c r="P18" s="520"/>
+      <c r="Q18" s="520"/>
+      <c r="R18" s="520"/>
+      <c r="S18" s="520"/>
+      <c r="T18" s="520"/>
+      <c r="U18" s="520"/>
+      <c r="V18" s="520"/>
+      <c r="W18" s="520"/>
+      <c r="X18" s="520"/>
+      <c r="Y18" s="520"/>
+      <c r="Z18" s="520"/>
+      <c r="AA18" s="520"/>
+      <c r="AB18" s="520"/>
+      <c r="AC18" s="520"/>
+      <c r="AD18" s="520"/>
+      <c r="AE18" s="520"/>
+      <c r="AF18" s="520"/>
+      <c r="AG18" s="520"/>
+      <c r="AH18" s="520"/>
+      <c r="AI18" s="520"/>
+      <c r="AJ18" s="520"/>
+      <c r="AK18" s="520"/>
+      <c r="AL18" s="520"/>
+      <c r="AM18" s="521"/>
       <c r="AN18" s="473"/>
       <c r="AO18" s="321"/>
     </row>
     <row r="19" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="491"/>
+      <c r="A19" s="512"/>
       <c r="B19" s="326"/>
       <c r="C19" s="327" t="s">
         <v>28</v>
@@ -11589,46 +11534,46 @@
       <c r="D19" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="498"/>
-      <c r="F19" s="499"/>
-      <c r="G19" s="499"/>
-      <c r="H19" s="499"/>
-      <c r="I19" s="499"/>
-      <c r="J19" s="499"/>
-      <c r="K19" s="499"/>
-      <c r="L19" s="500"/>
-      <c r="M19" s="498"/>
-      <c r="N19" s="499"/>
-      <c r="O19" s="499"/>
-      <c r="P19" s="499"/>
-      <c r="Q19" s="499"/>
-      <c r="R19" s="499"/>
-      <c r="S19" s="499"/>
-      <c r="T19" s="499"/>
-      <c r="U19" s="499"/>
-      <c r="V19" s="499"/>
-      <c r="W19" s="499"/>
-      <c r="X19" s="499"/>
-      <c r="Y19" s="499"/>
-      <c r="Z19" s="499"/>
-      <c r="AA19" s="499"/>
-      <c r="AB19" s="499"/>
-      <c r="AC19" s="499"/>
-      <c r="AD19" s="499"/>
-      <c r="AE19" s="499"/>
-      <c r="AF19" s="499"/>
-      <c r="AG19" s="499"/>
-      <c r="AH19" s="499"/>
-      <c r="AI19" s="499"/>
-      <c r="AJ19" s="499"/>
-      <c r="AK19" s="499"/>
-      <c r="AL19" s="499"/>
-      <c r="AM19" s="500"/>
+      <c r="E19" s="519"/>
+      <c r="F19" s="520"/>
+      <c r="G19" s="520"/>
+      <c r="H19" s="520"/>
+      <c r="I19" s="520"/>
+      <c r="J19" s="520"/>
+      <c r="K19" s="520"/>
+      <c r="L19" s="521"/>
+      <c r="M19" s="519"/>
+      <c r="N19" s="520"/>
+      <c r="O19" s="520"/>
+      <c r="P19" s="520"/>
+      <c r="Q19" s="520"/>
+      <c r="R19" s="520"/>
+      <c r="S19" s="520"/>
+      <c r="T19" s="520"/>
+      <c r="U19" s="520"/>
+      <c r="V19" s="520"/>
+      <c r="W19" s="520"/>
+      <c r="X19" s="520"/>
+      <c r="Y19" s="520"/>
+      <c r="Z19" s="520"/>
+      <c r="AA19" s="520"/>
+      <c r="AB19" s="520"/>
+      <c r="AC19" s="520"/>
+      <c r="AD19" s="520"/>
+      <c r="AE19" s="520"/>
+      <c r="AF19" s="520"/>
+      <c r="AG19" s="520"/>
+      <c r="AH19" s="520"/>
+      <c r="AI19" s="520"/>
+      <c r="AJ19" s="520"/>
+      <c r="AK19" s="520"/>
+      <c r="AL19" s="520"/>
+      <c r="AM19" s="521"/>
       <c r="AN19" s="473"/>
       <c r="AO19" s="321"/>
     </row>
     <row r="20" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="491"/>
+      <c r="A20" s="512"/>
       <c r="B20" s="326" t="s">
         <v>97</v>
       </c>
@@ -11638,46 +11583,46 @@
       <c r="D20" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="498"/>
-      <c r="F20" s="499"/>
-      <c r="G20" s="499"/>
-      <c r="H20" s="499"/>
-      <c r="I20" s="499"/>
-      <c r="J20" s="499"/>
-      <c r="K20" s="499"/>
-      <c r="L20" s="500"/>
-      <c r="M20" s="498"/>
-      <c r="N20" s="499"/>
-      <c r="O20" s="499"/>
-      <c r="P20" s="499"/>
-      <c r="Q20" s="499"/>
-      <c r="R20" s="499"/>
-      <c r="S20" s="499"/>
-      <c r="T20" s="499"/>
-      <c r="U20" s="499"/>
-      <c r="V20" s="499"/>
-      <c r="W20" s="499"/>
-      <c r="X20" s="499"/>
-      <c r="Y20" s="499"/>
-      <c r="Z20" s="499"/>
-      <c r="AA20" s="499"/>
-      <c r="AB20" s="499"/>
-      <c r="AC20" s="499"/>
-      <c r="AD20" s="499"/>
-      <c r="AE20" s="499"/>
-      <c r="AF20" s="499"/>
-      <c r="AG20" s="499"/>
-      <c r="AH20" s="499"/>
-      <c r="AI20" s="499"/>
-      <c r="AJ20" s="499"/>
-      <c r="AK20" s="499"/>
-      <c r="AL20" s="499"/>
-      <c r="AM20" s="500"/>
+      <c r="E20" s="519"/>
+      <c r="F20" s="520"/>
+      <c r="G20" s="520"/>
+      <c r="H20" s="520"/>
+      <c r="I20" s="520"/>
+      <c r="J20" s="520"/>
+      <c r="K20" s="520"/>
+      <c r="L20" s="521"/>
+      <c r="M20" s="519"/>
+      <c r="N20" s="520"/>
+      <c r="O20" s="520"/>
+      <c r="P20" s="520"/>
+      <c r="Q20" s="520"/>
+      <c r="R20" s="520"/>
+      <c r="S20" s="520"/>
+      <c r="T20" s="520"/>
+      <c r="U20" s="520"/>
+      <c r="V20" s="520"/>
+      <c r="W20" s="520"/>
+      <c r="X20" s="520"/>
+      <c r="Y20" s="520"/>
+      <c r="Z20" s="520"/>
+      <c r="AA20" s="520"/>
+      <c r="AB20" s="520"/>
+      <c r="AC20" s="520"/>
+      <c r="AD20" s="520"/>
+      <c r="AE20" s="520"/>
+      <c r="AF20" s="520"/>
+      <c r="AG20" s="520"/>
+      <c r="AH20" s="520"/>
+      <c r="AI20" s="520"/>
+      <c r="AJ20" s="520"/>
+      <c r="AK20" s="520"/>
+      <c r="AL20" s="520"/>
+      <c r="AM20" s="521"/>
       <c r="AN20" s="473"/>
       <c r="AO20" s="321"/>
     </row>
     <row r="21" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="491"/>
+      <c r="A21" s="512"/>
       <c r="B21" s="326" t="s">
         <v>45</v>
       </c>
@@ -11687,46 +11632,46 @@
       <c r="D21" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="498"/>
-      <c r="F21" s="499"/>
-      <c r="G21" s="499"/>
-      <c r="H21" s="499"/>
-      <c r="I21" s="499"/>
-      <c r="J21" s="499"/>
-      <c r="K21" s="499"/>
-      <c r="L21" s="500"/>
-      <c r="M21" s="498"/>
-      <c r="N21" s="499"/>
-      <c r="O21" s="499"/>
-      <c r="P21" s="499"/>
-      <c r="Q21" s="499"/>
-      <c r="R21" s="499"/>
-      <c r="S21" s="499"/>
-      <c r="T21" s="499"/>
-      <c r="U21" s="499"/>
-      <c r="V21" s="499"/>
-      <c r="W21" s="499"/>
-      <c r="X21" s="499"/>
-      <c r="Y21" s="499"/>
-      <c r="Z21" s="499"/>
-      <c r="AA21" s="499"/>
-      <c r="AB21" s="499"/>
-      <c r="AC21" s="499"/>
-      <c r="AD21" s="499"/>
-      <c r="AE21" s="499"/>
-      <c r="AF21" s="499"/>
-      <c r="AG21" s="499"/>
-      <c r="AH21" s="499"/>
-      <c r="AI21" s="499"/>
-      <c r="AJ21" s="499"/>
-      <c r="AK21" s="499"/>
-      <c r="AL21" s="499"/>
-      <c r="AM21" s="500"/>
+      <c r="E21" s="519"/>
+      <c r="F21" s="520"/>
+      <c r="G21" s="520"/>
+      <c r="H21" s="520"/>
+      <c r="I21" s="520"/>
+      <c r="J21" s="520"/>
+      <c r="K21" s="520"/>
+      <c r="L21" s="521"/>
+      <c r="M21" s="519"/>
+      <c r="N21" s="520"/>
+      <c r="O21" s="520"/>
+      <c r="P21" s="520"/>
+      <c r="Q21" s="520"/>
+      <c r="R21" s="520"/>
+      <c r="S21" s="520"/>
+      <c r="T21" s="520"/>
+      <c r="U21" s="520"/>
+      <c r="V21" s="520"/>
+      <c r="W21" s="520"/>
+      <c r="X21" s="520"/>
+      <c r="Y21" s="520"/>
+      <c r="Z21" s="520"/>
+      <c r="AA21" s="520"/>
+      <c r="AB21" s="520"/>
+      <c r="AC21" s="520"/>
+      <c r="AD21" s="520"/>
+      <c r="AE21" s="520"/>
+      <c r="AF21" s="520"/>
+      <c r="AG21" s="520"/>
+      <c r="AH21" s="520"/>
+      <c r="AI21" s="520"/>
+      <c r="AJ21" s="520"/>
+      <c r="AK21" s="520"/>
+      <c r="AL21" s="520"/>
+      <c r="AM21" s="521"/>
       <c r="AN21" s="473"/>
       <c r="AO21" s="322"/>
     </row>
     <row r="22" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="491"/>
+      <c r="A22" s="512"/>
       <c r="B22" s="326"/>
       <c r="C22" s="327" t="s">
         <v>318</v>
@@ -11734,46 +11679,46 @@
       <c r="D22" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="498"/>
-      <c r="F22" s="499"/>
-      <c r="G22" s="499"/>
-      <c r="H22" s="499"/>
-      <c r="I22" s="499"/>
-      <c r="J22" s="499"/>
-      <c r="K22" s="499"/>
-      <c r="L22" s="500"/>
-      <c r="M22" s="498"/>
-      <c r="N22" s="499"/>
-      <c r="O22" s="499"/>
-      <c r="P22" s="499"/>
-      <c r="Q22" s="499"/>
-      <c r="R22" s="499"/>
-      <c r="S22" s="499"/>
-      <c r="T22" s="499"/>
-      <c r="U22" s="499"/>
-      <c r="V22" s="499"/>
-      <c r="W22" s="499"/>
-      <c r="X22" s="499"/>
-      <c r="Y22" s="499"/>
-      <c r="Z22" s="499"/>
-      <c r="AA22" s="499"/>
-      <c r="AB22" s="499"/>
-      <c r="AC22" s="499"/>
-      <c r="AD22" s="499"/>
-      <c r="AE22" s="499"/>
-      <c r="AF22" s="499"/>
-      <c r="AG22" s="499"/>
-      <c r="AH22" s="499"/>
-      <c r="AI22" s="499"/>
-      <c r="AJ22" s="499"/>
-      <c r="AK22" s="499"/>
-      <c r="AL22" s="499"/>
-      <c r="AM22" s="500"/>
+      <c r="E22" s="519"/>
+      <c r="F22" s="520"/>
+      <c r="G22" s="520"/>
+      <c r="H22" s="520"/>
+      <c r="I22" s="520"/>
+      <c r="J22" s="520"/>
+      <c r="K22" s="520"/>
+      <c r="L22" s="521"/>
+      <c r="M22" s="519"/>
+      <c r="N22" s="520"/>
+      <c r="O22" s="520"/>
+      <c r="P22" s="520"/>
+      <c r="Q22" s="520"/>
+      <c r="R22" s="520"/>
+      <c r="S22" s="520"/>
+      <c r="T22" s="520"/>
+      <c r="U22" s="520"/>
+      <c r="V22" s="520"/>
+      <c r="W22" s="520"/>
+      <c r="X22" s="520"/>
+      <c r="Y22" s="520"/>
+      <c r="Z22" s="520"/>
+      <c r="AA22" s="520"/>
+      <c r="AB22" s="520"/>
+      <c r="AC22" s="520"/>
+      <c r="AD22" s="520"/>
+      <c r="AE22" s="520"/>
+      <c r="AF22" s="520"/>
+      <c r="AG22" s="520"/>
+      <c r="AH22" s="520"/>
+      <c r="AI22" s="520"/>
+      <c r="AJ22" s="520"/>
+      <c r="AK22" s="520"/>
+      <c r="AL22" s="520"/>
+      <c r="AM22" s="521"/>
       <c r="AN22" s="473"/>
       <c r="AO22" s="322"/>
     </row>
     <row r="23" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="491"/>
+      <c r="A23" s="512"/>
       <c r="B23" s="326"/>
       <c r="C23" s="327" t="s">
         <v>290</v>
@@ -11781,46 +11726,46 @@
       <c r="D23" s="328" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="498"/>
-      <c r="F23" s="499"/>
-      <c r="G23" s="499"/>
-      <c r="H23" s="499"/>
-      <c r="I23" s="499"/>
-      <c r="J23" s="499"/>
-      <c r="K23" s="499"/>
-      <c r="L23" s="500"/>
-      <c r="M23" s="498"/>
-      <c r="N23" s="499"/>
-      <c r="O23" s="499"/>
-      <c r="P23" s="499"/>
-      <c r="Q23" s="499"/>
-      <c r="R23" s="499"/>
-      <c r="S23" s="499"/>
-      <c r="T23" s="499"/>
-      <c r="U23" s="499"/>
-      <c r="V23" s="499"/>
-      <c r="W23" s="499"/>
-      <c r="X23" s="499"/>
-      <c r="Y23" s="499"/>
-      <c r="Z23" s="499"/>
-      <c r="AA23" s="499"/>
-      <c r="AB23" s="499"/>
-      <c r="AC23" s="499"/>
-      <c r="AD23" s="499"/>
-      <c r="AE23" s="499"/>
-      <c r="AF23" s="499"/>
-      <c r="AG23" s="499"/>
-      <c r="AH23" s="499"/>
-      <c r="AI23" s="499"/>
-      <c r="AJ23" s="499"/>
-      <c r="AK23" s="499"/>
-      <c r="AL23" s="499"/>
-      <c r="AM23" s="500"/>
+      <c r="E23" s="519"/>
+      <c r="F23" s="520"/>
+      <c r="G23" s="520"/>
+      <c r="H23" s="520"/>
+      <c r="I23" s="520"/>
+      <c r="J23" s="520"/>
+      <c r="K23" s="520"/>
+      <c r="L23" s="521"/>
+      <c r="M23" s="519"/>
+      <c r="N23" s="520"/>
+      <c r="O23" s="520"/>
+      <c r="P23" s="520"/>
+      <c r="Q23" s="520"/>
+      <c r="R23" s="520"/>
+      <c r="S23" s="520"/>
+      <c r="T23" s="520"/>
+      <c r="U23" s="520"/>
+      <c r="V23" s="520"/>
+      <c r="W23" s="520"/>
+      <c r="X23" s="520"/>
+      <c r="Y23" s="520"/>
+      <c r="Z23" s="520"/>
+      <c r="AA23" s="520"/>
+      <c r="AB23" s="520"/>
+      <c r="AC23" s="520"/>
+      <c r="AD23" s="520"/>
+      <c r="AE23" s="520"/>
+      <c r="AF23" s="520"/>
+      <c r="AG23" s="520"/>
+      <c r="AH23" s="520"/>
+      <c r="AI23" s="520"/>
+      <c r="AJ23" s="520"/>
+      <c r="AK23" s="520"/>
+      <c r="AL23" s="520"/>
+      <c r="AM23" s="521"/>
       <c r="AN23" s="473"/>
       <c r="AO23" s="322"/>
     </row>
     <row r="24" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="491"/>
+      <c r="A24" s="512"/>
       <c r="B24" s="326"/>
       <c r="C24" s="327" t="s">
         <v>184</v>
@@ -11828,46 +11773,46 @@
       <c r="D24" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="498"/>
-      <c r="F24" s="499"/>
-      <c r="G24" s="499"/>
-      <c r="H24" s="499"/>
-      <c r="I24" s="499"/>
-      <c r="J24" s="499"/>
-      <c r="K24" s="499"/>
-      <c r="L24" s="500"/>
-      <c r="M24" s="498"/>
-      <c r="N24" s="499"/>
-      <c r="O24" s="499"/>
-      <c r="P24" s="499"/>
-      <c r="Q24" s="499"/>
-      <c r="R24" s="499"/>
-      <c r="S24" s="499"/>
-      <c r="T24" s="499"/>
-      <c r="U24" s="499"/>
-      <c r="V24" s="499"/>
-      <c r="W24" s="499"/>
-      <c r="X24" s="499"/>
-      <c r="Y24" s="499"/>
-      <c r="Z24" s="499"/>
-      <c r="AA24" s="499"/>
-      <c r="AB24" s="499"/>
-      <c r="AC24" s="499"/>
-      <c r="AD24" s="499"/>
-      <c r="AE24" s="499"/>
-      <c r="AF24" s="499"/>
-      <c r="AG24" s="499"/>
-      <c r="AH24" s="499"/>
-      <c r="AI24" s="499"/>
-      <c r="AJ24" s="499"/>
-      <c r="AK24" s="499"/>
-      <c r="AL24" s="499"/>
-      <c r="AM24" s="500"/>
+      <c r="E24" s="519"/>
+      <c r="F24" s="520"/>
+      <c r="G24" s="520"/>
+      <c r="H24" s="520"/>
+      <c r="I24" s="520"/>
+      <c r="J24" s="520"/>
+      <c r="K24" s="520"/>
+      <c r="L24" s="521"/>
+      <c r="M24" s="519"/>
+      <c r="N24" s="520"/>
+      <c r="O24" s="520"/>
+      <c r="P24" s="520"/>
+      <c r="Q24" s="520"/>
+      <c r="R24" s="520"/>
+      <c r="S24" s="520"/>
+      <c r="T24" s="520"/>
+      <c r="U24" s="520"/>
+      <c r="V24" s="520"/>
+      <c r="W24" s="520"/>
+      <c r="X24" s="520"/>
+      <c r="Y24" s="520"/>
+      <c r="Z24" s="520"/>
+      <c r="AA24" s="520"/>
+      <c r="AB24" s="520"/>
+      <c r="AC24" s="520"/>
+      <c r="AD24" s="520"/>
+      <c r="AE24" s="520"/>
+      <c r="AF24" s="520"/>
+      <c r="AG24" s="520"/>
+      <c r="AH24" s="520"/>
+      <c r="AI24" s="520"/>
+      <c r="AJ24" s="520"/>
+      <c r="AK24" s="520"/>
+      <c r="AL24" s="520"/>
+      <c r="AM24" s="521"/>
       <c r="AN24" s="473"/>
       <c r="AO24" s="322"/>
     </row>
     <row r="25" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="491"/>
+      <c r="A25" s="512"/>
       <c r="B25" s="326"/>
       <c r="C25" s="327" t="s">
         <v>72</v>
@@ -11875,46 +11820,46 @@
       <c r="D25" s="328" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="498"/>
-      <c r="F25" s="499"/>
-      <c r="G25" s="499"/>
-      <c r="H25" s="499"/>
-      <c r="I25" s="499"/>
-      <c r="J25" s="499"/>
-      <c r="K25" s="499"/>
-      <c r="L25" s="500"/>
-      <c r="M25" s="498"/>
-      <c r="N25" s="499"/>
-      <c r="O25" s="499"/>
-      <c r="P25" s="499"/>
-      <c r="Q25" s="499"/>
-      <c r="R25" s="499"/>
-      <c r="S25" s="499"/>
-      <c r="T25" s="499"/>
-      <c r="U25" s="499"/>
-      <c r="V25" s="499"/>
-      <c r="W25" s="499"/>
-      <c r="X25" s="499"/>
-      <c r="Y25" s="499"/>
-      <c r="Z25" s="499"/>
-      <c r="AA25" s="499"/>
-      <c r="AB25" s="499"/>
-      <c r="AC25" s="499"/>
-      <c r="AD25" s="499"/>
-      <c r="AE25" s="499"/>
-      <c r="AF25" s="499"/>
-      <c r="AG25" s="499"/>
-      <c r="AH25" s="499"/>
-      <c r="AI25" s="499"/>
-      <c r="AJ25" s="499"/>
-      <c r="AK25" s="499"/>
-      <c r="AL25" s="499"/>
-      <c r="AM25" s="500"/>
+      <c r="E25" s="519"/>
+      <c r="F25" s="520"/>
+      <c r="G25" s="520"/>
+      <c r="H25" s="520"/>
+      <c r="I25" s="520"/>
+      <c r="J25" s="520"/>
+      <c r="K25" s="520"/>
+      <c r="L25" s="521"/>
+      <c r="M25" s="519"/>
+      <c r="N25" s="520"/>
+      <c r="O25" s="520"/>
+      <c r="P25" s="520"/>
+      <c r="Q25" s="520"/>
+      <c r="R25" s="520"/>
+      <c r="S25" s="520"/>
+      <c r="T25" s="520"/>
+      <c r="U25" s="520"/>
+      <c r="V25" s="520"/>
+      <c r="W25" s="520"/>
+      <c r="X25" s="520"/>
+      <c r="Y25" s="520"/>
+      <c r="Z25" s="520"/>
+      <c r="AA25" s="520"/>
+      <c r="AB25" s="520"/>
+      <c r="AC25" s="520"/>
+      <c r="AD25" s="520"/>
+      <c r="AE25" s="520"/>
+      <c r="AF25" s="520"/>
+      <c r="AG25" s="520"/>
+      <c r="AH25" s="520"/>
+      <c r="AI25" s="520"/>
+      <c r="AJ25" s="520"/>
+      <c r="AK25" s="520"/>
+      <c r="AL25" s="520"/>
+      <c r="AM25" s="521"/>
       <c r="AN25" s="473"/>
       <c r="AO25" s="322"/>
     </row>
     <row r="26" spans="1:41" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="491"/>
+      <c r="A26" s="512"/>
       <c r="B26" s="330"/>
       <c r="C26" s="331" t="s">
         <v>74</v>
@@ -11922,53 +11867,53 @@
       <c r="D26" s="332" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="501"/>
-      <c r="F26" s="502"/>
-      <c r="G26" s="502"/>
-      <c r="H26" s="502"/>
-      <c r="I26" s="502"/>
-      <c r="J26" s="502"/>
-      <c r="K26" s="502"/>
-      <c r="L26" s="503"/>
-      <c r="M26" s="501"/>
-      <c r="N26" s="502"/>
-      <c r="O26" s="502"/>
-      <c r="P26" s="502"/>
-      <c r="Q26" s="502"/>
-      <c r="R26" s="502"/>
-      <c r="S26" s="502"/>
-      <c r="T26" s="502"/>
-      <c r="U26" s="502"/>
-      <c r="V26" s="502"/>
-      <c r="W26" s="502"/>
-      <c r="X26" s="502"/>
-      <c r="Y26" s="502"/>
-      <c r="Z26" s="502"/>
-      <c r="AA26" s="502"/>
-      <c r="AB26" s="502"/>
-      <c r="AC26" s="502"/>
-      <c r="AD26" s="502"/>
-      <c r="AE26" s="502"/>
-      <c r="AF26" s="502"/>
-      <c r="AG26" s="502"/>
-      <c r="AH26" s="502"/>
-      <c r="AI26" s="502"/>
-      <c r="AJ26" s="502"/>
-      <c r="AK26" s="502"/>
-      <c r="AL26" s="499"/>
-      <c r="AM26" s="500"/>
+      <c r="E26" s="522"/>
+      <c r="F26" s="523"/>
+      <c r="G26" s="523"/>
+      <c r="H26" s="523"/>
+      <c r="I26" s="523"/>
+      <c r="J26" s="523"/>
+      <c r="K26" s="523"/>
+      <c r="L26" s="524"/>
+      <c r="M26" s="522"/>
+      <c r="N26" s="523"/>
+      <c r="O26" s="523"/>
+      <c r="P26" s="523"/>
+      <c r="Q26" s="523"/>
+      <c r="R26" s="523"/>
+      <c r="S26" s="523"/>
+      <c r="T26" s="523"/>
+      <c r="U26" s="523"/>
+      <c r="V26" s="523"/>
+      <c r="W26" s="523"/>
+      <c r="X26" s="523"/>
+      <c r="Y26" s="523"/>
+      <c r="Z26" s="523"/>
+      <c r="AA26" s="523"/>
+      <c r="AB26" s="523"/>
+      <c r="AC26" s="523"/>
+      <c r="AD26" s="523"/>
+      <c r="AE26" s="523"/>
+      <c r="AF26" s="523"/>
+      <c r="AG26" s="523"/>
+      <c r="AH26" s="523"/>
+      <c r="AI26" s="523"/>
+      <c r="AJ26" s="523"/>
+      <c r="AK26" s="523"/>
+      <c r="AL26" s="520"/>
+      <c r="AM26" s="521"/>
       <c r="AN26" s="473"/>
       <c r="AO26" s="322"/>
     </row>
     <row r="27" spans="1:41" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="491"/>
+      <c r="A27" s="512"/>
       <c r="B27" s="41" t="s">
         <v>293</v>
       </c>
       <c r="C27" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="492" t="s">
+      <c r="D27" s="513" t="s">
         <v>363</v>
       </c>
       <c r="E27" s="102"/>
@@ -12066,12 +12011,12 @@
       <c r="AO27" s="66"/>
     </row>
     <row r="28" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="491"/>
+      <c r="A28" s="512"/>
       <c r="B28" s="47"/>
       <c r="C28" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="493"/>
+      <c r="D28" s="514"/>
       <c r="E28" s="103"/>
       <c r="F28" s="31"/>
       <c r="G28" s="31"/>
@@ -12167,12 +12112,12 @@
       <c r="AO28" s="179"/>
     </row>
     <row r="29" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="491"/>
+      <c r="A29" s="512"/>
       <c r="B29" s="47"/>
       <c r="C29" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D29" s="493"/>
+      <c r="D29" s="514"/>
       <c r="E29" s="103"/>
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
@@ -12268,12 +12213,12 @@
       <c r="AO29" s="179"/>
     </row>
     <row r="30" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="491"/>
+      <c r="A30" s="512"/>
       <c r="B30" s="47"/>
       <c r="C30" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D30" s="493"/>
+      <c r="D30" s="514"/>
       <c r="E30" s="103"/>
       <c r="F30" s="31"/>
       <c r="G30" s="31"/>
@@ -12371,12 +12316,12 @@
       </c>
     </row>
     <row r="31" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="491"/>
+      <c r="A31" s="512"/>
       <c r="B31" s="47"/>
       <c r="C31" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D31" s="493"/>
+      <c r="D31" s="514"/>
       <c r="E31" s="103"/>
       <c r="F31" s="31"/>
       <c r="G31" s="31"/>
@@ -12472,12 +12417,12 @@
       <c r="AO31" s="179"/>
     </row>
     <row r="32" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="491"/>
+      <c r="A32" s="512"/>
       <c r="B32" s="47"/>
       <c r="C32" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="D32" s="493"/>
+      <c r="D32" s="514"/>
       <c r="E32" s="103"/>
       <c r="F32" s="31"/>
       <c r="G32" s="31"/>
@@ -12573,12 +12518,12 @@
       <c r="AO32" s="179"/>
     </row>
     <row r="33" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="491"/>
+      <c r="A33" s="512"/>
       <c r="B33" s="47"/>
       <c r="C33" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="493"/>
+      <c r="D33" s="514"/>
       <c r="E33" s="103"/>
       <c r="F33" s="31"/>
       <c r="G33" s="31"/>
@@ -12674,12 +12619,12 @@
       <c r="AO33" s="179"/>
     </row>
     <row r="34" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="491"/>
+      <c r="A34" s="512"/>
       <c r="B34" s="47"/>
       <c r="C34" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D34" s="493"/>
+      <c r="D34" s="514"/>
       <c r="E34" s="103"/>
       <c r="F34" s="31"/>
       <c r="G34" s="31"/>
@@ -12745,12 +12690,12 @@
       <c r="AO34" s="180"/>
     </row>
     <row r="35" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="491"/>
+      <c r="A35" s="512"/>
       <c r="B35" s="47"/>
       <c r="C35" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="493"/>
+      <c r="D35" s="514"/>
       <c r="E35" s="103"/>
       <c r="F35" s="31"/>
       <c r="G35" s="31"/>
@@ -12846,12 +12791,12 @@
       <c r="AO35" s="179"/>
     </row>
     <row r="36" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="491"/>
+      <c r="A36" s="512"/>
       <c r="B36" s="47"/>
       <c r="C36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="493"/>
+      <c r="D36" s="514"/>
       <c r="E36" s="103"/>
       <c r="F36" s="31"/>
       <c r="G36" s="31"/>
@@ -12933,12 +12878,12 @@
       <c r="AO36" s="179"/>
     </row>
     <row r="37" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="491"/>
+      <c r="A37" s="512"/>
       <c r="B37" s="47"/>
       <c r="C37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="493"/>
+      <c r="D37" s="514"/>
       <c r="E37" s="103"/>
       <c r="F37" s="31"/>
       <c r="G37" s="31"/>
@@ -13022,12 +12967,12 @@
       </c>
     </row>
     <row r="38" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="491"/>
+      <c r="A38" s="512"/>
       <c r="B38" s="47"/>
       <c r="C38" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="D38" s="493"/>
+      <c r="D38" s="514"/>
       <c r="E38" s="103"/>
       <c r="F38" s="31"/>
       <c r="G38" s="31"/>
@@ -13101,12 +13046,12 @@
       <c r="AO38" s="179"/>
     </row>
     <row r="39" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="491"/>
+      <c r="A39" s="512"/>
       <c r="B39" s="49"/>
       <c r="C39" s="305" t="s">
         <v>272</v>
       </c>
-      <c r="D39" s="493"/>
+      <c r="D39" s="514"/>
       <c r="E39" s="306"/>
       <c r="F39" s="307"/>
       <c r="G39" s="307"/>
@@ -13146,12 +13091,12 @@
       <c r="AO39" s="183"/>
     </row>
     <row r="40" spans="1:42" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="491"/>
+      <c r="A40" s="512"/>
       <c r="B40" s="67"/>
       <c r="C40" s="421" t="s">
         <v>436</v>
       </c>
-      <c r="D40" s="493"/>
+      <c r="D40" s="514"/>
       <c r="E40" s="105"/>
       <c r="F40" s="69"/>
       <c r="G40" s="69"/>
@@ -13217,14 +13162,14 @@
       <c r="AO40" s="181"/>
     </row>
     <row r="41" spans="1:42" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="491"/>
+      <c r="A41" s="512"/>
       <c r="B41" s="48" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="D41" s="493"/>
+      <c r="D41" s="514"/>
       <c r="E41" s="109"/>
       <c r="F41" s="40"/>
       <c r="G41" s="40"/>
@@ -13320,12 +13265,12 @@
       <c r="AO41" s="182"/>
     </row>
     <row r="42" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="491"/>
+      <c r="A42" s="512"/>
       <c r="B42" s="47"/>
       <c r="C42" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="493"/>
+      <c r="D42" s="514"/>
       <c r="E42" s="103"/>
       <c r="F42" s="31"/>
       <c r="G42" s="31"/>
@@ -13381,12 +13326,12 @@
       <c r="AO42" s="179"/>
     </row>
     <row r="43" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="491"/>
+      <c r="A43" s="512"/>
       <c r="B43" s="47"/>
       <c r="C43" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="D43" s="493"/>
+      <c r="D43" s="514"/>
       <c r="E43" s="103"/>
       <c r="F43" s="31"/>
       <c r="G43" s="31"/>
@@ -13442,12 +13387,12 @@
       <c r="AO43" s="179"/>
     </row>
     <row r="44" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="491"/>
+      <c r="A44" s="512"/>
       <c r="B44" s="49"/>
       <c r="C44" s="420" t="s">
         <v>495</v>
       </c>
-      <c r="D44" s="493"/>
+      <c r="D44" s="514"/>
       <c r="E44" s="306"/>
       <c r="F44" s="307"/>
       <c r="G44" s="307"/>
@@ -13543,12 +13488,12 @@
       <c r="AO44" s="183"/>
     </row>
     <row r="45" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="491"/>
+      <c r="A45" s="512"/>
       <c r="B45" s="49"/>
       <c r="C45" s="420" t="s">
         <v>496</v>
       </c>
-      <c r="D45" s="493"/>
+      <c r="D45" s="514"/>
       <c r="E45" s="306"/>
       <c r="F45" s="307"/>
       <c r="G45" s="307"/>
@@ -13588,12 +13533,12 @@
       <c r="AO45" s="183"/>
     </row>
     <row r="46" spans="1:42" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="491"/>
+      <c r="A46" s="512"/>
       <c r="B46" s="67"/>
       <c r="C46" s="68" t="s">
         <v>275</v>
       </c>
-      <c r="D46" s="493"/>
+      <c r="D46" s="514"/>
       <c r="E46" s="105"/>
       <c r="F46" s="69"/>
       <c r="G46" s="69"/>
@@ -13659,14 +13604,14 @@
       <c r="AO46" s="181"/>
     </row>
     <row r="47" spans="1:42" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="491"/>
+      <c r="A47" s="512"/>
       <c r="B47" s="41" t="s">
         <v>97</v>
       </c>
       <c r="C47" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="D47" s="493"/>
+      <c r="D47" s="514"/>
       <c r="E47" s="102"/>
       <c r="F47" s="43"/>
       <c r="G47" s="43"/>
@@ -13764,12 +13709,12 @@
       </c>
     </row>
     <row r="48" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="491"/>
+      <c r="A48" s="512"/>
       <c r="B48" s="47"/>
       <c r="C48" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="493"/>
+      <c r="D48" s="514"/>
       <c r="E48" s="103"/>
       <c r="F48" s="31"/>
       <c r="G48" s="31"/>
@@ -13870,12 +13815,12 @@
       </c>
     </row>
     <row r="49" spans="1:41" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="491"/>
+      <c r="A49" s="512"/>
       <c r="B49" s="381"/>
       <c r="C49" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D49" s="493"/>
+      <c r="D49" s="514"/>
       <c r="E49" s="116"/>
       <c r="F49" s="32"/>
       <c r="G49" s="32"/>
@@ -13941,12 +13886,12 @@
       <c r="AO49" s="180"/>
     </row>
     <row r="50" spans="1:41" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="491"/>
+      <c r="A50" s="512"/>
       <c r="B50" s="368"/>
       <c r="C50" s="369" t="s">
         <v>458</v>
       </c>
-      <c r="D50" s="493"/>
+      <c r="D50" s="514"/>
       <c r="E50" s="370"/>
       <c r="F50" s="371"/>
       <c r="G50" s="371"/>
@@ -14042,14 +13987,14 @@
       <c r="AO50" s="374"/>
     </row>
     <row r="51" spans="1:41" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="491"/>
+      <c r="A51" s="512"/>
       <c r="B51" s="41" t="s">
         <v>35</v>
       </c>
       <c r="C51" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="493"/>
+      <c r="D51" s="514"/>
       <c r="E51" s="102" t="s">
         <v>18</v>
       </c>
@@ -14161,12 +14106,12 @@
       <c r="AO51" s="66"/>
     </row>
     <row r="52" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="491"/>
+      <c r="A52" s="512"/>
       <c r="B52" s="48"/>
       <c r="C52" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="D52" s="493"/>
+      <c r="D52" s="514"/>
       <c r="E52" s="107"/>
       <c r="F52" s="40" t="s">
         <v>9</v>
@@ -14276,12 +14221,12 @@
       <c r="AO52" s="182"/>
     </row>
     <row r="53" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="491"/>
+      <c r="A53" s="512"/>
       <c r="B53" s="48"/>
       <c r="C53" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="D53" s="493"/>
+      <c r="D53" s="514"/>
       <c r="E53" s="109" t="s">
         <v>9</v>
       </c>
@@ -14393,12 +14338,12 @@
       <c r="AO53" s="182"/>
     </row>
     <row r="54" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="491"/>
+      <c r="A54" s="512"/>
       <c r="B54" s="47"/>
       <c r="C54" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="D54" s="493"/>
+      <c r="D54" s="514"/>
       <c r="E54" s="103" t="s">
         <v>9</v>
       </c>
@@ -14510,12 +14455,12 @@
       <c r="AO54" s="179"/>
     </row>
     <row r="55" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="491"/>
+      <c r="A55" s="512"/>
       <c r="B55" s="47"/>
       <c r="C55" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="D55" s="493"/>
+      <c r="D55" s="514"/>
       <c r="E55" s="110"/>
       <c r="F55" s="35"/>
       <c r="G55" s="35"/>
@@ -14597,12 +14542,12 @@
       </c>
     </row>
     <row r="56" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="491"/>
+      <c r="A56" s="512"/>
       <c r="B56" s="47"/>
       <c r="C56" s="198" t="s">
         <v>271</v>
       </c>
-      <c r="D56" s="493"/>
+      <c r="D56" s="514"/>
       <c r="E56" s="103" t="s">
         <v>18</v>
       </c>
@@ -14714,12 +14659,12 @@
       <c r="AO56" s="179"/>
     </row>
     <row r="57" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="491"/>
+      <c r="A57" s="512"/>
       <c r="B57" s="47"/>
       <c r="C57" s="198" t="s">
         <v>454</v>
       </c>
-      <c r="D57" s="493"/>
+      <c r="D57" s="514"/>
       <c r="E57" s="103" t="s">
         <v>48</v>
       </c>
@@ -14831,12 +14776,12 @@
       <c r="AO57" s="179"/>
     </row>
     <row r="58" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="491"/>
+      <c r="A58" s="512"/>
       <c r="B58" s="47"/>
       <c r="C58" s="199" t="s">
         <v>474</v>
       </c>
-      <c r="D58" s="493"/>
+      <c r="D58" s="514"/>
       <c r="E58" s="110"/>
       <c r="F58" s="35"/>
       <c r="G58" s="35"/>
@@ -14918,12 +14863,12 @@
       </c>
     </row>
     <row r="59" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="491"/>
+      <c r="A59" s="512"/>
       <c r="B59" s="47"/>
       <c r="C59" s="198" t="s">
         <v>37</v>
       </c>
-      <c r="D59" s="493"/>
+      <c r="D59" s="514"/>
       <c r="E59" s="103" t="s">
         <v>9</v>
       </c>
@@ -15035,12 +14980,12 @@
       <c r="AO59" s="179"/>
     </row>
     <row r="60" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="491"/>
+      <c r="A60" s="512"/>
       <c r="B60" s="47"/>
       <c r="C60" s="198" t="s">
         <v>234</v>
       </c>
-      <c r="D60" s="493"/>
+      <c r="D60" s="514"/>
       <c r="E60" s="103" t="s">
         <v>9</v>
       </c>
@@ -15154,12 +15099,12 @@
       </c>
     </row>
     <row r="61" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="491"/>
+      <c r="A61" s="512"/>
       <c r="B61" s="47"/>
       <c r="C61" s="198" t="s">
         <v>235</v>
       </c>
-      <c r="D61" s="493"/>
+      <c r="D61" s="514"/>
       <c r="E61" s="103" t="s">
         <v>9</v>
       </c>
@@ -15273,12 +15218,12 @@
       </c>
     </row>
     <row r="62" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="491"/>
+      <c r="A62" s="512"/>
       <c r="B62" s="47"/>
       <c r="C62" s="198" t="s">
         <v>236</v>
       </c>
-      <c r="D62" s="493"/>
+      <c r="D62" s="514"/>
       <c r="E62" s="103" t="s">
         <v>9</v>
       </c>
@@ -15390,12 +15335,12 @@
       <c r="AO62" s="179"/>
     </row>
     <row r="63" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="491"/>
+      <c r="A63" s="512"/>
       <c r="B63" s="47"/>
       <c r="C63" s="424" t="s">
         <v>498</v>
       </c>
-      <c r="D63" s="493"/>
+      <c r="D63" s="514"/>
       <c r="E63" s="111"/>
       <c r="F63" s="34"/>
       <c r="G63" s="34"/>
@@ -15439,12 +15384,12 @@
       <c r="AO63" s="179"/>
     </row>
     <row r="64" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="491"/>
+      <c r="A64" s="512"/>
       <c r="B64" s="47"/>
       <c r="C64" s="198" t="s">
         <v>480</v>
       </c>
-      <c r="D64" s="493"/>
+      <c r="D64" s="514"/>
       <c r="E64" s="111"/>
       <c r="F64" s="34"/>
       <c r="G64" s="34"/>
@@ -15490,12 +15435,12 @@
       <c r="AO64" s="179"/>
     </row>
     <row r="65" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="491"/>
+      <c r="A65" s="512"/>
       <c r="B65" s="47"/>
       <c r="C65" s="198" t="s">
         <v>228</v>
       </c>
-      <c r="D65" s="493"/>
+      <c r="D65" s="514"/>
       <c r="E65" s="111"/>
       <c r="F65" s="34"/>
       <c r="G65" s="34"/>
@@ -15571,12 +15516,12 @@
       <c r="AO65" s="179"/>
     </row>
     <row r="66" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="491"/>
+      <c r="A66" s="512"/>
       <c r="B66" s="47"/>
       <c r="C66" s="199" t="s">
         <v>38</v>
       </c>
-      <c r="D66" s="493"/>
+      <c r="D66" s="514"/>
       <c r="E66" s="110"/>
       <c r="F66" s="35"/>
       <c r="G66" s="35"/>
@@ -15658,12 +15603,12 @@
       </c>
     </row>
     <row r="67" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="491"/>
+      <c r="A67" s="512"/>
       <c r="B67" s="47"/>
       <c r="C67" s="199" t="s">
         <v>39</v>
       </c>
-      <c r="D67" s="493"/>
+      <c r="D67" s="514"/>
       <c r="E67" s="110"/>
       <c r="F67" s="35"/>
       <c r="G67" s="35"/>
@@ -15745,12 +15690,12 @@
       </c>
     </row>
     <row r="68" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="491"/>
+      <c r="A68" s="512"/>
       <c r="B68" s="47"/>
       <c r="C68" s="198" t="s">
         <v>499</v>
       </c>
-      <c r="D68" s="493"/>
+      <c r="D68" s="514"/>
       <c r="E68" s="103" t="s">
         <v>9</v>
       </c>
@@ -15862,12 +15807,12 @@
       <c r="AO68" s="179"/>
     </row>
     <row r="69" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="491"/>
+      <c r="A69" s="512"/>
       <c r="B69" s="47"/>
       <c r="C69" s="198" t="s">
         <v>500</v>
       </c>
-      <c r="D69" s="493"/>
+      <c r="D69" s="514"/>
       <c r="E69" s="103" t="s">
         <v>9</v>
       </c>
@@ -15979,12 +15924,12 @@
       <c r="AO69" s="179"/>
     </row>
     <row r="70" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="491"/>
+      <c r="A70" s="512"/>
       <c r="B70" s="47"/>
       <c r="C70" s="198" t="s">
         <v>237</v>
       </c>
-      <c r="D70" s="493"/>
+      <c r="D70" s="514"/>
       <c r="E70" s="103" t="s">
         <v>9</v>
       </c>
@@ -16096,12 +16041,12 @@
       <c r="AO70" s="179"/>
     </row>
     <row r="71" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="491"/>
+      <c r="A71" s="512"/>
       <c r="B71" s="47"/>
       <c r="C71" s="424" t="s">
         <v>501</v>
       </c>
-      <c r="D71" s="493"/>
+      <c r="D71" s="514"/>
       <c r="E71" s="111"/>
       <c r="F71" s="34"/>
       <c r="G71" s="34"/>
@@ -16145,12 +16090,12 @@
       <c r="AO71" s="179"/>
     </row>
     <row r="72" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="491"/>
+      <c r="A72" s="512"/>
       <c r="B72" s="47"/>
       <c r="C72" s="198" t="s">
         <v>40</v>
       </c>
-      <c r="D72" s="493"/>
+      <c r="D72" s="514"/>
       <c r="E72" s="111"/>
       <c r="F72" s="34"/>
       <c r="G72" s="34"/>
@@ -16230,12 +16175,12 @@
       <c r="AO72" s="179"/>
     </row>
     <row r="73" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="491"/>
+      <c r="A73" s="512"/>
       <c r="B73" s="47"/>
       <c r="C73" s="198" t="s">
         <v>260</v>
       </c>
-      <c r="D73" s="493"/>
+      <c r="D73" s="514"/>
       <c r="E73" s="111"/>
       <c r="F73" s="34"/>
       <c r="G73" s="34"/>
@@ -16307,12 +16252,12 @@
       <c r="AO73" s="179"/>
     </row>
     <row r="74" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="491"/>
+      <c r="A74" s="512"/>
       <c r="B74" s="47"/>
       <c r="C74" s="424" t="s">
         <v>502</v>
       </c>
-      <c r="D74" s="493"/>
+      <c r="D74" s="514"/>
       <c r="E74" s="111"/>
       <c r="F74" s="34"/>
       <c r="G74" s="34"/>
@@ -16356,12 +16301,12 @@
       <c r="AO74" s="179"/>
     </row>
     <row r="75" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="491"/>
+      <c r="A75" s="512"/>
       <c r="B75" s="47"/>
       <c r="C75" s="198" t="s">
         <v>452</v>
       </c>
-      <c r="D75" s="493"/>
+      <c r="D75" s="514"/>
       <c r="E75" s="111"/>
       <c r="F75" s="34"/>
       <c r="G75" s="34"/>
@@ -16437,12 +16382,12 @@
       <c r="AO75" s="179"/>
     </row>
     <row r="76" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="491"/>
+      <c r="A76" s="512"/>
       <c r="B76" s="47"/>
       <c r="C76" s="198" t="s">
         <v>453</v>
       </c>
-      <c r="D76" s="493"/>
+      <c r="D76" s="514"/>
       <c r="E76" s="111"/>
       <c r="F76" s="34"/>
       <c r="G76" s="34"/>
@@ -16508,12 +16453,12 @@
       <c r="AO76" s="179"/>
     </row>
     <row r="77" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="491"/>
+      <c r="A77" s="512"/>
       <c r="B77" s="47"/>
       <c r="C77" s="198" t="s">
         <v>41</v>
       </c>
-      <c r="D77" s="493"/>
+      <c r="D77" s="514"/>
       <c r="E77" s="103" t="s">
         <v>18</v>
       </c>
@@ -16625,12 +16570,12 @@
       <c r="AO77" s="179"/>
     </row>
     <row r="78" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="491"/>
+      <c r="A78" s="512"/>
       <c r="B78" s="47"/>
       <c r="C78" s="198" t="s">
         <v>222</v>
       </c>
-      <c r="D78" s="493"/>
+      <c r="D78" s="514"/>
       <c r="E78" s="103" t="s">
         <v>9</v>
       </c>
@@ -16742,12 +16687,12 @@
       <c r="AO78" s="179"/>
     </row>
     <row r="79" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="491"/>
+      <c r="A79" s="512"/>
       <c r="B79" s="47"/>
       <c r="C79" s="198" t="s">
         <v>223</v>
       </c>
-      <c r="D79" s="493"/>
+      <c r="D79" s="514"/>
       <c r="E79" s="111"/>
       <c r="F79" s="34"/>
       <c r="G79" s="34"/>
@@ -16819,12 +16764,12 @@
       <c r="AO79" s="179"/>
     </row>
     <row r="80" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="491"/>
+      <c r="A80" s="512"/>
       <c r="B80" s="47"/>
       <c r="C80" s="424" t="s">
         <v>503</v>
       </c>
-      <c r="D80" s="493"/>
+      <c r="D80" s="514"/>
       <c r="E80" s="111"/>
       <c r="F80" s="34"/>
       <c r="G80" s="34"/>
@@ -16868,12 +16813,12 @@
       <c r="AO80" s="179"/>
     </row>
     <row r="81" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="491"/>
+      <c r="A81" s="512"/>
       <c r="B81" s="47"/>
       <c r="C81" s="198" t="s">
         <v>481</v>
       </c>
-      <c r="D81" s="493"/>
+      <c r="D81" s="514"/>
       <c r="E81" s="111"/>
       <c r="F81" s="34"/>
       <c r="G81" s="34"/>
@@ -16921,12 +16866,12 @@
       <c r="AO81" s="179"/>
     </row>
     <row r="82" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="491"/>
+      <c r="A82" s="512"/>
       <c r="B82" s="47"/>
       <c r="C82" s="198" t="s">
         <v>42</v>
       </c>
-      <c r="D82" s="493"/>
+      <c r="D82" s="514"/>
       <c r="E82" s="103" t="s">
         <v>18</v>
       </c>
@@ -17040,12 +16985,12 @@
       </c>
     </row>
     <row r="83" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="491"/>
+      <c r="A83" s="512"/>
       <c r="B83" s="47"/>
       <c r="C83" s="198" t="s">
         <v>109</v>
       </c>
-      <c r="D83" s="493"/>
+      <c r="D83" s="514"/>
       <c r="E83" s="103" t="s">
         <v>9</v>
       </c>
@@ -17157,12 +17102,12 @@
       <c r="AO83" s="179"/>
     </row>
     <row r="84" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="491"/>
+      <c r="A84" s="512"/>
       <c r="B84" s="47"/>
       <c r="C84" s="198" t="s">
         <v>43</v>
       </c>
-      <c r="D84" s="493"/>
+      <c r="D84" s="514"/>
       <c r="E84" s="103" t="s">
         <v>18</v>
       </c>
@@ -17276,12 +17221,12 @@
       </c>
     </row>
     <row r="85" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="491"/>
+      <c r="A85" s="512"/>
       <c r="B85" s="47"/>
       <c r="C85" s="198" t="s">
         <v>304</v>
       </c>
-      <c r="D85" s="493"/>
+      <c r="D85" s="514"/>
       <c r="E85" s="111"/>
       <c r="F85" s="34"/>
       <c r="G85" s="34"/>
@@ -17353,12 +17298,12 @@
       <c r="AO85" s="179"/>
     </row>
     <row r="86" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="491"/>
+      <c r="A86" s="512"/>
       <c r="B86" s="253"/>
       <c r="C86" s="254" t="s">
         <v>245</v>
       </c>
-      <c r="D86" s="493"/>
+      <c r="D86" s="514"/>
       <c r="E86" s="31" t="s">
         <v>361</v>
       </c>
@@ -17470,12 +17415,12 @@
       <c r="AO86" s="259"/>
     </row>
     <row r="87" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="491"/>
+      <c r="A87" s="512"/>
       <c r="B87" s="253"/>
       <c r="C87" s="425" t="s">
         <v>504</v>
       </c>
-      <c r="D87" s="493"/>
+      <c r="D87" s="514"/>
       <c r="E87" s="349"/>
       <c r="F87" s="34"/>
       <c r="G87" s="34"/>
@@ -17519,12 +17464,12 @@
       <c r="AO87" s="259"/>
     </row>
     <row r="88" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="491"/>
+      <c r="A88" s="512"/>
       <c r="B88" s="47"/>
       <c r="C88" s="198" t="s">
         <v>350</v>
       </c>
-      <c r="D88" s="493"/>
+      <c r="D88" s="514"/>
       <c r="E88" s="202"/>
       <c r="F88" s="34"/>
       <c r="G88" s="34"/>
@@ -17570,12 +17515,12 @@
       <c r="AO88" s="179"/>
     </row>
     <row r="89" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="491"/>
+      <c r="A89" s="512"/>
       <c r="B89" s="47"/>
       <c r="C89" s="198" t="s">
         <v>239</v>
       </c>
-      <c r="D89" s="493"/>
+      <c r="D89" s="514"/>
       <c r="E89" s="112" t="s">
         <v>18</v>
       </c>
@@ -17687,12 +17632,12 @@
       <c r="AO89" s="179"/>
     </row>
     <row r="90" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="491"/>
+      <c r="A90" s="512"/>
       <c r="B90" s="47"/>
       <c r="C90" s="198" t="s">
         <v>482</v>
       </c>
-      <c r="D90" s="493"/>
+      <c r="D90" s="514"/>
       <c r="E90" s="202"/>
       <c r="F90" s="34"/>
       <c r="G90" s="34"/>
@@ -17733,19 +17678,19 @@
       <c r="AL90" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="AM90" s="414" t="s">
-        <v>18</v>
+      <c r="AM90" s="525" t="s">
+        <v>9</v>
       </c>
       <c r="AN90" s="269"/>
       <c r="AO90" s="179"/>
     </row>
     <row r="91" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="491"/>
+      <c r="A91" s="512"/>
       <c r="B91" s="47"/>
       <c r="C91" s="424" t="s">
         <v>490</v>
       </c>
-      <c r="D91" s="493"/>
+      <c r="D91" s="514"/>
       <c r="E91" s="202"/>
       <c r="F91" s="34"/>
       <c r="G91" s="34"/>
@@ -17791,12 +17736,12 @@
       <c r="AO91" s="179"/>
     </row>
     <row r="92" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="491"/>
+      <c r="A92" s="512"/>
       <c r="B92" s="47"/>
       <c r="C92" s="198" t="s">
         <v>202</v>
       </c>
-      <c r="D92" s="493"/>
+      <c r="D92" s="514"/>
       <c r="E92" s="111"/>
       <c r="F92" s="34"/>
       <c r="G92" s="34"/>
@@ -17880,12 +17825,12 @@
       <c r="AO92" s="179"/>
     </row>
     <row r="93" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="491"/>
+      <c r="A93" s="512"/>
       <c r="B93" s="47"/>
       <c r="C93" s="198" t="s">
         <v>110</v>
       </c>
-      <c r="D93" s="493"/>
+      <c r="D93" s="514"/>
       <c r="E93" s="111"/>
       <c r="F93" s="34"/>
       <c r="G93" s="34"/>
@@ -17965,12 +17910,12 @@
       <c r="AO93" s="179"/>
     </row>
     <row r="94" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="491"/>
+      <c r="A94" s="512"/>
       <c r="B94" s="47"/>
       <c r="C94" s="198" t="s">
         <v>111</v>
       </c>
-      <c r="D94" s="493"/>
+      <c r="D94" s="514"/>
       <c r="E94" s="111"/>
       <c r="F94" s="34"/>
       <c r="G94" s="34"/>
@@ -18046,12 +17991,12 @@
       <c r="AO94" s="179"/>
     </row>
     <row r="95" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="491"/>
+      <c r="A95" s="512"/>
       <c r="B95" s="47"/>
       <c r="C95" s="198" t="s">
         <v>505</v>
       </c>
-      <c r="D95" s="493"/>
+      <c r="D95" s="514"/>
       <c r="E95" s="111"/>
       <c r="F95" s="34"/>
       <c r="G95" s="34"/>
@@ -18122,8 +18067,8 @@
       <c r="AL95" s="413" t="s">
         <v>18</v>
       </c>
-      <c r="AM95" s="414" t="s">
-        <v>9</v>
+      <c r="AM95" s="525" t="s">
+        <v>18</v>
       </c>
       <c r="AN95" s="434" t="s">
         <v>9</v>
@@ -18131,12 +18076,12 @@
       <c r="AO95" s="179"/>
     </row>
     <row r="96" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="491"/>
+      <c r="A96" s="512"/>
       <c r="B96" s="47"/>
       <c r="C96" s="424" t="s">
         <v>506</v>
       </c>
-      <c r="D96" s="493"/>
+      <c r="D96" s="514"/>
       <c r="E96" s="349"/>
       <c r="F96" s="34"/>
       <c r="G96" s="34"/>
@@ -18173,19 +18118,19 @@
       <c r="AL96" s="413" t="s">
         <v>9</v>
       </c>
-      <c r="AM96" s="414" t="s">
-        <v>18</v>
+      <c r="AM96" s="525" t="s">
+        <v>9</v>
       </c>
       <c r="AN96" s="380"/>
       <c r="AO96" s="179"/>
     </row>
     <row r="97" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="491"/>
+      <c r="A97" s="512"/>
       <c r="B97" s="47"/>
       <c r="C97" s="424" t="s">
         <v>507</v>
       </c>
-      <c r="D97" s="493"/>
+      <c r="D97" s="514"/>
       <c r="E97" s="111"/>
       <c r="F97" s="34"/>
       <c r="G97" s="34"/>
@@ -18229,12 +18174,12 @@
       <c r="AO97" s="179"/>
     </row>
     <row r="98" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="491"/>
+      <c r="A98" s="512"/>
       <c r="B98" s="47"/>
       <c r="C98" s="424" t="s">
         <v>508</v>
       </c>
-      <c r="D98" s="493"/>
+      <c r="D98" s="514"/>
       <c r="E98" s="111"/>
       <c r="F98" s="34"/>
       <c r="G98" s="34"/>
@@ -18278,12 +18223,12 @@
       <c r="AO98" s="179"/>
     </row>
     <row r="99" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="491"/>
+      <c r="A99" s="512"/>
       <c r="B99" s="47"/>
       <c r="C99" s="424" t="s">
         <v>509</v>
       </c>
-      <c r="D99" s="493"/>
+      <c r="D99" s="514"/>
       <c r="E99" s="111"/>
       <c r="F99" s="34"/>
       <c r="G99" s="34"/>
@@ -18327,12 +18272,12 @@
       <c r="AO99" s="179"/>
     </row>
     <row r="100" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="491"/>
+      <c r="A100" s="512"/>
       <c r="B100" s="47"/>
       <c r="C100" s="198" t="s">
         <v>451</v>
       </c>
-      <c r="D100" s="493"/>
+      <c r="D100" s="514"/>
       <c r="E100" s="111"/>
       <c r="F100" s="34"/>
       <c r="G100" s="34"/>
@@ -18412,12 +18357,12 @@
       <c r="AO100" s="179"/>
     </row>
     <row r="101" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="491"/>
+      <c r="A101" s="512"/>
       <c r="B101" s="49"/>
       <c r="C101" s="424" t="s">
         <v>510</v>
       </c>
-      <c r="D101" s="493"/>
+      <c r="D101" s="514"/>
       <c r="E101" s="238"/>
       <c r="F101" s="239"/>
       <c r="G101" s="239"/>
@@ -18461,12 +18406,12 @@
       <c r="AO101" s="183"/>
     </row>
     <row r="102" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="491"/>
+      <c r="A102" s="512"/>
       <c r="B102" s="49"/>
       <c r="C102" s="74" t="s">
         <v>351</v>
       </c>
-      <c r="D102" s="493"/>
+      <c r="D102" s="514"/>
       <c r="E102" s="238"/>
       <c r="F102" s="239"/>
       <c r="G102" s="239"/>
@@ -18512,12 +18457,12 @@
       <c r="AO102" s="183"/>
     </row>
     <row r="103" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="491"/>
+      <c r="A103" s="512"/>
       <c r="B103" s="49"/>
       <c r="C103" s="420" t="s">
         <v>511</v>
       </c>
-      <c r="D103" s="493"/>
+      <c r="D103" s="514"/>
       <c r="E103" s="238"/>
       <c r="F103" s="239"/>
       <c r="G103" s="239"/>
@@ -18561,12 +18506,12 @@
       <c r="AO103" s="183"/>
     </row>
     <row r="104" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="491"/>
+      <c r="A104" s="512"/>
       <c r="B104" s="49"/>
       <c r="C104" s="420" t="s">
         <v>512</v>
       </c>
-      <c r="D104" s="493"/>
+      <c r="D104" s="514"/>
       <c r="E104" s="238"/>
       <c r="F104" s="239"/>
       <c r="G104" s="239"/>
@@ -18610,12 +18555,12 @@
       <c r="AO104" s="183"/>
     </row>
     <row r="105" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="491"/>
+      <c r="A105" s="512"/>
       <c r="B105" s="49"/>
       <c r="C105" s="74" t="s">
         <v>288</v>
       </c>
-      <c r="D105" s="493"/>
+      <c r="D105" s="514"/>
       <c r="E105" s="114" t="s">
         <v>243</v>
       </c>
@@ -18727,12 +18672,12 @@
       <c r="AO105" s="183"/>
     </row>
     <row r="106" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="491"/>
+      <c r="A106" s="512"/>
       <c r="B106" s="49"/>
       <c r="C106" s="74" t="s">
         <v>536</v>
       </c>
-      <c r="D106" s="493"/>
+      <c r="D106" s="514"/>
       <c r="E106" s="483"/>
       <c r="F106" s="477"/>
       <c r="G106" s="477"/>
@@ -18774,12 +18719,12 @@
       <c r="AO106" s="183"/>
     </row>
     <row r="107" spans="1:42" s="38" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="491"/>
+      <c r="A107" s="512"/>
       <c r="B107" s="73"/>
       <c r="C107" s="74" t="s">
         <v>229</v>
       </c>
-      <c r="D107" s="493"/>
+      <c r="D107" s="514"/>
       <c r="E107" s="114" t="s">
         <v>230</v>
       </c>
@@ -18894,14 +18839,14 @@
       </c>
     </row>
     <row r="108" spans="1:42" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="491"/>
+      <c r="A108" s="512"/>
       <c r="B108" s="41" t="s">
         <v>45</v>
       </c>
       <c r="C108" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="D108" s="493"/>
+      <c r="D108" s="514"/>
       <c r="E108" s="102"/>
       <c r="F108" s="43"/>
       <c r="G108" s="43"/>
@@ -18999,12 +18944,12 @@
       </c>
     </row>
     <row r="109" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="491"/>
+      <c r="A109" s="512"/>
       <c r="B109" s="48"/>
       <c r="C109" s="39" t="s">
         <v>305</v>
       </c>
-      <c r="D109" s="493"/>
+      <c r="D109" s="514"/>
       <c r="E109" s="109"/>
       <c r="F109" s="40"/>
       <c r="G109" s="40"/>
@@ -19070,12 +19015,12 @@
       <c r="AO109" s="182"/>
     </row>
     <row r="110" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="491"/>
+      <c r="A110" s="512"/>
       <c r="B110" s="47"/>
       <c r="C110" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D110" s="493"/>
+      <c r="D110" s="514"/>
       <c r="E110" s="103"/>
       <c r="F110" s="31"/>
       <c r="G110" s="31"/>
@@ -19171,12 +19116,12 @@
       <c r="AO110" s="179"/>
     </row>
     <row r="111" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="491"/>
+      <c r="A111" s="512"/>
       <c r="B111" s="47"/>
       <c r="C111" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D111" s="493"/>
+      <c r="D111" s="514"/>
       <c r="E111" s="103"/>
       <c r="F111" s="31"/>
       <c r="G111" s="31"/>
@@ -19272,12 +19217,12 @@
       <c r="AO111" s="179"/>
     </row>
     <row r="112" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="491"/>
+      <c r="A112" s="512"/>
       <c r="B112" s="47"/>
       <c r="C112" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D112" s="493"/>
+      <c r="D112" s="514"/>
       <c r="E112" s="103"/>
       <c r="F112" s="31"/>
       <c r="G112" s="31"/>
@@ -19373,12 +19318,12 @@
       <c r="AO112" s="179"/>
     </row>
     <row r="113" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="491"/>
+      <c r="A113" s="512"/>
       <c r="B113" s="47"/>
       <c r="C113" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D113" s="493"/>
+      <c r="D113" s="514"/>
       <c r="E113" s="103"/>
       <c r="F113" s="31"/>
       <c r="G113" s="31"/>
@@ -19479,12 +19424,12 @@
       </c>
     </row>
     <row r="114" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="491"/>
+      <c r="A114" s="512"/>
       <c r="B114" s="47"/>
       <c r="C114" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D114" s="493"/>
+      <c r="D114" s="514"/>
       <c r="E114" s="103"/>
       <c r="F114" s="31"/>
       <c r="G114" s="31"/>
@@ -19583,12 +19528,12 @@
       </c>
     </row>
     <row r="115" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="491"/>
+      <c r="A115" s="512"/>
       <c r="B115" s="47"/>
       <c r="C115" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D115" s="493"/>
+      <c r="D115" s="514"/>
       <c r="E115" s="103"/>
       <c r="F115" s="31"/>
       <c r="G115" s="31"/>
@@ -19689,12 +19634,12 @@
       </c>
     </row>
     <row r="116" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="491"/>
+      <c r="A116" s="512"/>
       <c r="B116" s="47"/>
       <c r="C116" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D116" s="493"/>
+      <c r="D116" s="514"/>
       <c r="E116" s="103"/>
       <c r="F116" s="31"/>
       <c r="G116" s="31"/>
@@ -19792,12 +19737,12 @@
       </c>
     </row>
     <row r="117" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="491"/>
+      <c r="A117" s="512"/>
       <c r="B117" s="47"/>
       <c r="C117" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D117" s="493"/>
+      <c r="D117" s="514"/>
       <c r="E117" s="103"/>
       <c r="F117" s="31"/>
       <c r="G117" s="31"/>
@@ -19895,12 +19840,12 @@
       </c>
     </row>
     <row r="118" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="491"/>
+      <c r="A118" s="512"/>
       <c r="B118" s="47"/>
       <c r="C118" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D118" s="493"/>
+      <c r="D118" s="514"/>
       <c r="E118" s="103"/>
       <c r="F118" s="31"/>
       <c r="G118" s="31"/>
@@ -19998,12 +19943,12 @@
       </c>
     </row>
     <row r="119" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="491"/>
+      <c r="A119" s="512"/>
       <c r="B119" s="47"/>
       <c r="C119" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="D119" s="493"/>
+      <c r="D119" s="514"/>
       <c r="E119" s="103"/>
       <c r="F119" s="31"/>
       <c r="G119" s="31"/>
@@ -20069,12 +20014,12 @@
       <c r="AO119" s="179"/>
     </row>
     <row r="120" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="491"/>
+      <c r="A120" s="512"/>
       <c r="B120" s="47"/>
       <c r="C120" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D120" s="493"/>
+      <c r="D120" s="514"/>
       <c r="E120" s="103"/>
       <c r="F120" s="31"/>
       <c r="G120" s="31"/>
@@ -20148,12 +20093,12 @@
       <c r="AO120" s="179"/>
     </row>
     <row r="121" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="491"/>
+      <c r="A121" s="512"/>
       <c r="B121" s="49"/>
       <c r="C121" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="D121" s="493"/>
+      <c r="D121" s="514"/>
       <c r="E121" s="103"/>
       <c r="F121" s="31"/>
       <c r="G121" s="31"/>
@@ -20213,12 +20158,12 @@
       <c r="AO121" s="179"/>
     </row>
     <row r="122" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="491"/>
+      <c r="A122" s="512"/>
       <c r="B122" s="49"/>
       <c r="C122" s="198" t="s">
         <v>435</v>
       </c>
-      <c r="D122" s="493"/>
+      <c r="D122" s="514"/>
       <c r="E122" s="103"/>
       <c r="F122" s="31"/>
       <c r="G122" s="31"/>
@@ -20284,12 +20229,12 @@
       <c r="AO122" s="179"/>
     </row>
     <row r="123" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="491"/>
+      <c r="A123" s="512"/>
       <c r="B123" s="49"/>
       <c r="C123" s="377" t="s">
         <v>477</v>
       </c>
-      <c r="D123" s="493"/>
+      <c r="D123" s="514"/>
       <c r="E123" s="103"/>
       <c r="F123" s="31"/>
       <c r="G123" s="31"/>
@@ -20335,12 +20280,12 @@
       <c r="AO123" s="179"/>
     </row>
     <row r="124" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="491"/>
+      <c r="A124" s="512"/>
       <c r="B124" s="49"/>
       <c r="C124" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="D124" s="493"/>
+      <c r="D124" s="514"/>
       <c r="E124" s="103"/>
       <c r="F124" s="31"/>
       <c r="G124" s="31"/>
@@ -20436,12 +20381,12 @@
       <c r="AO124" s="179"/>
     </row>
     <row r="125" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="491"/>
+      <c r="A125" s="512"/>
       <c r="B125" s="295"/>
       <c r="C125" s="199" t="s">
         <v>181</v>
       </c>
-      <c r="D125" s="493"/>
+      <c r="D125" s="514"/>
       <c r="E125" s="103"/>
       <c r="F125" s="31"/>
       <c r="G125" s="31"/>
@@ -20537,12 +20482,12 @@
       <c r="AO125" s="179"/>
     </row>
     <row r="126" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="491"/>
+      <c r="A126" s="512"/>
       <c r="B126" s="48"/>
       <c r="C126" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D126" s="493"/>
+      <c r="D126" s="514"/>
       <c r="E126" s="103"/>
       <c r="F126" s="31"/>
       <c r="G126" s="31"/>
@@ -20626,12 +20571,12 @@
       </c>
     </row>
     <row r="127" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="491"/>
+      <c r="A127" s="512"/>
       <c r="B127" s="47"/>
       <c r="C127" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="D127" s="493"/>
+      <c r="D127" s="514"/>
       <c r="E127" s="103"/>
       <c r="F127" s="31"/>
       <c r="G127" s="31"/>
@@ -20727,12 +20672,12 @@
       <c r="AO127" s="185"/>
     </row>
     <row r="128" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="491"/>
+      <c r="A128" s="512"/>
       <c r="B128" s="47"/>
       <c r="C128" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="D128" s="493"/>
+      <c r="D128" s="514"/>
       <c r="E128" s="103"/>
       <c r="F128" s="31"/>
       <c r="G128" s="31"/>
@@ -20828,12 +20773,12 @@
       <c r="AO128" s="179"/>
     </row>
     <row r="129" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="491"/>
+      <c r="A129" s="512"/>
       <c r="B129" s="47"/>
       <c r="C129" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="D129" s="493"/>
+      <c r="D129" s="514"/>
       <c r="E129" s="103"/>
       <c r="F129" s="31"/>
       <c r="G129" s="31"/>
@@ -20929,12 +20874,12 @@
       <c r="AO129" s="179"/>
     </row>
     <row r="130" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="491"/>
+      <c r="A130" s="512"/>
       <c r="B130" s="47"/>
       <c r="C130" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D130" s="493"/>
+      <c r="D130" s="514"/>
       <c r="E130" s="103"/>
       <c r="F130" s="31"/>
       <c r="G130" s="31"/>
@@ -21030,12 +20975,12 @@
       <c r="AO130" s="185"/>
     </row>
     <row r="131" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="491"/>
+      <c r="A131" s="512"/>
       <c r="B131" s="47"/>
       <c r="C131" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="D131" s="493"/>
+      <c r="D131" s="514"/>
       <c r="E131" s="103"/>
       <c r="F131" s="31"/>
       <c r="G131" s="31"/>
@@ -21131,12 +21076,12 @@
       <c r="AO131" s="179"/>
     </row>
     <row r="132" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="491"/>
+      <c r="A132" s="512"/>
       <c r="B132" s="47"/>
       <c r="C132" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="D132" s="493"/>
+      <c r="D132" s="514"/>
       <c r="E132" s="103"/>
       <c r="F132" s="31"/>
       <c r="G132" s="31"/>
@@ -21232,12 +21177,12 @@
       <c r="AO132" s="185"/>
     </row>
     <row r="133" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="491"/>
+      <c r="A133" s="512"/>
       <c r="B133" s="47"/>
       <c r="C133" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="D133" s="493"/>
+      <c r="D133" s="514"/>
       <c r="E133" s="103"/>
       <c r="F133" s="31"/>
       <c r="G133" s="31"/>
@@ -21333,12 +21278,12 @@
       <c r="AO133" s="179"/>
     </row>
     <row r="134" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="491"/>
+      <c r="A134" s="512"/>
       <c r="B134" s="47"/>
       <c r="C134" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="D134" s="493"/>
+      <c r="D134" s="514"/>
       <c r="E134" s="103"/>
       <c r="F134" s="31"/>
       <c r="G134" s="31"/>
@@ -21434,12 +21379,12 @@
       <c r="AO134" s="179"/>
     </row>
     <row r="135" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="491"/>
+      <c r="A135" s="512"/>
       <c r="B135" s="47"/>
       <c r="C135" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D135" s="493"/>
+      <c r="D135" s="514"/>
       <c r="E135" s="103"/>
       <c r="F135" s="31"/>
       <c r="G135" s="31"/>
@@ -21537,12 +21482,12 @@
       </c>
     </row>
     <row r="136" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="491"/>
+      <c r="A136" s="512"/>
       <c r="B136" s="47"/>
       <c r="C136" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D136" s="493"/>
+      <c r="D136" s="514"/>
       <c r="E136" s="103"/>
       <c r="F136" s="31"/>
       <c r="G136" s="31"/>
@@ -21640,12 +21585,12 @@
       </c>
     </row>
     <row r="137" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="491"/>
+      <c r="A137" s="512"/>
       <c r="B137" s="47"/>
       <c r="C137" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D137" s="493"/>
+      <c r="D137" s="514"/>
       <c r="E137" s="103"/>
       <c r="F137" s="31"/>
       <c r="G137" s="31"/>
@@ -21743,12 +21688,12 @@
       </c>
     </row>
     <row r="138" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="491"/>
+      <c r="A138" s="512"/>
       <c r="B138" s="47"/>
       <c r="C138" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D138" s="493"/>
+      <c r="D138" s="514"/>
       <c r="E138" s="103"/>
       <c r="F138" s="31"/>
       <c r="G138" s="31"/>
@@ -21846,12 +21791,12 @@
       </c>
     </row>
     <row r="139" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="491"/>
+      <c r="A139" s="512"/>
       <c r="B139" s="47"/>
       <c r="C139" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D139" s="493"/>
+      <c r="D139" s="514"/>
       <c r="E139" s="103"/>
       <c r="F139" s="31"/>
       <c r="G139" s="31"/>
@@ -21949,12 +21894,12 @@
       </c>
     </row>
     <row r="140" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="491"/>
+      <c r="A140" s="512"/>
       <c r="B140" s="47"/>
       <c r="C140" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D140" s="493"/>
+      <c r="D140" s="514"/>
       <c r="E140" s="103"/>
       <c r="F140" s="31"/>
       <c r="G140" s="31"/>
@@ -22055,12 +22000,12 @@
       </c>
     </row>
     <row r="141" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="491"/>
+      <c r="A141" s="512"/>
       <c r="B141" s="47"/>
       <c r="C141" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D141" s="493"/>
+      <c r="D141" s="514"/>
       <c r="E141" s="103"/>
       <c r="F141" s="31"/>
       <c r="G141" s="31"/>
@@ -22158,12 +22103,12 @@
       </c>
     </row>
     <row r="142" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="491"/>
+      <c r="A142" s="512"/>
       <c r="B142" s="47"/>
       <c r="C142" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D142" s="493"/>
+      <c r="D142" s="514"/>
       <c r="E142" s="103"/>
       <c r="F142" s="31"/>
       <c r="G142" s="31"/>
@@ -22231,12 +22176,12 @@
       <c r="AO142" s="179"/>
     </row>
     <row r="143" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="491"/>
+      <c r="A143" s="512"/>
       <c r="B143" s="47"/>
       <c r="C143" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D143" s="493"/>
+      <c r="D143" s="514"/>
       <c r="E143" s="103"/>
       <c r="F143" s="31"/>
       <c r="G143" s="31"/>
@@ -22304,12 +22249,12 @@
       <c r="AO143" s="179"/>
     </row>
     <row r="144" spans="1:42" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="491"/>
+      <c r="A144" s="512"/>
       <c r="B144" s="47"/>
       <c r="C144" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D144" s="493"/>
+      <c r="D144" s="514"/>
       <c r="E144" s="103"/>
       <c r="F144" s="31"/>
       <c r="G144" s="31"/>
@@ -22377,12 +22322,12 @@
       <c r="AO144" s="179"/>
     </row>
     <row r="145" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="491"/>
+      <c r="A145" s="512"/>
       <c r="B145" s="47"/>
       <c r="C145" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D145" s="493"/>
+      <c r="D145" s="514"/>
       <c r="E145" s="103"/>
       <c r="F145" s="31"/>
       <c r="G145" s="31"/>
@@ -22450,12 +22395,12 @@
       <c r="AO145" s="179"/>
     </row>
     <row r="146" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="491"/>
+      <c r="A146" s="512"/>
       <c r="B146" s="47"/>
       <c r="C146" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D146" s="493"/>
+      <c r="D146" s="514"/>
       <c r="E146" s="103"/>
       <c r="F146" s="31"/>
       <c r="G146" s="31"/>
@@ -22523,12 +22468,12 @@
       <c r="AO146" s="179"/>
     </row>
     <row r="147" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="491"/>
+      <c r="A147" s="512"/>
       <c r="B147" s="47"/>
       <c r="C147" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D147" s="493"/>
+      <c r="D147" s="514"/>
       <c r="E147" s="103"/>
       <c r="F147" s="31"/>
       <c r="G147" s="31"/>
@@ -22596,12 +22541,12 @@
       <c r="AO147" s="179"/>
     </row>
     <row r="148" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="491"/>
+      <c r="A148" s="512"/>
       <c r="B148" s="47"/>
       <c r="C148" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D148" s="493"/>
+      <c r="D148" s="514"/>
       <c r="E148" s="103"/>
       <c r="F148" s="31"/>
       <c r="G148" s="31"/>
@@ -22669,12 +22614,12 @@
       <c r="AO148" s="179"/>
     </row>
     <row r="149" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="491"/>
+      <c r="A149" s="512"/>
       <c r="B149" s="47"/>
       <c r="C149" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D149" s="493"/>
+      <c r="D149" s="514"/>
       <c r="E149" s="103"/>
       <c r="F149" s="31"/>
       <c r="G149" s="31"/>
@@ -22742,12 +22687,12 @@
       <c r="AO149" s="179"/>
     </row>
     <row r="150" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="491"/>
+      <c r="A150" s="512"/>
       <c r="B150" s="47"/>
       <c r="C150" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D150" s="493"/>
+      <c r="D150" s="514"/>
       <c r="E150" s="103"/>
       <c r="F150" s="31"/>
       <c r="G150" s="31"/>
@@ -22815,12 +22760,12 @@
       <c r="AO150" s="179"/>
     </row>
     <row r="151" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="491"/>
+      <c r="A151" s="512"/>
       <c r="B151" s="47"/>
       <c r="C151" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D151" s="493"/>
+      <c r="D151" s="514"/>
       <c r="E151" s="103"/>
       <c r="F151" s="31"/>
       <c r="G151" s="31"/>
@@ -22888,12 +22833,12 @@
       <c r="AO151" s="179"/>
     </row>
     <row r="152" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="491"/>
+      <c r="A152" s="512"/>
       <c r="B152" s="47"/>
       <c r="C152" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D152" s="493"/>
+      <c r="D152" s="514"/>
       <c r="E152" s="103"/>
       <c r="F152" s="31"/>
       <c r="G152" s="31"/>
@@ -22961,12 +22906,12 @@
       <c r="AO152" s="179"/>
     </row>
     <row r="153" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="491"/>
+      <c r="A153" s="512"/>
       <c r="B153" s="47"/>
       <c r="C153" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D153" s="493"/>
+      <c r="D153" s="514"/>
       <c r="E153" s="103"/>
       <c r="F153" s="31"/>
       <c r="G153" s="31"/>
@@ -23046,12 +22991,12 @@
       </c>
     </row>
     <row r="154" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="491"/>
+      <c r="A154" s="512"/>
       <c r="B154" s="47"/>
       <c r="C154" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D154" s="493"/>
+      <c r="D154" s="514"/>
       <c r="E154" s="103"/>
       <c r="F154" s="31"/>
       <c r="G154" s="31"/>
@@ -23149,12 +23094,12 @@
       </c>
     </row>
     <row r="155" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="491"/>
+      <c r="A155" s="512"/>
       <c r="B155" s="47"/>
       <c r="C155" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D155" s="493"/>
+      <c r="D155" s="514"/>
       <c r="E155" s="116"/>
       <c r="F155" s="32"/>
       <c r="G155" s="32"/>
@@ -23194,12 +23139,12 @@
       <c r="AO155" s="179"/>
     </row>
     <row r="156" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="491"/>
+      <c r="A156" s="512"/>
       <c r="B156" s="47"/>
       <c r="C156" s="199" t="s">
         <v>67</v>
       </c>
-      <c r="D156" s="493"/>
+      <c r="D156" s="514"/>
       <c r="E156" s="116"/>
       <c r="F156" s="32"/>
       <c r="G156" s="32"/>
@@ -23297,12 +23242,12 @@
       </c>
     </row>
     <row r="157" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="491"/>
+      <c r="A157" s="512"/>
       <c r="B157" s="47"/>
       <c r="C157" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="D157" s="493"/>
+      <c r="D157" s="514"/>
       <c r="E157" s="116"/>
       <c r="F157" s="32"/>
       <c r="G157" s="32"/>
@@ -23398,12 +23343,12 @@
       <c r="AO157" s="179"/>
     </row>
     <row r="158" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="491"/>
+      <c r="A158" s="512"/>
       <c r="B158" s="47"/>
       <c r="C158" s="422" t="s">
         <v>192</v>
       </c>
-      <c r="D158" s="493"/>
+      <c r="D158" s="514"/>
       <c r="E158" s="116"/>
       <c r="F158" s="32"/>
       <c r="G158" s="32"/>
@@ -23499,12 +23444,12 @@
       <c r="AO158" s="179"/>
     </row>
     <row r="159" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="491"/>
+      <c r="A159" s="512"/>
       <c r="B159" s="47"/>
       <c r="C159" s="422" t="s">
         <v>408</v>
       </c>
-      <c r="D159" s="493"/>
+      <c r="D159" s="514"/>
       <c r="E159" s="116"/>
       <c r="F159" s="32"/>
       <c r="G159" s="32"/>
@@ -23602,12 +23547,12 @@
       </c>
     </row>
     <row r="160" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="491"/>
+      <c r="A160" s="512"/>
       <c r="B160" s="47"/>
       <c r="C160" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="D160" s="493"/>
+      <c r="D160" s="514"/>
       <c r="E160" s="116"/>
       <c r="F160" s="32"/>
       <c r="G160" s="32"/>
@@ -23705,12 +23650,12 @@
       </c>
     </row>
     <row r="161" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="491"/>
+      <c r="A161" s="512"/>
       <c r="B161" s="47"/>
       <c r="C161" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D161" s="493"/>
+      <c r="D161" s="514"/>
       <c r="E161" s="116"/>
       <c r="F161" s="32"/>
       <c r="G161" s="32"/>
@@ -23808,12 +23753,12 @@
       </c>
     </row>
     <row r="162" spans="1:41" s="283" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="491"/>
+      <c r="A162" s="512"/>
       <c r="B162" s="286"/>
       <c r="C162" s="423" t="s">
         <v>183</v>
       </c>
-      <c r="D162" s="493"/>
+      <c r="D162" s="514"/>
       <c r="E162" s="281"/>
       <c r="F162" s="255"/>
       <c r="G162" s="255"/>
@@ -23909,12 +23854,12 @@
       <c r="AO162" s="282"/>
     </row>
     <row r="163" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="491"/>
+      <c r="A163" s="512"/>
       <c r="B163" s="49"/>
       <c r="C163" s="199" t="s">
         <v>66</v>
       </c>
-      <c r="D163" s="493"/>
+      <c r="D163" s="514"/>
       <c r="E163" s="116"/>
       <c r="F163" s="32"/>
       <c r="G163" s="32"/>
@@ -24010,12 +23955,12 @@
       <c r="AO163" s="179"/>
     </row>
     <row r="164" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="491"/>
+      <c r="A164" s="512"/>
       <c r="B164" s="286"/>
       <c r="C164" s="199" t="s">
         <v>73</v>
       </c>
-      <c r="D164" s="493"/>
+      <c r="D164" s="514"/>
       <c r="E164" s="116"/>
       <c r="F164" s="32"/>
       <c r="G164" s="32"/>
@@ -24113,12 +24058,12 @@
       </c>
     </row>
     <row r="165" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="491"/>
+      <c r="A165" s="512"/>
       <c r="B165" s="48"/>
       <c r="C165" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="D165" s="493"/>
+      <c r="D165" s="514"/>
       <c r="E165" s="116"/>
       <c r="F165" s="32"/>
       <c r="G165" s="32"/>
@@ -24216,12 +24161,12 @@
       </c>
     </row>
     <row r="166" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="491"/>
+      <c r="A166" s="512"/>
       <c r="B166" s="47"/>
       <c r="C166" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D166" s="493"/>
+      <c r="D166" s="514"/>
       <c r="E166" s="116"/>
       <c r="F166" s="32"/>
       <c r="G166" s="32"/>
@@ -24317,12 +24262,12 @@
       <c r="AO166" s="179"/>
     </row>
     <row r="167" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="491"/>
+      <c r="A167" s="512"/>
       <c r="B167" s="47"/>
       <c r="C167" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D167" s="493"/>
+      <c r="D167" s="514"/>
       <c r="E167" s="116"/>
       <c r="F167" s="32"/>
       <c r="G167" s="32"/>
@@ -24392,12 +24337,12 @@
       <c r="AO167" s="179"/>
     </row>
     <row r="168" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="491"/>
+      <c r="A168" s="512"/>
       <c r="B168" s="47"/>
       <c r="C168" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D168" s="493"/>
+      <c r="D168" s="514"/>
       <c r="E168" s="116"/>
       <c r="F168" s="32"/>
       <c r="G168" s="32"/>
@@ -24495,12 +24440,12 @@
       </c>
     </row>
     <row r="169" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="491"/>
+      <c r="A169" s="512"/>
       <c r="B169" s="47"/>
       <c r="C169" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D169" s="493"/>
+      <c r="D169" s="514"/>
       <c r="E169" s="116"/>
       <c r="F169" s="32"/>
       <c r="G169" s="32"/>
@@ -24596,12 +24541,12 @@
       <c r="AO169" s="179"/>
     </row>
     <row r="170" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="491"/>
+      <c r="A170" s="512"/>
       <c r="B170" s="49"/>
       <c r="C170" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="D170" s="493"/>
+      <c r="D170" s="514"/>
       <c r="E170" s="417"/>
       <c r="F170" s="359"/>
       <c r="G170" s="359"/>
@@ -24697,12 +24642,12 @@
       <c r="AO170" s="183"/>
     </row>
     <row r="171" spans="1:41" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="491"/>
+      <c r="A171" s="512"/>
       <c r="B171" s="67"/>
       <c r="C171" s="68" t="s">
         <v>226</v>
       </c>
-      <c r="D171" s="493"/>
+      <c r="D171" s="514"/>
       <c r="E171" s="106"/>
       <c r="F171" s="72"/>
       <c r="G171" s="72"/>
@@ -24770,14 +24715,14 @@
       <c r="AO171" s="181"/>
     </row>
     <row r="172" spans="1:41" ht="26.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="491"/>
+      <c r="A172" s="512"/>
       <c r="B172" s="85" t="s">
         <v>75</v>
       </c>
       <c r="C172" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="D172" s="493"/>
+      <c r="D172" s="514"/>
       <c r="E172" s="117"/>
       <c r="F172" s="86"/>
       <c r="G172" s="86"/>
@@ -24875,12 +24820,12 @@
       </c>
     </row>
     <row r="173" spans="1:41" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A173" s="491"/>
+      <c r="A173" s="512"/>
       <c r="B173" s="47"/>
       <c r="C173" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D173" s="493"/>
+      <c r="D173" s="514"/>
       <c r="E173" s="116"/>
       <c r="F173" s="32"/>
       <c r="G173" s="32"/>
@@ -24978,12 +24923,12 @@
       </c>
     </row>
     <row r="174" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="491"/>
+      <c r="A174" s="512"/>
       <c r="B174" s="47"/>
       <c r="C174" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D174" s="493"/>
+      <c r="D174" s="514"/>
       <c r="E174" s="116"/>
       <c r="F174" s="32"/>
       <c r="G174" s="32"/>
@@ -25079,12 +25024,12 @@
       <c r="AO174" s="179"/>
     </row>
     <row r="175" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="491"/>
+      <c r="A175" s="512"/>
       <c r="B175" s="47"/>
       <c r="C175" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D175" s="493"/>
+      <c r="D175" s="514"/>
       <c r="E175" s="116"/>
       <c r="F175" s="32"/>
       <c r="G175" s="32"/>
@@ -25180,12 +25125,12 @@
       <c r="AO175" s="179"/>
     </row>
     <row r="176" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="491"/>
+      <c r="A176" s="512"/>
       <c r="B176" s="47"/>
       <c r="C176" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D176" s="493"/>
+      <c r="D176" s="514"/>
       <c r="E176" s="116"/>
       <c r="F176" s="32"/>
       <c r="G176" s="32"/>
@@ -25281,12 +25226,12 @@
       <c r="AO176" s="179"/>
     </row>
     <row r="177" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="491"/>
+      <c r="A177" s="512"/>
       <c r="B177" s="47"/>
       <c r="C177" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D177" s="493"/>
+      <c r="D177" s="514"/>
       <c r="E177" s="116"/>
       <c r="F177" s="32"/>
       <c r="G177" s="32"/>
@@ -25382,12 +25327,12 @@
       <c r="AO177" s="179"/>
     </row>
     <row r="178" spans="1:41" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A178" s="491"/>
+      <c r="A178" s="512"/>
       <c r="B178" s="47"/>
       <c r="C178" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D178" s="493"/>
+      <c r="D178" s="514"/>
       <c r="E178" s="116"/>
       <c r="F178" s="32"/>
       <c r="G178" s="32"/>
@@ -25485,12 +25430,12 @@
       </c>
     </row>
     <row r="179" spans="1:41" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A179" s="491"/>
+      <c r="A179" s="512"/>
       <c r="B179" s="47"/>
       <c r="C179" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D179" s="493"/>
+      <c r="D179" s="514"/>
       <c r="E179" s="116"/>
       <c r="F179" s="32"/>
       <c r="G179" s="32"/>
@@ -25586,12 +25531,12 @@
       <c r="AO179" s="185"/>
     </row>
     <row r="180" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="491"/>
+      <c r="A180" s="512"/>
       <c r="B180" s="47"/>
       <c r="C180" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D180" s="493"/>
+      <c r="D180" s="514"/>
       <c r="E180" s="116"/>
       <c r="F180" s="32"/>
       <c r="G180" s="32"/>
@@ -25687,12 +25632,12 @@
       <c r="AO180" s="185"/>
     </row>
     <row r="181" spans="1:41" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A181" s="491"/>
+      <c r="A181" s="512"/>
       <c r="B181" s="47"/>
       <c r="C181" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D181" s="493"/>
+      <c r="D181" s="514"/>
       <c r="E181" s="116"/>
       <c r="F181" s="32"/>
       <c r="G181" s="32"/>
@@ -25790,12 +25735,12 @@
       </c>
     </row>
     <row r="182" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A182" s="491"/>
+      <c r="A182" s="512"/>
       <c r="B182" s="47"/>
       <c r="C182" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D182" s="493"/>
+      <c r="D182" s="514"/>
       <c r="E182" s="116"/>
       <c r="F182" s="32"/>
       <c r="G182" s="32"/>
@@ -25893,12 +25838,12 @@
       </c>
     </row>
     <row r="183" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="491"/>
+      <c r="A183" s="512"/>
       <c r="B183" s="47"/>
       <c r="C183" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D183" s="493"/>
+      <c r="D183" s="514"/>
       <c r="E183" s="116"/>
       <c r="F183" s="32"/>
       <c r="G183" s="32"/>
@@ -25994,12 +25939,12 @@
       <c r="AO183" s="179"/>
     </row>
     <row r="184" spans="1:41" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A184" s="491"/>
+      <c r="A184" s="512"/>
       <c r="B184" s="47"/>
       <c r="C184" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D184" s="493"/>
+      <c r="D184" s="514"/>
       <c r="E184" s="116"/>
       <c r="F184" s="32"/>
       <c r="G184" s="32"/>
@@ -26097,12 +26042,12 @@
       </c>
     </row>
     <row r="185" spans="1:41" ht="51" x14ac:dyDescent="0.25">
-      <c r="A185" s="491"/>
+      <c r="A185" s="512"/>
       <c r="B185" s="47"/>
       <c r="C185" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D185" s="493"/>
+      <c r="D185" s="514"/>
       <c r="E185" s="116"/>
       <c r="F185" s="32"/>
       <c r="G185" s="32"/>
@@ -26198,12 +26143,12 @@
       <c r="AO185" s="179"/>
     </row>
     <row r="186" spans="1:41" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="491"/>
+      <c r="A186" s="512"/>
       <c r="B186" s="67"/>
       <c r="C186" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="D186" s="493"/>
+      <c r="D186" s="514"/>
       <c r="E186" s="106"/>
       <c r="F186" s="72"/>
       <c r="G186" s="72"/>
@@ -26281,14 +26226,14 @@
       <c r="AO186" s="181"/>
     </row>
     <row r="187" spans="1:41" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="491"/>
+      <c r="A187" s="512"/>
       <c r="B187" s="55" t="s">
         <v>135</v>
       </c>
       <c r="C187" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="D187" s="493"/>
+      <c r="D187" s="514"/>
       <c r="E187" s="118"/>
       <c r="F187" s="57"/>
       <c r="G187" s="57"/>
@@ -26384,12 +26329,12 @@
       <c r="AO187" s="186"/>
     </row>
     <row r="188" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="491"/>
+      <c r="A188" s="512"/>
       <c r="B188" s="59"/>
       <c r="C188" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D188" s="493"/>
+      <c r="D188" s="514"/>
       <c r="E188" s="119"/>
       <c r="F188" s="33"/>
       <c r="G188" s="33"/>
@@ -26485,12 +26430,12 @@
       <c r="AO188" s="187"/>
     </row>
     <row r="189" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="491"/>
+      <c r="A189" s="512"/>
       <c r="B189" s="59"/>
       <c r="C189" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D189" s="493"/>
+      <c r="D189" s="514"/>
       <c r="E189" s="119"/>
       <c r="F189" s="33"/>
       <c r="G189" s="33"/>
@@ -26588,12 +26533,12 @@
       </c>
     </row>
     <row r="190" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="491"/>
+      <c r="A190" s="512"/>
       <c r="B190" s="59"/>
       <c r="C190" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D190" s="493"/>
+      <c r="D190" s="514"/>
       <c r="E190" s="119"/>
       <c r="F190" s="33"/>
       <c r="G190" s="33"/>
@@ -26689,12 +26634,12 @@
       <c r="AO190" s="187"/>
     </row>
     <row r="191" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="491"/>
+      <c r="A191" s="512"/>
       <c r="B191" s="59"/>
       <c r="C191" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D191" s="493"/>
+      <c r="D191" s="514"/>
       <c r="E191" s="119"/>
       <c r="F191" s="33"/>
       <c r="G191" s="33"/>
@@ -26790,12 +26735,12 @@
       <c r="AO191" s="187"/>
     </row>
     <row r="192" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="491"/>
+      <c r="A192" s="512"/>
       <c r="B192" s="59"/>
       <c r="C192" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D192" s="493"/>
+      <c r="D192" s="514"/>
       <c r="E192" s="119"/>
       <c r="F192" s="33"/>
       <c r="G192" s="33"/>
@@ -26893,12 +26838,12 @@
       </c>
     </row>
     <row r="193" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="491"/>
+      <c r="A193" s="512"/>
       <c r="B193" s="59"/>
       <c r="C193" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D193" s="493"/>
+      <c r="D193" s="514"/>
       <c r="E193" s="119"/>
       <c r="F193" s="33"/>
       <c r="G193" s="33"/>
@@ -26994,12 +26939,12 @@
       <c r="AO193" s="187"/>
     </row>
     <row r="194" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="491"/>
+      <c r="A194" s="512"/>
       <c r="B194" s="59"/>
       <c r="C194" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D194" s="493"/>
+      <c r="D194" s="514"/>
       <c r="E194" s="119"/>
       <c r="F194" s="33"/>
       <c r="G194" s="33"/>
@@ -27095,12 +27040,12 @@
       <c r="AO194" s="187"/>
     </row>
     <row r="195" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="491"/>
+      <c r="A195" s="512"/>
       <c r="B195" s="59"/>
       <c r="C195" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D195" s="493"/>
+      <c r="D195" s="514"/>
       <c r="E195" s="119"/>
       <c r="F195" s="33"/>
       <c r="G195" s="33"/>
@@ -27196,12 +27141,12 @@
       <c r="AO195" s="187"/>
     </row>
     <row r="196" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="491"/>
+      <c r="A196" s="512"/>
       <c r="B196" s="59"/>
       <c r="C196" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="D196" s="493"/>
+      <c r="D196" s="514"/>
       <c r="E196" s="119"/>
       <c r="F196" s="33"/>
       <c r="G196" s="33"/>
@@ -27299,12 +27244,12 @@
       </c>
     </row>
     <row r="197" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A197" s="491"/>
+      <c r="A197" s="512"/>
       <c r="B197" s="59"/>
       <c r="C197" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D197" s="493"/>
+      <c r="D197" s="514"/>
       <c r="E197" s="119"/>
       <c r="F197" s="33"/>
       <c r="G197" s="33"/>
@@ -27400,12 +27345,12 @@
       <c r="AO197" s="187"/>
     </row>
     <row r="198" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="491"/>
+      <c r="A198" s="512"/>
       <c r="B198" s="59"/>
       <c r="C198" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="D198" s="493"/>
+      <c r="D198" s="514"/>
       <c r="E198" s="119"/>
       <c r="F198" s="33"/>
       <c r="G198" s="33"/>
@@ -27501,12 +27446,12 @@
       <c r="AO198" s="187"/>
     </row>
     <row r="199" spans="1:41" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="491"/>
+      <c r="A199" s="512"/>
       <c r="B199" s="60"/>
       <c r="C199" s="61" t="s">
         <v>150</v>
       </c>
-      <c r="D199" s="494"/>
+      <c r="D199" s="515"/>
       <c r="E199" s="120"/>
       <c r="F199" s="62"/>
       <c r="G199" s="62"/>
@@ -27605,6 +27550,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="A27:A199"/>
+    <mergeCell ref="D27:D199"/>
+    <mergeCell ref="E5:L26"/>
+    <mergeCell ref="M5:AM26"/>
+    <mergeCell ref="A5:A26"/>
     <mergeCell ref="AO3:AO4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="T3:V3"/>
@@ -27614,12 +27565,6 @@
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="AL4:AM4"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="A27:A199"/>
-    <mergeCell ref="D27:D199"/>
-    <mergeCell ref="E5:L26"/>
-    <mergeCell ref="M5:AM26"/>
-    <mergeCell ref="A5:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#143 Change PCH-S CSME 4.8 SMT configure from x3 to x6 to be same as ADP-S. It was typo error.
[git-p4: depot-paths = "//depot/projects/coe/CSME/": change = 789314]
</commit_message>
<xml_diff>
--- a/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
+++ b/ArchSpecs/Working/CSME IE OCS Hardware Architecture Features Per Project.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0A61DF-FD65-4C3E-AA57-CC78AC5186EB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD571F08-6993-48DB-B447-8170568A289D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="19788" windowHeight="10524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="2" r:id="rId1"/>
@@ -948,6 +948,28 @@
         </r>
       </text>
     </comment>
+    <comment ref="AS33" authorId="0" shapeId="0" xr:uid="{7829B00B-EFCE-4F1B-87D9-6367C7EF217E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+assume LMT3D8 (MTL GEN) for PCH can give enough margin to meeting 400MHz w/ 1.25x PV. In SOC TSMC process, Min PV Freq 500MHz/435MHz, taget PV Freq is 800Mhz/580MHz </t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AT33" authorId="0" shapeId="0" xr:uid="{E7562668-8C2B-47EB-B60F-D5321558C2D4}">
       <text>
         <r>
@@ -10487,7 +10509,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5760" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5762" uniqueCount="654">
   <si>
     <t>CNP-LP</t>
   </si>
@@ -12875,6 +12897,9 @@
   <si>
     <t>add additional note for the reasoning of having 0.75KB buffer for "HW Save &amp; Restore AON Memory" on PCH CSME vs ADP-S was No</t>
   </si>
+  <si>
+    <t>Change PCH-S CSME 4.8 SMT configure from x3 to x6 to be same as ADP-S. It was typo error.</t>
+  </si>
 </sst>
 </file>
 
@@ -12884,7 +12909,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13076,6 +13101,17 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="18">
@@ -16550,13 +16586,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:E155"/>
+  <dimension ref="B2:E156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B153" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B154" sqref="B154"/>
+      <selection pane="bottomRight" activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18710,10 +18746,24 @@
       </c>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B155" s="171"/>
-      <c r="C155" s="9"/>
-      <c r="D155" s="10"/>
-      <c r="E155" s="4"/>
+      <c r="B155" s="171">
+        <v>143</v>
+      </c>
+      <c r="C155" s="9">
+        <v>44022</v>
+      </c>
+      <c r="D155" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="E155" s="4" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B156" s="171"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="10"/>
+      <c r="E156" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18727,11 +18777,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:MA205"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="AP164" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="AH191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AS171" sqref="AS171"/>
+      <selection pane="bottomRight" activeCell="AS193" sqref="AS193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -39537,7 +39587,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="189" spans="1:50" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:50" ht="69" x14ac:dyDescent="0.3">
       <c r="A189" s="622"/>
       <c r="B189" s="47"/>
       <c r="C189" s="3" t="s">
@@ -40137,7 +40187,7 @@
       <c r="AQ193" s="439"/>
       <c r="AR193" s="460"/>
       <c r="AS193" s="115" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AT193" s="341" t="s">
         <v>18</v>

</xml_diff>